<commit_message>
- geckodriver 0.20.1 - implemented "delayed" logging strategy (LogbackUtils)   - when nexial first started, all file-based logs are pointing to ${java.io.tmpdir}   - when the "out" directory is determined, file-based logs are redirected to ${out}/logs directory - implemented performance improvement on reading Excel files   - delete "temp" Excel files ONLY if they were "dup-then-open"   - implemented functional calls to eliminate excessive worksheet reads - base.verbose()   - reduce console log for base.verbose() command (not necessary)   - add original script param as comment when generating result of a base.verbose() call
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2904" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="417">
   <si>
     <t>description</t>
   </si>
@@ -1316,7 +1316,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="80">
+  <fonts count="104">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1821,8 +1821,160 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="129">
+  <fills count="171">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2549,8 +2701,246 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="122">
+  <borders count="162">
     <border>
       <left/>
       <right/>
@@ -3737,13 +4127,401 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="115">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3986,40 +4764,112 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="67" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="110" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="109" fillId="110" fontId="68" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="69" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="113" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="113" fontId="70" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="71" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="116" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="116" fontId="72" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="119" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="117" fillId="119" fontId="73" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="122" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="122" fontId="74" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="122" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="122" fontId="75" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="76" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="128" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="128" fontId="77" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="78" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="79" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="131" fontId="80" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="81" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="82" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="83" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="133" fillId="137" fontId="84" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="137" fillId="140" fontId="85" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="143" fontId="86" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="143" fontId="87" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="146" fontId="88" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="149" fontId="89" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="146" fontId="90" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="91" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="152" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="155" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="158" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="161" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="164" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="164" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="167" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="170" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="167" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
- [base &raquo; `section(steps)`](../commands/base/section(steps)): fixed logic so that we can properly 'skipped' any   enclosed [base &raquo; `repeatUntil(steps,maxWaitMs)`](../commands/base/repeatUntil(steps,maxWaitMs)) steps when   the section command is 'skipped'.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A679D9-665F-704F-AFE9-51A4E898E88D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF040F0C-62D2-0044-B062-3E15E493F8D7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-10580" windowWidth="38400" windowHeight="10580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="440" windowWidth="38400" windowHeight="10580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="450">
   <si>
     <t>description</t>
   </si>
@@ -1358,6 +1358,64 @@
   </si>
   <si>
     <t>ProceedIf (2 between [1|5])</t>
+  </si>
+  <si>
+    <t>macro-with-repeat</t>
+  </si>
+  <si>
+    <t>step 2: loop start</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>step 3: check for loop exit</t>
+  </si>
+  <si>
+    <t>step 4: in-loop task</t>
+  </si>
+  <si>
+    <t>step 5: increment loop control</t>
+  </si>
+  <si>
+    <t>step 6: out of loop now / checking</t>
+  </si>
+  <si>
+    <t>step 7: last statement</t>
+  </si>
+  <si>
+    <t>step 1: setup for loop</t>
+  </si>
+  <si>
+    <t>${counter}</t>
+  </si>
+  <si>
+    <t>This is line 6.  We should all done now.. $(sysdate|now|MM/dd/yyyy HH:mm:ss)</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/in-macro.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$(sysdate|now|yyyy-MM-dd HH:mm:ss) - the counter is now ${counter}
+</t>
+  </si>
+  <si>
+    <t>SkipIf(${counter} &gt; 2)</t>
   </si>
 </sst>
 </file>
@@ -3340,7 +3398,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3349,8 +3407,9 @@
     <col min="2" max="2" width="47.83203125" style="8" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.83203125" style="12" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="42.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.83203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="18.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="40.83203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="68.5" style="9" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="18.33203125" style="9" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="28.6640625" style="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="10" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" style="14" customWidth="1" collapsed="1"/>
@@ -3581,12 +3640,24 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="A10" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>437</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -3596,11 +3667,21 @@
     </row>
     <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>434</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -3610,11 +3691,21 @@
     </row>
     <row r="12" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="B12" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>436</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -3622,27 +3713,51 @@
       <c r="K12" s="2"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>446</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="15" t="s">
+        <v>449</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>437</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -3652,11 +3767,21 @@
     </row>
     <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="B15" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>433</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -3666,10 +3791,18 @@
     </row>
     <row r="16" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>445</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>

</xml_diff>

<commit_message>
[web command] - [`saveTableAsCsv(locator,nextPageLocator,file)`](../commands/web/saveTableAsCsv(locator,nextPageLocator,file)):   **NEW** command to automate the collection of HTML table data into a CSV file. - added firefox-specific fix for selecting option from a <SELECT> element. Only tested on single-option <SELECT> for now. - [`assertTable(locator,row,column,text)`](../commands/web/assertTable(locator,row,column,text)): fixed internal   locator to find cell data with more coverage. - [`savePageAsFile(sessionId,url,file)`](../commands/web/savePageAsFile(sessionId,url,file)): shorten parameter   `fileName` to just `file`.
[genera]
- DataVariableUpdater: remove dead code and typos
- DataVariableUpdater: fixed wrong verbiage for option -p
- DataVariableUpdater: minor refactoring
- TestScriptUpdater: minor fixes to program output to improve clarity

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10806"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{55B3D360-E400-DE46-A8B0-10A78870F93C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CF388224-2B55-8B4C-8431-C0020A5D6873}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="10580" windowWidth="25600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-21160"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="10580" windowWidth="25600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -37,27 +37,22 @@
     <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
     <definedName name="rdbms">'#system'!$O$2:$O$7</definedName>
     <definedName name="redis">'#system'!$P$2:$P$10</definedName>
+    <definedName name="sms">'#system'!$Q$2:$Q$2</definedName>
     <definedName name="sound">'#system'!$R$2:$R$5</definedName>
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$108</definedName>
+    <definedName name="web">'#system'!$U$2:$U$111</definedName>
     <definedName name="webalert">'#system'!$V$2:$V$6</definedName>
     <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
     <definedName name="ws">'#system'!$X$2:$X$16</definedName>
+    <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="xml">'#system'!$Z$2:$Z$11</definedName>
-    <definedName name="sms">'#system'!$Q$2:$Q$2</definedName>
-    <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -67,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3177" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="475">
   <si>
     <t>description</t>
   </si>
@@ -492,9 +487,6 @@
     <t>saveLocation(var)</t>
   </si>
   <si>
-    <t>savePageAsFile(sessionIdName,url,fileName)</t>
-  </si>
-  <si>
     <t>scrollLeft(locator,pixel)</t>
   </si>
   <si>
@@ -1303,9 +1295,6 @@
   </si>
   <si>
     <t>saveTableRowsRange(var,beginRow,endRow)</t>
-  </si>
-  <si>
-    <t>assertBetween(num,min,max)</t>
   </si>
   <si>
     <t>clear(vars)</t>
@@ -1480,34 +1469,25 @@
     <t>assertEqual(num1,num2)</t>
   </si>
   <si>
-    <t>average(variableName,array)</t>
-  </si>
-  <si>
-    <t>ceiling(variableName)</t>
-  </si>
-  <si>
-    <t>decrement(variableName,amount)</t>
-  </si>
-  <si>
-    <t>floor(variableName)</t>
-  </si>
-  <si>
-    <t>increment(variableName,amount)</t>
-  </si>
-  <si>
-    <t>max(variableName,array)</t>
-  </si>
-  <si>
-    <t>min(variableName,array)</t>
-  </si>
-  <si>
-    <t>round(variableName,closestDigit)</t>
-  </si>
-  <si>
     <t>delete(url,body,output)</t>
   </si>
   <si>
     <t>decrement(var,amount)</t>
+  </si>
+  <si>
+    <t>assertTextMatches(text,minMatch,scrollTo)</t>
+  </si>
+  <si>
+    <t>jsSelect(locator,text)</t>
+  </si>
+  <si>
+    <t>savePageAsFile(sessionIdName,url,file)</t>
+  </si>
+  <si>
+    <t>saveTableAsCsv(locator,file)</t>
+  </si>
+  <si>
+    <t>saveTableAsCsv(locator,nextPageLocator,file)</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1495,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="98" x14ac:knownFonts="1">
+  <fonts count="53" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1851,290 +1831,8 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="823C3C"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="823C3C"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="823C3C"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="165">
+  <fills count="84">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2606,467 +2304,8 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6D7D7"/>
-        <bgColor rgb="E6D7D7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="170">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -3935,859 +3174,13 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin">
-        <color rgb="BEC8CD"/>
-      </right>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDC3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin">
-        <color rgb="BEC8CD"/>
-      </right>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDC3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="BEC8CD"/>
-      </left>
-      <right style="thin">
-        <color rgb="BEC8CD"/>
-      </right>
-      <top style="thin">
-        <color rgb="BEC8CD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="BEC8CD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDC3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDC3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDC3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDC3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="64">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4940,184 +3333,49 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="65" fillId="59" fontId="38" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="38" fillId="59" borderId="65" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="69" fillId="62" fontId="40" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="40" fillId="62" borderId="69" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="65" fontId="41" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="41" fillId="65" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="43" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="43" fillId="68" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="44" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="71" fontId="45" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="45" fillId="71" borderId="77" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="81" fillId="74" fontId="46" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="46" fillId="74" borderId="81" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="77" fontId="47" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="47" fillId="77" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="77" fontId="48" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="48" fillId="77" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="49" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="49" fillId="80" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="50" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="50" fillId="83" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="51" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="51" fillId="80" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="52" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="93" fillId="86" fontId="53" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="54" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="97" fillId="89" fontId="55" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="101" fillId="92" fontId="56" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="57" numFmtId="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="58" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="59" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="105" fillId="98" fontId="60" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="109" fillId="101" fontId="61" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="104" fontId="62" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="104" fontId="63" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="64" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="65" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="66" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="67" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="113" fontId="68" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="69" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="125" fillId="116" fontId="70" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="119" fontId="71" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="72" numFmtId="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="73" numFmtId="0" xfId="0">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="74" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="133" fillId="125" fontId="75" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="137" fillId="128" fontId="76" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="131" fontId="77" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="131" fontId="78" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="79" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="137" fontId="80" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="81" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="82" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="140" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="143" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="146" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="149" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="152" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="155" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="164" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5415,7 +3673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA108"/>
+  <dimension ref="A1:AA111"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -5429,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -5447,43 +3705,43 @@
         <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K1" t="s">
         <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M1" t="s">
         <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O1" t="s">
         <v>45</v>
       </c>
       <c r="P1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="S1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="T1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="U1" t="s">
         <v>46</v>
@@ -5498,18 +3756,18 @@
         <v>49</v>
       </c>
       <c r="Y1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="Z1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" t="s">
         <v>373</v>
-      </c>
-      <c r="B2" t="s">
-        <v>374</v>
       </c>
       <c r="C2" t="s">
         <v>50</v>
@@ -5527,61 +3785,61 @@
         <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="M2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="R2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="S2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="U2" t="s">
         <v>89</v>
       </c>
       <c r="V2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="W2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Y2" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="Z2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
@@ -5589,73 +3847,73 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E3" t="s">
         <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K3" t="s">
         <v>78</v>
       </c>
       <c r="M3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="N3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="R3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="S3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="U3" t="s">
         <v>90</v>
       </c>
       <c r="V3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Y3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Z3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4">
@@ -5663,7 +3921,7 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -5672,19 +3930,19 @@
         <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -5693,40 +3951,40 @@
         <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R4" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="S4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="U4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="V4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="W4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="X4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Y4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="Z4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5">
@@ -5734,19 +3992,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I5" t="s">
         <v>64</v>
@@ -5758,37 +4016,37 @@
         <v>23</v>
       </c>
       <c r="N5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="S5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="U5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="V5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="X5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Y5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Z5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6">
@@ -5796,16 +4054,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
@@ -5817,34 +4075,34 @@
         <v>24</v>
       </c>
       <c r="N6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="P6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="S6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="U6" t="s">
         <v>91</v>
       </c>
       <c r="V6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="Z6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7">
@@ -5852,16 +4110,16 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I7" t="s">
         <v>72</v>
@@ -5873,48 +4131,48 @@
         <v>26</v>
       </c>
       <c r="N7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="P7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="U7" t="s">
         <v>92</v>
       </c>
       <c r="W7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Y7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="Z7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I8" t="s">
         <v>31</v>
@@ -5926,28 +4184,28 @@
         <v>83</v>
       </c>
       <c r="N8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="S8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U8" t="s">
         <v>93</v>
       </c>
       <c r="W8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="Z8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9">
@@ -5955,16 +4213,16 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K9" t="s">
         <v>29</v>
@@ -5973,33 +4231,33 @@
         <v>84</v>
       </c>
       <c r="N9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="S9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="U9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -6008,22 +4266,22 @@
         <v>32</v>
       </c>
       <c r="M10" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="N10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="U10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11">
@@ -6031,10 +4289,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I11" t="s">
         <v>35</v>
@@ -6046,27 +4304,27 @@
         <v>85</v>
       </c>
       <c r="N11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U11" t="s">
+        <v>259</v>
+      </c>
+      <c r="X11" t="s">
         <v>260</v>
       </c>
-      <c r="X11" t="s">
-        <v>261</v>
-      </c>
       <c r="Z11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I12" t="s">
         <v>73</v>
@@ -6078,13 +4336,13 @@
         <v>34</v>
       </c>
       <c r="N12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U12" t="s">
         <v>94</v>
       </c>
       <c r="X12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13">
@@ -6095,7 +4353,7 @@
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I13" t="s">
         <v>74</v>
@@ -6104,24 +4362,24 @@
         <v>86</v>
       </c>
       <c r="N13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="X13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I14" t="s">
         <v>75</v>
@@ -6130,13 +4388,13 @@
         <v>87</v>
       </c>
       <c r="N14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U14" t="s">
         <v>95</v>
       </c>
       <c r="X14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15">
@@ -6144,10 +4402,10 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I15" t="s">
         <v>76</v>
@@ -6156,41 +4414,41 @@
         <v>88</v>
       </c>
       <c r="N15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U15" t="s">
         <v>96</v>
       </c>
       <c r="X15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C16" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U16" t="s">
         <v>67</v>
       </c>
       <c r="X16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
@@ -6207,7 +4465,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
@@ -6216,7 +4474,7 @@
         <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="U18" t="s">
         <v>98</v>
@@ -6224,13 +4482,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I19" t="s">
         <v>77</v>
@@ -6241,13 +4499,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I20" t="s">
         <v>38</v>
@@ -6264,7 +4522,7 @@
         <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I21" t="s">
         <v>39</v>
@@ -6278,10 +4536,10 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U22" t="s">
         <v>102</v>
@@ -6292,10 +4550,10 @@
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U23" t="s">
         <v>103</v>
@@ -6306,10 +4564,10 @@
         <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="U24" t="s">
         <v>104</v>
@@ -6317,7 +4575,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
@@ -6331,13 +4589,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U26" t="s">
         <v>106</v>
@@ -6348,10 +4606,10 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28">
@@ -6359,7 +4617,7 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U28" t="s">
         <v>107</v>
@@ -6370,7 +4628,7 @@
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U29" t="s">
         <v>108</v>
@@ -6381,7 +4639,7 @@
         <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U30" t="s">
         <v>109</v>
@@ -6392,7 +4650,7 @@
         <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="U31" t="s">
         <v>110</v>
@@ -6403,7 +4661,7 @@
         <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U32" t="s">
         <v>111</v>
@@ -6411,7 +4669,7 @@
     </row>
     <row r="33">
       <c r="E33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U33" t="s">
         <v>112</v>
@@ -6419,15 +4677,15 @@
     </row>
     <row r="34">
       <c r="E34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35">
       <c r="E35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U35" t="s">
         <v>113</v>
@@ -6435,26 +4693,26 @@
     </row>
     <row r="36">
       <c r="E36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="37">
       <c r="E37" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U37" t="s">
-        <v>395</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38">
       <c r="E38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U38" t="s">
-        <v>114</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39">
@@ -6462,511 +4720,526 @@
         <v>70</v>
       </c>
       <c r="U39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40">
       <c r="E40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41">
       <c r="E41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42">
       <c r="E42" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43">
       <c r="E43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44">
       <c r="E44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U44" t="s">
-        <v>206</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45">
       <c r="E45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U45" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46">
       <c r="E46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U46" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
       <c r="E47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="U47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48">
       <c r="E48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="U48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49">
       <c r="E49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="U49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50">
       <c r="E50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="U50" t="s">
-        <v>348</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51">
       <c r="E51" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="U51" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
     </row>
     <row r="52">
       <c r="E52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53">
       <c r="E53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54">
       <c r="E54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="U54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55">
       <c r="E55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="U55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56">
       <c r="E56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="U56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57">
       <c r="E57" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58">
       <c r="E58" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U58" t="s">
-        <v>207</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59">
       <c r="E59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="U59" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60">
       <c r="E60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U60" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61">
       <c r="E61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62">
       <c r="E62" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63">
       <c r="E63" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U63" t="s">
-        <v>134</v>
+        <v>471</v>
       </c>
     </row>
     <row r="64">
       <c r="E64" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="U64" t="s">
-        <v>190</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65">
       <c r="E65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U65" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66">
       <c r="E66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U66" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67">
       <c r="E67" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="U67" t="s">
-        <v>136</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68">
       <c r="E68" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69">
       <c r="E69" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="U69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70">
       <c r="E70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71">
       <c r="E71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="U71" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72">
       <c r="E72" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U72" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73">
       <c r="E73" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="U73" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74">
       <c r="E74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="U74" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75">
       <c r="E75" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U75" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76">
       <c r="E76" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="U76" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77">
       <c r="E77" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="U77" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78">
       <c r="E78" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79">
       <c r="E79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U79" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80">
       <c r="E80" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U80" t="s">
-        <v>198</v>
+        <v>472</v>
       </c>
     </row>
     <row r="81">
       <c r="E81" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="U81" t="s">
-        <v>199</v>
+        <v>474</v>
       </c>
     </row>
     <row r="82">
       <c r="E82" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="U82" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83">
       <c r="E83" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="U83" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84">
       <c r="E84" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="U84" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85">
       <c r="E85" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U85" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86">
       <c r="E86" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U86" t="s">
-        <v>385</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87">
       <c r="E87" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U87" t="s">
-        <v>143</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88">
       <c r="E88" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U88" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89">
       <c r="E89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="U89" t="s">
-        <v>145</v>
+        <v>384</v>
       </c>
     </row>
     <row r="90">
       <c r="E90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="U90" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91">
       <c r="E91" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U91" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92">
       <c r="E92" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="U92" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93">
       <c r="U93" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94">
       <c r="U94" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95">
       <c r="U95" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96">
       <c r="U96" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97">
       <c r="U97" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98">
       <c r="U98" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99">
       <c r="U99" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100">
       <c r="U100" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101">
       <c r="U101" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102">
       <c r="U102" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103">
       <c r="U103" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104">
       <c r="U104" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
     </row>
     <row r="105">
       <c r="U105" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="106">
       <c r="U106" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="107">
       <c r="U107" t="s">
-        <v>162</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108">
       <c r="U108" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="U109" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="U110" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="U111" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -6980,7 +5253,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A7" ySplit="1"/>
-      <selection activeCell="B22" pane="bottomLeft" sqref="B22"/>
+      <selection activeCell="D15" pane="bottomLeft" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7000,13 +5273,13 @@
   <sheetData>
     <row customFormat="1" customHeight="1" ht="20" r="1" s="5" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>2</v>
@@ -7036,10 +5309,10 @@
     </row>
     <row customHeight="1" ht="18" r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>9</v>
@@ -7048,7 +5321,7 @@
         <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -7060,10 +5333,10 @@
     </row>
     <row customHeight="1" ht="19" r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>9</v>
@@ -7072,7 +5345,7 @@
         <v>62</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -7085,7 +5358,7 @@
     <row customHeight="1" ht="19" r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>9</v>
@@ -7094,7 +5367,7 @@
         <v>62</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -7110,7 +5383,7 @@
     <row customHeight="1" ht="19" r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -7119,7 +5392,7 @@
         <v>62</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -7132,7 +5405,7 @@
     <row customHeight="1" ht="19" r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>9</v>
@@ -7141,7 +5414,7 @@
         <v>62</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -7161,20 +5434,20 @@
         <v>61</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>425</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>427</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="13"/>
@@ -7186,10 +5459,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -7201,7 +5474,7 @@
     </row>
     <row customHeight="1" ht="19" r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="11" t="s">
@@ -7211,7 +5484,7 @@
         <v>62</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -7223,10 +5496,10 @@
     </row>
     <row customHeight="1" ht="19" r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -7235,10 +5508,10 @@
         <v>55</v>
       </c>
       <c r="E10" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -7250,19 +5523,19 @@
     <row customHeight="1" ht="19" r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -7274,7 +5547,7 @@
     <row customHeight="1" ht="19" r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>44</v>
@@ -7283,10 +5556,10 @@
         <v>19</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -7298,7 +5571,7 @@
     <row customHeight="1" ht="36" r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>10</v>
@@ -7307,18 +5580,18 @@
         <v>77</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="13"/>
@@ -7326,7 +5599,7 @@
     <row customHeight="1" ht="19" r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>44</v>
@@ -7335,10 +5608,10 @@
         <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -7350,19 +5623,19 @@
     <row customHeight="1" ht="19" r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>318</v>
+        <v>467</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -7374,7 +5647,7 @@
     <row customHeight="1" ht="19" r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>9</v>
@@ -7383,7 +5656,7 @@
         <v>62</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -7396,19 +5669,19 @@
     <row customHeight="1" ht="19" r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -7420,7 +5693,7 @@
     <row customHeight="1" ht="19" r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>44</v>
@@ -7429,10 +5702,10 @@
         <v>23</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -7444,7 +5717,7 @@
     <row customHeight="1" ht="19" r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>9</v>
@@ -7453,7 +5726,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -7466,7 +5739,7 @@
     <row customHeight="1" ht="19" r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>44</v>
@@ -7475,10 +5748,10 @@
         <v>34</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -7490,7 +5763,7 @@
     <row customHeight="1" ht="19" r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>9</v>
@@ -7499,7 +5772,7 @@
         <v>62</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>

</xml_diff>

<commit_message>
- `dragAndDrop(fromLocator,toLocator)`: **NEW** command to support drag-and-drop automation from one element to another on the same page.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -42,7 +42,7 @@
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$111</definedName>
+    <definedName name="web">'#system'!$U$2:$U$112</definedName>
     <definedName name="webalert">'#system'!$V$2:$V$6</definedName>
     <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
     <definedName name="ws">'#system'!$X$2:$X$16</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="476">
   <si>
     <t>description</t>
   </si>
@@ -1488,6 +1488,9 @@
   </si>
   <si>
     <t>saveTableAsCsv(locator,nextPageLocator,file)</t>
+  </si>
+  <si>
+    <t>dragAndDrop(fromLocator,toLocator)</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1498,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="68" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1831,8 +1834,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="84">
+  <fills count="111">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2304,8 +2401,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="86">
+  <borders count="114">
     <border>
       <left/>
       <right/>
@@ -3174,13 +3424,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3333,49 +3865,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="59" borderId="65" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="65" fillId="59" fontId="38" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="62" borderId="69" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="69" fillId="62" fontId="40" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="65" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="65" fontId="41" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="42" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="68" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="43" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="44" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="71" borderId="77" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="71" fontId="45" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="74" borderId="81" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="81" fillId="74" fontId="46" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="77" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="77" fontId="47" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="77" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="77" fontId="48" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="80" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="49" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="83" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="50" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="80" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="80" fontId="51" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="52" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="86" borderId="93" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="89" borderId="97" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="92" borderId="101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="98" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="101" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="104" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="104" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="110" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3673,7 +4250,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA111"/>
+  <dimension ref="A1:AA112"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -4880,7 +5457,7 @@
         <v>338</v>
       </c>
       <c r="U59" t="s">
-        <v>206</v>
+        <v>475</v>
       </c>
     </row>
     <row r="60">
@@ -4888,7 +5465,7 @@
         <v>311</v>
       </c>
       <c r="U60" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61">
@@ -4896,7 +5473,7 @@
         <v>312</v>
       </c>
       <c r="U61" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62">
@@ -4904,7 +5481,7 @@
         <v>370</v>
       </c>
       <c r="U62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63">
@@ -4912,7 +5489,7 @@
         <v>371</v>
       </c>
       <c r="U63" t="s">
-        <v>471</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64">
@@ -4920,7 +5497,7 @@
         <v>346</v>
       </c>
       <c r="U64" t="s">
-        <v>133</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65">
@@ -4928,7 +5505,7 @@
         <v>315</v>
       </c>
       <c r="U65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66">
@@ -4936,7 +5513,7 @@
         <v>270</v>
       </c>
       <c r="U66" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67">
@@ -4944,7 +5521,7 @@
         <v>354</v>
       </c>
       <c r="U67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68">
@@ -4952,7 +5529,7 @@
         <v>316</v>
       </c>
       <c r="U68" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69">
@@ -4960,7 +5537,7 @@
         <v>409</v>
       </c>
       <c r="U69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70">
@@ -4968,7 +5545,7 @@
         <v>306</v>
       </c>
       <c r="U70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71">
@@ -4976,7 +5553,7 @@
         <v>410</v>
       </c>
       <c r="U71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72">
@@ -4984,7 +5561,7 @@
         <v>263</v>
       </c>
       <c r="U72" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73">
@@ -4992,7 +5569,7 @@
         <v>345</v>
       </c>
       <c r="U73" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74">
@@ -5000,7 +5577,7 @@
         <v>281</v>
       </c>
       <c r="U74" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75">
@@ -5008,7 +5585,7 @@
         <v>287</v>
       </c>
       <c r="U75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76">
@@ -5016,7 +5593,7 @@
         <v>292</v>
       </c>
       <c r="U76" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77">
@@ -5024,7 +5601,7 @@
         <v>464</v>
       </c>
       <c r="U77" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78">
@@ -5032,7 +5609,7 @@
         <v>333</v>
       </c>
       <c r="U78" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79">
@@ -5040,7 +5617,7 @@
         <v>271</v>
       </c>
       <c r="U79" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80">
@@ -5048,7 +5625,7 @@
         <v>282</v>
       </c>
       <c r="U80" t="s">
-        <v>472</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81">
@@ -5056,7 +5633,7 @@
         <v>288</v>
       </c>
       <c r="U81" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="82">
@@ -5064,7 +5641,7 @@
         <v>277</v>
       </c>
       <c r="U82" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
     </row>
     <row r="83">
@@ -5072,7 +5649,7 @@
         <v>272</v>
       </c>
       <c r="U83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84">
@@ -5080,7 +5657,7 @@
         <v>289</v>
       </c>
       <c r="U84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85">
@@ -5088,7 +5665,7 @@
         <v>273</v>
       </c>
       <c r="U85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86">
@@ -5096,7 +5673,7 @@
         <v>274</v>
       </c>
       <c r="U86" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87">
@@ -5104,7 +5681,7 @@
         <v>307</v>
       </c>
       <c r="U87" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88">
@@ -5112,7 +5689,7 @@
         <v>313</v>
       </c>
       <c r="U88" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89">
@@ -5120,7 +5697,7 @@
         <v>296</v>
       </c>
       <c r="U89" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90">
@@ -5128,7 +5705,7 @@
         <v>341</v>
       </c>
       <c r="U90" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="91">
@@ -5136,7 +5713,7 @@
         <v>278</v>
       </c>
       <c r="U91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92">
@@ -5144,101 +5721,106 @@
         <v>279</v>
       </c>
       <c r="U92" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93">
       <c r="U93" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94">
       <c r="U94" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95">
       <c r="U95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96">
       <c r="U96" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97">
       <c r="U97" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98">
       <c r="U98" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99">
       <c r="U99" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100">
       <c r="U100" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101">
       <c r="U101" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102">
       <c r="U102" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103">
       <c r="U103" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104">
       <c r="U104" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105">
       <c r="U105" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106">
       <c r="U106" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107">
       <c r="U107" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108">
       <c r="U108" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109">
       <c r="U109" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110">
       <c r="U110" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111">
       <c r="U111" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="U112" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[base] - [`nexial.currentActivity`](../systemvars/index#nexial.currentActivity): **NEW** System variable to indicate the   Activity currently in execution
[webalert]
- [`replyOK(text)`](../commands/webalert/replyOK(text)): **NEW** command to automate prompt reply and then click OK.
- [`replyCancel(text)`](../commands/webalert/replyCancel(text)): **NEW** command to automate prompt reply and then click
  Cancel.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,16 +19,16 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="base">'#system'!$C$2:$C$33</definedName>
-    <definedName name="csv">'#system'!$D$2:$D$4</definedName>
+    <definedName name="csv">'#system'!$D$2:$D$5</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
     <definedName name="excel">'#system'!$F$2:$F$8</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
-    <definedName name="io">'#system'!$I$2:$I$21</definedName>
+    <definedName name="io">'#system'!$I$2:$I$22</definedName>
     <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="json">'#system'!$K$2:$K$12</definedName>
+    <definedName name="json">'#system'!$K$2:$K$13</definedName>
     <definedName name="mail">'#system'!$L$2:$L$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -42,8 +42,8 @@
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$112</definedName>
-    <definedName name="webalert">'#system'!$V$2:$V$6</definedName>
+    <definedName name="web">'#system'!$U$2:$U$114</definedName>
+    <definedName name="webalert">'#system'!$V$2:$V$8</definedName>
     <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
     <definedName name="ws">'#system'!$X$2:$X$16</definedName>
     <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2792" uniqueCount="484">
   <si>
     <t>description</t>
   </si>
@@ -1491,6 +1491,30 @@
   </si>
   <si>
     <t>dragAndDrop(fromLocator,toLocator)</t>
+  </si>
+  <si>
+    <t>fromExcel(excel,worksheet,csvFile)</t>
+  </si>
+  <si>
+    <t>writeFileAsIs(file,content,append)</t>
+  </si>
+  <si>
+    <t>fromCsv(csv,header,jsonFile)</t>
+  </si>
+  <si>
+    <t>checkAll(locator)</t>
+  </si>
+  <si>
+    <t>focus(locator)</t>
+  </si>
+  <si>
+    <t>uncheckAll(locator)</t>
+  </si>
+  <si>
+    <t>replyCancel(text)</t>
+  </si>
+  <si>
+    <t>replyOK(text)</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1522,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="68" x14ac:knownFonts="1">
+  <fonts count="83" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1928,8 +1952,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="111">
+  <fills count="138">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2554,8 +2672,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="114">
+  <borders count="142">
     <border>
       <left/>
       <right/>
@@ -3706,13 +3977,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3910,49 +4463,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="52" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="86" borderId="93" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="93" fillId="86" fontId="53" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="54" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="89" borderId="97" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="97" fillId="89" fontId="55" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="92" borderId="101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="101" fillId="92" fontId="56" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="57" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="58" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="59" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="98" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="105" fillId="98" fontId="60" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="101" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="109" fillId="101" fontId="61" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="104" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="104" fontId="62" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="104" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="104" fontId="63" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="64" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="110" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="65" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="66" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="67" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="113" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="116" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="119" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="125" borderId="133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="128" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="131" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="131" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4250,7 +4848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA112"/>
+  <dimension ref="A1:AA114"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -4574,6 +5172,9 @@
       <c r="C5" t="s">
         <v>215</v>
       </c>
+      <c r="D5" t="s">
+        <v>476</v>
+      </c>
       <c r="E5" t="s">
         <v>337</v>
       </c>
@@ -4667,7 +5268,7 @@
         <v>91</v>
       </c>
       <c r="V6" t="s">
-        <v>167</v>
+        <v>482</v>
       </c>
       <c r="W6" t="s">
         <v>172</v>
@@ -4722,6 +5323,9 @@
       <c r="U7" t="s">
         <v>92</v>
       </c>
+      <c r="V7" t="s">
+        <v>483</v>
+      </c>
       <c r="W7" t="s">
         <v>173</v>
       </c>
@@ -4772,6 +5376,9 @@
       <c r="U8" t="s">
         <v>93</v>
       </c>
+      <c r="V8" t="s">
+        <v>167</v>
+      </c>
       <c r="W8" t="s">
         <v>174</v>
       </c>
@@ -4840,7 +5447,7 @@
         <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>478</v>
       </c>
       <c r="M10" t="s">
         <v>469</v>
@@ -4875,7 +5482,7 @@
         <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M11" t="s">
         <v>85</v>
@@ -4907,7 +5514,7 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M12" t="s">
         <v>34</v>
@@ -4935,6 +5542,9 @@
       <c r="I13" t="s">
         <v>74</v>
       </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
       <c r="M13" t="s">
         <v>86</v>
       </c>
@@ -5085,7 +5695,7 @@
         <v>298</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>477</v>
       </c>
       <c r="U20" t="s">
         <v>100</v>
@@ -5102,7 +5712,7 @@
         <v>299</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U21" t="s">
         <v>101</v>
@@ -5118,6 +5728,9 @@
       <c r="E22" t="s">
         <v>300</v>
       </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
       <c r="U22" t="s">
         <v>102</v>
       </c>
@@ -5345,7 +5958,7 @@
         <v>343</v>
       </c>
       <c r="U45" t="s">
-        <v>205</v>
+        <v>479</v>
       </c>
     </row>
     <row r="46">
@@ -5353,7 +5966,7 @@
         <v>203</v>
       </c>
       <c r="U46" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47">
@@ -5361,7 +5974,7 @@
         <v>303</v>
       </c>
       <c r="U47" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48">
@@ -5369,7 +5982,7 @@
         <v>340</v>
       </c>
       <c r="U48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49">
@@ -5377,7 +5990,7 @@
         <v>369</v>
       </c>
       <c r="U49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50">
@@ -5385,7 +5998,7 @@
         <v>304</v>
       </c>
       <c r="U50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51">
@@ -5393,7 +6006,7 @@
         <v>357</v>
       </c>
       <c r="U51" t="s">
-        <v>347</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52">
@@ -5401,7 +6014,7 @@
         <v>332</v>
       </c>
       <c r="U52" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
     </row>
     <row r="53">
@@ -5409,7 +6022,7 @@
         <v>269</v>
       </c>
       <c r="U53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54">
@@ -5417,7 +6030,7 @@
         <v>293</v>
       </c>
       <c r="U54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55">
@@ -5425,7 +6038,7 @@
         <v>294</v>
       </c>
       <c r="U55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56">
@@ -5433,7 +6046,7 @@
         <v>295</v>
       </c>
       <c r="U56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57">
@@ -5441,7 +6054,7 @@
         <v>305</v>
       </c>
       <c r="U57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58">
@@ -5449,7 +6062,7 @@
         <v>314</v>
       </c>
       <c r="U58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59">
@@ -5457,7 +6070,7 @@
         <v>338</v>
       </c>
       <c r="U59" t="s">
-        <v>475</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60">
@@ -5465,7 +6078,7 @@
         <v>311</v>
       </c>
       <c r="U60" t="s">
-        <v>206</v>
+        <v>475</v>
       </c>
     </row>
     <row r="61">
@@ -5473,7 +6086,7 @@
         <v>312</v>
       </c>
       <c r="U61" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62">
@@ -5481,7 +6094,7 @@
         <v>370</v>
       </c>
       <c r="U62" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63">
@@ -5489,7 +6102,7 @@
         <v>371</v>
       </c>
       <c r="U63" t="s">
-        <v>132</v>
+        <v>480</v>
       </c>
     </row>
     <row r="64">
@@ -5497,7 +6110,7 @@
         <v>346</v>
       </c>
       <c r="U64" t="s">
-        <v>471</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65">
@@ -5505,7 +6118,7 @@
         <v>315</v>
       </c>
       <c r="U65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66">
@@ -5513,7 +6126,7 @@
         <v>270</v>
       </c>
       <c r="U66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67">
@@ -5521,7 +6134,7 @@
         <v>354</v>
       </c>
       <c r="U67" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68">
@@ -5529,7 +6142,7 @@
         <v>316</v>
       </c>
       <c r="U68" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69">
@@ -5537,7 +6150,7 @@
         <v>409</v>
       </c>
       <c r="U69" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70">
@@ -5545,7 +6158,7 @@
         <v>306</v>
       </c>
       <c r="U70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71">
@@ -5553,7 +6166,7 @@
         <v>410</v>
       </c>
       <c r="U71" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72">
@@ -5561,7 +6174,7 @@
         <v>263</v>
       </c>
       <c r="U72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73">
@@ -5569,7 +6182,7 @@
         <v>345</v>
       </c>
       <c r="U73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74">
@@ -5577,7 +6190,7 @@
         <v>281</v>
       </c>
       <c r="U74" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75">
@@ -5585,7 +6198,7 @@
         <v>287</v>
       </c>
       <c r="U75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76">
@@ -5593,7 +6206,7 @@
         <v>292</v>
       </c>
       <c r="U76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77">
@@ -5601,7 +6214,7 @@
         <v>464</v>
       </c>
       <c r="U77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78">
@@ -5609,7 +6222,7 @@
         <v>333</v>
       </c>
       <c r="U78" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79">
@@ -5617,7 +6230,7 @@
         <v>271</v>
       </c>
       <c r="U79" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80">
@@ -5625,7 +6238,7 @@
         <v>282</v>
       </c>
       <c r="U80" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="81">
@@ -5633,7 +6246,7 @@
         <v>288</v>
       </c>
       <c r="U81" t="s">
-        <v>472</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82">
@@ -5641,7 +6254,7 @@
         <v>277</v>
       </c>
       <c r="U82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="83">
@@ -5649,7 +6262,7 @@
         <v>272</v>
       </c>
       <c r="U83" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
     </row>
     <row r="84">
@@ -5657,7 +6270,7 @@
         <v>289</v>
       </c>
       <c r="U84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85">
@@ -5665,7 +6278,7 @@
         <v>273</v>
       </c>
       <c r="U85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86">
@@ -5673,7 +6286,7 @@
         <v>274</v>
       </c>
       <c r="U86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87">
@@ -5681,7 +6294,7 @@
         <v>307</v>
       </c>
       <c r="U87" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88">
@@ -5689,7 +6302,7 @@
         <v>313</v>
       </c>
       <c r="U88" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="89">
@@ -5697,7 +6310,7 @@
         <v>296</v>
       </c>
       <c r="U89" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90">
@@ -5705,7 +6318,7 @@
         <v>341</v>
       </c>
       <c r="U90" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91">
@@ -5713,7 +6326,7 @@
         <v>278</v>
       </c>
       <c r="U91" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="92">
@@ -5721,106 +6334,116 @@
         <v>279</v>
       </c>
       <c r="U92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93">
       <c r="U93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94">
       <c r="U94" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95">
       <c r="U95" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96">
       <c r="U96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97">
       <c r="U97" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98">
       <c r="U98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="99">
       <c r="U99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100">
       <c r="U100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101">
       <c r="U101" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102">
       <c r="U102" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103">
       <c r="U103" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104">
       <c r="U104" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105">
       <c r="U105" t="s">
-        <v>156</v>
+        <v>481</v>
       </c>
     </row>
     <row r="106">
       <c r="U106" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107">
       <c r="U107" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108">
       <c r="U108" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109">
       <c r="U109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110">
       <c r="U110" t="s">
-        <v>160</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111">
       <c r="U111" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112">
       <c r="U112" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="U113" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="U114" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- [DATE expression]: fixed date operation with negative values.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2792" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3246" uniqueCount="484">
   <si>
     <t>description</t>
   </si>
@@ -1522,7 +1522,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="83" x14ac:knownFonts="1">
+  <fonts count="98" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2046,8 +2046,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="138">
+  <fills count="165">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2825,8 +2919,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="142">
+  <borders count="170">
     <border>
       <left/>
       <right/>
@@ -4259,13 +4506,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="109">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4508,49 +5037,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="67" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="113" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="113" fontId="68" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="69" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="116" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="125" fillId="116" fontId="70" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="119" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="119" fontId="71" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="72" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="73" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="74" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="125" borderId="133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="133" fillId="125" fontId="75" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="128" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="137" fillId="128" fontId="76" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="131" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="131" fontId="77" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="131" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="131" fontId="78" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="79" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="137" fontId="80" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="81" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="82" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="140" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="143" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="146" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="149" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="152" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="155" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="164" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
- support default output directory via environment variable `NEXIAL_OUTPUT` - update code to avoid using deprecated references in POI - hide internal commandline options from being printed to console
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3246" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="484">
   <si>
     <t>description</t>
   </si>
@@ -1522,7 +1522,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="98" x14ac:knownFonts="1">
+  <fonts count="113" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2140,8 +2140,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="165">
+  <fills count="192">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3072,8 +3166,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="170">
+  <borders count="198">
     <border>
       <left/>
       <right/>
@@ -4788,13 +5035,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="124">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5082,49 +5611,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="82" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="140" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="149" fillId="140" fontId="83" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="84" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="143" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="153" fillId="143" fontId="85" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="86" fillId="146" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="157" fillId="146" fontId="86" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="87" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="88" fillId="149" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="149" fontId="88" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="89" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="90" fillId="152" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="161" fillId="152" fontId="90" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="91" fillId="155" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="165" fillId="155" fontId="91" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="92" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="169" fillId="158" fontId="92" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="158" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="169" fillId="158" fontId="93" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="94" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="161" fontId="94" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="164" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="164" fontId="95" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="96" fillId="161" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="161" fontId="96" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="97" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="167" borderId="177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="170" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="173" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="179" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="182" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="185" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="185" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
- [`assertEqual(expected,actual)](../commands/json/assertEqual(expected,actual)): **NEW** command to compare JSON documents.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -28,7 +28,7 @@
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
     <definedName name="io">'#system'!$I$2:$I$22</definedName>
     <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="json">'#system'!$K$2:$K$13</definedName>
+    <definedName name="json">'#system'!$K$2:$K$14</definedName>
     <definedName name="mail">'#system'!$L$2:$L$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="484">
   <si>
     <t>description</t>
   </si>
@@ -1522,7 +1522,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="113" x14ac:knownFonts="1">
+  <fonts count="128" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2234,8 +2234,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="192">
+  <fills count="219">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3319,8 +3413,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="198">
+  <borders count="226">
     <border>
       <left/>
       <right/>
@@ -5317,13 +5564,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="139">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5656,49 +6185,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="97" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="98" fillId="167" borderId="177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="177" fillId="167" fontId="98" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="99" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="100" fillId="170" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="181" fillId="170" fontId="100" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="101" fillId="173" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="185" fillId="173" fontId="101" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="102" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="103" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="176" fontId="103" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="104" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="179" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="189" fillId="179" fontId="105" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="106" fillId="182" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="193" fillId="182" fontId="106" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="107" fillId="185" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="197" fillId="185" fontId="107" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="108" fillId="185" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="197" fillId="185" fontId="108" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="109" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="188" fontId="109" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="110" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="191" fontId="110" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="188" fontId="111" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="112" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="194" borderId="205" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="197" borderId="209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="200" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="206" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="209" borderId="221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="212" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="212" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="215" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="218" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="215" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6451,7 +7025,7 @@
         <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>317</v>
       </c>
       <c r="M7" t="s">
         <v>26</v>
@@ -6507,7 +7081,7 @@
         <v>31</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
         <v>83</v>
@@ -6557,7 +7131,7 @@
         <v>391</v>
       </c>
       <c r="K9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M9" t="s">
         <v>84</v>
@@ -6595,7 +7169,7 @@
         <v>13</v>
       </c>
       <c r="K10" t="s">
-        <v>478</v>
+        <v>29</v>
       </c>
       <c r="M10" t="s">
         <v>469</v>
@@ -6630,7 +7204,7 @@
         <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>478</v>
       </c>
       <c r="M11" t="s">
         <v>85</v>
@@ -6662,7 +7236,7 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M12" t="s">
         <v>34</v>
@@ -6691,7 +7265,7 @@
         <v>74</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M13" t="s">
         <v>86</v>
@@ -6718,6 +7292,9 @@
       </c>
       <c r="I14" t="s">
         <v>75</v>
+      </c>
+      <c r="K14" t="s">
+        <v>36</v>
       </c>
       <c r="M14" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
- [`saveDivsAsCsv(headers,rows,cells,nextPage,file)`](../commands/web/saveDivsAsCsv(headers,rows,cells,nextPage,file)):   **NEW** command to save a "DIV"-style grid data to CSV file.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -42,7 +42,7 @@
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$114</definedName>
+    <definedName name="web">'#system'!$U$2:$U$115</definedName>
     <definedName name="webalert">'#system'!$V$2:$V$8</definedName>
     <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
     <definedName name="ws">'#system'!$X$2:$X$16</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5534" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6458" uniqueCount="493">
   <si>
     <t>description</t>
   </si>
@@ -1536,6 +1536,12 @@
   </si>
   <si>
     <t>setPassword(file,password)</t>
+  </si>
+  <si>
+    <t>saveDivsAsCsv(headerCellsLoc,rowLocator,cellLocator,nextPageLocator,file)</t>
+  </si>
+  <si>
+    <t>saveDivsAsCsv(headers,rows,cells,nextPage,file)</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1549,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="173" x14ac:knownFonts="1">
+  <fonts count="203" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2631,8 +2637,196 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="300">
+  <fills count="354">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4328,8 +4522,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="310">
+  <borders count="366">
     <border>
       <left/>
       <right/>
@@ -7454,13 +7954,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="214">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -7973,49 +9037,139 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="157" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="158" fillId="275" borderId="289" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="289" fillId="275" fontId="158" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="159" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="160" fillId="278" borderId="293" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="293" fillId="278" fontId="160" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="161" fillId="281" borderId="297" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="297" fillId="281" fontId="161" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="162" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="163" fillId="284" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="284" fontId="163" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="164" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="164" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="165" fillId="287" borderId="301" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="301" fillId="287" fontId="165" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="166" fillId="290" borderId="305" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="305" fillId="290" fontId="166" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="167" fillId="293" borderId="309" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="309" fillId="293" fontId="167" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="168" fillId="293" borderId="309" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="309" fillId="293" fontId="168" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="169" fillId="296" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="296" fontId="169" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="170" fillId="299" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="299" fontId="170" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="171" fillId="296" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="296" fontId="171" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="172" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="172" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="317" fillId="302" fontId="173" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="174" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="321" fillId="305" fontId="175" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="325" fillId="308" fontId="176" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="177" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="311" fontId="178" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="179" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="329" fillId="314" fontId="180" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="333" fillId="317" fontId="181" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="337" fillId="320" fontId="182" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="337" fillId="320" fontId="183" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="323" fontId="184" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="326" fontId="185" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="323" fontId="186" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="187" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="188" fillId="329" borderId="345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="332" borderId="349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="191" fillId="335" borderId="353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="338" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="194" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="195" fillId="341" borderId="357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="196" fillId="344" borderId="361" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="197" fillId="347" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="198" fillId="347" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="199" fillId="350" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="200" fillId="353" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="201" fillId="350" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="202" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -8313,7 +9467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA114"/>
+  <dimension ref="A1:AA115"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -9700,7 +10854,7 @@
         <v>464</v>
       </c>
       <c r="U77" t="s">
-        <v>193</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78">
@@ -9708,7 +10862,7 @@
         <v>333</v>
       </c>
       <c r="U78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79">
@@ -9716,7 +10870,7 @@
         <v>271</v>
       </c>
       <c r="U79" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80">
@@ -9724,7 +10878,7 @@
         <v>282</v>
       </c>
       <c r="U80" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81">
@@ -9732,7 +10886,7 @@
         <v>288</v>
       </c>
       <c r="U81" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82">
@@ -9740,7 +10894,7 @@
         <v>277</v>
       </c>
       <c r="U82" t="s">
-        <v>472</v>
+        <v>195</v>
       </c>
     </row>
     <row r="83">
@@ -9748,7 +10902,7 @@
         <v>272</v>
       </c>
       <c r="U83" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="84">
@@ -9756,7 +10910,7 @@
         <v>289</v>
       </c>
       <c r="U84" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
     </row>
     <row r="85">
@@ -9764,7 +10918,7 @@
         <v>273</v>
       </c>
       <c r="U85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86">
@@ -9772,7 +10926,7 @@
         <v>274</v>
       </c>
       <c r="U86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="87">
@@ -9780,7 +10934,7 @@
         <v>307</v>
       </c>
       <c r="U87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="88">
@@ -9788,7 +10942,7 @@
         <v>313</v>
       </c>
       <c r="U88" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89">
@@ -9796,7 +10950,7 @@
         <v>296</v>
       </c>
       <c r="U89" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90">
@@ -9804,7 +10958,7 @@
         <v>341</v>
       </c>
       <c r="U90" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91">
@@ -9812,7 +10966,7 @@
         <v>278</v>
       </c>
       <c r="U91" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92">
@@ -9820,116 +10974,121 @@
         <v>279</v>
       </c>
       <c r="U92" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="93">
       <c r="U93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94">
       <c r="U94" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95">
       <c r="U95" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96">
       <c r="U96" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97">
       <c r="U97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98">
       <c r="U98" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99">
       <c r="U99" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100">
       <c r="U100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101">
       <c r="U101" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102">
       <c r="U102" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103">
       <c r="U103" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104">
       <c r="U104" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105">
       <c r="U105" t="s">
-        <v>481</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106">
       <c r="U106" t="s">
-        <v>155</v>
+        <v>481</v>
       </c>
     </row>
     <row r="107">
       <c r="U107" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108">
       <c r="U108" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109">
       <c r="U109" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110">
       <c r="U110" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111">
       <c r="U111" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112">
       <c r="U112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113">
       <c r="U113" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="114">
       <c r="U114" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="U115" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- [`columnarCsv(file,worksheet,ranges,output)`]: support merging of multiple ranges from the same worksheet. The merge is performend columnwise (not adding new rows).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -23,7 +23,7 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
-    <definedName name="excel">'#system'!$F$2:$F$13</definedName>
+    <definedName name="excel">'#system'!$F$2:$F$14</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
     <definedName name="io">'#system'!$I$2:$I$22</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6921" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7385" uniqueCount="495">
   <si>
     <t>description</t>
   </si>
@@ -1545,6 +1545,9 @@
   </si>
   <si>
     <t>openHttpBasic(url,username,password)</t>
+  </si>
+  <si>
+    <t>columnarCsv(file,worksheet,ranges,output)</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1555,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="218" x14ac:knownFonts="1">
+  <fonts count="233" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2922,8 +2925,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="381">
+  <fills count="408">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5078,8 +5175,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="394">
+  <borders count="422">
     <border>
       <left/>
       <right/>
@@ -9050,13 +9300,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="244">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9704,49 +10236,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="202" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="203" fillId="356" borderId="373" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="373" fillId="356" fontId="203" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="204" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="204" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="205" fillId="359" borderId="377" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="377" fillId="359" fontId="205" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="206" fillId="362" borderId="381" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="381" fillId="362" fontId="206" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="207" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="207" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="208" fillId="365" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="365" fontId="208" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="209" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="209" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="210" fillId="368" borderId="385" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="385" fillId="368" fontId="210" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="211" fillId="371" borderId="389" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="389" fillId="371" fontId="211" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="212" fillId="374" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="393" fillId="374" fontId="212" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="213" fillId="374" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="393" fillId="374" fontId="213" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="214" fillId="377" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="377" fontId="214" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="215" fillId="380" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="380" fontId="215" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="216" fillId="377" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="377" fontId="216" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="217" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="217" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="218" fillId="383" borderId="401" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="219" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="220" fillId="386" borderId="405" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="221" fillId="389" borderId="409" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="222" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="223" fillId="392" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="224" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="225" fillId="395" borderId="413" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="226" fillId="398" borderId="417" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="227" fillId="401" borderId="421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="228" fillId="401" borderId="421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="229" fillId="404" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="230" fillId="407" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="231" fillId="404" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="232" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10375,7 +10952,7 @@
         <v>337</v>
       </c>
       <c r="F5" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="H5" t="s">
         <v>349</v>
@@ -10437,7 +11014,7 @@
         <v>389</v>
       </c>
       <c r="F6" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
@@ -10493,7 +11070,7 @@
         <v>367</v>
       </c>
       <c r="F7" t="s">
-        <v>329</v>
+        <v>485</v>
       </c>
       <c r="I7" t="s">
         <v>72</v>
@@ -10549,7 +11126,7 @@
         <v>368</v>
       </c>
       <c r="F8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I8" t="s">
         <v>31</v>
@@ -10602,7 +11179,7 @@
         <v>308</v>
       </c>
       <c r="F9" t="s">
-        <v>490</v>
+        <v>330</v>
       </c>
       <c r="I9" t="s">
         <v>391</v>
@@ -10643,7 +11220,7 @@
         <v>353</v>
       </c>
       <c r="F10" t="s">
-        <v>323</v>
+        <v>490</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -10681,7 +11258,7 @@
         <v>275</v>
       </c>
       <c r="F11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I11" t="s">
         <v>35</v>
@@ -10716,7 +11293,7 @@
         <v>264</v>
       </c>
       <c r="F12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I12" t="s">
         <v>73</v>
@@ -10748,7 +11325,7 @@
         <v>318</v>
       </c>
       <c r="F13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I13" t="s">
         <v>74</v>
@@ -10778,6 +11355,9 @@
       </c>
       <c r="E14" t="s">
         <v>265</v>
+      </c>
+      <c r="F14" t="s">
+        <v>326</v>
       </c>
       <c r="I14" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
[io] - [`rename(target,newFile)`](../commands/io/rename(target,newName)): **NEW** command to rename file or directory.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -26,7 +26,7 @@
     <definedName name="excel">'#system'!$F$2:$F$14</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
-    <definedName name="io">'#system'!$I$2:$I$22</definedName>
+    <definedName name="io">'#system'!$I$2:$I$23</definedName>
     <definedName name="jms">'#system'!$J$2:$J$4</definedName>
     <definedName name="json">'#system'!$K$2:$K$14</definedName>
     <definedName name="mail">'#system'!$L$2:$L$2</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7385" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8314" uniqueCount="496">
   <si>
     <t>description</t>
   </si>
@@ -1548,6 +1548,9 @@
   </si>
   <si>
     <t>columnarCsv(file,worksheet,ranges,output)</t>
+  </si>
+  <si>
+    <t>rename(target,newName)</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1558,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="233" x14ac:knownFonts="1">
+  <fonts count="263" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3019,8 +3022,196 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="408">
+  <fills count="462">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5328,8 +5519,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="422">
+  <borders count="478">
     <border>
       <left/>
       <right/>
@@ -9582,13 +10079,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="274">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -10281,49 +11342,139 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="217" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="218" fillId="383" borderId="401" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="401" fillId="383" fontId="218" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="219" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="219" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="220" fillId="386" borderId="405" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="405" fillId="386" fontId="220" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="221" fillId="389" borderId="409" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="409" fillId="389" fontId="221" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="222" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="222" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="223" fillId="392" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="392" fontId="223" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="224" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="224" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="225" fillId="395" borderId="413" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="413" fillId="395" fontId="225" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="226" fillId="398" borderId="417" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="417" fillId="398" fontId="226" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="227" fillId="401" borderId="421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="421" fillId="401" fontId="227" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="228" fillId="401" borderId="421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="421" fillId="401" fontId="228" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="229" fillId="404" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="404" fontId="229" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="230" fillId="407" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="407" fontId="230" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="231" fillId="404" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="404" fontId="231" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="232" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="232" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="429" fillId="410" fontId="233" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="234" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="433" fillId="413" fontId="235" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="437" fillId="416" fontId="236" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="237" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="419" fontId="238" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="239" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="441" fillId="422" fontId="240" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="445" fillId="425" fontId="241" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="449" fillId="428" fontId="242" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="449" fillId="428" fontId="243" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="431" fontId="244" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="434" fontId="245" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="431" fontId="246" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="247" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="248" fillId="437" borderId="457" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="249" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="250" fillId="440" borderId="461" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="251" fillId="443" borderId="465" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="252" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="253" fillId="446" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="254" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="255" fillId="449" borderId="469" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="256" fillId="452" borderId="473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="257" fillId="455" borderId="477" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="258" fillId="455" borderId="477" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="259" fillId="458" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="260" fillId="461" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="261" fillId="458" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="262" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -11360,7 +12511,7 @@
         <v>326</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>495</v>
       </c>
       <c r="K14" t="s">
         <v>36</v>
@@ -11389,7 +12540,7 @@
         <v>266</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M15" t="s">
         <v>88</v>
@@ -11415,7 +12566,7 @@
         <v>319</v>
       </c>
       <c r="I16" t="s">
-        <v>381</v>
+        <v>76</v>
       </c>
       <c r="N16" t="s">
         <v>243</v>
@@ -11438,7 +12589,7 @@
         <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>381</v>
       </c>
       <c r="U17" t="s">
         <v>97</v>
@@ -11455,7 +12606,7 @@
         <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>393</v>
+        <v>37</v>
       </c>
       <c r="U18" t="s">
         <v>98</v>
@@ -11472,7 +12623,7 @@
         <v>297</v>
       </c>
       <c r="I19" t="s">
-        <v>77</v>
+        <v>393</v>
       </c>
       <c r="U19" t="s">
         <v>99</v>
@@ -11489,7 +12640,7 @@
         <v>298</v>
       </c>
       <c r="I20" t="s">
-        <v>477</v>
+        <v>77</v>
       </c>
       <c r="U20" t="s">
         <v>100</v>
@@ -11506,7 +12657,7 @@
         <v>299</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>477</v>
       </c>
       <c r="U21" t="s">
         <v>101</v>
@@ -11523,7 +12674,7 @@
         <v>300</v>
       </c>
       <c r="I22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U22" t="s">
         <v>102</v>
@@ -11538,6 +12689,9 @@
       </c>
       <c r="E23" t="s">
         <v>291</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
       </c>
       <c r="U23" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
[ssh] - support empty password (use `(empty)`) for cases where the target SSH server allows for it.
[web]
- [`select(locator,text)`](../commands/web/select(locator,text)): now supports selection based on regular expression.
  Use `REGEX:` as prefix to enable regex-based text selection. Note that for SELECT element that supports only single
  selection, only the first match will be selected.
- [`deselect(locator,text)`](../commands/web/deselect(locator,text)): **NEW** command to deselect (unselect?) from a
  SELECT element based on `text`. For regex-based deselect, add `REGEX:` prefix to `text`.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -42,7 +42,7 @@
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$116</definedName>
+    <definedName name="web">'#system'!$U$2:$U$117</definedName>
     <definedName name="webalert">'#system'!$V$2:$V$8</definedName>
     <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
     <definedName name="ws">'#system'!$X$2:$X$16</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8781" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9249" uniqueCount="499">
   <si>
     <t>description</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>assertArrayNotContain(array,unexpected)</t>
+  </si>
+  <si>
+    <t>deselect(locator,text)</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1567,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="278" x14ac:knownFonts="1">
+  <fonts count="293" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3310,8 +3313,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="489">
+  <fills count="516">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6078,8 +6175,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="506">
+  <borders count="534">
     <border>
       <left/>
       <right/>
@@ -11178,13 +11428,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="289">
+  <cellXfs count="304">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12012,49 +12544,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="262" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="263" fillId="464" borderId="485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="485" fillId="464" fontId="263" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="264" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="264" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="265" fillId="467" borderId="489" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="489" fillId="467" fontId="265" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="266" fillId="470" borderId="493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="493" fillId="470" fontId="266" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="267" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="267" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="268" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="473" fontId="268" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="269" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="269" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="270" fillId="476" borderId="497" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="497" fillId="476" fontId="270" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="271" fillId="479" borderId="501" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="501" fillId="479" fontId="271" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="272" fillId="482" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="505" fillId="482" fontId="272" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="273" fillId="482" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="505" fillId="482" fontId="273" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="274" fillId="485" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="485" fontId="274" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="275" fillId="488" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="488" fontId="275" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="276" fillId="485" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="485" fontId="276" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="277" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="277" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="278" fillId="491" borderId="513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="279" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="280" fillId="494" borderId="517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="281" fillId="497" borderId="521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="282" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="283" fillId="500" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="284" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="285" fillId="503" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="286" fillId="506" borderId="529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="287" fillId="509" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="288" fillId="509" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="289" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="290" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="291" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="292" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12352,7 +12929,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA116"/>
+  <dimension ref="A1:AA117"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -13559,7 +14136,7 @@
         <v>269</v>
       </c>
       <c r="U53" t="s">
-        <v>124</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54">
@@ -13567,7 +14144,7 @@
         <v>293</v>
       </c>
       <c r="U54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55">
@@ -13575,7 +14152,7 @@
         <v>294</v>
       </c>
       <c r="U55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56">
@@ -13583,7 +14160,7 @@
         <v>295</v>
       </c>
       <c r="U56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57">
@@ -13591,7 +14168,7 @@
         <v>305</v>
       </c>
       <c r="U57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58">
@@ -13599,7 +14176,7 @@
         <v>314</v>
       </c>
       <c r="U58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59">
@@ -13607,7 +14184,7 @@
         <v>338</v>
       </c>
       <c r="U59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60">
@@ -13615,7 +14192,7 @@
         <v>311</v>
       </c>
       <c r="U60" t="s">
-        <v>475</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61">
@@ -13623,7 +14200,7 @@
         <v>312</v>
       </c>
       <c r="U61" t="s">
-        <v>206</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62">
@@ -13631,7 +14208,7 @@
         <v>370</v>
       </c>
       <c r="U62" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63">
@@ -13639,7 +14216,7 @@
         <v>371</v>
       </c>
       <c r="U63" t="s">
-        <v>480</v>
+        <v>390</v>
       </c>
     </row>
     <row r="64">
@@ -13647,7 +14224,7 @@
         <v>346</v>
       </c>
       <c r="U64" t="s">
-        <v>131</v>
+        <v>480</v>
       </c>
     </row>
     <row r="65">
@@ -13655,7 +14232,7 @@
         <v>315</v>
       </c>
       <c r="U65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66">
@@ -13663,7 +14240,7 @@
         <v>270</v>
       </c>
       <c r="U66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67">
@@ -13671,7 +14248,7 @@
         <v>354</v>
       </c>
       <c r="U67" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68">
@@ -13679,7 +14256,7 @@
         <v>316</v>
       </c>
       <c r="U68" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69">
@@ -13687,7 +14264,7 @@
         <v>409</v>
       </c>
       <c r="U69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70">
@@ -13695,7 +14272,7 @@
         <v>306</v>
       </c>
       <c r="U70" t="s">
-        <v>493</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71">
@@ -13703,7 +14280,7 @@
         <v>410</v>
       </c>
       <c r="U71" t="s">
-        <v>135</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72">
@@ -13711,7 +14288,7 @@
         <v>263</v>
       </c>
       <c r="U72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73">
@@ -13719,7 +14296,7 @@
         <v>345</v>
       </c>
       <c r="U73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74">
@@ -13727,7 +14304,7 @@
         <v>281</v>
       </c>
       <c r="U74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75">
@@ -13735,7 +14312,7 @@
         <v>287</v>
       </c>
       <c r="U75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76">
@@ -13743,7 +14320,7 @@
         <v>292</v>
       </c>
       <c r="U76" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77">
@@ -13751,7 +14328,7 @@
         <v>464</v>
       </c>
       <c r="U77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78">
@@ -13759,7 +14336,7 @@
         <v>333</v>
       </c>
       <c r="U78" t="s">
-        <v>492</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79">
@@ -13767,7 +14344,7 @@
         <v>271</v>
       </c>
       <c r="U79" t="s">
-        <v>193</v>
+        <v>492</v>
       </c>
     </row>
     <row r="80">
@@ -13775,7 +14352,7 @@
         <v>282</v>
       </c>
       <c r="U80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81">
@@ -13783,7 +14360,7 @@
         <v>288</v>
       </c>
       <c r="U81" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="82">
@@ -13791,7 +14368,7 @@
         <v>277</v>
       </c>
       <c r="U82" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83">
@@ -13799,7 +14376,7 @@
         <v>272</v>
       </c>
       <c r="U83" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84">
@@ -13807,7 +14384,7 @@
         <v>289</v>
       </c>
       <c r="U84" t="s">
-        <v>472</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85">
@@ -13815,7 +14392,7 @@
         <v>273</v>
       </c>
       <c r="U85" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="86">
@@ -13823,7 +14400,7 @@
         <v>274</v>
       </c>
       <c r="U86" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
     </row>
     <row r="87">
@@ -13831,7 +14408,7 @@
         <v>307</v>
       </c>
       <c r="U87" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="88">
@@ -13839,7 +14416,7 @@
         <v>313</v>
       </c>
       <c r="U88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="89">
@@ -13847,7 +14424,7 @@
         <v>296</v>
       </c>
       <c r="U89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90">
@@ -13855,7 +14432,7 @@
         <v>341</v>
       </c>
       <c r="U90" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91">
@@ -13863,7 +14440,7 @@
         <v>278</v>
       </c>
       <c r="U91" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92">
@@ -13871,126 +14448,131 @@
         <v>279</v>
       </c>
       <c r="U92" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93">
       <c r="U93" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94">
       <c r="U94" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="95">
       <c r="U95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96">
       <c r="U96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97">
       <c r="U97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98">
       <c r="U98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99">
       <c r="U99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100">
       <c r="U100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101">
       <c r="U101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="102">
       <c r="U102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103">
       <c r="U103" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104">
       <c r="U104" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105">
       <c r="U105" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106">
       <c r="U106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107">
       <c r="U107" t="s">
-        <v>481</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108">
       <c r="U108" t="s">
-        <v>155</v>
+        <v>481</v>
       </c>
     </row>
     <row r="109">
       <c r="U109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="110">
       <c r="U110" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="111">
       <c r="U111" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112">
       <c r="U112" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="113">
       <c r="U113" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114">
       <c r="U114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115">
       <c r="U115" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116">
       <c r="U116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="U117" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- enhanced nexial mailer to handle inflight mail configuration changes (e.g. between iterations) and to support AWS SES. - fixed overflow condition when generating new command-listing JSON that has more than 26 command types.
### [aws.ses commands]
- [`sendHtmlMail(profile,to,subject,body)`]: **NEW** command to send email via AWS SES.
- [`sendTextMail(profile,to,subject,body)`]: **NEW** command to send email via AWS SES.

### [built-in functions]
- [`$(execution|meta|nexial)`]: display current Nexial version
- [`$(execution|meta|java)`]: display current Java version

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -18,36 +18,37 @@
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
-    <definedName name="base">'#system'!$C$2:$C$36</definedName>
-    <definedName name="csv">'#system'!$D$2:$D$5</definedName>
+    <definedName name="base">'#system'!$D$2:$D$36</definedName>
+    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
-    <definedName name="excel">'#system'!$F$2:$F$14</definedName>
-    <definedName name="external">'#system'!$G$2:$G$3</definedName>
-    <definedName name="image">'#system'!$H$2:$H$5</definedName>
-    <definedName name="io">'#system'!$I$2:$I$24</definedName>
-    <definedName name="jms">'#system'!$J$2:$J$4</definedName>
-    <definedName name="json">'#system'!$K$2:$K$14</definedName>
-    <definedName name="mail">'#system'!$L$2:$L$2</definedName>
+    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
+    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
+    <definedName name="external">'#system'!$H$2:$H$3</definedName>
+    <definedName name="image">'#system'!$I$2:$I$5</definedName>
+    <definedName name="io">'#system'!$J$2:$J$24</definedName>
+    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
+    <definedName name="json">'#system'!$L$2:$L$14</definedName>
+    <definedName name="mail">'#system'!$M$2:$M$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$M$2:$M$15</definedName>
-    <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
-    <definedName name="rdbms">'#system'!$O$2:$O$7</definedName>
-    <definedName name="redis">'#system'!$P$2:$P$10</definedName>
-    <definedName name="sms">'#system'!$Q$2:$Q$2</definedName>
-    <definedName name="sound">'#system'!$R$2:$R$5</definedName>
-    <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
-    <definedName name="step">'#system'!$T$2:$T$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$26</definedName>
-    <definedName name="web">'#system'!$U$2:$U$117</definedName>
-    <definedName name="webalert">'#system'!$V$2:$V$8</definedName>
-    <definedName name="webcookie">'#system'!$W$2:$W$8</definedName>
-    <definedName name="ws">'#system'!$X$2:$X$17</definedName>
-    <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
-    <definedName name="xml">'#system'!$Z$2:$Z$11</definedName>
+    <definedName name="number">'#system'!$N$2:$N$15</definedName>
+    <definedName name="pdf">'#system'!$O$2:$O$16</definedName>
+    <definedName name="rdbms">'#system'!$P$2:$P$7</definedName>
+    <definedName name="redis">'#system'!$Q$2:$Q$10</definedName>
+    <definedName name="sms">'#system'!$R$2:$R$2</definedName>
+    <definedName name="sound">'#system'!$S$2:$S$5</definedName>
+    <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
+    <definedName name="step">'#system'!$U$2:$U$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$27</definedName>
+    <definedName name="web">'#system'!$V$2:$V$117</definedName>
+    <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
+    <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
+    <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
+    <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="xml">'#system'!$AA$2:$AA$11</definedName>
+    <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9719" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10193" uniqueCount="504">
   <si>
     <t>description</t>
   </si>
@@ -1566,6 +1567,15 @@
   </si>
   <si>
     <t>upload(url,body,fileParams,var)</t>
+  </si>
+  <si>
+    <t>aws.ses</t>
+  </si>
+  <si>
+    <t>sendMail(profile,to,subject,body)</t>
+  </si>
+  <si>
+    <t>sendTextMail(profile,to,subject,body)</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1583,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="309" x14ac:knownFonts="1">
+  <fonts count="325" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3514,8 +3524,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="543">
+  <fills count="570">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6588,8 +6699,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="562">
+  <borders count="590">
     <border>
       <left/>
       <right/>
@@ -12252,13 +12516,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="320">
+  <cellXfs count="336">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -13176,52 +13722,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="292" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="293" fillId="518" borderId="541" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="541" fillId="518" fontId="293" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="294" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="294" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="295" fillId="521" borderId="545" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="545" fillId="521" fontId="295" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="296" fillId="524" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="549" fillId="524" fontId="296" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="297" fillId="527" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="549" fillId="527" fontId="297" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="298" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="298" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="299" fillId="530" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="530" fontId="299" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="300" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="300" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="301" fillId="533" borderId="553" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="553" fillId="533" fontId="301" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="302" fillId="536" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="557" fillId="536" fontId="302" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="303" fillId="539" borderId="561" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="561" fillId="539" fontId="303" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="304" fillId="539" borderId="561" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="561" fillId="539" fontId="304" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="305" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="305" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="306" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="542" fontId="306" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="307" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="307" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="308" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="308" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="309" fillId="545" borderId="569" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="310" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="311" fillId="548" borderId="573" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="312" fillId="551" borderId="577" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="313" fillId="554" borderId="577" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="314" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="315" fillId="557" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="316" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="317" fillId="560" borderId="581" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="318" fillId="563" borderId="585" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="319" fillId="566" borderId="589" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="320" fillId="566" borderId="589" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="321" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="322" fillId="569" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="323" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="324" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13519,7 +14113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA117"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -13536,75 +14130,78 @@
         <v>372</v>
       </c>
       <c r="C1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>348</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>334</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>188</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>230</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>399</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>456</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>413</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>358</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>395</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>47</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>458</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -13616,1559 +14213,1568 @@
         <v>373</v>
       </c>
       <c r="C2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>66</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>487</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>350</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>317</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>385</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>465</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>412</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>466</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>244</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>209</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>400</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>457</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>454</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>382</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>396</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>89</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>163</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>168</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>175</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>468</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>501</v>
       </c>
       <c r="B3" t="s">
         <v>374</v>
       </c>
       <c r="C3" t="s">
+        <v>503</v>
+      </c>
+      <c r="D3" t="s">
         <v>496</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>366</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>351</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>342</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>335</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>78</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>467</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>231</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>210</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>401</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>415</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>383</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>397</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>90</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>164</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>169</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>365</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>176</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>388</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>488</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>352</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>229</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>336</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>232</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>211</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>402</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>416</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>359</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>398</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>355</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>165</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>170</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>176</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>459</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>497</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>476</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>337</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>494</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>349</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>499</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>79</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>233</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>212</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>403</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>417</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>360</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>356</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>166</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>171</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>177</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>460</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>389</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>489</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>64</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>234</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>392</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>404</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>362</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>91</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>482</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>172</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>178</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>461</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>215</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>367</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>485</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>317</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>235</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>414</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>405</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>361</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>92</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>483</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>173</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>179</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>462</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>320</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>368</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>329</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>72</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>27</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>83</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>236</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>406</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>363</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>93</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>167</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>174</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>180</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>463</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>348</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>308</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>330</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>31</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>84</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>237</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>407</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>364</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>201</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>181</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>334</v>
-      </c>
-      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>317</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>353</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>490</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>391</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>469</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>238</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>408</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>258</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>182</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" t="s">
         <v>250</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>275</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>323</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>478</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>85</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>239</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>259</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>260</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
         <v>321</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>264</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>324</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>35</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>34</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>240</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>94</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
         <v>342</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>318</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>325</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>73</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>33</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>86</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>245</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>327</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>265</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>326</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>74</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>36</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>87</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>241</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>95</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>266</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>495</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>88</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>242</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>96</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>399</v>
-      </c>
-      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
         <v>386</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>319</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>75</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>243</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>67</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>456</v>
-      </c>
-      <c r="C17" t="s">
+        <v>399</v>
+      </c>
+      <c r="D17" t="s">
         <v>387</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>81</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>76</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>97</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>413</v>
-      </c>
-      <c r="C18" t="s">
+        <v>456</v>
+      </c>
+      <c r="D18" t="s">
         <v>411</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>82</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>381</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>358</v>
-      </c>
-      <c r="C19" t="s">
+        <v>413</v>
+      </c>
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>297</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>37</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>395</v>
-      </c>
-      <c r="C20" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>298</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>393</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
+        <v>395</v>
+      </c>
+      <c r="D21" t="s">
         <v>54</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>299</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>77</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
         <v>322</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>300</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>477</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
         <v>55</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>291</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>38</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
         <v>486</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>280</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>39</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>458</v>
-      </c>
-      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
         <v>216</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>68</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>458</v>
+      </c>
+      <c r="D26" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" t="s">
+        <v>283</v>
+      </c>
+      <c r="V26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>218</v>
       </c>
-      <c r="C26" t="s">
-        <v>217</v>
-      </c>
-      <c r="E26" t="s">
-        <v>283</v>
-      </c>
-      <c r="U26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>453</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>267</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>56</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>284</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>57</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>285</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>58</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>208</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>59</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>276</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32">
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>60</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>286</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>61</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>261</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>62</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>331</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>63</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>309</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36">
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>262</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="37">
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>310</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="38">
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>268</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="39">
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>70</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40">
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>204</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="41">
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>290</v>
       </c>
-      <c r="U41" t="s">
+      <c r="V41" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="42">
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>301</v>
       </c>
-      <c r="U42" t="s">
+      <c r="V42" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="43">
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>302</v>
       </c>
-      <c r="U43" t="s">
+      <c r="V43" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="44">
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>344</v>
       </c>
-      <c r="U44" t="s">
+      <c r="V44" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="45">
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>343</v>
       </c>
-      <c r="U45" t="s">
+      <c r="V45" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="46">
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>203</v>
       </c>
-      <c r="U46" t="s">
+      <c r="V46" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="47">
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>303</v>
       </c>
-      <c r="U47" t="s">
+      <c r="V47" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="48">
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>340</v>
       </c>
-      <c r="U48" t="s">
+      <c r="V48" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="49">
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>369</v>
       </c>
-      <c r="U49" t="s">
+      <c r="V49" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="50">
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>304</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="51">
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>357</v>
       </c>
-      <c r="U51" t="s">
+      <c r="V51" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="52">
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>332</v>
       </c>
-      <c r="U52" t="s">
+      <c r="V52" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="53">
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>269</v>
       </c>
-      <c r="U53" t="s">
+      <c r="V53" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="54">
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>293</v>
       </c>
-      <c r="U54" t="s">
+      <c r="V54" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="55">
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>294</v>
       </c>
-      <c r="U55" t="s">
+      <c r="V55" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="56">
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>295</v>
       </c>
-      <c r="U56" t="s">
+      <c r="V56" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="57">
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>305</v>
       </c>
-      <c r="U57" t="s">
+      <c r="V57" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="58">
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>314</v>
       </c>
-      <c r="U58" t="s">
+      <c r="V58" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="59">
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>338</v>
       </c>
-      <c r="U59" t="s">
+      <c r="V59" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="60">
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>311</v>
       </c>
-      <c r="U60" t="s">
+      <c r="V60" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="61">
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>312</v>
       </c>
-      <c r="U61" t="s">
+      <c r="V61" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="62">
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>370</v>
       </c>
-      <c r="U62" t="s">
+      <c r="V62" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="63">
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>371</v>
       </c>
-      <c r="U63" t="s">
+      <c r="V63" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="64">
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>346</v>
       </c>
-      <c r="U64" t="s">
+      <c r="V64" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="65">
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>315</v>
       </c>
-      <c r="U65" t="s">
+      <c r="V65" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="66">
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>270</v>
       </c>
-      <c r="U66" t="s">
+      <c r="V66" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="67">
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>354</v>
       </c>
-      <c r="U67" t="s">
+      <c r="V67" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="68">
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>316</v>
       </c>
-      <c r="U68" t="s">
+      <c r="V68" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="69">
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>409</v>
       </c>
-      <c r="U69" t="s">
+      <c r="V69" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="70">
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>306</v>
       </c>
-      <c r="U70" t="s">
+      <c r="V70" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="71">
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>410</v>
       </c>
-      <c r="U71" t="s">
+      <c r="V71" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="72">
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>263</v>
       </c>
-      <c r="U72" t="s">
+      <c r="V72" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="73">
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>345</v>
       </c>
-      <c r="U73" t="s">
+      <c r="V73" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="74">
-      <c r="E74" t="s">
+      <c r="F74" t="s">
         <v>281</v>
       </c>
-      <c r="U74" t="s">
+      <c r="V74" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="75">
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>287</v>
       </c>
-      <c r="U75" t="s">
+      <c r="V75" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="76">
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>292</v>
       </c>
-      <c r="U76" t="s">
+      <c r="V76" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="77">
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>464</v>
       </c>
-      <c r="U77" t="s">
+      <c r="V77" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="78">
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>333</v>
       </c>
-      <c r="U78" t="s">
+      <c r="V78" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="79">
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>271</v>
       </c>
-      <c r="U79" t="s">
+      <c r="V79" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="80">
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>282</v>
       </c>
-      <c r="U80" t="s">
+      <c r="V80" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="81">
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>288</v>
       </c>
-      <c r="U81" t="s">
+      <c r="V81" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="82">
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>277</v>
       </c>
-      <c r="U82" t="s">
+      <c r="V82" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="83">
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>272</v>
       </c>
-      <c r="U83" t="s">
+      <c r="V83" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="84">
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>289</v>
       </c>
-      <c r="U84" t="s">
+      <c r="V84" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="85">
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>273</v>
       </c>
-      <c r="U85" t="s">
+      <c r="V85" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="86">
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>274</v>
       </c>
-      <c r="U86" t="s">
+      <c r="V86" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="87">
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>307</v>
       </c>
-      <c r="U87" t="s">
+      <c r="V87" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="88">
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>313</v>
       </c>
-      <c r="U88" t="s">
+      <c r="V88" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="89">
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>296</v>
       </c>
-      <c r="U89" t="s">
+      <c r="V89" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="90">
-      <c r="E90" t="s">
+      <c r="F90" t="s">
         <v>341</v>
       </c>
-      <c r="U90" t="s">
+      <c r="V90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="91">
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>278</v>
       </c>
-      <c r="U91" t="s">
+      <c r="V91" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="92">
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>279</v>
       </c>
-      <c r="U92" t="s">
+      <c r="V92" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="93">
-      <c r="U93" t="s">
+      <c r="V93" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="94">
-      <c r="U94" t="s">
+      <c r="V94" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="95">
-      <c r="U95" t="s">
+      <c r="V95" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="96">
-      <c r="U96" t="s">
+      <c r="V96" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="97">
-      <c r="U97" t="s">
+      <c r="V97" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="98">
-      <c r="U98" t="s">
+      <c r="V98" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="99">
-      <c r="U99" t="s">
+      <c r="V99" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="100">
-      <c r="U100" t="s">
+      <c r="V100" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="101">
-      <c r="U101" t="s">
+      <c r="V101" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="102">
-      <c r="U102" t="s">
+      <c r="V102" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="103">
-      <c r="U103" t="s">
+      <c r="V103" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="104">
-      <c r="U104" t="s">
+      <c r="V104" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="105">
-      <c r="U105" t="s">
+      <c r="V105" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="106">
-      <c r="U106" t="s">
+      <c r="V106" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="107">
-      <c r="U107" t="s">
+      <c r="V107" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="108">
-      <c r="U108" t="s">
+      <c r="V108" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="109">
-      <c r="U109" t="s">
+      <c r="V109" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="110">
-      <c r="U110" t="s">
+      <c r="V110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="111">
-      <c r="U111" t="s">
+      <c r="V111" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="112">
-      <c r="U112" t="s">
+      <c r="V112" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="113">
-      <c r="U113" t="s">
+      <c r="V113" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="114">
-      <c r="U114" t="s">
+      <c r="V114" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="115">
-      <c r="U115" t="s">
+      <c r="V115" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="116">
-      <c r="U116" t="s">
+      <c r="V116" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="117">
-      <c r="U117" t="s">
+      <c r="V117" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- alpha version of Nexial Interactive now available! Not fully tested; please kindly report issues on GitHub. - optimize the resolution of hostname (of test harness). -
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -42,7 +42,7 @@
     <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
     <definedName name="step">'#system'!$U$2:$U$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$27</definedName>
-    <definedName name="web">'#system'!$V$2:$V$117</definedName>
+    <definedName name="web">'#system'!$V$2:$V$118</definedName>
     <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
     <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
     <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10193" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10668" uniqueCount="506">
   <si>
     <t>description</t>
   </si>
@@ -1576,6 +1576,12 @@
   </si>
   <si>
     <t>sendTextMail(profile,to,subject,body)</t>
+  </si>
+  <si>
+    <t>sendHtmlMail(profile,to,subject,body)</t>
+  </si>
+  <si>
+    <t>clickWithKeys(locator,keys)</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1589,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="325" x14ac:knownFonts="1">
+  <fonts count="341" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3625,8 +3631,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="570">
+  <fills count="597">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6852,8 +6959,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="590">
+  <borders count="618">
     <border>
       <left/>
       <right/>
@@ -6875,6 +7135,288 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -12804,7 +13346,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="336">
+  <cellXfs count="352">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -13770,52 +14312,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="308" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="309" fillId="545" borderId="569" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="569" fillId="545" fontId="309" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="310" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="310" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="311" fillId="548" borderId="573" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="573" fillId="548" fontId="311" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="312" fillId="551" borderId="577" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="577" fillId="551" fontId="312" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="313" fillId="554" borderId="577" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="577" fillId="554" fontId="313" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="314" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="314" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="315" fillId="557" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="557" fontId="315" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="316" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="316" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="317" fillId="560" borderId="581" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="581" fillId="560" fontId="317" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="318" fillId="563" borderId="585" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="585" fillId="563" fontId="318" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="319" fillId="566" borderId="589" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="566" fontId="319" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="320" fillId="566" borderId="589" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="566" fontId="320" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="321" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="554" fontId="321" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="322" fillId="569" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="569" fontId="322" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="323" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="554" fontId="323" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="324" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="324" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="325" fillId="572" borderId="597" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="326" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="327" fillId="575" borderId="601" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="328" fillId="578" borderId="605" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="329" fillId="581" borderId="605" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="330" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="331" fillId="584" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="332" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="333" fillId="587" borderId="609" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="334" fillId="590" borderId="613" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="335" fillId="593" borderId="617" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="336" fillId="593" borderId="617" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="337" fillId="581" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="338" fillId="596" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="339" fillId="581" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="340" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -14113,7 +14703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB117"/>
+  <dimension ref="A1:AB118"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -14213,7 +14803,7 @@
         <v>373</v>
       </c>
       <c r="C2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
@@ -15322,7 +15912,7 @@
         <v>357</v>
       </c>
       <c r="V51" t="s">
-        <v>123</v>
+        <v>505</v>
       </c>
     </row>
     <row r="52">
@@ -15330,7 +15920,7 @@
         <v>332</v>
       </c>
       <c r="V52" t="s">
-        <v>347</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53">
@@ -15338,7 +15928,7 @@
         <v>269</v>
       </c>
       <c r="V53" t="s">
-        <v>498</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54">
@@ -15346,7 +15936,7 @@
         <v>293</v>
       </c>
       <c r="V54" t="s">
-        <v>124</v>
+        <v>498</v>
       </c>
     </row>
     <row r="55">
@@ -15354,7 +15944,7 @@
         <v>294</v>
       </c>
       <c r="V55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56">
@@ -15362,7 +15952,7 @@
         <v>295</v>
       </c>
       <c r="V56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57">
@@ -15370,7 +15960,7 @@
         <v>305</v>
       </c>
       <c r="V57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58">
@@ -15378,7 +15968,7 @@
         <v>314</v>
       </c>
       <c r="V58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59">
@@ -15386,7 +15976,7 @@
         <v>338</v>
       </c>
       <c r="V59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60">
@@ -15394,7 +15984,7 @@
         <v>311</v>
       </c>
       <c r="V60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61">
@@ -15402,7 +15992,7 @@
         <v>312</v>
       </c>
       <c r="V61" t="s">
-        <v>475</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62">
@@ -15410,7 +16000,7 @@
         <v>370</v>
       </c>
       <c r="V62" t="s">
-        <v>206</v>
+        <v>475</v>
       </c>
     </row>
     <row r="63">
@@ -15418,7 +16008,7 @@
         <v>371</v>
       </c>
       <c r="V63" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64">
@@ -15426,7 +16016,7 @@
         <v>346</v>
       </c>
       <c r="V64" t="s">
-        <v>480</v>
+        <v>390</v>
       </c>
     </row>
     <row r="65">
@@ -15434,7 +16024,7 @@
         <v>315</v>
       </c>
       <c r="V65" t="s">
-        <v>131</v>
+        <v>480</v>
       </c>
     </row>
     <row r="66">
@@ -15442,7 +16032,7 @@
         <v>270</v>
       </c>
       <c r="V66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67">
@@ -15450,7 +16040,7 @@
         <v>354</v>
       </c>
       <c r="V67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68">
@@ -15458,7 +16048,7 @@
         <v>316</v>
       </c>
       <c r="V68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69">
@@ -15466,7 +16056,7 @@
         <v>409</v>
       </c>
       <c r="V69" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70">
@@ -15474,7 +16064,7 @@
         <v>306</v>
       </c>
       <c r="V70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71">
@@ -15482,7 +16072,7 @@
         <v>410</v>
       </c>
       <c r="V71" t="s">
-        <v>493</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72">
@@ -15490,7 +16080,7 @@
         <v>263</v>
       </c>
       <c r="V72" t="s">
-        <v>135</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73">
@@ -15498,7 +16088,7 @@
         <v>345</v>
       </c>
       <c r="V73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74">
@@ -15506,7 +16096,7 @@
         <v>281</v>
       </c>
       <c r="V74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75">
@@ -15514,7 +16104,7 @@
         <v>287</v>
       </c>
       <c r="V75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76">
@@ -15522,7 +16112,7 @@
         <v>292</v>
       </c>
       <c r="V76" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77">
@@ -15530,7 +16120,7 @@
         <v>464</v>
       </c>
       <c r="V77" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78">
@@ -15538,7 +16128,7 @@
         <v>333</v>
       </c>
       <c r="V78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79">
@@ -15546,7 +16136,7 @@
         <v>271</v>
       </c>
       <c r="V79" t="s">
-        <v>492</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80">
@@ -15554,7 +16144,7 @@
         <v>282</v>
       </c>
       <c r="V80" t="s">
-        <v>193</v>
+        <v>492</v>
       </c>
     </row>
     <row r="81">
@@ -15562,7 +16152,7 @@
         <v>288</v>
       </c>
       <c r="V81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82">
@@ -15570,7 +16160,7 @@
         <v>277</v>
       </c>
       <c r="V82" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83">
@@ -15578,7 +16168,7 @@
         <v>272</v>
       </c>
       <c r="V83" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84">
@@ -15586,7 +16176,7 @@
         <v>289</v>
       </c>
       <c r="V84" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85">
@@ -15594,7 +16184,7 @@
         <v>273</v>
       </c>
       <c r="V85" t="s">
-        <v>472</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86">
@@ -15602,7 +16192,7 @@
         <v>274</v>
       </c>
       <c r="V86" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="87">
@@ -15610,7 +16200,7 @@
         <v>307</v>
       </c>
       <c r="V87" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
     </row>
     <row r="88">
@@ -15618,7 +16208,7 @@
         <v>313</v>
       </c>
       <c r="V88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89">
@@ -15626,7 +16216,7 @@
         <v>296</v>
       </c>
       <c r="V89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90">
@@ -15634,7 +16224,7 @@
         <v>341</v>
       </c>
       <c r="V90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91">
@@ -15642,7 +16232,7 @@
         <v>278</v>
       </c>
       <c r="V91" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92">
@@ -15650,131 +16240,136 @@
         <v>279</v>
       </c>
       <c r="V92" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93">
       <c r="V93" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94">
       <c r="V94" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95">
       <c r="V95" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="96">
       <c r="V96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97">
       <c r="V97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98">
       <c r="V98" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99">
       <c r="V99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100">
       <c r="V100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101">
       <c r="V101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102">
       <c r="V102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103">
       <c r="V103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104">
       <c r="V104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105">
       <c r="V105" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106">
       <c r="V106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107">
       <c r="V107" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="108">
       <c r="V108" t="s">
-        <v>481</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109">
       <c r="V109" t="s">
-        <v>155</v>
+        <v>481</v>
       </c>
     </row>
     <row r="110">
       <c r="V110" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111">
       <c r="V111" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="112">
       <c r="V112" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="113">
       <c r="V113" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114">
       <c r="V114" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115">
       <c r="V115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116">
       <c r="V116" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117">
       <c r="V117" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="V118" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- update documentation on io.saveFileMeta()
[Nexial Expression]
- [JSON &raquo; `beautify`]: *NEW* beautify `json` to improve readability.
- [JSON &raquo; `minify`]: *NEW* minify `json` to improve data transfer efficiency.

### [json command]
- [`beautify(json,var)`]: *NEW* beautify `json` to improve readability.
- [`minify(json,var)`]: *NEW* minify `json` to improve data transfer efficiency.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -29,7 +29,7 @@
     <definedName name="image">'#system'!$I$2:$I$6</definedName>
     <definedName name="io">'#system'!$J$2:$J$25</definedName>
     <definedName name="jms">'#system'!$K$2:$K$4</definedName>
-    <definedName name="json">'#system'!$L$2:$L$14</definedName>
+    <definedName name="json">'#system'!$L$2:$L$16</definedName>
     <definedName name="mail">'#system'!$M$2:$M$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2020" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="508">
   <si>
     <t>description</t>
   </si>
@@ -1582,6 +1582,12 @@
   </si>
   <si>
     <t>searchAndReplace(file,config,saveAs)</t>
+  </si>
+  <si>
+    <t>minify(json,var)</t>
+  </si>
+  <si>
+    <t>beautify(json,var)</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1595,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="88" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1946,8 +1952,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="84">
+  <fills count="138">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2419,8 +2627,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="86">
+  <borders count="142">
     <border>
       <left/>
       <right/>
@@ -3289,13 +3803,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="99">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3454,52 +4532,148 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="59" borderId="65" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="65" fillId="59" fontId="40" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="41" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="62" borderId="69" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="69" fillId="62" fontId="42" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="65" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="65" fontId="43" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="68" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="68" fontId="44" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="45" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="71" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="71" fontId="46" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="47" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="74" borderId="77" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="74" fontId="48" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="77" borderId="81" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="81" fillId="77" fontId="49" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="80" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="80" fontId="50" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="80" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="80" fontId="51" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="68" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="52" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="83" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="53" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="68" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="68" fontId="54" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="55" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="93" fillId="86" fontId="56" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="57" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="97" fillId="89" fontId="58" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="101" fillId="92" fontId="59" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="101" fillId="95" fontId="60" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="61" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="98" fontId="62" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="63" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="105" fillId="101" fontId="64" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="109" fillId="104" fontId="65" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="107" fontId="66" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="107" fontId="67" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="68" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="69" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="70" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="71" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="113" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="116" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="119" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="122" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="128" borderId="133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="131" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="134" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="134" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4452,7 +5626,7 @@
         <v>13</v>
       </c>
       <c r="L11" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="N11" t="s">
         <v>85</v>
@@ -4487,7 +5661,7 @@
         <v>35</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>476</v>
       </c>
       <c r="N12" t="s">
         <v>34</v>
@@ -4519,7 +5693,7 @@
         <v>73</v>
       </c>
       <c r="L13" t="s">
-        <v>33</v>
+        <v>506</v>
       </c>
       <c r="N13" t="s">
         <v>86</v>
@@ -4551,7 +5725,7 @@
         <v>74</v>
       </c>
       <c r="L14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N14" t="s">
         <v>87</v>
@@ -4579,6 +5753,9 @@
       <c r="J15" t="s">
         <v>491</v>
       </c>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
       <c r="N15" t="s">
         <v>88</v>
       </c>
@@ -4604,6 +5781,9 @@
       </c>
       <c r="J16" t="s">
         <v>75</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
       </c>
       <c r="O16" t="s">
         <v>243</v>

</xml_diff>

<commit_message>
[System Variables]: - [`nexial.web.dragFrom`]: **NEW** determine where the "drag" action on a web element should start from.
[Nexial Expression]:
- code fix to enable the use of `]` character as part of operation parameter.

[web commands]
- [`dragTo(fromLocator,xOffset,yOffset)`]: **NEW** automates the "drag" action on a web element.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,12 +43,12 @@
     <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
     <definedName name="step">'#system'!$U$2:$U$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$27</definedName>
-    <definedName name="web">'#system'!$V$2:$V$119</definedName>
+    <definedName name="web">'#system'!$V$2:$V$120</definedName>
     <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
     <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
     <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
     <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="xml">'#system'!$AA$2:$AA$11</definedName>
+    <definedName name="xml">'#system'!$AA$2:$AA$13</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3468" uniqueCount="511">
   <si>
     <t>description</t>
   </si>
@@ -1588,6 +1588,15 @@
   </si>
   <si>
     <t>beautify(json,var)</t>
+  </si>
+  <si>
+    <t>dragTo(fromLocator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>beautify(xml,var)</t>
+  </si>
+  <si>
+    <t>minify(xml,var)</t>
   </si>
 </sst>
 </file>
@@ -1595,7 +1604,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="88" x14ac:knownFonts="1">
+  <fonts count="104" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2154,8 +2163,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="138">
+  <fills count="165">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2933,8 +3043,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="142">
+  <borders count="170">
     <border>
       <left/>
       <right/>
@@ -4367,13 +4630,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="115">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4628,52 +5173,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="71" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="113" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="113" fontId="72" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="73" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="116" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="125" fillId="116" fontId="74" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="119" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="119" fontId="75" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="122" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="122" fontId="76" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="77" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="78" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="79" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="128" borderId="133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="133" fillId="128" fontId="80" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="131" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="137" fillId="131" fontId="81" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="134" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="134" fontId="82" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="134" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="141" fillId="134" fontId="83" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="84" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="84" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="137" fontId="85" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="86" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="122" fontId="86" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="87" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="140" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="143" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="146" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="149" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="152" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="155" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="158" borderId="165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="161" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="161" borderId="169" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="149" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="164" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="149" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4971,7 +5564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB119"/>
+  <dimension ref="A1:AB120"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -5568,7 +6161,7 @@
         <v>181</v>
       </c>
       <c r="AA9" t="s">
-        <v>226</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10">
@@ -5606,7 +6199,7 @@
         <v>182</v>
       </c>
       <c r="AA10" t="s">
-        <v>227</v>
+        <v>510</v>
       </c>
     </row>
     <row r="11">
@@ -5641,7 +6234,7 @@
         <v>260</v>
       </c>
       <c r="AA11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12">
@@ -5675,6 +6268,9 @@
       <c r="Y12" t="s">
         <v>183</v>
       </c>
+      <c r="AA12" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -5707,6 +6303,9 @@
       <c r="Y13" t="s">
         <v>184</v>
       </c>
+      <c r="AA13" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -6294,7 +6893,7 @@
         <v>371</v>
       </c>
       <c r="V63" t="s">
-        <v>206</v>
+        <v>508</v>
       </c>
     </row>
     <row r="64">
@@ -6302,7 +6901,7 @@
         <v>346</v>
       </c>
       <c r="V64" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65">
@@ -6310,7 +6909,7 @@
         <v>315</v>
       </c>
       <c r="V65" t="s">
-        <v>478</v>
+        <v>390</v>
       </c>
     </row>
     <row r="66">
@@ -6318,7 +6917,7 @@
         <v>270</v>
       </c>
       <c r="V66" t="s">
-        <v>131</v>
+        <v>478</v>
       </c>
     </row>
     <row r="67">
@@ -6326,7 +6925,7 @@
         <v>354</v>
       </c>
       <c r="V67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68">
@@ -6334,7 +6933,7 @@
         <v>316</v>
       </c>
       <c r="V68" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69">
@@ -6342,7 +6941,7 @@
         <v>409</v>
       </c>
       <c r="V69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70">
@@ -6350,7 +6949,7 @@
         <v>306</v>
       </c>
       <c r="V70" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71">
@@ -6358,7 +6957,7 @@
         <v>410</v>
       </c>
       <c r="V71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72">
@@ -6366,7 +6965,7 @@
         <v>263</v>
       </c>
       <c r="V72" t="s">
-        <v>489</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73">
@@ -6374,7 +6973,7 @@
         <v>345</v>
       </c>
       <c r="V73" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
     </row>
     <row r="74">
@@ -6382,7 +6981,7 @@
         <v>281</v>
       </c>
       <c r="V74" t="s">
-        <v>135</v>
+        <v>502</v>
       </c>
     </row>
     <row r="75">
@@ -6390,7 +6989,7 @@
         <v>287</v>
       </c>
       <c r="V75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76">
@@ -6398,7 +6997,7 @@
         <v>292</v>
       </c>
       <c r="V76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77">
@@ -6406,7 +7005,7 @@
         <v>464</v>
       </c>
       <c r="V77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78">
@@ -6414,7 +7013,7 @@
         <v>333</v>
       </c>
       <c r="V78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79">
@@ -6422,7 +7021,7 @@
         <v>271</v>
       </c>
       <c r="V79" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80">
@@ -6430,7 +7029,7 @@
         <v>282</v>
       </c>
       <c r="V80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81">
@@ -6438,7 +7037,7 @@
         <v>288</v>
       </c>
       <c r="V81" t="s">
-        <v>488</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82">
@@ -6446,7 +7045,7 @@
         <v>277</v>
       </c>
       <c r="V82" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
     </row>
     <row r="83">
@@ -6454,7 +7053,7 @@
         <v>272</v>
       </c>
       <c r="V83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84">
@@ -6462,7 +7061,7 @@
         <v>289</v>
       </c>
       <c r="V84" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85">
@@ -6470,7 +7069,7 @@
         <v>273</v>
       </c>
       <c r="V85" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86">
@@ -6478,7 +7077,7 @@
         <v>274</v>
       </c>
       <c r="V86" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87">
@@ -6486,7 +7085,7 @@
         <v>307</v>
       </c>
       <c r="V87" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88">
@@ -6494,7 +7093,7 @@
         <v>313</v>
       </c>
       <c r="V88" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="89">
@@ -6502,7 +7101,7 @@
         <v>296</v>
       </c>
       <c r="V89" t="s">
-        <v>196</v>
+        <v>472</v>
       </c>
     </row>
     <row r="90">
@@ -6510,7 +7109,7 @@
         <v>341</v>
       </c>
       <c r="V90" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91">
@@ -6518,7 +7117,7 @@
         <v>278</v>
       </c>
       <c r="V91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92">
@@ -6526,141 +7125,146 @@
         <v>279</v>
       </c>
       <c r="V92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93">
       <c r="V93" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94">
       <c r="V94" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95">
       <c r="V95" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96">
       <c r="V96" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="97">
       <c r="V97" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="98">
       <c r="V98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99">
       <c r="V99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100">
       <c r="V100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101">
       <c r="V101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102">
       <c r="V102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103">
       <c r="V103" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104">
       <c r="V104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105">
       <c r="V105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106">
       <c r="V106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107">
       <c r="V107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108">
       <c r="V108" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109">
       <c r="V109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110">
       <c r="V110" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111">
       <c r="V111" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="112">
       <c r="V112" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="113">
       <c r="V113" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="114">
       <c r="V114" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115">
       <c r="V115" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="116">
       <c r="V116" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="117">
       <c r="V117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118">
       <c r="V118" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119">
       <c r="V119" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="V120" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Nexial now supports email notification with customized `subject`, `cc`, `bcc`, `from`, `footer`. One can optionally configure such email to be sent as HTML or plain text (default). See [Execution Event Notification] for more details.   - remove `nexial.notifyAsHTML` System variable removed. - SMS notification: now supports configurable execution metada inclusion as a footer. - [base &raquo; `repeatUntil(steps,maxWaitMs)`]: enhanced with additional logging to aid in troubleshooting and debugging.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4454" uniqueCount="519">
   <si>
     <t>description</t>
   </si>
@@ -1619,6 +1619,9 @@
   </si>
   <si>
     <t>saveAttributeList(var,locator,attrName)</t>
+  </si>
+  <si>
+    <t>assertIENativeMode()</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1629,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="120" x14ac:knownFonts="1">
+  <fonts count="136" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2387,8 +2390,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="192">
+  <fills count="219">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3472,8 +3576,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="198">
+  <borders count="226">
     <border>
       <left/>
       <right/>
@@ -5470,13 +5727,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="147">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5827,52 +6366,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="103" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="104" fillId="167" borderId="177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="177" fillId="167" fontId="104" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="105" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="106" fillId="170" borderId="181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="181" fillId="170" fontId="106" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="107" fillId="173" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="185" fillId="173" fontId="107" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="108" fillId="176" borderId="185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="185" fillId="176" fontId="108" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="109" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="110" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="179" fontId="110" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="111" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="112" fillId="182" borderId="189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="189" fillId="182" fontId="112" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="113" fillId="185" borderId="193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="193" fillId="185" fontId="113" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="114" fillId="188" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="197" fillId="188" fontId="114" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="115" fillId="188" borderId="197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="197" fillId="188" fontId="115" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="116" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="176" fontId="116" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="117" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="191" fontId="117" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="118" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="176" fontId="118" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="119" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="194" borderId="205" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="197" borderId="209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="200" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="203" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="206" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="209" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="212" borderId="221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="215" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="215" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="218" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7100,7 +7687,7 @@
         <v>393</v>
       </c>
       <c r="W21" t="s">
-        <v>101</v>
+        <v>518</v>
       </c>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
- [project id binding]: use `.meta/project.id` to bind project identification across sandboxes (local project directory) instead of using project directory name. The same binding now affects cloud storage location to keep output of the same project together. - move `nexial-3rdparty.log` under execution-specific log directory
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4454" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4947" uniqueCount="519">
   <si>
     <t>description</t>
   </si>
@@ -1629,7 +1629,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="136" x14ac:knownFonts="1">
+  <fonts count="152" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2491,8 +2491,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="219">
+  <fills count="246">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3729,8 +3830,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="226">
+  <borders count="254">
     <border>
       <left/>
       <right/>
@@ -6009,13 +6263,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="163">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -6414,52 +6950,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="119" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="120" fillId="194" borderId="205" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="205" fillId="194" fontId="120" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="121" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="122" fillId="197" borderId="209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="209" fillId="197" fontId="122" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="123" fillId="200" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="213" fillId="200" fontId="123" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="124" fillId="203" borderId="213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="213" fillId="203" fontId="124" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="125" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="126" fillId="206" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="206" fontId="126" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="127" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="128" fillId="209" borderId="217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="217" fillId="209" fontId="128" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="129" fillId="212" borderId="221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="221" fillId="212" fontId="129" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="130" fillId="215" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="225" fillId="215" fontId="130" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="131" fillId="215" borderId="225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="225" fillId="215" fontId="131" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="132" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="203" fontId="132" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="133" fillId="218" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="218" fontId="133" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="134" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="203" fontId="134" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="135" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="221" borderId="233" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="224" borderId="237" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="227" borderId="241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="230" borderId="241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="233" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="236" borderId="245" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="239" borderId="249" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="242" borderId="253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="242" borderId="253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="230" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="245" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="230" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[aws.sqs] - [`deleteMessage(profile,queue,receiptHandle)`]: **NEW** command to delete a message from a AWS SQS queue. - add support for read timeout for 'receiveMessage' - add support for visibility timeout for 'receiveMessage'
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,37 +19,38 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$D$2:$D$38</definedName>
-    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
+    <definedName name="base">'#system'!$E$2:$E$38</definedName>
+    <definedName name="csv">'#system'!$F$2:$F$5</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
-    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
-    <definedName name="external">'#system'!$H$2:$H$4</definedName>
-    <definedName name="image">'#system'!$I$2:$I$6</definedName>
-    <definedName name="io">'#system'!$J$2:$J$25</definedName>
-    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
-    <definedName name="json">'#system'!$L$2:$L$16</definedName>
-    <definedName name="mail">'#system'!$N$2:$N$2</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$92</definedName>
+    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
+    <definedName name="external">'#system'!$I$2:$I$4</definedName>
+    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="io">'#system'!$K$2:$K$25</definedName>
+    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
+    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="mail">'#system'!$O$2:$O$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$O$2:$O$15</definedName>
-    <definedName name="pdf">'#system'!$P$2:$P$16</definedName>
-    <definedName name="rdbms">'#system'!$Q$2:$Q$7</definedName>
-    <definedName name="redis">'#system'!$R$2:$R$10</definedName>
-    <definedName name="sms">'#system'!$S$2:$S$2</definedName>
-    <definedName name="sound">'#system'!$T$2:$T$5</definedName>
-    <definedName name="ssh">'#system'!$U$2:$U$9</definedName>
-    <definedName name="step">'#system'!$V$2:$V$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$28</definedName>
-    <definedName name="web">'#system'!$W$2:$W$122</definedName>
-    <definedName name="webalert">'#system'!$X$2:$X$8</definedName>
-    <definedName name="webcookie">'#system'!$Y$2:$Y$8</definedName>
-    <definedName name="ws">'#system'!$Z$2:$Z$17</definedName>
-    <definedName name="ws.async">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="xml">'#system'!$AB$2:$AB$13</definedName>
-    <definedName name="macro">'#system'!$M$2:$M$4</definedName>
+    <definedName name="number">'#system'!$P$2:$P$15</definedName>
+    <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
+    <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
+    <definedName name="redis">'#system'!$S$2:$S$10</definedName>
+    <definedName name="sms">'#system'!$T$2:$T$2</definedName>
+    <definedName name="sound">'#system'!$U$2:$U$5</definedName>
+    <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
+    <definedName name="step">'#system'!$W$2:$W$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$29</definedName>
+    <definedName name="web">'#system'!$X$2:$X$122</definedName>
+    <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
+    <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
+    <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="xml">'#system'!$AC$2:$AC$13</definedName>
+    <definedName name="macro">'#system'!$N$2:$N$4</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4947" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6432" uniqueCount="524">
   <si>
     <t>description</t>
   </si>
@@ -1622,6 +1623,21 @@
   </si>
   <si>
     <t>assertIENativeMode()</t>
+  </si>
+  <si>
+    <t>aws.sqs</t>
+  </si>
+  <si>
+    <t>deleteMessage(profile,queue,receiptHandle)</t>
+  </si>
+  <si>
+    <t>receiveMessage(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>receiveMessages(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>sendMessage(profile,queue,message,var)</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1645,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="152" x14ac:knownFonts="1">
+  <fonts count="200" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2592,8 +2608,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="246">
+  <fills count="327">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3983,8 +4302,467 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="254">
+  <borders count="338">
     <border>
       <left/>
       <right/>
@@ -6545,13 +7323,859 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="211">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -6998,52 +8622,196 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="135" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="136" fillId="221" borderId="233" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="233" fillId="221" fontId="136" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="137" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="138" fillId="224" borderId="237" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="237" fillId="224" fontId="138" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="139" fillId="227" borderId="241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="241" fillId="227" fontId="139" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="140" fillId="230" borderId="241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="241" fillId="230" fontId="140" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="141" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="142" fillId="233" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="233" fontId="142" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="143" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="144" fillId="236" borderId="245" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="245" fillId="236" fontId="144" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="145" fillId="239" borderId="249" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="249" fillId="239" fontId="145" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="146" fillId="242" borderId="253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="253" fillId="242" fontId="146" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="147" fillId="242" borderId="253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="253" fillId="242" fontId="147" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="148" fillId="230" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="230" fontId="148" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="149" fillId="245" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="245" fontId="149" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="150" fillId="230" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="230" fontId="150" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="151" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="261" fillId="248" fontId="152" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="153" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="265" fillId="251" fontId="154" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="269" fillId="254" fontId="155" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="269" fillId="257" fontId="156" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="157" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="260" fontId="158" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="159" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="273" fillId="263" fontId="160" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="277" fillId="266" fontId="161" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="281" fillId="269" fontId="162" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="281" fillId="269" fontId="163" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="257" fontId="164" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="272" fontId="165" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="257" fontId="166" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="167" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="289" fillId="275" fontId="168" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="169" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="293" fillId="278" fontId="170" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="297" fillId="281" fontId="171" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="297" fillId="284" fontId="172" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="173" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="287" fontId="174" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="175" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="301" fillId="290" fontId="176" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="305" fillId="293" fontId="177" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="309" fillId="296" fontId="178" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="309" fillId="296" fontId="179" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="284" fontId="180" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="299" fontId="181" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="284" fontId="182" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="183" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="302" borderId="317" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="305" borderId="321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="187" fillId="308" borderId="325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="188" fillId="311" borderId="325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="314" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="191" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="317" borderId="329" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="193" fillId="320" borderId="333" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="194" fillId="323" borderId="337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="195" fillId="323" borderId="337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="196" fillId="311" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="197" fillId="326" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="198" fillId="311" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="199" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7341,7 +9109,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC122"/>
+  <dimension ref="A1:AD122"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -7361,78 +9129,81 @@
         <v>497</v>
       </c>
       <c r="D1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>348</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>334</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>246</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>188</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>230</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>399</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>456</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>413</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>358</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>395</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>458</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -7447,78 +9218,81 @@
         <v>499</v>
       </c>
       <c r="D2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>484</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>71</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>501</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>317</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>385</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>465</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>513</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>412</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>466</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>244</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>209</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>400</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>457</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>454</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>382</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>396</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>89</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>163</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>168</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>175</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>468</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>219</v>
       </c>
     </row>
@@ -7533,1543 +9307,1555 @@
         <v>498</v>
       </c>
       <c r="D3" t="s">
+        <v>521</v>
+      </c>
+      <c r="E3" t="s">
         <v>492</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>366</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>511</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>350</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>342</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>335</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>78</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>514</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>467</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>231</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>210</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>401</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>415</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>383</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>397</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>90</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>164</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>169</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>365</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>176</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>519</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
       </c>
       <c r="D4" t="s">
+        <v>522</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>388</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>485</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>512</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>351</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>229</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>336</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>515</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>232</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>211</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>402</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>416</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>359</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>398</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>355</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>165</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>170</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>176</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>459</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
       </c>
       <c r="D5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E5" t="s">
         <v>493</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>474</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>337</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>490</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>352</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>495</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>79</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>23</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>233</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>212</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>403</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>417</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>360</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>356</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>166</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>171</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>177</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>460</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>389</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>486</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>349</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>24</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>234</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>392</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>404</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>362</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>91</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>480</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>172</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>178</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>461</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>215</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>367</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>482</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>317</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>26</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>235</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>414</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>405</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>361</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>92</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>481</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>173</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>179</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>462</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>320</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>368</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>329</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>72</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>27</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>83</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>236</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>406</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>363</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>93</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>167</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>174</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>180</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>463</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>308</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>330</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>31</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>84</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>237</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>407</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>364</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>201</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>181</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
         <v>317</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>353</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>487</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>391</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>469</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>238</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>408</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>258</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>182</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>334</v>
-      </c>
-      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>250</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>275</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>323</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>13</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>507</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>85</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>239</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>259</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>260</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E12" t="s">
         <v>321</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>264</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>324</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>35</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>476</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>34</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>240</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>94</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>183</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>246</v>
-      </c>
-      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
         <v>342</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>318</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>325</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>73</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>506</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>86</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>245</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>327</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>184</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>188</v>
-      </c>
-      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>265</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>326</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>74</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>32</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>87</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>241</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>95</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>266</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>491</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>33</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>88</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>242</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>96</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
         <v>386</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>319</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>75</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>36</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>243</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>67</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" t="s">
         <v>387</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>81</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>76</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>97</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>399</v>
-      </c>
-      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
         <v>411</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>82</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>381</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>456</v>
-      </c>
-      <c r="D19" t="s">
+        <v>399</v>
+      </c>
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>297</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>505</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>413</v>
-      </c>
-      <c r="D20" t="s">
+        <v>456</v>
+      </c>
+      <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>298</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>37</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>358</v>
-      </c>
-      <c r="D21" t="s">
+        <v>413</v>
+      </c>
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>299</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>393</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>395</v>
-      </c>
-      <c r="D22" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" t="s">
         <v>322</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>300</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>77</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s">
+        <v>395</v>
+      </c>
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>291</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>475</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
         <v>483</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>280</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>38</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
         <v>216</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>39</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="s">
         <v>217</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>283</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>458</v>
-      </c>
-      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
         <v>503</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>267</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>458</v>
+      </c>
+      <c r="E28" t="s">
+        <v>504</v>
+      </c>
+      <c r="G28" t="s">
+        <v>284</v>
+      </c>
+      <c r="X28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
         <v>218</v>
       </c>
-      <c r="D28" t="s">
-        <v>504</v>
-      </c>
-      <c r="F28" t="s">
-        <v>284</v>
-      </c>
-      <c r="W28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>453</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>285</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30">
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>56</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>208</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="31">
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>57</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>276</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32">
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>58</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>286</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33">
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>59</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>261</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="34">
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>331</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="35">
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>61</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>309</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36">
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>62</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>262</v>
       </c>
-      <c r="W36" t="s">
+      <c r="X36" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="37">
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>63</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>310</v>
       </c>
-      <c r="W37" t="s">
+      <c r="X37" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="38">
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>268</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="39">
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>70</v>
       </c>
-      <c r="W39" t="s">
+      <c r="X39" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40">
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>204</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="41">
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>290</v>
       </c>
-      <c r="W41" t="s">
+      <c r="X41" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="42">
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>301</v>
       </c>
-      <c r="W42" t="s">
+      <c r="X42" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="43">
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>302</v>
       </c>
-      <c r="W43" t="s">
+      <c r="X43" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="44">
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>344</v>
       </c>
-      <c r="W44" t="s">
+      <c r="X44" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="45">
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>343</v>
       </c>
-      <c r="W45" t="s">
+      <c r="X45" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="46">
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>203</v>
       </c>
-      <c r="W46" t="s">
+      <c r="X46" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="47">
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>303</v>
       </c>
-      <c r="W47" t="s">
+      <c r="X47" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="48">
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>340</v>
       </c>
-      <c r="W48" t="s">
+      <c r="X48" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="49">
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>369</v>
       </c>
-      <c r="W49" t="s">
+      <c r="X49" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="50">
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>304</v>
       </c>
-      <c r="W50" t="s">
+      <c r="X50" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="51">
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>357</v>
       </c>
-      <c r="W51" t="s">
+      <c r="X51" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="52">
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>332</v>
       </c>
-      <c r="W52" t="s">
+      <c r="X52" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="53">
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>269</v>
       </c>
-      <c r="W53" t="s">
+      <c r="X53" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="54">
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>293</v>
       </c>
-      <c r="W54" t="s">
+      <c r="X54" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="55">
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>294</v>
       </c>
-      <c r="W55" t="s">
+      <c r="X55" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="56">
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>295</v>
       </c>
-      <c r="W56" t="s">
+      <c r="X56" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="57">
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>305</v>
       </c>
-      <c r="W57" t="s">
+      <c r="X57" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58">
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>314</v>
       </c>
-      <c r="W58" t="s">
+      <c r="X58" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="59">
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>338</v>
       </c>
-      <c r="W59" t="s">
+      <c r="X59" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="60">
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>311</v>
       </c>
-      <c r="W60" t="s">
+      <c r="X60" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="61">
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>312</v>
       </c>
-      <c r="W61" t="s">
+      <c r="X61" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="62">
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>370</v>
       </c>
-      <c r="W62" t="s">
+      <c r="X62" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="63">
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>371</v>
       </c>
-      <c r="W63" t="s">
+      <c r="X63" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="64">
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>346</v>
       </c>
-      <c r="W64" t="s">
+      <c r="X64" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="65">
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>315</v>
       </c>
-      <c r="W65" t="s">
+      <c r="X65" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="66">
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>270</v>
       </c>
-      <c r="W66" t="s">
+      <c r="X66" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="67">
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>354</v>
       </c>
-      <c r="W67" t="s">
+      <c r="X67" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="68">
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>316</v>
       </c>
-      <c r="W68" t="s">
+      <c r="X68" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="69">
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>409</v>
       </c>
-      <c r="W69" t="s">
+      <c r="X69" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="70">
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>306</v>
       </c>
-      <c r="W70" t="s">
+      <c r="X70" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="71">
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>410</v>
       </c>
-      <c r="W71" t="s">
+      <c r="X71" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="72">
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>263</v>
       </c>
-      <c r="W72" t="s">
+      <c r="X72" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="73">
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>345</v>
       </c>
-      <c r="W73" t="s">
+      <c r="X73" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="74">
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>281</v>
       </c>
-      <c r="W74" t="s">
+      <c r="X74" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="75">
-      <c r="F75" t="s">
+      <c r="G75" t="s">
         <v>287</v>
       </c>
-      <c r="W75" t="s">
+      <c r="X75" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="76">
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>292</v>
       </c>
-      <c r="W76" t="s">
+      <c r="X76" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="77">
-      <c r="F77" t="s">
+      <c r="G77" t="s">
         <v>464</v>
       </c>
-      <c r="W77" t="s">
+      <c r="X77" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="78">
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>333</v>
       </c>
-      <c r="W78" t="s">
+      <c r="X78" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="79">
-      <c r="F79" t="s">
+      <c r="G79" t="s">
         <v>271</v>
       </c>
-      <c r="W79" t="s">
+      <c r="X79" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="80">
-      <c r="F80" t="s">
+      <c r="G80" t="s">
         <v>282</v>
       </c>
-      <c r="W80" t="s">
+      <c r="X80" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="81">
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>288</v>
       </c>
-      <c r="W81" t="s">
+      <c r="X81" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="82">
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>277</v>
       </c>
-      <c r="W82" t="s">
+      <c r="X82" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="83">
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>272</v>
       </c>
-      <c r="W83" t="s">
+      <c r="X83" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="84">
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>289</v>
       </c>
-      <c r="W84" t="s">
+      <c r="X84" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="85">
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>273</v>
       </c>
-      <c r="W85" t="s">
+      <c r="X85" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="86">
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>274</v>
       </c>
-      <c r="W86" t="s">
+      <c r="X86" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="87">
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>307</v>
       </c>
-      <c r="W87" t="s">
+      <c r="X87" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="88">
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>313</v>
       </c>
-      <c r="W88" t="s">
+      <c r="X88" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="89">
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>296</v>
       </c>
-      <c r="W89" t="s">
+      <c r="X89" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="90">
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>341</v>
       </c>
-      <c r="W90" t="s">
+      <c r="X90" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="91">
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>278</v>
       </c>
-      <c r="W91" t="s">
+      <c r="X91" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="92">
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>279</v>
       </c>
-      <c r="W92" t="s">
+      <c r="X92" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="93">
-      <c r="W93" t="s">
+      <c r="X93" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="94">
-      <c r="W94" t="s">
+      <c r="X94" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="95">
-      <c r="W95" t="s">
+      <c r="X95" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="96">
-      <c r="W96" t="s">
+      <c r="X96" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="97">
-      <c r="W97" t="s">
+      <c r="X97" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="98">
-      <c r="W98" t="s">
+      <c r="X98" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="99">
-      <c r="W99" t="s">
+      <c r="X99" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="100">
-      <c r="W100" t="s">
+      <c r="X100" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="101">
-      <c r="W101" t="s">
+      <c r="X101" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="102">
-      <c r="W102" t="s">
+      <c r="X102" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="103">
-      <c r="W103" t="s">
+      <c r="X103" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="104">
-      <c r="W104" t="s">
+      <c r="X104" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="105">
-      <c r="W105" t="s">
+      <c r="X105" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="106">
-      <c r="W106" t="s">
+      <c r="X106" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="107">
-      <c r="W107" t="s">
+      <c r="X107" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="108">
-      <c r="W108" t="s">
+      <c r="X108" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="109">
-      <c r="W109" t="s">
+      <c r="X109" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="110">
-      <c r="W110" t="s">
+      <c r="X110" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="111">
-      <c r="W111" t="s">
+      <c r="X111" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="112">
-      <c r="W112" t="s">
+      <c r="X112" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="113">
-      <c r="W113" t="s">
+      <c r="X113" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="114">
-      <c r="W114" t="s">
+      <c r="X114" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="115">
-      <c r="W115" t="s">
+      <c r="X115" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="116">
-      <c r="W116" t="s">
+      <c r="X116" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="117">
-      <c r="W117" t="s">
+      <c r="X117" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="118">
-      <c r="W118" t="s">
+      <c r="X118" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="119">
-      <c r="W119" t="s">
+      <c r="X119" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="120">
-      <c r="W120" t="s">
+      <c r="X120" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="121">
-      <c r="W121" t="s">
+      <c r="X121" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="122">
-      <c r="W122" t="s">
+      <c r="X122" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- [`nexial.web.clearWithBackspace`]: **NEW** System variable to forcefully clear out text input using BACKSPACE keystrokes. Default is `false` (i.e. not enabled).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,12 +43,12 @@
     <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
     <definedName name="step">'#system'!$W$2:$W$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$29</definedName>
-    <definedName name="web">'#system'!$X$2:$X$122</definedName>
+    <definedName name="web">'#system'!$X$2:$X$123</definedName>
     <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
     <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
-    <definedName name="xml">'#system'!$AC$2:$AC$18</definedName>
+    <definedName name="xml">'#system'!$AC$2:$AC$21</definedName>
     <definedName name="macro">'#system'!$N$2:$N$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
   </definedNames>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7444" uniqueCount="533">
   <si>
     <t>description</t>
   </si>
@@ -1653,6 +1653,18 @@
   </si>
   <si>
     <t>replace(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>rightClick(locator)</t>
+  </si>
+  <si>
+    <t>insertAfter(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>insertBefore(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replaceIn(xml,xpath,content,var)</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1672,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="216" x14ac:knownFonts="1">
+  <fonts count="232" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3027,8 +3039,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="354">
+  <fills count="381">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5030,8 +5143,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="366">
+  <borders count="394">
     <border>
       <left/>
       <right/>
@@ -8720,13 +8986,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="243">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9365,52 +9913,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="199" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="200" fillId="329" borderId="345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="345" fillId="329" fontId="200" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="201" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="201" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="202" fillId="332" borderId="349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="349" fillId="332" fontId="202" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="203" fillId="335" borderId="353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="353" fillId="335" fontId="203" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="204" fillId="338" borderId="353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="353" fillId="338" fontId="204" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="205" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="205" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="206" fillId="341" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="341" fontId="206" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="207" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="207" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="208" fillId="344" borderId="357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="357" fillId="344" fontId="208" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="209" fillId="347" borderId="361" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="361" fillId="347" fontId="209" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="210" fillId="350" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="365" fillId="350" fontId="210" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="211" fillId="350" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="365" fillId="350" fontId="211" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="212" fillId="338" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="338" fontId="212" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="213" fillId="353" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="353" fontId="213" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="214" fillId="338" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="338" fontId="214" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="215" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="215" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="216" fillId="356" borderId="373" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="217" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="218" fillId="359" borderId="377" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="219" fillId="362" borderId="381" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="220" fillId="365" borderId="381" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="221" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="222" fillId="368" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="223" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="224" fillId="371" borderId="385" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="225" fillId="374" borderId="389" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="226" fillId="377" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="227" fillId="377" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="228" fillId="365" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="229" fillId="380" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="230" fillId="365" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="231" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9708,7 +10304,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD122"/>
+  <dimension ref="A1:AD123"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -10478,7 +11074,7 @@
         <v>184</v>
       </c>
       <c r="AC13" t="s">
-        <v>510</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14">
@@ -10513,7 +11109,7 @@
         <v>185</v>
       </c>
       <c r="AC14" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15">
@@ -10545,7 +11141,7 @@
         <v>186</v>
       </c>
       <c r="AC15" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16">
@@ -10574,7 +11170,7 @@
         <v>187</v>
       </c>
       <c r="AC16" t="s">
-        <v>226</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17">
@@ -10597,7 +11193,7 @@
         <v>496</v>
       </c>
       <c r="AC17" t="s">
-        <v>227</v>
+        <v>528</v>
       </c>
     </row>
     <row r="18">
@@ -10617,7 +11213,7 @@
         <v>98</v>
       </c>
       <c r="AC18" t="s">
-        <v>228</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19">
@@ -10636,6 +11232,9 @@
       <c r="X19" t="s">
         <v>99</v>
       </c>
+      <c r="AC19" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -10653,6 +11252,9 @@
       <c r="X20" t="s">
         <v>100</v>
       </c>
+      <c r="AC20" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -10670,6 +11272,9 @@
       <c r="X21" t="s">
         <v>518</v>
       </c>
+      <c r="AC21" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -11216,7 +11821,7 @@
         <v>271</v>
       </c>
       <c r="X79" t="s">
-        <v>138</v>
+        <v>529</v>
       </c>
     </row>
     <row r="80">
@@ -11224,7 +11829,7 @@
         <v>282</v>
       </c>
       <c r="X80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81">
@@ -11232,7 +11837,7 @@
         <v>288</v>
       </c>
       <c r="X81" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82">
@@ -11240,7 +11845,7 @@
         <v>277</v>
       </c>
       <c r="X82" t="s">
-        <v>517</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83">
@@ -11248,7 +11853,7 @@
         <v>272</v>
       </c>
       <c r="X83" t="s">
-        <v>192</v>
+        <v>517</v>
       </c>
     </row>
     <row r="84">
@@ -11256,7 +11861,7 @@
         <v>289</v>
       </c>
       <c r="X84" t="s">
-        <v>488</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85">
@@ -11264,7 +11869,7 @@
         <v>273</v>
       </c>
       <c r="X85" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
     </row>
     <row r="86">
@@ -11272,7 +11877,7 @@
         <v>274</v>
       </c>
       <c r="X86" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87">
@@ -11280,7 +11885,7 @@
         <v>307</v>
       </c>
       <c r="X87" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88">
@@ -11288,7 +11893,7 @@
         <v>313</v>
       </c>
       <c r="X88" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="89">
@@ -11296,7 +11901,7 @@
         <v>296</v>
       </c>
       <c r="X89" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90">
@@ -11304,7 +11909,7 @@
         <v>341</v>
       </c>
       <c r="X90" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91">
@@ -11312,7 +11917,7 @@
         <v>278</v>
       </c>
       <c r="X91" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="92">
@@ -11320,156 +11925,161 @@
         <v>279</v>
       </c>
       <c r="X92" t="s">
-        <v>196</v>
+        <v>472</v>
       </c>
     </row>
     <row r="93">
       <c r="X93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94">
       <c r="X94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95">
       <c r="X95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96">
       <c r="X96" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97">
       <c r="X97" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98">
       <c r="X98" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99">
       <c r="X99" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100">
       <c r="X100" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="101">
       <c r="X101" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102">
       <c r="X102" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103">
       <c r="X103" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104">
       <c r="X104" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105">
       <c r="X105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106">
       <c r="X106" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107">
       <c r="X107" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108">
       <c r="X108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109">
       <c r="X109" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110">
       <c r="X110" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="111">
       <c r="X111" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="112">
       <c r="X112" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="113">
       <c r="X113" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="114">
       <c r="X114" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115">
       <c r="X115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116">
       <c r="X116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="117">
       <c r="X117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118">
       <c r="X118" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119">
       <c r="X119" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="120">
       <c r="X120" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121">
       <c r="X121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122">
       <c r="X122" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="X123" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- [`assertElementsPresent(prefix)`]: *NEW* command to assert a series   of web elements via their respective locators. - support propagation of execution metadata as shell environment variables.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -34,7 +34,7 @@
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$P$2:$P$15</definedName>
+    <definedName name="number">'#system'!$P$2:$P$16</definedName>
     <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
     <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
     <definedName name="redis">'#system'!$S$2:$S$10</definedName>
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
     <definedName name="step">'#system'!$W$2:$W$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$29</definedName>
-    <definedName name="web">'#system'!$X$2:$X$123</definedName>
+    <definedName name="web">'#system'!$X$2:$X$124</definedName>
     <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7444" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8463" uniqueCount="536">
   <si>
     <t>description</t>
   </si>
@@ -1665,6 +1665,15 @@
   </si>
   <si>
     <t>replaceIn(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>roundTo(var,closestDigit)</t>
+  </si>
+  <si>
+    <t>whole(var)</t>
+  </si>
+  <si>
+    <t>assertElementsPresent(prefix)</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1681,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="232" x14ac:knownFonts="1">
+  <fonts count="264" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3140,8 +3149,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="381">
+  <fills count="435">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5296,8 +5507,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="394">
+  <borders count="450">
     <border>
       <left/>
       <right/>
@@ -9268,13 +9785,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="275">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9961,52 +11042,148 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="215" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="216" fillId="356" borderId="373" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="373" fillId="356" fontId="216" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="217" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="217" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="218" fillId="359" borderId="377" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="377" fillId="359" fontId="218" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="219" fillId="362" borderId="381" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="381" fillId="362" fontId="219" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="220" fillId="365" borderId="381" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="381" fillId="365" fontId="220" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="221" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="221" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="222" fillId="368" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="368" fontId="222" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="223" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="223" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="224" fillId="371" borderId="385" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="385" fillId="371" fontId="224" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="225" fillId="374" borderId="389" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="389" fillId="374" fontId="225" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="226" fillId="377" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="393" fillId="377" fontId="226" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="227" fillId="377" borderId="393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="393" fillId="377" fontId="227" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="228" fillId="365" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="365" fontId="228" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="229" fillId="380" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="380" fontId="229" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="230" fillId="365" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="365" fontId="230" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="231" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="231" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="401" fillId="383" fontId="232" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="233" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="405" fillId="386" fontId="234" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="409" fillId="389" fontId="235" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="409" fillId="392" fontId="236" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="237" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="395" fontId="238" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="239" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="413" fillId="398" fontId="240" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="417" fillId="401" fontId="241" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="421" fillId="404" fontId="242" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="421" fillId="404" fontId="243" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="392" fontId="244" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="407" fontId="245" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="392" fontId="246" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="247" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="248" fillId="410" borderId="429" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="249" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="250" fillId="413" borderId="433" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="251" fillId="416" borderId="437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="252" fillId="419" borderId="437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="253" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="254" fillId="422" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="255" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="256" fillId="425" borderId="441" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="257" fillId="428" borderId="445" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="258" fillId="431" borderId="449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="259" fillId="431" borderId="449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="260" fillId="419" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="261" fillId="434" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="262" fillId="419" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="263" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10304,7 +11481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD123"/>
+  <dimension ref="A1:AD124"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -11129,7 +12306,7 @@
         <v>33</v>
       </c>
       <c r="P15" t="s">
-        <v>88</v>
+        <v>533</v>
       </c>
       <c r="Q15" t="s">
         <v>242</v>
@@ -11160,6 +12337,9 @@
       <c r="M16" t="s">
         <v>36</v>
       </c>
+      <c r="P16" t="s">
+        <v>534</v>
+      </c>
       <c r="Q16" t="s">
         <v>243</v>
       </c>
@@ -11187,7 +12367,7 @@
         <v>76</v>
       </c>
       <c r="X17" t="s">
-        <v>97</v>
+        <v>535</v>
       </c>
       <c r="AA17" t="s">
         <v>496</v>
@@ -11210,7 +12390,7 @@
         <v>381</v>
       </c>
       <c r="X18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC18" t="s">
         <v>532</v>
@@ -11230,7 +12410,7 @@
         <v>505</v>
       </c>
       <c r="X19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC19" t="s">
         <v>226</v>
@@ -11250,7 +12430,7 @@
         <v>37</v>
       </c>
       <c r="X20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC20" t="s">
         <v>227</v>
@@ -11270,7 +12450,7 @@
         <v>393</v>
       </c>
       <c r="X21" t="s">
-        <v>518</v>
+        <v>100</v>
       </c>
       <c r="AC21" t="s">
         <v>228</v>
@@ -11290,7 +12470,7 @@
         <v>77</v>
       </c>
       <c r="X22" t="s">
-        <v>102</v>
+        <v>518</v>
       </c>
     </row>
     <row r="23">
@@ -11307,7 +12487,7 @@
         <v>475</v>
       </c>
       <c r="X23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24">
@@ -11324,7 +12504,7 @@
         <v>38</v>
       </c>
       <c r="X24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25">
@@ -11341,7 +12521,7 @@
         <v>39</v>
       </c>
       <c r="X25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
@@ -11355,7 +12535,7 @@
         <v>283</v>
       </c>
       <c r="X26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
@@ -11369,7 +12549,7 @@
         <v>267</v>
       </c>
       <c r="X27" t="s">
-        <v>328</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28">
@@ -11383,7 +12563,7 @@
         <v>284</v>
       </c>
       <c r="X28" t="s">
-        <v>107</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29">
@@ -11397,7 +12577,7 @@
         <v>285</v>
       </c>
       <c r="X29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30">
@@ -11408,7 +12588,7 @@
         <v>208</v>
       </c>
       <c r="X30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31">
@@ -11419,7 +12599,7 @@
         <v>276</v>
       </c>
       <c r="X31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32">
@@ -11430,7 +12610,7 @@
         <v>286</v>
       </c>
       <c r="X32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33">
@@ -11441,7 +12621,7 @@
         <v>261</v>
       </c>
       <c r="X33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34">
@@ -11452,7 +12632,7 @@
         <v>331</v>
       </c>
       <c r="X34" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35">
@@ -11463,7 +12643,7 @@
         <v>309</v>
       </c>
       <c r="X35" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36">
@@ -11474,7 +12654,7 @@
         <v>262</v>
       </c>
       <c r="X36" t="s">
-        <v>339</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37">
@@ -11485,7 +12665,7 @@
         <v>310</v>
       </c>
       <c r="X37" t="s">
-        <v>470</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38">
@@ -11493,7 +12673,7 @@
         <v>268</v>
       </c>
       <c r="X38" t="s">
-        <v>394</v>
+        <v>470</v>
       </c>
     </row>
     <row r="39">
@@ -11501,7 +12681,7 @@
         <v>70</v>
       </c>
       <c r="X39" t="s">
-        <v>114</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40">
@@ -11509,7 +12689,7 @@
         <v>204</v>
       </c>
       <c r="X40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41">
@@ -11517,7 +12697,7 @@
         <v>290</v>
       </c>
       <c r="X41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42">
@@ -11525,7 +12705,7 @@
         <v>301</v>
       </c>
       <c r="X42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43">
@@ -11533,7 +12713,7 @@
         <v>302</v>
       </c>
       <c r="X43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44">
@@ -11541,7 +12721,7 @@
         <v>344</v>
       </c>
       <c r="X44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45">
@@ -11549,7 +12729,7 @@
         <v>343</v>
       </c>
       <c r="X45" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46">
@@ -11557,7 +12737,7 @@
         <v>203</v>
       </c>
       <c r="X46" t="s">
-        <v>205</v>
+        <v>477</v>
       </c>
     </row>
     <row r="47">
@@ -11565,7 +12745,7 @@
         <v>303</v>
       </c>
       <c r="X47" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48">
@@ -11573,7 +12753,7 @@
         <v>340</v>
       </c>
       <c r="X48" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49">
@@ -11581,7 +12761,7 @@
         <v>369</v>
       </c>
       <c r="X49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50">
@@ -11589,7 +12769,7 @@
         <v>304</v>
       </c>
       <c r="X50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51">
@@ -11597,7 +12777,7 @@
         <v>357</v>
       </c>
       <c r="X51" t="s">
-        <v>516</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52">
@@ -11605,7 +12785,7 @@
         <v>332</v>
       </c>
       <c r="X52" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
     </row>
     <row r="53">
@@ -11613,7 +12793,7 @@
         <v>269</v>
       </c>
       <c r="X53" t="s">
-        <v>123</v>
+        <v>500</v>
       </c>
     </row>
     <row r="54">
@@ -11621,7 +12801,7 @@
         <v>293</v>
       </c>
       <c r="X54" t="s">
-        <v>347</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55">
@@ -11629,7 +12809,7 @@
         <v>294</v>
       </c>
       <c r="X55" t="s">
-        <v>494</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56">
@@ -11637,7 +12817,7 @@
         <v>295</v>
       </c>
       <c r="X56" t="s">
-        <v>124</v>
+        <v>494</v>
       </c>
     </row>
     <row r="57">
@@ -11645,7 +12825,7 @@
         <v>305</v>
       </c>
       <c r="X57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58">
@@ -11653,7 +12833,7 @@
         <v>314</v>
       </c>
       <c r="X58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59">
@@ -11661,7 +12841,7 @@
         <v>338</v>
       </c>
       <c r="X59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60">
@@ -11669,7 +12849,7 @@
         <v>311</v>
       </c>
       <c r="X60" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61">
@@ -11677,7 +12857,7 @@
         <v>312</v>
       </c>
       <c r="X61" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62">
@@ -11685,7 +12865,7 @@
         <v>370</v>
       </c>
       <c r="X62" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63">
@@ -11693,7 +12873,7 @@
         <v>371</v>
       </c>
       <c r="X63" t="s">
-        <v>473</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64">
@@ -11701,7 +12881,7 @@
         <v>346</v>
       </c>
       <c r="X64" t="s">
-        <v>508</v>
+        <v>473</v>
       </c>
     </row>
     <row r="65">
@@ -11709,7 +12889,7 @@
         <v>315</v>
       </c>
       <c r="X65" t="s">
-        <v>206</v>
+        <v>508</v>
       </c>
     </row>
     <row r="66">
@@ -11717,7 +12897,7 @@
         <v>270</v>
       </c>
       <c r="X66" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67">
@@ -11725,7 +12905,7 @@
         <v>354</v>
       </c>
       <c r="X67" t="s">
-        <v>478</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68">
@@ -11733,7 +12913,7 @@
         <v>316</v>
       </c>
       <c r="X68" t="s">
-        <v>131</v>
+        <v>478</v>
       </c>
     </row>
     <row r="69">
@@ -11741,7 +12921,7 @@
         <v>409</v>
       </c>
       <c r="X69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70">
@@ -11749,7 +12929,7 @@
         <v>306</v>
       </c>
       <c r="X70" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71">
@@ -11757,7 +12937,7 @@
         <v>410</v>
       </c>
       <c r="X71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72">
@@ -11765,7 +12945,7 @@
         <v>263</v>
       </c>
       <c r="X72" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73">
@@ -11773,7 +12953,7 @@
         <v>345</v>
       </c>
       <c r="X73" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74">
@@ -11781,7 +12961,7 @@
         <v>281</v>
       </c>
       <c r="X74" t="s">
-        <v>489</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75">
@@ -11789,7 +12969,7 @@
         <v>287</v>
       </c>
       <c r="X75" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
     </row>
     <row r="76">
@@ -11797,7 +12977,7 @@
         <v>292</v>
       </c>
       <c r="X76" t="s">
-        <v>135</v>
+        <v>502</v>
       </c>
     </row>
     <row r="77">
@@ -11805,7 +12985,7 @@
         <v>464</v>
       </c>
       <c r="X77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78">
@@ -11813,7 +12993,7 @@
         <v>333</v>
       </c>
       <c r="X78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79">
@@ -11821,7 +13001,7 @@
         <v>271</v>
       </c>
       <c r="X79" t="s">
-        <v>529</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80">
@@ -11829,7 +13009,7 @@
         <v>282</v>
       </c>
       <c r="X80" t="s">
-        <v>138</v>
+        <v>529</v>
       </c>
     </row>
     <row r="81">
@@ -11837,7 +13017,7 @@
         <v>288</v>
       </c>
       <c r="X81" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82">
@@ -11845,7 +13025,7 @@
         <v>277</v>
       </c>
       <c r="X82" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83">
@@ -11853,7 +13033,7 @@
         <v>272</v>
       </c>
       <c r="X83" t="s">
-        <v>517</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84">
@@ -11861,7 +13041,7 @@
         <v>289</v>
       </c>
       <c r="X84" t="s">
-        <v>192</v>
+        <v>517</v>
       </c>
     </row>
     <row r="85">
@@ -11869,7 +13049,7 @@
         <v>273</v>
       </c>
       <c r="X85" t="s">
-        <v>488</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86">
@@ -11877,7 +13057,7 @@
         <v>274</v>
       </c>
       <c r="X86" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
     </row>
     <row r="87">
@@ -11885,7 +13065,7 @@
         <v>307</v>
       </c>
       <c r="X87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88">
@@ -11893,7 +13073,7 @@
         <v>313</v>
       </c>
       <c r="X88" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89">
@@ -11901,7 +13081,7 @@
         <v>296</v>
       </c>
       <c r="X89" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90">
@@ -11909,7 +13089,7 @@
         <v>341</v>
       </c>
       <c r="X90" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91">
@@ -11917,7 +13097,7 @@
         <v>278</v>
       </c>
       <c r="X91" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92">
@@ -11925,161 +13105,166 @@
         <v>279</v>
       </c>
       <c r="X92" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="93">
       <c r="X93" t="s">
-        <v>196</v>
+        <v>472</v>
       </c>
     </row>
     <row r="94">
       <c r="X94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95">
       <c r="X95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96">
       <c r="X96" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97">
       <c r="X97" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98">
       <c r="X98" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="99">
       <c r="X99" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100">
       <c r="X100" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="101">
       <c r="X101" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="102">
       <c r="X102" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103">
       <c r="X103" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104">
       <c r="X104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105">
       <c r="X105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106">
       <c r="X106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107">
       <c r="X107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108">
       <c r="X108" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109">
       <c r="X109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="110">
       <c r="X110" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111">
       <c r="X111" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112">
       <c r="X112" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="113">
       <c r="X113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="114">
       <c r="X114" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115">
       <c r="X115" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="116">
       <c r="X116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117">
       <c r="X117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118">
       <c r="X118" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119">
       <c r="X119" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120">
       <c r="X120" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121">
       <c r="X121" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="122">
       <c r="X122" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123">
       <c r="X123" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="X124" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Nexial Expression] - fix the storage of large decimal numbers when using `[NUMBER(...) => ...]` expression. The previous scientific representation has been replaced with plain numeric representation.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
     <definedName name="step">'#system'!$W$2:$W$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$29</definedName>
-    <definedName name="web">'#system'!$X$2:$X$124</definedName>
+    <definedName name="web">'#system'!$X$2:$X$125</definedName>
     <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8463" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9484" uniqueCount="537">
   <si>
     <t>description</t>
   </si>
@@ -1674,6 +1674,9 @@
   </si>
   <si>
     <t>assertElementsPresent(prefix)</t>
+  </si>
+  <si>
+    <t>saveValues(var,locator)</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1684,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="264" x14ac:knownFonts="1">
+  <fonts count="296" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3351,8 +3354,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="435">
+  <fills count="489">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5813,8 +6018,314 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="450">
+  <borders count="506">
     <border>
       <left/>
       <right/>
@@ -10349,13 +10860,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="307">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -11138,52 +12213,148 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="247" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="248" fillId="410" borderId="429" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="429" fillId="410" fontId="248" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="249" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="249" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="250" fillId="413" borderId="433" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="433" fillId="413" fontId="250" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="251" fillId="416" borderId="437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="437" fillId="416" fontId="251" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="252" fillId="419" borderId="437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="437" fillId="419" fontId="252" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="253" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="253" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="254" fillId="422" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="422" fontId="254" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="255" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="255" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="256" fillId="425" borderId="441" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="441" fillId="425" fontId="256" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="257" fillId="428" borderId="445" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="445" fillId="428" fontId="257" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="258" fillId="431" borderId="449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="449" fillId="431" fontId="258" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="259" fillId="431" borderId="449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="449" fillId="431" fontId="259" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="260" fillId="419" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="419" fontId="260" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="261" fillId="434" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="434" fontId="261" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="262" fillId="419" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="419" fontId="262" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="263" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="263" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="457" fillId="437" fontId="264" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="265" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="461" fillId="440" fontId="266" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="465" fillId="443" fontId="267" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="465" fillId="446" fontId="268" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="269" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="449" fontId="270" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="271" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="469" fillId="452" fontId="272" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="473" fillId="455" fontId="273" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="477" fillId="458" fontId="274" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="477" fillId="458" fontId="275" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="446" fontId="276" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="461" fontId="277" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="446" fontId="278" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="279" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="280" fillId="464" borderId="485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="282" fillId="467" borderId="489" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="283" fillId="470" borderId="493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="284" fillId="473" borderId="493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="286" fillId="476" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="288" fillId="479" borderId="497" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="289" fillId="482" borderId="501" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="290" fillId="485" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="291" fillId="485" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="292" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="293" fillId="488" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="294" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="295" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -11481,7 +12652,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD124"/>
+  <dimension ref="A1:AD125"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -13145,126 +14316,131 @@
     </row>
     <row r="100">
       <c r="X100" t="s">
-        <v>141</v>
+        <v>536</v>
       </c>
     </row>
     <row r="101">
       <c r="X101" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102">
       <c r="X102" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="103">
       <c r="X103" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104">
       <c r="X104" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="105">
       <c r="X105" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106">
       <c r="X106" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107">
       <c r="X107" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108">
       <c r="X108" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109">
       <c r="X109" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110">
       <c r="X110" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111">
       <c r="X111" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112">
       <c r="X112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113">
       <c r="X113" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="114">
       <c r="X114" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="115">
       <c r="X115" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116">
       <c r="X116" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="117">
       <c r="X117" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="118">
       <c r="X118" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="119">
       <c r="X119" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120">
       <c r="X120" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="121">
       <c r="X121" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="122">
       <c r="X122" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123">
       <c r="X123" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124">
       <c r="X124" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="X125" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[csv] - [`toExcel`]: **NEW** command to export CSV content into new/existing Excel file.
[web]
- [`assertElementsPresent(prefix)`]: improved logging.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -20,14 +20,14 @@
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="base">'#system'!$E$2:$E$38</definedName>
-    <definedName name="csv">'#system'!$F$2:$F$5</definedName>
+    <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$G$2:$G$92</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$4</definedName>
     <definedName name="image">'#system'!$J$2:$J$6</definedName>
-    <definedName name="io">'#system'!$K$2:$K$25</definedName>
+    <definedName name="io">'#system'!$K$2:$K$28</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
     <definedName name="json">'#system'!$M$2:$M$16</definedName>
     <definedName name="mail">'#system'!$O$2:$O$2</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9484" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9999" uniqueCount="541">
   <si>
     <t>description</t>
   </si>
@@ -1677,6 +1677,18 @@
   </si>
   <si>
     <t>saveValues(var,locator)</t>
+  </si>
+  <si>
+    <t>toExcel(csvFile,excel,worksheet,startCell)</t>
+  </si>
+  <si>
+    <t>copyFilesByRegex(sourceDir,regex,target)</t>
+  </si>
+  <si>
+    <t>deleteFilesByRegex(sourceDir,regex)</t>
+  </si>
+  <si>
+    <t>moveFilesByRegex(sourceDir,regex,target)</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1696,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="296" x14ac:knownFonts="1">
+  <fonts count="312" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3556,8 +3568,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="489">
+  <fills count="516">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6324,8 +6437,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="506">
+  <borders count="534">
     <border>
       <left/>
       <right/>
@@ -11424,13 +11690,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="323">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12309,52 +12857,100 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="279" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="280" fillId="464" borderId="485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="485" fillId="464" fontId="280" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="281" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="282" fillId="467" borderId="489" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="489" fillId="467" fontId="282" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="283" fillId="470" borderId="493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="493" fillId="470" fontId="283" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="284" fillId="473" borderId="493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="493" fillId="473" fontId="284" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="285" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="286" fillId="476" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="476" fontId="286" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="287" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="288" fillId="479" borderId="497" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="497" fillId="479" fontId="288" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="289" fillId="482" borderId="501" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="501" fillId="482" fontId="289" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="290" fillId="485" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="505" fillId="485" fontId="290" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="291" fillId="485" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="505" fillId="485" fontId="291" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="292" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="473" fontId="292" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="293" fillId="488" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="488" fontId="293" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="294" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="473" fontId="294" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="295" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="295" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="296" fillId="491" borderId="513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="297" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="298" fillId="494" borderId="517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="299" fillId="497" borderId="521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="300" fillId="500" borderId="521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="301" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="302" fillId="503" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="303" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="304" fillId="506" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="305" fillId="509" borderId="529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="306" fillId="512" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="307" fillId="512" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="308" fillId="500" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="309" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="310" fillId="500" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="311" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13080,6 +13676,9 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
+      <c r="F6" t="s">
+        <v>537</v>
+      </c>
       <c r="G6" t="s">
         <v>389</v>
       </c>
@@ -13202,7 +13801,7 @@
         <v>329</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>538</v>
       </c>
       <c r="M8" t="s">
         <v>27</v>
@@ -13255,7 +13854,7 @@
         <v>330</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
         <v>28</v>
@@ -13296,7 +13895,7 @@
         <v>487</v>
       </c>
       <c r="K10" t="s">
-        <v>391</v>
+        <v>31</v>
       </c>
       <c r="M10" t="s">
         <v>29</v>
@@ -13334,7 +13933,7 @@
         <v>323</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>539</v>
       </c>
       <c r="M11" t="s">
         <v>507</v>
@@ -13369,7 +13968,7 @@
         <v>324</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>391</v>
       </c>
       <c r="M12" t="s">
         <v>476</v>
@@ -13404,7 +14003,7 @@
         <v>325</v>
       </c>
       <c r="K13" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="M13" t="s">
         <v>506</v>
@@ -13439,7 +14038,7 @@
         <v>326</v>
       </c>
       <c r="K14" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="M14" t="s">
         <v>32</v>
@@ -13471,7 +14070,7 @@
         <v>266</v>
       </c>
       <c r="K15" t="s">
-        <v>491</v>
+        <v>540</v>
       </c>
       <c r="M15" t="s">
         <v>33</v>
@@ -13503,7 +14102,7 @@
         <v>319</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M16" t="s">
         <v>36</v>
@@ -13535,7 +14134,7 @@
         <v>81</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="X17" t="s">
         <v>535</v>
@@ -13558,7 +14157,7 @@
         <v>82</v>
       </c>
       <c r="K18" t="s">
-        <v>381</v>
+        <v>491</v>
       </c>
       <c r="X18" t="s">
         <v>97</v>
@@ -13578,7 +14177,7 @@
         <v>297</v>
       </c>
       <c r="K19" t="s">
-        <v>505</v>
+        <v>75</v>
       </c>
       <c r="X19" t="s">
         <v>98</v>
@@ -13598,7 +14197,7 @@
         <v>298</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="X20" t="s">
         <v>99</v>
@@ -13618,7 +14217,7 @@
         <v>299</v>
       </c>
       <c r="K21" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="X21" t="s">
         <v>100</v>
@@ -13638,7 +14237,7 @@
         <v>300</v>
       </c>
       <c r="K22" t="s">
-        <v>77</v>
+        <v>505</v>
       </c>
       <c r="X22" t="s">
         <v>518</v>
@@ -13655,7 +14254,7 @@
         <v>291</v>
       </c>
       <c r="K23" t="s">
-        <v>475</v>
+        <v>37</v>
       </c>
       <c r="X23" t="s">
         <v>102</v>
@@ -13672,7 +14271,7 @@
         <v>280</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>393</v>
       </c>
       <c r="X24" t="s">
         <v>103</v>
@@ -13689,7 +14288,7 @@
         <v>68</v>
       </c>
       <c r="K25" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="X25" t="s">
         <v>104</v>
@@ -13705,6 +14304,9 @@
       <c r="G26" t="s">
         <v>283</v>
       </c>
+      <c r="K26" t="s">
+        <v>475</v>
+      </c>
       <c r="X26" t="s">
         <v>105</v>
       </c>
@@ -13719,6 +14321,9 @@
       <c r="G27" t="s">
         <v>267</v>
       </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
       <c r="X27" t="s">
         <v>106</v>
       </c>
@@ -13732,6 +14337,9 @@
       </c>
       <c r="G28" t="s">
         <v>284</v>
+      </c>
+      <c r="K28" t="s">
+        <v>39</v>
       </c>
       <c r="X28" t="s">
         <v>328</v>

</xml_diff>

<commit_message>
- support the change of expression parameter delimiter from the default `,` to the value of `nexial.textDelim`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
     <definedName name="step">'#system'!$W$2:$W$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$29</definedName>
-    <definedName name="web">'#system'!$X$2:$X$125</definedName>
+    <definedName name="web">'#system'!$X$2:$X$127</definedName>
     <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
     <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10516" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11554" uniqueCount="545">
   <si>
     <t>description</t>
   </si>
@@ -1695,6 +1695,12 @@
   </si>
   <si>
     <t>saveTextByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>scrollElement(locator,xOffset,yOffset)</t>
+  </si>
+  <si>
+    <t>scrollPage(xOffset,yOffset)</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1708,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="328" x14ac:knownFonts="1">
+  <fonts count="360" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3776,8 +3782,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="543">
+  <fills count="603">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6850,8 +7058,348 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="562">
+  <borders count="618">
     <border>
       <left/>
       <right/>
@@ -12514,13 +13062,577 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="339">
+  <cellXfs count="371">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -13495,52 +14607,148 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="311" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="312" fillId="518" borderId="541" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="541" fillId="518" fontId="312" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="313" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="313" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="314" fillId="521" borderId="545" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="545" fillId="521" fontId="314" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="315" fillId="524" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="549" fillId="524" fontId="315" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="316" fillId="527" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="549" fillId="527" fontId="316" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="317" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="317" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="318" fillId="530" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="530" fontId="318" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="319" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="319" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="320" fillId="533" borderId="553" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="553" fillId="533" fontId="320" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="321" fillId="536" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="557" fillId="536" fontId="321" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="322" fillId="539" borderId="561" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="561" fillId="539" fontId="322" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="323" fillId="539" borderId="561" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="561" fillId="539" fontId="323" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="324" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="324" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="325" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="542" fontId="325" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="326" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="326" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="327" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="327" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="569" fillId="545" fontId="328" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="329" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="573" fillId="548" fontId="330" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="577" fillId="551" fontId="331" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="577" fillId="554" fontId="332" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="333" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="557" fontId="334" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="335" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="581" fillId="560" fontId="336" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="585" fillId="563" fontId="337" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="566" fontId="338" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="566" fontId="339" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="554" fontId="340" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="569" fontId="341" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="554" fontId="342" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="572" fontId="343" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="344" fillId="575" borderId="597" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="345" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="346" fillId="578" borderId="601" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="347" fillId="581" borderId="605" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="348" fillId="584" borderId="605" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="349" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="350" fillId="587" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="351" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="590" borderId="609" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="593" borderId="613" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="354" fillId="596" borderId="617" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="355" fillId="596" borderId="617" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="356" fillId="584" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="357" fillId="599" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="358" fillId="584" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="359" fillId="602" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13838,7 +15046,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD125"/>
+  <dimension ref="A1:AD127"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -15525,126 +16733,136 @@
     </row>
     <row r="101">
       <c r="X101" t="s">
-        <v>141</v>
+        <v>543</v>
       </c>
     </row>
     <row r="102">
       <c r="X102" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103">
       <c r="X103" t="s">
-        <v>142</v>
+        <v>544</v>
       </c>
     </row>
     <row r="104">
       <c r="X104" t="s">
-        <v>143</v>
+        <v>384</v>
       </c>
     </row>
     <row r="105">
       <c r="X105" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106">
       <c r="X106" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="107">
       <c r="X107" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108">
       <c r="X108" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109">
       <c r="X109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="110">
       <c r="X110" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111">
       <c r="X111" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="112">
       <c r="X112" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113">
       <c r="X113" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114">
       <c r="X114" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="115">
       <c r="X115" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116">
       <c r="X116" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
     </row>
     <row r="117">
       <c r="X117" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="118">
       <c r="X118" t="s">
-        <v>156</v>
+        <v>479</v>
       </c>
     </row>
     <row r="119">
       <c r="X119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120">
       <c r="X120" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="121">
       <c r="X121" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122">
       <c r="X122" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="123">
       <c r="X123" t="s">
-        <v>160</v>
+        <v>40</v>
       </c>
     </row>
     <row r="124">
       <c r="X124" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125">
       <c r="X125" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="X126" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="X127" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update scripts and templates
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -50,8 +50,8 @@
     <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
     <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
-    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
-    <definedName name="localdb">'#system'!$N$2:$N$10</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
+    <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14203" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14737" uniqueCount="560">
   <si>
     <t>description</t>
   </si>
@@ -1735,6 +1735,18 @@
   </si>
   <si>
     <t>writeBase64decode(encodedSource,decodedTarget)</t>
+  </si>
+  <si>
+    <t>purgeQueue(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>writeBase64decode(encodedSource,decodedTarget,append)</t>
+  </si>
+  <si>
+    <t>exportEXCEL(sql,output,sheet,start)</t>
+  </si>
+  <si>
+    <t>importEXCEL(var,excel,sheet,ranges,table)</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1754,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="440" x14ac:knownFonts="1">
+  <fonts count="456" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4523,8 +4535,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="753">
+  <fills count="783">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8787,8 +8900,178 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="758">
+  <borders count="786">
     <border>
       <left/>
       <right/>
@@ -8810,6 +9093,288 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -16431,7 +16996,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="451">
+  <cellXfs count="467">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -17742,52 +18307,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="722" fontId="423" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="424" fillId="725" borderId="737" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="737" fillId="725" fontId="424" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="425" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="425" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="426" fillId="728" borderId="741" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="741" fillId="728" fontId="426" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="427" fillId="731" borderId="745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="745" fillId="731" fontId="427" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="428" fillId="734" borderId="745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="745" fillId="734" fontId="428" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="429" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="429" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="430" fillId="737" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="737" fontId="430" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="431" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="431" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="432" fillId="740" borderId="749" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="749" fillId="740" fontId="432" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="433" fillId="743" borderId="753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="753" fillId="743" fontId="433" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="434" fillId="746" borderId="757" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="757" fillId="746" fontId="434" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="435" fillId="746" borderId="757" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="757" fillId="746" fontId="435" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="436" fillId="734" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="734" fontId="436" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="437" fillId="749" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="749" fontId="437" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="438" fillId="734" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="734" fontId="438" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="439" fillId="752" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="752" fontId="439" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="440" fillId="755" borderId="765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="441" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="442" fillId="758" borderId="769" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="443" fillId="761" borderId="773" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="444" fillId="764" borderId="773" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="445" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="446" fillId="767" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="447" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="448" fillId="770" borderId="777" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="449" fillId="773" borderId="781" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="450" fillId="776" borderId="785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="451" fillId="776" borderId="785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="452" fillId="764" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="453" fillId="779" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="454" fillId="764" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="455" fillId="782" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -18289,7 +18902,7 @@
         <v>498</v>
       </c>
       <c r="D3" t="s">
-        <v>521</v>
+        <v>556</v>
       </c>
       <c r="E3" t="s">
         <v>492</v>
@@ -18372,7 +18985,7 @@
         <v>375</v>
       </c>
       <c r="D4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -18455,7 +19068,7 @@
         <v>376</v>
       </c>
       <c r="D5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E5" t="s">
         <v>493</v>
@@ -18479,7 +19092,7 @@
         <v>79</v>
       </c>
       <c r="N5" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="Q5" t="s">
         <v>23</v>
@@ -18525,6 +19138,9 @@
       <c r="B6" t="s">
         <v>377</v>
       </c>
+      <c r="D6" t="s">
+        <v>523</v>
+      </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -18547,7 +19163,7 @@
         <v>22</v>
       </c>
       <c r="N6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="Q6" t="s">
         <v>24</v>
@@ -18606,7 +19222,7 @@
         <v>317</v>
       </c>
       <c r="N7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q7" t="s">
         <v>26</v>
@@ -18665,7 +19281,7 @@
         <v>27</v>
       </c>
       <c r="N8" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="Q8" t="s">
         <v>83</v>
@@ -18721,7 +19337,7 @@
         <v>28</v>
       </c>
       <c r="N9" t="s">
-        <v>550</v>
+        <v>559</v>
       </c>
       <c r="Q9" t="s">
         <v>84</v>
@@ -18765,7 +19381,7 @@
         <v>29</v>
       </c>
       <c r="N10" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="Q10" t="s">
         <v>469</v>
@@ -18805,6 +19421,9 @@
       <c r="M11" t="s">
         <v>507</v>
       </c>
+      <c r="N11" t="s">
+        <v>550</v>
+      </c>
       <c r="Q11" t="s">
         <v>85</v>
       </c>
@@ -18840,6 +19459,9 @@
       <c r="M12" t="s">
         <v>476</v>
       </c>
+      <c r="N12" t="s">
+        <v>551</v>
+      </c>
       <c r="Q12" t="s">
         <v>34</v>
       </c>
@@ -19155,7 +19777,7 @@
         <v>68</v>
       </c>
       <c r="K25" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="Y25" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
[csv] - [`compareExtended(var,profile,expected,actual)`]: enhanced with configuration option to compare some fields as number, compare case-insensitively or before-compare trim.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -23,13 +23,13 @@
     <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$94</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$95</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$5</definedName>
-    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="image">'#system'!$J$2:$J$7</definedName>
     <definedName name="io">'#system'!$K$2:$K$29</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="json">'#system'!$M$2:$M$17</definedName>
     <definedName name="mail">'#system'!$P$2:$P$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -43,12 +43,12 @@
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$128</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
     <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
     <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
+    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15273" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15819" uniqueCount="573">
   <si>
     <t>description</t>
   </si>
@@ -1753,6 +1753,39 @@
   </si>
   <si>
     <t>assertTextNotContains(locator,text)</t>
+  </si>
+  <si>
+    <t>saveModalDialogTextByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>typeKeys(os,keystrokes)</t>
+  </si>
+  <si>
+    <t>saveDiff(var,baseline,actual)</t>
+  </si>
+  <si>
+    <t>compact(var,json,removeEmpty)</t>
+  </si>
+  <si>
+    <t>clickAll(locator)</t>
+  </si>
+  <si>
+    <t>assertSoap(wsdl,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultCode(expected,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultString(expected,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultCode(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultDetail(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultString(var,xml)</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1793,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="472" x14ac:knownFonts="1">
+  <fonts count="488" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4743,8 +4776,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="813">
+  <fills count="840">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9347,8 +9481,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="814">
+  <borders count="846">
     <border>
       <left/>
       <right/>
@@ -17371,6 +17658,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -17555,7 +18168,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="483">
+  <cellXfs count="499">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -18962,52 +19575,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="782" fontId="455" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="456" fillId="785" borderId="793" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="793" fillId="785" fontId="456" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="457" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="457" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="458" fillId="788" borderId="797" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="797" fillId="788" fontId="458" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="459" fillId="791" borderId="801" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="801" fillId="791" fontId="459" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="460" fillId="794" borderId="801" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="801" fillId="794" fontId="460" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="461" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="461" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="462" fillId="797" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="797" fontId="462" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="463" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="463" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="464" fillId="800" borderId="805" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="805" fillId="800" fontId="464" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="465" fillId="803" borderId="809" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="809" fillId="803" fontId="465" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="466" fillId="806" borderId="813" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="813" fillId="806" fontId="466" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="467" fillId="806" borderId="813" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="813" fillId="806" fontId="467" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="468" fillId="794" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="794" fontId="468" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="469" fillId="809" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="809" fontId="469" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="470" fillId="794" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="794" fontId="470" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="471" fillId="812" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="812" fontId="471" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="472" fillId="815" borderId="821" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="473" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="474" fillId="818" borderId="825" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="475" fillId="821" borderId="829" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="476" fillId="824" borderId="833" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="477" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="478" fillId="827" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="479" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="480" fillId="830" borderId="837" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="481" fillId="821" borderId="841" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="482" fillId="833" borderId="845" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="483" fillId="833" borderId="845" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="484" fillId="824" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="485" fillId="836" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="486" fillId="824" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="487" fillId="839" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -19305,7 +19966,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -19825,6 +20486,9 @@
       <c r="H7" t="s">
         <v>482</v>
       </c>
+      <c r="J7" t="s">
+        <v>564</v>
+      </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>
@@ -19865,7 +20529,7 @@
         <v>462</v>
       </c>
       <c r="AD7" t="s">
-        <v>223</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8">
@@ -19921,7 +20585,7 @@
         <v>463</v>
       </c>
       <c r="AD8" t="s">
-        <v>224</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9">
@@ -19968,7 +20632,7 @@
         <v>181</v>
       </c>
       <c r="AD9" t="s">
-        <v>225</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10">
@@ -20009,7 +20673,7 @@
         <v>182</v>
       </c>
       <c r="AD10" t="s">
-        <v>509</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
@@ -20047,7 +20711,7 @@
         <v>260</v>
       </c>
       <c r="AD11" t="s">
-        <v>525</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12">
@@ -20067,7 +20731,7 @@
         <v>391</v>
       </c>
       <c r="M12" t="s">
-        <v>476</v>
+        <v>565</v>
       </c>
       <c r="N12" t="s">
         <v>551</v>
@@ -20085,7 +20749,7 @@
         <v>183</v>
       </c>
       <c r="AD12" t="s">
-        <v>526</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
@@ -20105,7 +20769,7 @@
         <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>506</v>
+        <v>476</v>
       </c>
       <c r="Q13" t="s">
         <v>86</v>
@@ -20120,7 +20784,7 @@
         <v>184</v>
       </c>
       <c r="AD13" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14">
@@ -20140,7 +20804,7 @@
         <v>35</v>
       </c>
       <c r="M14" t="s">
-        <v>32</v>
+        <v>506</v>
       </c>
       <c r="Q14" t="s">
         <v>87</v>
@@ -20155,7 +20819,7 @@
         <v>185</v>
       </c>
       <c r="AD14" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
     </row>
     <row r="15">
@@ -20172,7 +20836,7 @@
         <v>540</v>
       </c>
       <c r="M15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q15" t="s">
         <v>533</v>
@@ -20187,7 +20851,7 @@
         <v>186</v>
       </c>
       <c r="AD15" t="s">
-        <v>510</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16">
@@ -20204,7 +20868,7 @@
         <v>73</v>
       </c>
       <c r="M16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q16" t="s">
         <v>534</v>
@@ -20219,7 +20883,7 @@
         <v>187</v>
       </c>
       <c r="AD16" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17">
@@ -20235,6 +20899,9 @@
       <c r="K17" t="s">
         <v>74</v>
       </c>
+      <c r="M17" t="s">
+        <v>36</v>
+      </c>
       <c r="Y17" t="s">
         <v>535</v>
       </c>
@@ -20242,7 +20909,7 @@
         <v>496</v>
       </c>
       <c r="AD17" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18">
@@ -20262,7 +20929,7 @@
         <v>97</v>
       </c>
       <c r="AD18" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19">
@@ -20282,7 +20949,7 @@
         <v>98</v>
       </c>
       <c r="AD19" t="s">
-        <v>226</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20">
@@ -20302,7 +20969,7 @@
         <v>99</v>
       </c>
       <c r="AD20" t="s">
-        <v>227</v>
+        <v>528</v>
       </c>
     </row>
     <row r="21">
@@ -20322,7 +20989,7 @@
         <v>100</v>
       </c>
       <c r="AD21" t="s">
-        <v>228</v>
+        <v>532</v>
       </c>
     </row>
     <row r="22">
@@ -20341,6 +21008,9 @@
       <c r="Y22" t="s">
         <v>518</v>
       </c>
+      <c r="AD22" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -20358,6 +21028,9 @@
       <c r="Y23" t="s">
         <v>102</v>
       </c>
+      <c r="AD23" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -20375,6 +21048,9 @@
       <c r="Y24" t="s">
         <v>103</v>
       </c>
+      <c r="AD24" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -20392,6 +21068,9 @@
       <c r="Y25" t="s">
         <v>104</v>
       </c>
+      <c r="AD25" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -20409,6 +21088,9 @@
       <c r="Y26" t="s">
         <v>105</v>
       </c>
+      <c r="AD26" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -20426,6 +21108,9 @@
       <c r="Y27" t="s">
         <v>106</v>
       </c>
+      <c r="AD27" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -20653,7 +21338,7 @@
         <v>369</v>
       </c>
       <c r="Y50" t="s">
-        <v>120</v>
+        <v>566</v>
       </c>
     </row>
     <row r="51">
@@ -20661,7 +21346,7 @@
         <v>304</v>
       </c>
       <c r="Y51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52">
@@ -20669,7 +21354,7 @@
         <v>357</v>
       </c>
       <c r="Y52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53">
@@ -20677,7 +21362,7 @@
         <v>332</v>
       </c>
       <c r="Y53" t="s">
-        <v>516</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54">
@@ -20685,7 +21370,7 @@
         <v>269</v>
       </c>
       <c r="Y54" t="s">
-        <v>500</v>
+        <v>516</v>
       </c>
     </row>
     <row r="55">
@@ -20693,7 +21378,7 @@
         <v>293</v>
       </c>
       <c r="Y55" t="s">
-        <v>123</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56">
@@ -20701,7 +21386,7 @@
         <v>294</v>
       </c>
       <c r="Y56" t="s">
-        <v>347</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57">
@@ -20709,7 +21394,7 @@
         <v>295</v>
       </c>
       <c r="Y57" t="s">
-        <v>494</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58">
@@ -20717,7 +21402,7 @@
         <v>305</v>
       </c>
       <c r="Y58" t="s">
-        <v>124</v>
+        <v>494</v>
       </c>
     </row>
     <row r="59">
@@ -20725,7 +21410,7 @@
         <v>314</v>
       </c>
       <c r="Y59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60">
@@ -20733,7 +21418,7 @@
         <v>338</v>
       </c>
       <c r="Y60" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61">
@@ -20741,7 +21426,7 @@
         <v>311</v>
       </c>
       <c r="Y61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62">
@@ -20749,7 +21434,7 @@
         <v>312</v>
       </c>
       <c r="Y62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63">
@@ -20757,7 +21442,7 @@
         <v>370</v>
       </c>
       <c r="Y63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64">
@@ -20765,7 +21450,7 @@
         <v>371</v>
       </c>
       <c r="Y64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65">
@@ -20773,7 +21458,7 @@
         <v>346</v>
       </c>
       <c r="Y65" t="s">
-        <v>473</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66">
@@ -20781,7 +21466,7 @@
         <v>315</v>
       </c>
       <c r="Y66" t="s">
-        <v>508</v>
+        <v>473</v>
       </c>
     </row>
     <row r="67">
@@ -20789,15 +21474,15 @@
         <v>270</v>
       </c>
       <c r="Y67" t="s">
-        <v>206</v>
+        <v>508</v>
       </c>
     </row>
     <row r="68">
       <c r="G68" t="s">
-        <v>354</v>
+        <v>562</v>
       </c>
       <c r="Y68" t="s">
-        <v>390</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69">
@@ -20805,7 +21490,7 @@
         <v>316</v>
       </c>
       <c r="Y69" t="s">
-        <v>478</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70">
@@ -20813,7 +21498,7 @@
         <v>409</v>
       </c>
       <c r="Y70" t="s">
-        <v>131</v>
+        <v>478</v>
       </c>
     </row>
     <row r="71">
@@ -20821,7 +21506,7 @@
         <v>306</v>
       </c>
       <c r="Y71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72">
@@ -20829,7 +21514,7 @@
         <v>410</v>
       </c>
       <c r="Y72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73">
@@ -20837,7 +21522,7 @@
         <v>263</v>
       </c>
       <c r="Y73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74">
@@ -20845,7 +21530,7 @@
         <v>542</v>
       </c>
       <c r="Y74" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75">
@@ -20853,7 +21538,7 @@
         <v>345</v>
       </c>
       <c r="Y75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76">
@@ -20861,7 +21546,7 @@
         <v>281</v>
       </c>
       <c r="Y76" t="s">
-        <v>489</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77">
@@ -20869,7 +21554,7 @@
         <v>287</v>
       </c>
       <c r="Y77" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
     </row>
     <row r="78">
@@ -20877,7 +21562,7 @@
         <v>292</v>
       </c>
       <c r="Y78" t="s">
-        <v>135</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79">
@@ -20885,7 +21570,7 @@
         <v>464</v>
       </c>
       <c r="Y79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80">
@@ -20893,7 +21578,7 @@
         <v>333</v>
       </c>
       <c r="Y80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81">
@@ -20901,7 +21586,7 @@
         <v>271</v>
       </c>
       <c r="Y81" t="s">
-        <v>529</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82">
@@ -20909,7 +21594,7 @@
         <v>282</v>
       </c>
       <c r="Y82" t="s">
-        <v>138</v>
+        <v>529</v>
       </c>
     </row>
     <row r="83">
@@ -20917,7 +21602,7 @@
         <v>288</v>
       </c>
       <c r="Y83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84">
@@ -20925,256 +21610,264 @@
         <v>277</v>
       </c>
       <c r="Y84" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85">
       <c r="G85" t="s">
-        <v>272</v>
+        <v>563</v>
       </c>
       <c r="Y85" t="s">
-        <v>517</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86">
       <c r="G86" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="Y86" t="s">
-        <v>192</v>
+        <v>517</v>
       </c>
     </row>
     <row r="87">
       <c r="G87" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="Y87" t="s">
-        <v>488</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88">
       <c r="G88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y88" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
     </row>
     <row r="89">
       <c r="G89" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="Y89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90">
       <c r="G90" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="Y90" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91">
       <c r="G91" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="Y91" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92">
       <c r="G92" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="Y92" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93">
       <c r="G93" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="Y93" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94">
       <c r="G94" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="G95" t="s">
         <v>279</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Y95" t="s">
         <v>472</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="Y95" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="96">
       <c r="Y96" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97">
       <c r="Y97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98">
       <c r="Y98" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99">
       <c r="Y99" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="100">
       <c r="Y100" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101">
       <c r="Y101" t="s">
-        <v>536</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102">
       <c r="Y102" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="103">
       <c r="Y103" t="s">
-        <v>141</v>
+        <v>543</v>
       </c>
     </row>
     <row r="104">
       <c r="Y104" t="s">
-        <v>544</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105">
       <c r="Y105" t="s">
-        <v>384</v>
+        <v>544</v>
       </c>
     </row>
     <row r="106">
       <c r="Y106" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107">
       <c r="Y107" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108">
       <c r="Y108" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="109">
       <c r="Y109" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110">
       <c r="Y110" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111">
       <c r="Y111" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="112">
       <c r="Y112" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113">
       <c r="Y113" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="114">
       <c r="Y114" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="115">
       <c r="Y115" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116">
       <c r="Y116" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117">
       <c r="Y117" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="118">
       <c r="Y118" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="119">
       <c r="Y119" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="120">
       <c r="Y120" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="121">
       <c r="Y121" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122">
       <c r="Y122" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="123">
       <c r="Y123" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="124">
       <c r="Y124" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="125">
       <c r="Y125" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="126">
       <c r="Y126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127">
       <c r="Y127" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128">
       <c r="Y128" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="Y129" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[fixes] - capture screenshot image file as `nexial.lastScreenshot` for `desktop` commands
[improvements]
- create backup screen capture capability in case we can't capture screen via WebDrivr of Winiun driver

[desktop]
- [`clickScreen(button,modifiers,x,y)`]: support English words for `x` and `y`

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -23,7 +23,7 @@
     <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$95</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$97</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$5</definedName>
     <definedName name="image">'#system'!$J$2:$J$7</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16369" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17473" uniqueCount="578">
   <si>
     <t>description</t>
   </si>
@@ -1796,6 +1796,12 @@
   </si>
   <si>
     <t>spellCheck(var,profile,text)</t>
+  </si>
+  <si>
+    <t>clickScreen(button,modifiers,x,y)</t>
+  </si>
+  <si>
+    <t>mouseWheel(amount,modifiers,x,y)</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1809,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="504" x14ac:knownFonts="1">
+  <fonts count="536" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4988,8 +4994,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="867">
+  <fills count="921">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9898,8 +10106,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="878">
+  <borders count="942">
     <border>
       <left/>
       <right/>
@@ -17922,6 +18436,658 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -18758,7 +19924,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="515">
+  <cellXfs count="547">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -20261,52 +21427,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="839" fontId="487" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="488" fillId="842" borderId="853" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="853" fillId="842" fontId="488" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="489" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="489" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="490" fillId="845" borderId="857" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="857" fillId="845" fontId="490" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="491" fillId="848" borderId="861" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="861" fillId="848" fontId="491" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="492" fillId="851" borderId="865" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="865" fillId="851" fontId="492" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="493" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="493" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="494" fillId="854" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="854" fontId="494" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="495" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="495" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="496" fillId="857" borderId="869" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="869" fillId="857" fontId="496" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="497" fillId="848" borderId="873" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="873" fillId="848" fontId="497" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="498" fillId="860" borderId="877" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="877" fillId="860" fontId="498" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="499" fillId="860" borderId="877" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="877" fillId="860" fontId="499" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="500" fillId="851" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="851" fontId="500" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="501" fillId="863" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="863" fontId="501" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="502" fillId="851" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="851" fontId="502" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="503" fillId="866" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="866" fontId="503" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="885" fillId="869" fontId="504" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="505" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="889" fillId="872" fontId="506" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="893" fillId="875" fontId="507" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="897" fillId="878" fontId="508" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="509" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="881" fontId="510" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="511" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="901" fillId="884" fontId="512" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="905" fillId="875" fontId="513" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="909" fillId="887" fontId="514" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="909" fillId="887" fontId="515" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="878" fontId="516" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="890" fontId="517" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="878" fontId="518" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="893" fontId="519" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="520" fillId="896" borderId="917" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="521" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="522" fillId="899" borderId="921" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="523" fillId="902" borderId="925" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="524" fillId="905" borderId="929" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="525" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="526" fillId="908" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="527" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="528" fillId="911" borderId="933" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="529" fillId="902" borderId="937" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="530" fillId="914" borderId="941" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="531" fillId="914" borderId="941" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="532" fillId="905" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="533" fillId="917" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="534" fillId="905" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="535" fillId="920" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -21921,7 +23183,7 @@
     </row>
     <row r="42">
       <c r="G42" t="s">
-        <v>290</v>
+        <v>576</v>
       </c>
       <c r="Z42" t="s">
         <v>115</v>
@@ -21929,7 +23191,7 @@
     </row>
     <row r="43">
       <c r="G43" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="Z43" t="s">
         <v>116</v>
@@ -21937,7 +23199,7 @@
     </row>
     <row r="44">
       <c r="G44" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Z44" t="s">
         <v>117</v>
@@ -21945,7 +23207,7 @@
     </row>
     <row r="45">
       <c r="G45" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="Z45" t="s">
         <v>118</v>
@@ -21953,7 +23215,7 @@
     </row>
     <row r="46">
       <c r="G46" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Z46" t="s">
         <v>119</v>
@@ -21961,7 +23223,7 @@
     </row>
     <row r="47">
       <c r="G47" t="s">
-        <v>203</v>
+        <v>343</v>
       </c>
       <c r="Z47" t="s">
         <v>477</v>
@@ -21969,7 +23231,7 @@
     </row>
     <row r="48">
       <c r="G48" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="Z48" t="s">
         <v>205</v>
@@ -21977,7 +23239,7 @@
     </row>
     <row r="49">
       <c r="G49" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="Z49" t="s">
         <v>69</v>
@@ -21985,7 +23247,7 @@
     </row>
     <row r="50">
       <c r="G50" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="Z50" t="s">
         <v>566</v>
@@ -21993,7 +23255,7 @@
     </row>
     <row r="51">
       <c r="G51" t="s">
-        <v>304</v>
+        <v>369</v>
       </c>
       <c r="Z51" t="s">
         <v>120</v>
@@ -22001,7 +23263,7 @@
     </row>
     <row r="52">
       <c r="G52" t="s">
-        <v>357</v>
+        <v>304</v>
       </c>
       <c r="Z52" t="s">
         <v>121</v>
@@ -22009,7 +23271,7 @@
     </row>
     <row r="53">
       <c r="G53" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="Z53" t="s">
         <v>122</v>
@@ -22017,7 +23279,7 @@
     </row>
     <row r="54">
       <c r="G54" t="s">
-        <v>269</v>
+        <v>332</v>
       </c>
       <c r="Z54" t="s">
         <v>516</v>
@@ -22025,7 +23287,7 @@
     </row>
     <row r="55">
       <c r="G55" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="Z55" t="s">
         <v>500</v>
@@ -22033,7 +23295,7 @@
     </row>
     <row r="56">
       <c r="G56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Z56" t="s">
         <v>123</v>
@@ -22041,7 +23303,7 @@
     </row>
     <row r="57">
       <c r="G57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Z57" t="s">
         <v>347</v>
@@ -22049,7 +23311,7 @@
     </row>
     <row r="58">
       <c r="G58" t="s">
-        <v>305</v>
+        <v>577</v>
       </c>
       <c r="Z58" t="s">
         <v>494</v>
@@ -22057,7 +23319,7 @@
     </row>
     <row r="59">
       <c r="G59" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="Z59" t="s">
         <v>124</v>
@@ -22065,7 +23327,7 @@
     </row>
     <row r="60">
       <c r="G60" t="s">
-        <v>338</v>
+        <v>305</v>
       </c>
       <c r="Z60" t="s">
         <v>125</v>
@@ -22073,7 +23335,7 @@
     </row>
     <row r="61">
       <c r="G61" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="Z61" t="s">
         <v>126</v>
@@ -22081,7 +23343,7 @@
     </row>
     <row r="62">
       <c r="G62" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="Z62" t="s">
         <v>127</v>
@@ -22089,7 +23351,7 @@
     </row>
     <row r="63">
       <c r="G63" t="s">
-        <v>370</v>
+        <v>311</v>
       </c>
       <c r="Z63" t="s">
         <v>128</v>
@@ -22097,7 +23359,7 @@
     </row>
     <row r="64">
       <c r="G64" t="s">
-        <v>371</v>
+        <v>312</v>
       </c>
       <c r="Z64" t="s">
         <v>129</v>
@@ -22105,7 +23367,7 @@
     </row>
     <row r="65">
       <c r="G65" t="s">
-        <v>346</v>
+        <v>370</v>
       </c>
       <c r="Z65" t="s">
         <v>130</v>
@@ -22113,7 +23375,7 @@
     </row>
     <row r="66">
       <c r="G66" t="s">
-        <v>315</v>
+        <v>371</v>
       </c>
       <c r="Z66" t="s">
         <v>473</v>
@@ -22121,7 +23383,7 @@
     </row>
     <row r="67">
       <c r="G67" t="s">
-        <v>270</v>
+        <v>346</v>
       </c>
       <c r="Z67" t="s">
         <v>508</v>
@@ -22129,7 +23391,7 @@
     </row>
     <row r="68">
       <c r="G68" t="s">
-        <v>562</v>
+        <v>315</v>
       </c>
       <c r="Z68" t="s">
         <v>206</v>
@@ -22137,7 +23399,7 @@
     </row>
     <row r="69">
       <c r="G69" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
       <c r="Z69" t="s">
         <v>390</v>
@@ -22145,7 +23407,7 @@
     </row>
     <row r="70">
       <c r="G70" t="s">
-        <v>409</v>
+        <v>562</v>
       </c>
       <c r="Z70" t="s">
         <v>478</v>
@@ -22153,7 +23415,7 @@
     </row>
     <row r="71">
       <c r="G71" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="Z71" t="s">
         <v>131</v>
@@ -22161,7 +23423,7 @@
     </row>
     <row r="72">
       <c r="G72" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z72" t="s">
         <v>132</v>
@@ -22169,7 +23431,7 @@
     </row>
     <row r="73">
       <c r="G73" t="s">
-        <v>263</v>
+        <v>306</v>
       </c>
       <c r="Z73" t="s">
         <v>133</v>
@@ -22177,7 +23439,7 @@
     </row>
     <row r="74">
       <c r="G74" t="s">
-        <v>542</v>
+        <v>410</v>
       </c>
       <c r="Z74" t="s">
         <v>134</v>
@@ -22185,7 +23447,7 @@
     </row>
     <row r="75">
       <c r="G75" t="s">
-        <v>345</v>
+        <v>263</v>
       </c>
       <c r="Z75" t="s">
         <v>189</v>
@@ -22193,7 +23455,7 @@
     </row>
     <row r="76">
       <c r="G76" t="s">
-        <v>281</v>
+        <v>542</v>
       </c>
       <c r="Z76" t="s">
         <v>190</v>
@@ -22201,7 +23463,7 @@
     </row>
     <row r="77">
       <c r="G77" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="Z77" t="s">
         <v>489</v>
@@ -22209,7 +23471,7 @@
     </row>
     <row r="78">
       <c r="G78" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="Z78" t="s">
         <v>502</v>
@@ -22217,7 +23479,7 @@
     </row>
     <row r="79">
       <c r="G79" t="s">
-        <v>464</v>
+        <v>287</v>
       </c>
       <c r="Z79" t="s">
         <v>135</v>
@@ -22225,7 +23487,7 @@
     </row>
     <row r="80">
       <c r="G80" t="s">
-        <v>333</v>
+        <v>292</v>
       </c>
       <c r="Z80" t="s">
         <v>136</v>
@@ -22233,7 +23495,7 @@
     </row>
     <row r="81">
       <c r="G81" t="s">
-        <v>271</v>
+        <v>464</v>
       </c>
       <c r="Z81" t="s">
         <v>137</v>
@@ -22241,7 +23503,7 @@
     </row>
     <row r="82">
       <c r="G82" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
       <c r="Z82" t="s">
         <v>529</v>
@@ -22249,7 +23511,7 @@
     </row>
     <row r="83">
       <c r="G83" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="Z83" t="s">
         <v>138</v>
@@ -22257,7 +23519,7 @@
     </row>
     <row r="84">
       <c r="G84" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="Z84" t="s">
         <v>139</v>
@@ -22265,7 +23527,7 @@
     </row>
     <row r="85">
       <c r="G85" t="s">
-        <v>563</v>
+        <v>288</v>
       </c>
       <c r="Z85" t="s">
         <v>191</v>
@@ -22273,7 +23535,7 @@
     </row>
     <row r="86">
       <c r="G86" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="Z86" t="s">
         <v>517</v>
@@ -22281,7 +23543,7 @@
     </row>
     <row r="87">
       <c r="G87" t="s">
-        <v>289</v>
+        <v>563</v>
       </c>
       <c r="Z87" t="s">
         <v>192</v>
@@ -22289,7 +23551,7 @@
     </row>
     <row r="88">
       <c r="G88" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z88" t="s">
         <v>488</v>
@@ -22297,7 +23559,7 @@
     </row>
     <row r="89">
       <c r="G89" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="Z89" t="s">
         <v>193</v>
@@ -22305,7 +23567,7 @@
     </row>
     <row r="90">
       <c r="G90" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
       <c r="Z90" t="s">
         <v>194</v>
@@ -22313,7 +23575,7 @@
     </row>
     <row r="91">
       <c r="G91" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="Z91" t="s">
         <v>207</v>
@@ -22321,7 +23583,7 @@
     </row>
     <row r="92">
       <c r="G92" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="Z92" t="s">
         <v>140</v>
@@ -22329,7 +23591,7 @@
     </row>
     <row r="93">
       <c r="G93" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
       <c r="Z93" t="s">
         <v>195</v>
@@ -22337,7 +23599,7 @@
     </row>
     <row r="94">
       <c r="G94" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="Z94" t="s">
         <v>471</v>
@@ -22345,18 +23607,24 @@
     </row>
     <row r="95">
       <c r="G95" t="s">
-        <v>279</v>
+        <v>341</v>
       </c>
       <c r="Z95" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="96">
+      <c r="G96" t="s">
+        <v>278</v>
+      </c>
       <c r="Z96" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="97">
+      <c r="G97" t="s">
+        <v>279</v>
+      </c>
       <c r="Z97" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
[improvements] - upgraded to Spring Boot 2.1.6
[expression]
- [JSON &raquo; `keys(jsonpath)`]: extract immediate keys of resolved JSON fragment based on `jsonpath`.

[json]
- [`storeKeys(json,jsonpath,var)`]: extract immediate keys of resolved JSON fragment based on `jsonpath`.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -29,7 +29,7 @@
     <definedName name="image">'#system'!$J$2:$J$7</definedName>
     <definedName name="io">'#system'!$K$2:$K$29</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$17</definedName>
+    <definedName name="json">'#system'!$M$2:$M$18</definedName>
     <definedName name="mail">'#system'!$P$2:$P$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -42,13 +42,13 @@
     <definedName name="sound">'#system'!$V$2:$V$5</definedName>
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$129</definedName>
-    <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
-    <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
-    <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
-    <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
+    <definedName name="target">'#system'!$A$2:$A$30</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
+    <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
+    <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
+    <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
+    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17473" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18023" uniqueCount="579">
   <si>
     <t>description</t>
   </si>
@@ -1802,6 +1802,9 @@
   </si>
   <si>
     <t>mouseWheel(amount,modifiers,x,y)</t>
+  </si>
+  <si>
+    <t>storeKeys(json,jsonpath,var)</t>
   </si>
 </sst>
 </file>
@@ -1809,7 +1812,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="536" x14ac:knownFonts="1">
+  <fonts count="552" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5196,8 +5199,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="921">
+  <fills count="948">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10412,8 +10516,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="942">
+  <borders count="974">
     <border>
       <left/>
       <right/>
@@ -18436,6 +18693,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -19924,7 +20507,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="547">
+  <cellXfs count="563">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -21523,52 +22106,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="893" fontId="519" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="520" fillId="896" borderId="917" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="917" fillId="896" fontId="520" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="521" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="521" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="522" fillId="899" borderId="921" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="921" fillId="899" fontId="522" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="523" fillId="902" borderId="925" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="925" fillId="902" fontId="523" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="524" fillId="905" borderId="929" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="929" fillId="905" fontId="524" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="525" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="525" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="526" fillId="908" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="908" fontId="526" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="527" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="527" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="528" fillId="911" borderId="933" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="933" fillId="911" fontId="528" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="529" fillId="902" borderId="937" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="937" fillId="902" fontId="529" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="530" fillId="914" borderId="941" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="941" fillId="914" fontId="530" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="531" fillId="914" borderId="941" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="941" fillId="914" fontId="531" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="532" fillId="905" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="905" fontId="532" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="533" fillId="917" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="917" fontId="533" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="534" fillId="905" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="905" fontId="534" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="535" fillId="920" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="920" fontId="535" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="536" fillId="923" borderId="949" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="537" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="538" fillId="926" borderId="953" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="539" fillId="929" borderId="957" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="540" fillId="932" borderId="961" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="541" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="542" fillId="935" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="543" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="544" fillId="938" borderId="965" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="545" fillId="929" borderId="969" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="546" fillId="941" borderId="973" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="547" fillId="941" borderId="973" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="548" fillId="932" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="549" fillId="944" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="550" fillId="932" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="551" fillId="947" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -21866,7 +22497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF129"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -21949,24 +22580,21 @@
         <v>395</v>
       </c>
       <c r="Y1" t="s">
-        <v>573</v>
+        <v>46</v>
       </c>
       <c r="Z1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AC1" t="s">
-        <v>49</v>
+        <v>458</v>
       </c>
       <c r="AD1" t="s">
-        <v>458</v>
-      </c>
-      <c r="AE1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -22044,24 +22672,21 @@
         <v>396</v>
       </c>
       <c r="Y2" t="s">
-        <v>575</v>
+        <v>89</v>
       </c>
       <c r="Z2" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="AA2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="AB2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="AC2" t="s">
-        <v>175</v>
+        <v>468</v>
       </c>
       <c r="AD2" t="s">
-        <v>468</v>
-      </c>
-      <c r="AE2" t="s">
         <v>524</v>
       </c>
     </row>
@@ -22132,22 +22757,22 @@
       <c r="X3" t="s">
         <v>397</v>
       </c>
+      <c r="Y3" t="s">
+        <v>90</v>
+      </c>
       <c r="Z3" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="AA3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="AB3" t="s">
-        <v>169</v>
+        <v>365</v>
       </c>
       <c r="AC3" t="s">
-        <v>365</v>
+        <v>176</v>
       </c>
       <c r="AD3" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -22215,22 +22840,22 @@
       <c r="X4" t="s">
         <v>398</v>
       </c>
+      <c r="Y4" t="s">
+        <v>355</v>
+      </c>
       <c r="Z4" t="s">
-        <v>355</v>
+        <v>165</v>
       </c>
       <c r="AA4" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="AB4" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AC4" t="s">
-        <v>176</v>
+        <v>459</v>
       </c>
       <c r="AD4" t="s">
-        <v>459</v>
-      </c>
-      <c r="AE4" t="s">
         <v>220</v>
       </c>
     </row>
@@ -22289,22 +22914,22 @@
       <c r="W5" t="s">
         <v>360</v>
       </c>
+      <c r="Y5" t="s">
+        <v>356</v>
+      </c>
       <c r="Z5" t="s">
-        <v>356</v>
+        <v>166</v>
       </c>
       <c r="AA5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="AB5" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="AC5" t="s">
-        <v>177</v>
+        <v>460</v>
       </c>
       <c r="AD5" t="s">
-        <v>460</v>
-      </c>
-      <c r="AE5" t="s">
         <v>221</v>
       </c>
     </row>
@@ -22357,22 +22982,22 @@
       <c r="W6" t="s">
         <v>362</v>
       </c>
+      <c r="Y6" t="s">
+        <v>91</v>
+      </c>
       <c r="Z6" t="s">
-        <v>91</v>
+        <v>480</v>
       </c>
       <c r="AA6" t="s">
-        <v>480</v>
+        <v>172</v>
       </c>
       <c r="AB6" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="AC6" t="s">
-        <v>178</v>
+        <v>461</v>
       </c>
       <c r="AD6" t="s">
-        <v>461</v>
-      </c>
-      <c r="AE6" t="s">
         <v>222</v>
       </c>
     </row>
@@ -22419,22 +23044,22 @@
       <c r="W7" t="s">
         <v>361</v>
       </c>
+      <c r="Y7" t="s">
+        <v>92</v>
+      </c>
       <c r="Z7" t="s">
-        <v>92</v>
+        <v>481</v>
       </c>
       <c r="AA7" t="s">
-        <v>481</v>
+        <v>173</v>
       </c>
       <c r="AB7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="AC7" t="s">
-        <v>179</v>
+        <v>462</v>
       </c>
       <c r="AD7" t="s">
-        <v>462</v>
-      </c>
-      <c r="AE7" t="s">
         <v>567</v>
       </c>
     </row>
@@ -22475,22 +23100,22 @@
       <c r="W8" t="s">
         <v>363</v>
       </c>
+      <c r="Y8" t="s">
+        <v>93</v>
+      </c>
       <c r="Z8" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="AA8" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="AB8" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="AC8" t="s">
-        <v>180</v>
+        <v>463</v>
       </c>
       <c r="AD8" t="s">
-        <v>463</v>
-      </c>
-      <c r="AE8" t="s">
         <v>568</v>
       </c>
     </row>
@@ -22531,13 +23156,13 @@
       <c r="W9" t="s">
         <v>364</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="Y9" t="s">
         <v>201</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AB9" t="s">
         <v>181</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AD9" t="s">
         <v>569</v>
       </c>
     </row>
@@ -22572,13 +23197,13 @@
       <c r="T10" t="s">
         <v>408</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="Y10" t="s">
         <v>258</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AB10" t="s">
         <v>182</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AD10" t="s">
         <v>223</v>
       </c>
     </row>
@@ -22610,13 +23235,13 @@
       <c r="R11" t="s">
         <v>239</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Y11" t="s">
         <v>259</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AB11" t="s">
         <v>260</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AD11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -22648,13 +23273,13 @@
       <c r="R12" t="s">
         <v>240</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="Y12" t="s">
         <v>94</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AB12" t="s">
         <v>183</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AD12" t="s">
         <v>225</v>
       </c>
     </row>
@@ -22683,13 +23308,13 @@
       <c r="R13" t="s">
         <v>245</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="Y13" t="s">
         <v>327</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AB13" t="s">
         <v>184</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AD13" t="s">
         <v>509</v>
       </c>
     </row>
@@ -22718,13 +23343,13 @@
       <c r="R14" t="s">
         <v>241</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="Y14" t="s">
         <v>95</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AB14" t="s">
         <v>185</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AD14" t="s">
         <v>525</v>
       </c>
     </row>
@@ -22750,13 +23375,13 @@
       <c r="R15" t="s">
         <v>242</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="Y15" t="s">
         <v>96</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AB15" t="s">
         <v>186</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AD15" t="s">
         <v>526</v>
       </c>
     </row>
@@ -22774,7 +23399,7 @@
         <v>73</v>
       </c>
       <c r="M16" t="s">
-        <v>33</v>
+        <v>578</v>
       </c>
       <c r="Q16" t="s">
         <v>534</v>
@@ -22782,13 +23407,13 @@
       <c r="R16" t="s">
         <v>243</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="Y16" t="s">
         <v>67</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AB16" t="s">
         <v>187</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AD16" t="s">
         <v>530</v>
       </c>
     </row>
@@ -22806,15 +23431,15 @@
         <v>74</v>
       </c>
       <c r="M17" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y17" t="s">
         <v>535</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AB17" t="s">
         <v>496</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AD17" t="s">
         <v>531</v>
       </c>
     </row>
@@ -22831,10 +23456,13 @@
       <c r="K18" t="s">
         <v>491</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y18" t="s">
         <v>97</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AD18" t="s">
         <v>510</v>
       </c>
     </row>
@@ -22851,10 +23479,10 @@
       <c r="K19" t="s">
         <v>75</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="Y19" t="s">
         <v>98</v>
       </c>
-      <c r="AE19" t="s">
+      <c r="AD19" t="s">
         <v>527</v>
       </c>
     </row>
@@ -22871,10 +23499,10 @@
       <c r="K20" t="s">
         <v>76</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="Y20" t="s">
         <v>99</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AD20" t="s">
         <v>528</v>
       </c>
     </row>
@@ -22891,10 +23519,10 @@
       <c r="K21" t="s">
         <v>381</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="Y21" t="s">
         <v>100</v>
       </c>
-      <c r="AE21" t="s">
+      <c r="AD21" t="s">
         <v>532</v>
       </c>
     </row>
@@ -22911,10 +23539,10 @@
       <c r="K22" t="s">
         <v>505</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="Y22" t="s">
         <v>518</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AD22" t="s">
         <v>226</v>
       </c>
     </row>
@@ -22931,10 +23559,10 @@
       <c r="K23" t="s">
         <v>37</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="Y23" t="s">
         <v>102</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AD23" t="s">
         <v>570</v>
       </c>
     </row>
@@ -22951,16 +23579,16 @@
       <c r="K24" t="s">
         <v>393</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="Y24" t="s">
         <v>103</v>
       </c>
-      <c r="AE24" t="s">
+      <c r="AD24" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>573</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
         <v>483</v>
@@ -22971,16 +23599,16 @@
       <c r="K25" t="s">
         <v>557</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="Y25" t="s">
         <v>104</v>
       </c>
-      <c r="AE25" t="s">
+      <c r="AD25" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
         <v>216</v>
@@ -22991,16 +23619,16 @@
       <c r="K26" t="s">
         <v>77</v>
       </c>
-      <c r="Z26" t="s">
+      <c r="Y26" t="s">
         <v>105</v>
       </c>
-      <c r="AE26" t="s">
+      <c r="AD26" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>217</v>
@@ -23011,16 +23639,16 @@
       <c r="K27" t="s">
         <v>475</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="Y27" t="s">
         <v>106</v>
       </c>
-      <c r="AE27" t="s">
+      <c r="AD27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
         <v>503</v>
@@ -23031,13 +23659,13 @@
       <c r="K28" t="s">
         <v>38</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="Y28" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>458</v>
       </c>
       <c r="E29" t="s">
         <v>504</v>
@@ -23048,13 +23676,13 @@
       <c r="K29" t="s">
         <v>39</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="Y29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>458</v>
+        <v>218</v>
       </c>
       <c r="E30" t="s">
         <v>453</v>
@@ -23062,21 +23690,18 @@
       <c r="G30" t="s">
         <v>208</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="Y30" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>218</v>
-      </c>
       <c r="E31" t="s">
         <v>56</v>
       </c>
       <c r="G31" t="s">
         <v>276</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="Y31" t="s">
         <v>109</v>
       </c>
     </row>
@@ -23087,7 +23712,7 @@
       <c r="G32" t="s">
         <v>286</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="Y32" t="s">
         <v>110</v>
       </c>
     </row>
@@ -23098,7 +23723,7 @@
       <c r="G33" t="s">
         <v>541</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="Y33" t="s">
         <v>111</v>
       </c>
     </row>
@@ -23109,7 +23734,7 @@
       <c r="G34" t="s">
         <v>261</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="Y34" t="s">
         <v>112</v>
       </c>
     </row>
@@ -23120,7 +23745,7 @@
       <c r="G35" t="s">
         <v>331</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="Y35" t="s">
         <v>202</v>
       </c>
     </row>
@@ -23131,7 +23756,7 @@
       <c r="G36" t="s">
         <v>309</v>
       </c>
-      <c r="Z36" t="s">
+      <c r="Y36" t="s">
         <v>113</v>
       </c>
     </row>
@@ -23142,7 +23767,7 @@
       <c r="G37" t="s">
         <v>262</v>
       </c>
-      <c r="Z37" t="s">
+      <c r="Y37" t="s">
         <v>339</v>
       </c>
     </row>
@@ -23153,7 +23778,7 @@
       <c r="G38" t="s">
         <v>310</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="Y38" t="s">
         <v>470</v>
       </c>
     </row>
@@ -23161,7 +23786,7 @@
       <c r="G39" t="s">
         <v>268</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="Y39" t="s">
         <v>561</v>
       </c>
     </row>
@@ -23169,7 +23794,7 @@
       <c r="G40" t="s">
         <v>70</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="Y40" t="s">
         <v>394</v>
       </c>
     </row>
@@ -23177,7 +23802,7 @@
       <c r="G41" t="s">
         <v>204</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="Y41" t="s">
         <v>114</v>
       </c>
     </row>
@@ -23185,7 +23810,7 @@
       <c r="G42" t="s">
         <v>576</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="Y42" t="s">
         <v>115</v>
       </c>
     </row>
@@ -23193,7 +23818,7 @@
       <c r="G43" t="s">
         <v>290</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="Y43" t="s">
         <v>116</v>
       </c>
     </row>
@@ -23201,7 +23826,7 @@
       <c r="G44" t="s">
         <v>301</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="Y44" t="s">
         <v>117</v>
       </c>
     </row>
@@ -23209,7 +23834,7 @@
       <c r="G45" t="s">
         <v>302</v>
       </c>
-      <c r="Z45" t="s">
+      <c r="Y45" t="s">
         <v>118</v>
       </c>
     </row>
@@ -23217,7 +23842,7 @@
       <c r="G46" t="s">
         <v>344</v>
       </c>
-      <c r="Z46" t="s">
+      <c r="Y46" t="s">
         <v>119</v>
       </c>
     </row>
@@ -23225,7 +23850,7 @@
       <c r="G47" t="s">
         <v>343</v>
       </c>
-      <c r="Z47" t="s">
+      <c r="Y47" t="s">
         <v>477</v>
       </c>
     </row>
@@ -23233,7 +23858,7 @@
       <c r="G48" t="s">
         <v>203</v>
       </c>
-      <c r="Z48" t="s">
+      <c r="Y48" t="s">
         <v>205</v>
       </c>
     </row>
@@ -23241,7 +23866,7 @@
       <c r="G49" t="s">
         <v>303</v>
       </c>
-      <c r="Z49" t="s">
+      <c r="Y49" t="s">
         <v>69</v>
       </c>
     </row>
@@ -23249,7 +23874,7 @@
       <c r="G50" t="s">
         <v>340</v>
       </c>
-      <c r="Z50" t="s">
+      <c r="Y50" t="s">
         <v>566</v>
       </c>
     </row>
@@ -23257,7 +23882,7 @@
       <c r="G51" t="s">
         <v>369</v>
       </c>
-      <c r="Z51" t="s">
+      <c r="Y51" t="s">
         <v>120</v>
       </c>
     </row>
@@ -23265,7 +23890,7 @@
       <c r="G52" t="s">
         <v>304</v>
       </c>
-      <c r="Z52" t="s">
+      <c r="Y52" t="s">
         <v>121</v>
       </c>
     </row>
@@ -23273,7 +23898,7 @@
       <c r="G53" t="s">
         <v>357</v>
       </c>
-      <c r="Z53" t="s">
+      <c r="Y53" t="s">
         <v>122</v>
       </c>
     </row>
@@ -23281,7 +23906,7 @@
       <c r="G54" t="s">
         <v>332</v>
       </c>
-      <c r="Z54" t="s">
+      <c r="Y54" t="s">
         <v>516</v>
       </c>
     </row>
@@ -23289,7 +23914,7 @@
       <c r="G55" t="s">
         <v>269</v>
       </c>
-      <c r="Z55" t="s">
+      <c r="Y55" t="s">
         <v>500</v>
       </c>
     </row>
@@ -23297,7 +23922,7 @@
       <c r="G56" t="s">
         <v>293</v>
       </c>
-      <c r="Z56" t="s">
+      <c r="Y56" t="s">
         <v>123</v>
       </c>
     </row>
@@ -23305,7 +23930,7 @@
       <c r="G57" t="s">
         <v>294</v>
       </c>
-      <c r="Z57" t="s">
+      <c r="Y57" t="s">
         <v>347</v>
       </c>
     </row>
@@ -23313,7 +23938,7 @@
       <c r="G58" t="s">
         <v>577</v>
       </c>
-      <c r="Z58" t="s">
+      <c r="Y58" t="s">
         <v>494</v>
       </c>
     </row>
@@ -23321,7 +23946,7 @@
       <c r="G59" t="s">
         <v>295</v>
       </c>
-      <c r="Z59" t="s">
+      <c r="Y59" t="s">
         <v>124</v>
       </c>
     </row>
@@ -23329,7 +23954,7 @@
       <c r="G60" t="s">
         <v>305</v>
       </c>
-      <c r="Z60" t="s">
+      <c r="Y60" t="s">
         <v>125</v>
       </c>
     </row>
@@ -23337,7 +23962,7 @@
       <c r="G61" t="s">
         <v>314</v>
       </c>
-      <c r="Z61" t="s">
+      <c r="Y61" t="s">
         <v>126</v>
       </c>
     </row>
@@ -23345,7 +23970,7 @@
       <c r="G62" t="s">
         <v>338</v>
       </c>
-      <c r="Z62" t="s">
+      <c r="Y62" t="s">
         <v>127</v>
       </c>
     </row>
@@ -23353,7 +23978,7 @@
       <c r="G63" t="s">
         <v>311</v>
       </c>
-      <c r="Z63" t="s">
+      <c r="Y63" t="s">
         <v>128</v>
       </c>
     </row>
@@ -23361,7 +23986,7 @@
       <c r="G64" t="s">
         <v>312</v>
       </c>
-      <c r="Z64" t="s">
+      <c r="Y64" t="s">
         <v>129</v>
       </c>
     </row>
@@ -23369,7 +23994,7 @@
       <c r="G65" t="s">
         <v>370</v>
       </c>
-      <c r="Z65" t="s">
+      <c r="Y65" t="s">
         <v>130</v>
       </c>
     </row>
@@ -23377,7 +24002,7 @@
       <c r="G66" t="s">
         <v>371</v>
       </c>
-      <c r="Z66" t="s">
+      <c r="Y66" t="s">
         <v>473</v>
       </c>
     </row>
@@ -23385,7 +24010,7 @@
       <c r="G67" t="s">
         <v>346</v>
       </c>
-      <c r="Z67" t="s">
+      <c r="Y67" t="s">
         <v>508</v>
       </c>
     </row>
@@ -23393,7 +24018,7 @@
       <c r="G68" t="s">
         <v>315</v>
       </c>
-      <c r="Z68" t="s">
+      <c r="Y68" t="s">
         <v>206</v>
       </c>
     </row>
@@ -23401,7 +24026,7 @@
       <c r="G69" t="s">
         <v>270</v>
       </c>
-      <c r="Z69" t="s">
+      <c r="Y69" t="s">
         <v>390</v>
       </c>
     </row>
@@ -23409,7 +24034,7 @@
       <c r="G70" t="s">
         <v>562</v>
       </c>
-      <c r="Z70" t="s">
+      <c r="Y70" t="s">
         <v>478</v>
       </c>
     </row>
@@ -23417,7 +24042,7 @@
       <c r="G71" t="s">
         <v>316</v>
       </c>
-      <c r="Z71" t="s">
+      <c r="Y71" t="s">
         <v>131</v>
       </c>
     </row>
@@ -23425,7 +24050,7 @@
       <c r="G72" t="s">
         <v>409</v>
       </c>
-      <c r="Z72" t="s">
+      <c r="Y72" t="s">
         <v>132</v>
       </c>
     </row>
@@ -23433,7 +24058,7 @@
       <c r="G73" t="s">
         <v>306</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="Y73" t="s">
         <v>133</v>
       </c>
     </row>
@@ -23441,7 +24066,7 @@
       <c r="G74" t="s">
         <v>410</v>
       </c>
-      <c r="Z74" t="s">
+      <c r="Y74" t="s">
         <v>134</v>
       </c>
     </row>
@@ -23449,7 +24074,7 @@
       <c r="G75" t="s">
         <v>263</v>
       </c>
-      <c r="Z75" t="s">
+      <c r="Y75" t="s">
         <v>189</v>
       </c>
     </row>
@@ -23457,7 +24082,7 @@
       <c r="G76" t="s">
         <v>542</v>
       </c>
-      <c r="Z76" t="s">
+      <c r="Y76" t="s">
         <v>190</v>
       </c>
     </row>
@@ -23465,7 +24090,7 @@
       <c r="G77" t="s">
         <v>345</v>
       </c>
-      <c r="Z77" t="s">
+      <c r="Y77" t="s">
         <v>489</v>
       </c>
     </row>
@@ -23473,7 +24098,7 @@
       <c r="G78" t="s">
         <v>281</v>
       </c>
-      <c r="Z78" t="s">
+      <c r="Y78" t="s">
         <v>502</v>
       </c>
     </row>
@@ -23481,7 +24106,7 @@
       <c r="G79" t="s">
         <v>287</v>
       </c>
-      <c r="Z79" t="s">
+      <c r="Y79" t="s">
         <v>135</v>
       </c>
     </row>
@@ -23489,7 +24114,7 @@
       <c r="G80" t="s">
         <v>292</v>
       </c>
-      <c r="Z80" t="s">
+      <c r="Y80" t="s">
         <v>136</v>
       </c>
     </row>
@@ -23497,7 +24122,7 @@
       <c r="G81" t="s">
         <v>464</v>
       </c>
-      <c r="Z81" t="s">
+      <c r="Y81" t="s">
         <v>137</v>
       </c>
     </row>
@@ -23505,7 +24130,7 @@
       <c r="G82" t="s">
         <v>333</v>
       </c>
-      <c r="Z82" t="s">
+      <c r="Y82" t="s">
         <v>529</v>
       </c>
     </row>
@@ -23513,7 +24138,7 @@
       <c r="G83" t="s">
         <v>271</v>
       </c>
-      <c r="Z83" t="s">
+      <c r="Y83" t="s">
         <v>138</v>
       </c>
     </row>
@@ -23521,7 +24146,7 @@
       <c r="G84" t="s">
         <v>282</v>
       </c>
-      <c r="Z84" t="s">
+      <c r="Y84" t="s">
         <v>139</v>
       </c>
     </row>
@@ -23529,7 +24154,7 @@
       <c r="G85" t="s">
         <v>288</v>
       </c>
-      <c r="Z85" t="s">
+      <c r="Y85" t="s">
         <v>191</v>
       </c>
     </row>
@@ -23537,7 +24162,7 @@
       <c r="G86" t="s">
         <v>277</v>
       </c>
-      <c r="Z86" t="s">
+      <c r="Y86" t="s">
         <v>517</v>
       </c>
     </row>
@@ -23545,7 +24170,7 @@
       <c r="G87" t="s">
         <v>563</v>
       </c>
-      <c r="Z87" t="s">
+      <c r="Y87" t="s">
         <v>192</v>
       </c>
     </row>
@@ -23553,7 +24178,7 @@
       <c r="G88" t="s">
         <v>272</v>
       </c>
-      <c r="Z88" t="s">
+      <c r="Y88" t="s">
         <v>488</v>
       </c>
     </row>
@@ -23561,7 +24186,7 @@
       <c r="G89" t="s">
         <v>289</v>
       </c>
-      <c r="Z89" t="s">
+      <c r="Y89" t="s">
         <v>193</v>
       </c>
     </row>
@@ -23569,7 +24194,7 @@
       <c r="G90" t="s">
         <v>273</v>
       </c>
-      <c r="Z90" t="s">
+      <c r="Y90" t="s">
         <v>194</v>
       </c>
     </row>
@@ -23577,7 +24202,7 @@
       <c r="G91" t="s">
         <v>274</v>
       </c>
-      <c r="Z91" t="s">
+      <c r="Y91" t="s">
         <v>207</v>
       </c>
     </row>
@@ -23585,7 +24210,7 @@
       <c r="G92" t="s">
         <v>307</v>
       </c>
-      <c r="Z92" t="s">
+      <c r="Y92" t="s">
         <v>140</v>
       </c>
     </row>
@@ -23593,7 +24218,7 @@
       <c r="G93" t="s">
         <v>313</v>
       </c>
-      <c r="Z93" t="s">
+      <c r="Y93" t="s">
         <v>195</v>
       </c>
     </row>
@@ -23601,7 +24226,7 @@
       <c r="G94" t="s">
         <v>296</v>
       </c>
-      <c r="Z94" t="s">
+      <c r="Y94" t="s">
         <v>471</v>
       </c>
     </row>
@@ -23609,7 +24234,7 @@
       <c r="G95" t="s">
         <v>341</v>
       </c>
-      <c r="Z95" t="s">
+      <c r="Y95" t="s">
         <v>472</v>
       </c>
     </row>
@@ -23617,7 +24242,7 @@
       <c r="G96" t="s">
         <v>278</v>
       </c>
-      <c r="Z96" t="s">
+      <c r="Y96" t="s">
         <v>196</v>
       </c>
     </row>
@@ -23625,167 +24250,167 @@
       <c r="G97" t="s">
         <v>279</v>
       </c>
-      <c r="Z97" t="s">
+      <c r="Y97" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="98">
-      <c r="Z98" t="s">
+      <c r="Y98" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="99">
-      <c r="Z99" t="s">
+      <c r="Y99" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="100">
-      <c r="Z100" t="s">
+      <c r="Y100" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="101">
-      <c r="Z101" t="s">
+      <c r="Y101" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="102">
-      <c r="Z102" t="s">
+      <c r="Y102" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="103">
-      <c r="Z103" t="s">
+      <c r="Y103" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="104">
-      <c r="Z104" t="s">
+      <c r="Y104" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="105">
-      <c r="Z105" t="s">
+      <c r="Y105" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="106">
-      <c r="Z106" t="s">
+      <c r="Y106" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="107">
-      <c r="Z107" t="s">
+      <c r="Y107" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="108">
-      <c r="Z108" t="s">
+      <c r="Y108" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="109">
-      <c r="Z109" t="s">
+      <c r="Y109" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="110">
-      <c r="Z110" t="s">
+      <c r="Y110" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="111">
-      <c r="Z111" t="s">
+      <c r="Y111" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="112">
-      <c r="Z112" t="s">
+      <c r="Y112" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="113">
-      <c r="Z113" t="s">
+      <c r="Y113" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="114">
-      <c r="Z114" t="s">
+      <c r="Y114" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="115">
-      <c r="Z115" t="s">
+      <c r="Y115" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="116">
-      <c r="Z116" t="s">
+      <c r="Y116" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="117">
-      <c r="Z117" t="s">
+      <c r="Y117" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="118">
-      <c r="Z118" t="s">
+      <c r="Y118" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="119">
-      <c r="Z119" t="s">
+      <c r="Y119" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="120">
-      <c r="Z120" t="s">
+      <c r="Y120" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="121">
-      <c r="Z121" t="s">
+      <c r="Y121" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="122">
-      <c r="Z122" t="s">
+      <c r="Y122" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="123">
-      <c r="Z123" t="s">
+      <c r="Y123" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="124">
-      <c r="Z124" t="s">
+      <c r="Y124" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="125">
-      <c r="Z125" t="s">
+      <c r="Y125" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="126">
-      <c r="Z126" t="s">
+      <c r="Y126" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="127">
-      <c r="Z127" t="s">
+      <c r="Y127" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="128">
-      <c r="Z128" t="s">
+      <c r="Y128" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="129">
-      <c r="Z129" t="s">
+      <c r="Y129" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[web] - [`saveISTDivsAsCsv`]: *NEW* command to export data from an Infinite Scroll Table (IST) to CSV. This is initial   implementation and further testing is yet to complete. Documentation forthcoming.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$133</definedName>
     <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18023" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19683" uniqueCount="583">
   <si>
     <t>description</t>
   </si>
@@ -1805,6 +1805,18 @@
   </si>
   <si>
     <t>storeKeys(json,jsonpath,var)</t>
+  </si>
+  <si>
+    <t>assertMultiSelect(locator)</t>
+  </si>
+  <si>
+    <t>assertSingleSelect(locator)</t>
+  </si>
+  <si>
+    <t>updateAttribute(locator,attrName,value)</t>
+  </si>
+  <si>
+    <t>saveISTDivsAsCsv(config,file)</t>
   </si>
 </sst>
 </file>
@@ -1812,7 +1824,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="552" x14ac:knownFonts="1">
+  <fonts count="600" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5300,8 +5312,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="948">
+  <fills count="1029">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10669,8 +10984,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="974">
+  <borders count="1070">
     <border>
       <left/>
       <right/>
@@ -18693,6 +19467,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -20507,7 +22259,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="563">
+  <cellXfs count="611">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -22154,52 +23906,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="920" fontId="535" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="536" fillId="923" borderId="949" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="537" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="949" fillId="923" fontId="536" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="537" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="538" fillId="926" borderId="953" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="953" fillId="926" fontId="538" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="539" fillId="929" borderId="957" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="957" fillId="929" fontId="539" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="540" fillId="932" borderId="961" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="961" fillId="932" fontId="540" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="541" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="541" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="542" fillId="935" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="935" fontId="542" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="543" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="544" fillId="938" borderId="965" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="545" fillId="929" borderId="969" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="546" fillId="941" borderId="973" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="547" fillId="941" borderId="973" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="548" fillId="932" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="549" fillId="944" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="550" fillId="932" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="551" fillId="947" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="543" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="965" fillId="938" fontId="544" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="969" fillId="929" fontId="545" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="973" fillId="941" fontId="546" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="973" fillId="941" fontId="547" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="932" fontId="548" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="944" fontId="549" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="932" fontId="550" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="947" fontId="551" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="981" fillId="950" fontId="552" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="553" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="985" fillId="953" fontId="554" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="989" fillId="956" fontId="555" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="993" fillId="959" fontId="556" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="557" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="962" fontId="558" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="559" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="997" fillId="965" fontId="560" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1001" fillId="956" fontId="561" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1005" fillId="968" fontId="562" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1005" fillId="968" fontId="563" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="959" fontId="564" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="971" fontId="565" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="959" fontId="566" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="974" fontId="567" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1013" fillId="977" fontId="568" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="569" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1017" fillId="980" fontId="570" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1021" fillId="983" fontId="571" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1025" fillId="986" fontId="572" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="573" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="989" fontId="574" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="575" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1029" fillId="992" fontId="576" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1033" fillId="983" fontId="577" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1037" fillId="995" fontId="578" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1037" fillId="995" fontId="579" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="986" fontId="580" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="998" fontId="581" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="986" fontId="582" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1001" fontId="583" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="584" fillId="1004" borderId="1045" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="585" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="586" fillId="1007" borderId="1049" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="587" fillId="1010" borderId="1053" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="588" fillId="1013" borderId="1057" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="589" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="590" fillId="1016" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="591" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="592" fillId="1019" borderId="1061" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="593" fillId="1010" borderId="1065" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="594" fillId="1022" borderId="1069" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="595" fillId="1022" borderId="1069" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="596" fillId="1013" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="597" fillId="1025" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="598" fillId="1013" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="599" fillId="1028" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -22497,7 +24393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE129"/>
+  <dimension ref="A1:AE133"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -23580,7 +25476,7 @@
         <v>393</v>
       </c>
       <c r="Y24" t="s">
-        <v>103</v>
+        <v>579</v>
       </c>
       <c r="AD24" t="s">
         <v>571</v>
@@ -23600,7 +25496,7 @@
         <v>557</v>
       </c>
       <c r="Y25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD25" t="s">
         <v>572</v>
@@ -23620,7 +25516,7 @@
         <v>77</v>
       </c>
       <c r="Y26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD26" t="s">
         <v>227</v>
@@ -23640,7 +25536,7 @@
         <v>475</v>
       </c>
       <c r="Y27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AD27" t="s">
         <v>228</v>
@@ -23660,7 +25556,7 @@
         <v>38</v>
       </c>
       <c r="Y28" t="s">
-        <v>328</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29">
@@ -23677,7 +25573,7 @@
         <v>39</v>
       </c>
       <c r="Y29" t="s">
-        <v>107</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30">
@@ -23691,7 +25587,7 @@
         <v>208</v>
       </c>
       <c r="Y30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31">
@@ -23702,7 +25598,7 @@
         <v>276</v>
       </c>
       <c r="Y31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -23713,7 +25609,7 @@
         <v>286</v>
       </c>
       <c r="Y32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33">
@@ -23724,7 +25620,7 @@
         <v>541</v>
       </c>
       <c r="Y33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34">
@@ -23735,7 +25631,7 @@
         <v>261</v>
       </c>
       <c r="Y34" t="s">
-        <v>112</v>
+        <v>580</v>
       </c>
     </row>
     <row r="35">
@@ -23746,7 +25642,7 @@
         <v>331</v>
       </c>
       <c r="Y35" t="s">
-        <v>202</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36">
@@ -23757,7 +25653,7 @@
         <v>309</v>
       </c>
       <c r="Y36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37">
@@ -23768,7 +25664,7 @@
         <v>262</v>
       </c>
       <c r="Y37" t="s">
-        <v>339</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38">
@@ -23779,7 +25675,7 @@
         <v>310</v>
       </c>
       <c r="Y38" t="s">
-        <v>470</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39">
@@ -23787,7 +25683,7 @@
         <v>268</v>
       </c>
       <c r="Y39" t="s">
-        <v>561</v>
+        <v>339</v>
       </c>
     </row>
     <row r="40">
@@ -23795,7 +25691,7 @@
         <v>70</v>
       </c>
       <c r="Y40" t="s">
-        <v>394</v>
+        <v>470</v>
       </c>
     </row>
     <row r="41">
@@ -23803,7 +25699,7 @@
         <v>204</v>
       </c>
       <c r="Y41" t="s">
-        <v>114</v>
+        <v>561</v>
       </c>
     </row>
     <row r="42">
@@ -23811,7 +25707,7 @@
         <v>576</v>
       </c>
       <c r="Y42" t="s">
-        <v>115</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43">
@@ -23819,7 +25715,7 @@
         <v>290</v>
       </c>
       <c r="Y43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44">
@@ -23827,7 +25723,7 @@
         <v>301</v>
       </c>
       <c r="Y44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45">
@@ -23835,7 +25731,7 @@
         <v>302</v>
       </c>
       <c r="Y45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46">
@@ -23843,7 +25739,7 @@
         <v>344</v>
       </c>
       <c r="Y46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47">
@@ -23851,7 +25747,7 @@
         <v>343</v>
       </c>
       <c r="Y47" t="s">
-        <v>477</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48">
@@ -23859,7 +25755,7 @@
         <v>203</v>
       </c>
       <c r="Y48" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49">
@@ -23867,7 +25763,7 @@
         <v>303</v>
       </c>
       <c r="Y49" t="s">
-        <v>69</v>
+        <v>477</v>
       </c>
     </row>
     <row r="50">
@@ -23875,7 +25771,7 @@
         <v>340</v>
       </c>
       <c r="Y50" t="s">
-        <v>566</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51">
@@ -23883,7 +25779,7 @@
         <v>369</v>
       </c>
       <c r="Y51" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52">
@@ -23891,7 +25787,7 @@
         <v>304</v>
       </c>
       <c r="Y52" t="s">
-        <v>121</v>
+        <v>566</v>
       </c>
     </row>
     <row r="53">
@@ -23899,7 +25795,7 @@
         <v>357</v>
       </c>
       <c r="Y53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54">
@@ -23907,7 +25803,7 @@
         <v>332</v>
       </c>
       <c r="Y54" t="s">
-        <v>516</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55">
@@ -23915,7 +25811,7 @@
         <v>269</v>
       </c>
       <c r="Y55" t="s">
-        <v>500</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56">
@@ -23923,7 +25819,7 @@
         <v>293</v>
       </c>
       <c r="Y56" t="s">
-        <v>123</v>
+        <v>516</v>
       </c>
     </row>
     <row r="57">
@@ -23931,7 +25827,7 @@
         <v>294</v>
       </c>
       <c r="Y57" t="s">
-        <v>347</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58">
@@ -23939,7 +25835,7 @@
         <v>577</v>
       </c>
       <c r="Y58" t="s">
-        <v>494</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59">
@@ -23947,7 +25843,7 @@
         <v>295</v>
       </c>
       <c r="Y59" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60">
@@ -23955,7 +25851,7 @@
         <v>305</v>
       </c>
       <c r="Y60" t="s">
-        <v>125</v>
+        <v>494</v>
       </c>
     </row>
     <row r="61">
@@ -23963,7 +25859,7 @@
         <v>314</v>
       </c>
       <c r="Y61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62">
@@ -23971,7 +25867,7 @@
         <v>338</v>
       </c>
       <c r="Y62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63">
@@ -23979,7 +25875,7 @@
         <v>311</v>
       </c>
       <c r="Y63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64">
@@ -23987,7 +25883,7 @@
         <v>312</v>
       </c>
       <c r="Y64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65">
@@ -23995,7 +25891,7 @@
         <v>370</v>
       </c>
       <c r="Y65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66">
@@ -24003,7 +25899,7 @@
         <v>371</v>
       </c>
       <c r="Y66" t="s">
-        <v>473</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67">
@@ -24011,7 +25907,7 @@
         <v>346</v>
       </c>
       <c r="Y67" t="s">
-        <v>508</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68">
@@ -24019,7 +25915,7 @@
         <v>315</v>
       </c>
       <c r="Y68" t="s">
-        <v>206</v>
+        <v>473</v>
       </c>
     </row>
     <row r="69">
@@ -24027,7 +25923,7 @@
         <v>270</v>
       </c>
       <c r="Y69" t="s">
-        <v>390</v>
+        <v>508</v>
       </c>
     </row>
     <row r="70">
@@ -24035,7 +25931,7 @@
         <v>562</v>
       </c>
       <c r="Y70" t="s">
-        <v>478</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71">
@@ -24043,7 +25939,7 @@
         <v>316</v>
       </c>
       <c r="Y71" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72">
@@ -24051,7 +25947,7 @@
         <v>409</v>
       </c>
       <c r="Y72" t="s">
-        <v>132</v>
+        <v>478</v>
       </c>
     </row>
     <row r="73">
@@ -24059,7 +25955,7 @@
         <v>306</v>
       </c>
       <c r="Y73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74">
@@ -24067,7 +25963,7 @@
         <v>410</v>
       </c>
       <c r="Y74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75">
@@ -24075,7 +25971,7 @@
         <v>263</v>
       </c>
       <c r="Y75" t="s">
-        <v>189</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76">
@@ -24083,7 +25979,7 @@
         <v>542</v>
       </c>
       <c r="Y76" t="s">
-        <v>190</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77">
@@ -24091,7 +25987,7 @@
         <v>345</v>
       </c>
       <c r="Y77" t="s">
-        <v>489</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78">
@@ -24099,7 +25995,7 @@
         <v>281</v>
       </c>
       <c r="Y78" t="s">
-        <v>502</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79">
@@ -24107,7 +26003,7 @@
         <v>287</v>
       </c>
       <c r="Y79" t="s">
-        <v>135</v>
+        <v>489</v>
       </c>
     </row>
     <row r="80">
@@ -24115,7 +26011,7 @@
         <v>292</v>
       </c>
       <c r="Y80" t="s">
-        <v>136</v>
+        <v>502</v>
       </c>
     </row>
     <row r="81">
@@ -24123,7 +26019,7 @@
         <v>464</v>
       </c>
       <c r="Y81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82">
@@ -24131,7 +26027,7 @@
         <v>333</v>
       </c>
       <c r="Y82" t="s">
-        <v>529</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83">
@@ -24139,7 +26035,7 @@
         <v>271</v>
       </c>
       <c r="Y83" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84">
@@ -24147,7 +26043,7 @@
         <v>282</v>
       </c>
       <c r="Y84" t="s">
-        <v>139</v>
+        <v>529</v>
       </c>
     </row>
     <row r="85">
@@ -24155,7 +26051,7 @@
         <v>288</v>
       </c>
       <c r="Y85" t="s">
-        <v>191</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86">
@@ -24163,7 +26059,7 @@
         <v>277</v>
       </c>
       <c r="Y86" t="s">
-        <v>517</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87">
@@ -24171,7 +26067,7 @@
         <v>563</v>
       </c>
       <c r="Y87" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88">
@@ -24179,7 +26075,7 @@
         <v>272</v>
       </c>
       <c r="Y88" t="s">
-        <v>488</v>
+        <v>517</v>
       </c>
     </row>
     <row r="89">
@@ -24187,7 +26083,7 @@
         <v>289</v>
       </c>
       <c r="Y89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90">
@@ -24195,7 +26091,7 @@
         <v>273</v>
       </c>
       <c r="Y90" t="s">
-        <v>194</v>
+        <v>488</v>
       </c>
     </row>
     <row r="91">
@@ -24203,7 +26099,7 @@
         <v>274</v>
       </c>
       <c r="Y91" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92">
@@ -24211,7 +26107,7 @@
         <v>307</v>
       </c>
       <c r="Y92" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93">
@@ -24219,7 +26115,7 @@
         <v>313</v>
       </c>
       <c r="Y93" t="s">
-        <v>195</v>
+        <v>582</v>
       </c>
     </row>
     <row r="94">
@@ -24227,7 +26123,7 @@
         <v>296</v>
       </c>
       <c r="Y94" t="s">
-        <v>471</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95">
@@ -24235,7 +26131,7 @@
         <v>341</v>
       </c>
       <c r="Y95" t="s">
-        <v>472</v>
+        <v>140</v>
       </c>
     </row>
     <row r="96">
@@ -24243,7 +26139,7 @@
         <v>278</v>
       </c>
       <c r="Y96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97">
@@ -24251,166 +26147,186 @@
         <v>279</v>
       </c>
       <c r="Y97" t="s">
-        <v>197</v>
+        <v>471</v>
       </c>
     </row>
     <row r="98">
       <c r="Y98" t="s">
-        <v>198</v>
+        <v>472</v>
       </c>
     </row>
     <row r="99">
       <c r="Y99" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100">
       <c r="Y100" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101">
       <c r="Y101" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102">
       <c r="Y102" t="s">
-        <v>536</v>
+        <v>199</v>
       </c>
     </row>
     <row r="103">
       <c r="Y103" t="s">
-        <v>543</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104">
       <c r="Y104" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105">
       <c r="Y105" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="106">
       <c r="Y106" t="s">
-        <v>384</v>
+        <v>543</v>
       </c>
     </row>
     <row r="107">
       <c r="Y107" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="108">
       <c r="Y108" t="s">
-        <v>143</v>
+        <v>544</v>
       </c>
     </row>
     <row r="109">
       <c r="Y109" t="s">
-        <v>144</v>
+        <v>384</v>
       </c>
     </row>
     <row r="110">
       <c r="Y110" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111">
       <c r="Y111" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112">
       <c r="Y112" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113">
       <c r="Y113" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114">
       <c r="Y114" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115">
       <c r="Y115" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116">
       <c r="Y116" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117">
       <c r="Y117" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118">
       <c r="Y118" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119">
       <c r="Y119" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="120">
       <c r="Y120" t="s">
-        <v>479</v>
+        <v>152</v>
       </c>
     </row>
     <row r="121">
       <c r="Y121" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="122">
       <c r="Y122" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="123">
       <c r="Y123" t="s">
-        <v>157</v>
+        <v>479</v>
       </c>
     </row>
     <row r="124">
       <c r="Y124" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125">
       <c r="Y125" t="s">
-        <v>40</v>
+        <v>581</v>
       </c>
     </row>
     <row r="126">
       <c r="Y126" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127">
       <c r="Y127" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128">
       <c r="Y128" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129">
       <c r="Y129" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="Y130" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="Y131" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="Y132" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="Y133" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[built-in functions] - [$(array)]: fixed previous erroneous parsing where surrounding `{...}` and `[...]` characters are removed necessarily.
[expression]
- [LIST expression]: fixed previous erroneous parsing where surrounding `{...}` and `[...]` characters are removed necessarily.

[web]
- [saveInfiniteDivsAsCsv(config,file)]: renamed from its previous command name `saveISTDivsAsCsv()`. The new name is more readable.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -23,7 +23,7 @@
     <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$97</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$98</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$5</definedName>
     <definedName name="image">'#system'!$J$2:$J$7</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19683" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20238" uniqueCount="585">
   <si>
     <t>description</t>
   </si>
@@ -1817,6 +1817,12 @@
   </si>
   <si>
     <t>saveISTDivsAsCsv(config,file)</t>
+  </si>
+  <si>
+    <t>assertElementNotPresent(name)</t>
+  </si>
+  <si>
+    <t>saveInfiniteDivsAsCsv(config,file)</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1830,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="600" x14ac:knownFonts="1">
+  <fonts count="616" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5615,8 +5621,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1029">
+  <fills count="1056">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11443,8 +11550,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1070">
+  <borders count="1102">
     <border>
       <left/>
       <right/>
@@ -19467,6 +19727,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -22259,7 +22845,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="611">
+  <cellXfs count="627">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -24050,52 +24636,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1001" fontId="583" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="584" fillId="1004" borderId="1045" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="585" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1045" fillId="1004" fontId="584" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="585" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="586" fillId="1007" borderId="1049" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1049" fillId="1007" fontId="586" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="587" fillId="1010" borderId="1053" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1053" fillId="1010" fontId="587" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="588" fillId="1013" borderId="1057" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1057" fillId="1013" fontId="588" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="589" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="589" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="590" fillId="1016" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1016" fontId="590" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="591" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="592" fillId="1019" borderId="1061" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="593" fillId="1010" borderId="1065" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="594" fillId="1022" borderId="1069" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="595" fillId="1022" borderId="1069" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="596" fillId="1013" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="597" fillId="1025" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="598" fillId="1013" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="599" fillId="1028" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="591" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1061" fillId="1019" fontId="592" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1065" fillId="1010" fontId="593" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1069" fillId="1022" fontId="594" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1069" fillId="1022" fontId="595" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1013" fontId="596" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1025" fontId="597" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1013" fontId="598" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1028" fontId="599" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="600" fillId="1031" borderId="1077" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="601" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="602" fillId="1034" borderId="1081" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="603" fillId="1037" borderId="1085" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="604" fillId="1040" borderId="1089" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="605" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="606" fillId="1043" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="607" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="608" fillId="1046" borderId="1093" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="609" fillId="1037" borderId="1097" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="610" fillId="1049" borderId="1101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="611" fillId="1049" borderId="1101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="612" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="613" fillId="1052" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="614" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="615" fillId="1055" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -24772,7 +25406,7 @@
         <v>474</v>
       </c>
       <c r="G5" t="s">
-        <v>337</v>
+        <v>583</v>
       </c>
       <c r="H5" t="s">
         <v>490</v>
@@ -24846,7 +25480,7 @@
         <v>537</v>
       </c>
       <c r="G6" t="s">
-        <v>389</v>
+        <v>337</v>
       </c>
       <c r="H6" t="s">
         <v>486</v>
@@ -24908,7 +25542,7 @@
         <v>215</v>
       </c>
       <c r="G7" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="H7" t="s">
         <v>482</v>
@@ -24970,7 +25604,7 @@
         <v>320</v>
       </c>
       <c r="G8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H8" t="s">
         <v>329</v>
@@ -25026,7 +25660,7 @@
         <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>308</v>
+        <v>368</v>
       </c>
       <c r="H9" t="s">
         <v>330</v>
@@ -25070,7 +25704,7 @@
         <v>317</v>
       </c>
       <c r="G10" t="s">
-        <v>353</v>
+        <v>308</v>
       </c>
       <c r="H10" t="s">
         <v>487</v>
@@ -25111,7 +25745,7 @@
         <v>250</v>
       </c>
       <c r="G11" t="s">
-        <v>275</v>
+        <v>353</v>
       </c>
       <c r="H11" t="s">
         <v>323</v>
@@ -25149,7 +25783,7 @@
         <v>321</v>
       </c>
       <c r="G12" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="H12" t="s">
         <v>324</v>
@@ -25187,7 +25821,7 @@
         <v>342</v>
       </c>
       <c r="G13" t="s">
-        <v>318</v>
+        <v>264</v>
       </c>
       <c r="H13" t="s">
         <v>325</v>
@@ -25222,7 +25856,7 @@
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="H14" t="s">
         <v>326</v>
@@ -25257,7 +25891,7 @@
         <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K15" t="s">
         <v>540</v>
@@ -25289,7 +25923,7 @@
         <v>386</v>
       </c>
       <c r="G16" t="s">
-        <v>319</v>
+        <v>266</v>
       </c>
       <c r="K16" t="s">
         <v>73</v>
@@ -25321,7 +25955,7 @@
         <v>387</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="K17" t="s">
         <v>74</v>
@@ -25347,7 +25981,7 @@
         <v>411</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K18" t="s">
         <v>491</v>
@@ -25370,7 +26004,7 @@
         <v>52</v>
       </c>
       <c r="G19" t="s">
-        <v>297</v>
+        <v>82</v>
       </c>
       <c r="K19" t="s">
         <v>75</v>
@@ -25390,7 +26024,7 @@
         <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K20" t="s">
         <v>76</v>
@@ -25410,7 +26044,7 @@
         <v>574</v>
       </c>
       <c r="G21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K21" t="s">
         <v>381</v>
@@ -25430,7 +26064,7 @@
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K22" t="s">
         <v>505</v>
@@ -25450,7 +26084,7 @@
         <v>322</v>
       </c>
       <c r="G23" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="K23" t="s">
         <v>37</v>
@@ -25470,7 +26104,7 @@
         <v>55</v>
       </c>
       <c r="G24" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="K24" t="s">
         <v>393</v>
@@ -25490,7 +26124,7 @@
         <v>483</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>280</v>
       </c>
       <c r="K25" t="s">
         <v>557</v>
@@ -25510,7 +26144,7 @@
         <v>216</v>
       </c>
       <c r="G26" t="s">
-        <v>283</v>
+        <v>68</v>
       </c>
       <c r="K26" t="s">
         <v>77</v>
@@ -25530,7 +26164,7 @@
         <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="K27" t="s">
         <v>475</v>
@@ -25550,7 +26184,7 @@
         <v>503</v>
       </c>
       <c r="G28" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="K28" t="s">
         <v>38</v>
@@ -25567,7 +26201,7 @@
         <v>504</v>
       </c>
       <c r="G29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K29" t="s">
         <v>39</v>
@@ -25584,7 +26218,7 @@
         <v>453</v>
       </c>
       <c r="G30" t="s">
-        <v>208</v>
+        <v>285</v>
       </c>
       <c r="Y30" t="s">
         <v>107</v>
@@ -25595,7 +26229,7 @@
         <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>276</v>
+        <v>208</v>
       </c>
       <c r="Y31" t="s">
         <v>108</v>
@@ -25606,7 +26240,7 @@
         <v>57</v>
       </c>
       <c r="G32" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="Y32" t="s">
         <v>109</v>
@@ -25617,7 +26251,7 @@
         <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>541</v>
+        <v>286</v>
       </c>
       <c r="Y33" t="s">
         <v>110</v>
@@ -25628,7 +26262,7 @@
         <v>59</v>
       </c>
       <c r="G34" t="s">
-        <v>261</v>
+        <v>541</v>
       </c>
       <c r="Y34" t="s">
         <v>580</v>
@@ -25639,7 +26273,7 @@
         <v>60</v>
       </c>
       <c r="G35" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
       <c r="Y35" t="s">
         <v>111</v>
@@ -25650,7 +26284,7 @@
         <v>61</v>
       </c>
       <c r="G36" t="s">
-        <v>309</v>
+        <v>331</v>
       </c>
       <c r="Y36" t="s">
         <v>112</v>
@@ -25661,7 +26295,7 @@
         <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>262</v>
+        <v>309</v>
       </c>
       <c r="Y37" t="s">
         <v>202</v>
@@ -25672,7 +26306,7 @@
         <v>63</v>
       </c>
       <c r="G38" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="Y38" t="s">
         <v>113</v>
@@ -25680,7 +26314,7 @@
     </row>
     <row r="39">
       <c r="G39" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="Y39" t="s">
         <v>339</v>
@@ -25688,7 +26322,7 @@
     </row>
     <row r="40">
       <c r="G40" t="s">
-        <v>70</v>
+        <v>268</v>
       </c>
       <c r="Y40" t="s">
         <v>470</v>
@@ -25696,7 +26330,7 @@
     </row>
     <row r="41">
       <c r="G41" t="s">
-        <v>204</v>
+        <v>70</v>
       </c>
       <c r="Y41" t="s">
         <v>561</v>
@@ -25704,7 +26338,7 @@
     </row>
     <row r="42">
       <c r="G42" t="s">
-        <v>576</v>
+        <v>204</v>
       </c>
       <c r="Y42" t="s">
         <v>394</v>
@@ -25712,7 +26346,7 @@
     </row>
     <row r="43">
       <c r="G43" t="s">
-        <v>290</v>
+        <v>576</v>
       </c>
       <c r="Y43" t="s">
         <v>114</v>
@@ -25720,7 +26354,7 @@
     </row>
     <row r="44">
       <c r="G44" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="Y44" t="s">
         <v>115</v>
@@ -25728,7 +26362,7 @@
     </row>
     <row r="45">
       <c r="G45" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Y45" t="s">
         <v>116</v>
@@ -25736,7 +26370,7 @@
     </row>
     <row r="46">
       <c r="G46" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="Y46" t="s">
         <v>117</v>
@@ -25744,7 +26378,7 @@
     </row>
     <row r="47">
       <c r="G47" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Y47" t="s">
         <v>118</v>
@@ -25752,7 +26386,7 @@
     </row>
     <row r="48">
       <c r="G48" t="s">
-        <v>203</v>
+        <v>343</v>
       </c>
       <c r="Y48" t="s">
         <v>119</v>
@@ -25760,7 +26394,7 @@
     </row>
     <row r="49">
       <c r="G49" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="Y49" t="s">
         <v>477</v>
@@ -25768,7 +26402,7 @@
     </row>
     <row r="50">
       <c r="G50" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="Y50" t="s">
         <v>205</v>
@@ -25776,7 +26410,7 @@
     </row>
     <row r="51">
       <c r="G51" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="Y51" t="s">
         <v>69</v>
@@ -25784,7 +26418,7 @@
     </row>
     <row r="52">
       <c r="G52" t="s">
-        <v>304</v>
+        <v>369</v>
       </c>
       <c r="Y52" t="s">
         <v>566</v>
@@ -25792,7 +26426,7 @@
     </row>
     <row r="53">
       <c r="G53" t="s">
-        <v>357</v>
+        <v>304</v>
       </c>
       <c r="Y53" t="s">
         <v>120</v>
@@ -25800,7 +26434,7 @@
     </row>
     <row r="54">
       <c r="G54" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="Y54" t="s">
         <v>121</v>
@@ -25808,7 +26442,7 @@
     </row>
     <row r="55">
       <c r="G55" t="s">
-        <v>269</v>
+        <v>332</v>
       </c>
       <c r="Y55" t="s">
         <v>122</v>
@@ -25816,7 +26450,7 @@
     </row>
     <row r="56">
       <c r="G56" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="Y56" t="s">
         <v>516</v>
@@ -25824,7 +26458,7 @@
     </row>
     <row r="57">
       <c r="G57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Y57" t="s">
         <v>500</v>
@@ -25832,7 +26466,7 @@
     </row>
     <row r="58">
       <c r="G58" t="s">
-        <v>577</v>
+        <v>294</v>
       </c>
       <c r="Y58" t="s">
         <v>123</v>
@@ -25840,7 +26474,7 @@
     </row>
     <row r="59">
       <c r="G59" t="s">
-        <v>295</v>
+        <v>577</v>
       </c>
       <c r="Y59" t="s">
         <v>347</v>
@@ -25848,7 +26482,7 @@
     </row>
     <row r="60">
       <c r="G60" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="Y60" t="s">
         <v>494</v>
@@ -25856,7 +26490,7 @@
     </row>
     <row r="61">
       <c r="G61" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="Y61" t="s">
         <v>124</v>
@@ -25864,7 +26498,7 @@
     </row>
     <row r="62">
       <c r="G62" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="Y62" t="s">
         <v>125</v>
@@ -25872,7 +26506,7 @@
     </row>
     <row r="63">
       <c r="G63" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="Y63" t="s">
         <v>126</v>
@@ -25880,7 +26514,7 @@
     </row>
     <row r="64">
       <c r="G64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Y64" t="s">
         <v>127</v>
@@ -25888,7 +26522,7 @@
     </row>
     <row r="65">
       <c r="G65" t="s">
-        <v>370</v>
+        <v>312</v>
       </c>
       <c r="Y65" t="s">
         <v>128</v>
@@ -25896,7 +26530,7 @@
     </row>
     <row r="66">
       <c r="G66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Y66" t="s">
         <v>129</v>
@@ -25904,7 +26538,7 @@
     </row>
     <row r="67">
       <c r="G67" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="Y67" t="s">
         <v>130</v>
@@ -25912,7 +26546,7 @@
     </row>
     <row r="68">
       <c r="G68" t="s">
-        <v>315</v>
+        <v>346</v>
       </c>
       <c r="Y68" t="s">
         <v>473</v>
@@ -25920,7 +26554,7 @@
     </row>
     <row r="69">
       <c r="G69" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="Y69" t="s">
         <v>508</v>
@@ -25928,7 +26562,7 @@
     </row>
     <row r="70">
       <c r="G70" t="s">
-        <v>562</v>
+        <v>270</v>
       </c>
       <c r="Y70" t="s">
         <v>206</v>
@@ -25936,7 +26570,7 @@
     </row>
     <row r="71">
       <c r="G71" t="s">
-        <v>316</v>
+        <v>562</v>
       </c>
       <c r="Y71" t="s">
         <v>390</v>
@@ -25944,7 +26578,7 @@
     </row>
     <row r="72">
       <c r="G72" t="s">
-        <v>409</v>
+        <v>316</v>
       </c>
       <c r="Y72" t="s">
         <v>478</v>
@@ -25952,7 +26586,7 @@
     </row>
     <row r="73">
       <c r="G73" t="s">
-        <v>306</v>
+        <v>409</v>
       </c>
       <c r="Y73" t="s">
         <v>131</v>
@@ -25960,7 +26594,7 @@
     </row>
     <row r="74">
       <c r="G74" t="s">
-        <v>410</v>
+        <v>306</v>
       </c>
       <c r="Y74" t="s">
         <v>132</v>
@@ -25968,7 +26602,7 @@
     </row>
     <row r="75">
       <c r="G75" t="s">
-        <v>263</v>
+        <v>410</v>
       </c>
       <c r="Y75" t="s">
         <v>133</v>
@@ -25976,7 +26610,7 @@
     </row>
     <row r="76">
       <c r="G76" t="s">
-        <v>542</v>
+        <v>263</v>
       </c>
       <c r="Y76" t="s">
         <v>134</v>
@@ -25984,7 +26618,7 @@
     </row>
     <row r="77">
       <c r="G77" t="s">
-        <v>345</v>
+        <v>542</v>
       </c>
       <c r="Y77" t="s">
         <v>189</v>
@@ -25992,7 +26626,7 @@
     </row>
     <row r="78">
       <c r="G78" t="s">
-        <v>281</v>
+        <v>345</v>
       </c>
       <c r="Y78" t="s">
         <v>190</v>
@@ -26000,7 +26634,7 @@
     </row>
     <row r="79">
       <c r="G79" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="Y79" t="s">
         <v>489</v>
@@ -26008,7 +26642,7 @@
     </row>
     <row r="80">
       <c r="G80" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="Y80" t="s">
         <v>502</v>
@@ -26016,7 +26650,7 @@
     </row>
     <row r="81">
       <c r="G81" t="s">
-        <v>464</v>
+        <v>292</v>
       </c>
       <c r="Y81" t="s">
         <v>135</v>
@@ -26024,7 +26658,7 @@
     </row>
     <row r="82">
       <c r="G82" t="s">
-        <v>333</v>
+        <v>464</v>
       </c>
       <c r="Y82" t="s">
         <v>136</v>
@@ -26032,7 +26666,7 @@
     </row>
     <row r="83">
       <c r="G83" t="s">
-        <v>271</v>
+        <v>333</v>
       </c>
       <c r="Y83" t="s">
         <v>137</v>
@@ -26040,7 +26674,7 @@
     </row>
     <row r="84">
       <c r="G84" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="Y84" t="s">
         <v>529</v>
@@ -26048,7 +26682,7 @@
     </row>
     <row r="85">
       <c r="G85" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="Y85" t="s">
         <v>138</v>
@@ -26056,7 +26690,7 @@
     </row>
     <row r="86">
       <c r="G86" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="Y86" t="s">
         <v>139</v>
@@ -26064,7 +26698,7 @@
     </row>
     <row r="87">
       <c r="G87" t="s">
-        <v>563</v>
+        <v>277</v>
       </c>
       <c r="Y87" t="s">
         <v>191</v>
@@ -26072,7 +26706,7 @@
     </row>
     <row r="88">
       <c r="G88" t="s">
-        <v>272</v>
+        <v>563</v>
       </c>
       <c r="Y88" t="s">
         <v>517</v>
@@ -26080,7 +26714,7 @@
     </row>
     <row r="89">
       <c r="G89" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="Y89" t="s">
         <v>192</v>
@@ -26088,7 +26722,7 @@
     </row>
     <row r="90">
       <c r="G90" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="Y90" t="s">
         <v>488</v>
@@ -26096,7 +26730,7 @@
     </row>
     <row r="91">
       <c r="G91" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y91" t="s">
         <v>193</v>
@@ -26104,7 +26738,7 @@
     </row>
     <row r="92">
       <c r="G92" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="Y92" t="s">
         <v>194</v>
@@ -26112,15 +26746,15 @@
     </row>
     <row r="93">
       <c r="G93" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="Y93" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="94">
       <c r="G94" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="Y94" t="s">
         <v>207</v>
@@ -26128,7 +26762,7 @@
     </row>
     <row r="95">
       <c r="G95" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="Y95" t="s">
         <v>140</v>
@@ -26136,7 +26770,7 @@
     </row>
     <row r="96">
       <c r="G96" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="Y96" t="s">
         <v>195</v>
@@ -26144,13 +26778,16 @@
     </row>
     <row r="97">
       <c r="G97" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y97" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="98">
+      <c r="G98" t="s">
+        <v>279</v>
+      </c>
       <c r="Y98" t="s">
         <v>472</v>
       </c>

</xml_diff>

<commit_message>
[localdb] - [`importCSV(var,csv,table)`]: fixed to support `(` and `)` characters in column name.
[web]
- [`saveInfiniteTableAsCsv`]: *NEW* command to harvest data from a Infinite Scrolling Table as CSV
- [`saveInfiniteTableAsCsv`] and [`saveInfiniteDivsAsCsv`]: supports long running headers that are rendered off-screen

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$133</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$134</definedName>
     <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20238" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20794" uniqueCount="586">
   <si>
     <t>description</t>
   </si>
@@ -1823,6 +1823,9 @@
   </si>
   <si>
     <t>saveInfiniteDivsAsCsv(config,file)</t>
+  </si>
+  <si>
+    <t>saveInfiniteTableAsCsv(config,file)</t>
   </si>
 </sst>
 </file>
@@ -1830,7 +1833,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="616" x14ac:knownFonts="1">
+  <fonts count="632" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5722,8 +5725,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1056">
+  <fills count="1083">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11703,8 +11807,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1102">
+  <borders count="1134">
     <border>
       <left/>
       <right/>
@@ -19727,6 +19984,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -22845,7 +23428,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="627">
+  <cellXfs count="643">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -24684,52 +25267,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1028" fontId="599" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="600" fillId="1031" borderId="1077" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="601" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1077" fillId="1031" fontId="600" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="601" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="602" fillId="1034" borderId="1081" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1081" fillId="1034" fontId="602" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="603" fillId="1037" borderId="1085" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1085" fillId="1037" fontId="603" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="604" fillId="1040" borderId="1089" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1089" fillId="1040" fontId="604" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="605" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="605" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="606" fillId="1043" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1043" fontId="606" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="607" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="608" fillId="1046" borderId="1093" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="609" fillId="1037" borderId="1097" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="610" fillId="1049" borderId="1101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="611" fillId="1049" borderId="1101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="612" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="613" fillId="1052" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="614" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="615" fillId="1055" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="607" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1093" fillId="1046" fontId="608" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1097" fillId="1037" fontId="609" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1101" fillId="1049" fontId="610" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1101" fillId="1049" fontId="611" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1040" fontId="612" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1052" fontId="613" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1040" fontId="614" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1055" fontId="615" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="616" fillId="1058" borderId="1109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="617" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="618" fillId="1061" borderId="1113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="619" fillId="1064" borderId="1117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="620" fillId="1067" borderId="1121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="621" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="622" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="623" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="624" fillId="1073" borderId="1125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="625" fillId="1064" borderId="1129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="626" fillId="1076" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="627" fillId="1076" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="628" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="629" fillId="1079" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="630" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="631" fillId="1082" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -25027,7 +25658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE133"/>
+  <dimension ref="A1:AE134"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -26757,7 +27388,7 @@
         <v>313</v>
       </c>
       <c r="Y94" t="s">
-        <v>207</v>
+        <v>585</v>
       </c>
     </row>
     <row r="95">
@@ -26765,7 +27396,7 @@
         <v>296</v>
       </c>
       <c r="Y95" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96">
@@ -26773,7 +27404,7 @@
         <v>341</v>
       </c>
       <c r="Y96" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97">
@@ -26781,7 +27412,7 @@
         <v>278</v>
       </c>
       <c r="Y97" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98">
@@ -26789,181 +27420,186 @@
         <v>279</v>
       </c>
       <c r="Y98" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="99">
       <c r="Y99" t="s">
-        <v>196</v>
+        <v>472</v>
       </c>
     </row>
     <row r="100">
       <c r="Y100" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="101">
       <c r="Y101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102">
       <c r="Y102" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103">
       <c r="Y103" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="104">
       <c r="Y104" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105">
       <c r="Y105" t="s">
-        <v>536</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106">
       <c r="Y106" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="107">
       <c r="Y107" t="s">
-        <v>141</v>
+        <v>543</v>
       </c>
     </row>
     <row r="108">
       <c r="Y108" t="s">
-        <v>544</v>
+        <v>141</v>
       </c>
     </row>
     <row r="109">
       <c r="Y109" t="s">
-        <v>384</v>
+        <v>544</v>
       </c>
     </row>
     <row r="110">
       <c r="Y110" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="111">
       <c r="Y111" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="112">
       <c r="Y112" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113">
       <c r="Y113" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114">
       <c r="Y114" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115">
       <c r="Y115" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116">
       <c r="Y116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117">
       <c r="Y117" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="118">
       <c r="Y118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119">
       <c r="Y119" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120">
       <c r="Y120" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121">
       <c r="Y121" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122">
       <c r="Y122" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123">
       <c r="Y123" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124">
       <c r="Y124" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="125">
       <c r="Y125" t="s">
-        <v>581</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126">
       <c r="Y126" t="s">
-        <v>156</v>
+        <v>581</v>
       </c>
     </row>
     <row r="127">
       <c r="Y127" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="128">
       <c r="Y128" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="129">
       <c r="Y129" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130">
       <c r="Y130" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="131">
       <c r="Y131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="132">
       <c r="Y132" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="133">
       <c r="Y133" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="Y134" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[base] - [`assertNotContain(text,substring)`]: renamed from `assertNotContains(text,substring)` (grammatically displeasing)
[web]
- [`assertAttributeContains(locator,attrName,contains)`]: support `REGEX:` in `contains` to trigger regular expression matching.
- [`assertAttributeNotContain(locator,attrName,contains)`]:
  - renamed from `assertAttributeNotContains(locator,attrName,contains)` (grammatically displeasing)
  - support `REGEX:` in `contains` to trigger regular expression matching.
- [`assertTextNotContain(locator,text)`]: renamed from `assertTextNotContains(locator,text)` (grammatically displeasing)

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,40 +19,41 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$E$2:$E$39</definedName>
-    <definedName name="csv">'#system'!$F$2:$F$6</definedName>
+    <definedName name="base">'#system'!$F$2:$F$39</definedName>
+    <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$98</definedName>
-    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
-    <definedName name="external">'#system'!$I$2:$I$5</definedName>
-    <definedName name="image">'#system'!$J$2:$J$7</definedName>
-    <definedName name="io">'#system'!$K$2:$K$29</definedName>
-    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$18</definedName>
-    <definedName name="mail">'#system'!$P$2:$P$2</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$14</definedName>
+    <definedName name="external">'#system'!$J$2:$J$5</definedName>
+    <definedName name="image">'#system'!$K$2:$K$7</definedName>
+    <definedName name="io">'#system'!$L$2:$L$29</definedName>
+    <definedName name="jms">'#system'!$M$2:$M$4</definedName>
+    <definedName name="json">'#system'!$N$2:$N$18</definedName>
+    <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$Q$2:$Q$16</definedName>
-    <definedName name="pdf">'#system'!$R$2:$R$16</definedName>
-    <definedName name="rdbms">'#system'!$S$2:$S$7</definedName>
-    <definedName name="redis">'#system'!$T$2:$T$10</definedName>
-    <definedName name="sms">'#system'!$U$2:$U$2</definedName>
-    <definedName name="sound">'#system'!$V$2:$V$5</definedName>
-    <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
-    <definedName name="step">'#system'!$X$2:$X$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$134</definedName>
-    <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
-    <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
-    <definedName name="macro">'#system'!$O$2:$O$4</definedName>
+    <definedName name="number">'#system'!$R$2:$R$16</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$16</definedName>
+    <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
+    <definedName name="redis">'#system'!$U$2:$U$10</definedName>
+    <definedName name="sms">'#system'!$V$2:$V$2</definedName>
+    <definedName name="sound">'#system'!$W$2:$W$5</definedName>
+    <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
+    <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$31</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
+    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
+    <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
+    <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
+    <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
-    <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
+    <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
+    <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20794" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21354" uniqueCount="592">
   <si>
     <t>description</t>
   </si>
@@ -1826,6 +1827,24 @@
   </si>
   <si>
     <t>saveInfiniteTableAsCsv(config,file)</t>
+  </si>
+  <si>
+    <t>aws.vision</t>
+  </si>
+  <si>
+    <t>saveText(profile,image,var)</t>
+  </si>
+  <si>
+    <t>assertNotContain(text,substring)</t>
+  </si>
+  <si>
+    <t>assertAttributeNotContain(locator,attrName,contains)</t>
+  </si>
+  <si>
+    <t>assertTextNotContain(locator,text)</t>
+  </si>
+  <si>
+    <t>screenshot(file,locator)</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1852,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="632" x14ac:knownFonts="1">
+  <fonts count="648" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5826,8 +5845,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1083">
+  <fills count="1110">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11960,8 +12080,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1134">
+  <borders count="1166">
     <border>
       <left/>
       <right/>
@@ -19984,6 +20257,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -23428,7 +24027,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="643">
+  <cellXfs count="659">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -25315,52 +25914,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1055" fontId="615" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="616" fillId="1058" borderId="1109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="617" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1109" fillId="1058" fontId="616" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="617" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="618" fillId="1061" borderId="1113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1113" fillId="1061" fontId="618" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="619" fillId="1064" borderId="1117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1117" fillId="1064" fontId="619" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="620" fillId="1067" borderId="1121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1121" fillId="1067" fontId="620" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="621" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="621" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="622" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1070" fontId="622" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="623" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="624" fillId="1073" borderId="1125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="625" fillId="1064" borderId="1129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="626" fillId="1076" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="627" fillId="1076" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="628" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="629" fillId="1079" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="630" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="631" fillId="1082" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="623" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1125" fillId="1073" fontId="624" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1129" fillId="1064" fontId="625" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1133" fillId="1076" fontId="626" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1133" fillId="1076" fontId="627" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1067" fontId="628" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1079" fontId="629" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1067" fontId="630" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1082" fontId="631" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="632" fillId="1085" borderId="1141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="633" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="634" fillId="1088" borderId="1145" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="635" fillId="1091" borderId="1149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="636" fillId="1094" borderId="1153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="637" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="638" fillId="1097" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="639" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="640" fillId="1100" borderId="1157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="641" fillId="1091" borderId="1161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="642" fillId="1103" borderId="1165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="643" fillId="1103" borderId="1165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="644" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="645" fillId="1106" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="646" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="647" fillId="1109" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -25658,7 +26305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE134"/>
+  <dimension ref="A1:AF135"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -25681,81 +26328,84 @@
         <v>519</v>
       </c>
       <c r="E1" t="s">
+        <v>586</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>348</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>334</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>545</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>246</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>188</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>44</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>230</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>399</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>456</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>413</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>358</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>395</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>458</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -25773,81 +26423,84 @@
         <v>520</v>
       </c>
       <c r="E2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>66</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>484</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>71</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>501</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>317</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>385</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>465</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>546</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>513</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>412</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>466</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>244</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>209</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>400</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>457</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>454</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>382</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>396</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>89</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>163</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>168</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>175</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>468</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>524</v>
       </c>
     </row>
@@ -25864,76 +26517,76 @@
       <c r="D3" t="s">
         <v>556</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>492</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>366</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>511</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>350</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>342</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>335</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>78</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>547</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>514</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>467</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>231</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>210</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>401</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>415</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>383</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>397</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>90</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>164</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>169</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>365</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>176</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -25947,82 +26600,82 @@
       <c r="D4" t="s">
         <v>521</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>65</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>388</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>485</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>512</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>351</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>229</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>336</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>548</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>515</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>19</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>232</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>211</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>402</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>416</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>359</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>398</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>355</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>165</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>170</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>176</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>459</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>586</v>
       </c>
       <c r="B5" t="s">
         <v>376</v>
@@ -26030,73 +26683,73 @@
       <c r="D5" t="s">
         <v>522</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>493</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>474</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>583</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>490</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>560</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>352</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>495</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>558</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>23</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>233</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>212</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>403</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>417</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>360</v>
       </c>
-      <c r="Y5" t="s">
-        <v>356</v>
-      </c>
       <c r="Z5" t="s">
+        <v>589</v>
+      </c>
+      <c r="AA5" t="s">
         <v>166</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>171</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>177</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>460</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>377</v>
@@ -26104,1502 +26757,1510 @@
       <c r="D6" t="s">
         <v>523</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>537</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>337</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>486</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>349</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>64</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>552</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>24</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>234</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>392</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>404</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>362</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>91</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>480</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>172</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>178</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>461</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>378</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>215</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>389</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>482</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>564</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>12</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>317</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>553</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>235</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>414</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>405</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>361</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>92</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>481</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>173</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>179</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>462</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>379</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>320</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>367</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>329</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>538</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>27</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>554</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>83</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>236</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>406</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>363</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>93</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>167</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>174</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>180</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>463</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>380</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>368</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>330</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>72</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>28</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>559</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>84</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>237</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>407</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>364</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>201</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>181</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>348</v>
-      </c>
-      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
         <v>317</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>308</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>487</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>31</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>29</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>549</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>469</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>238</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>408</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>258</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>182</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>250</v>
-      </c>
-      <c r="G11" t="s">
+        <v>348</v>
+      </c>
+      <c r="F11" t="s">
+        <v>588</v>
+      </c>
+      <c r="H11" t="s">
         <v>353</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>323</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>539</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>507</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>550</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>85</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>239</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>259</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>260</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>334</v>
-      </c>
-      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>321</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>275</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>324</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>391</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>565</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>551</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>34</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>240</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>94</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>183</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" t="s">
         <v>342</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>264</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>325</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>13</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>476</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>86</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>245</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>327</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>184</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>545</v>
-      </c>
-      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
         <v>30</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>318</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>326</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>35</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>506</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>87</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>241</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>95</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>185</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E15" t="s">
+        <v>545</v>
+      </c>
+      <c r="F15" t="s">
         <v>51</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>265</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>540</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>32</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>533</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>242</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>96</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>186</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>188</v>
-      </c>
-      <c r="E16" t="s">
+        <v>246</v>
+      </c>
+      <c r="F16" t="s">
         <v>386</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>266</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>73</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>578</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>534</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>243</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>67</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>187</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" t="s">
         <v>387</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>319</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>74</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>33</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>535</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>496</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
         <v>411</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>81</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>491</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>36</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>97</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" t="s">
         <v>52</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>82</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>75</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>98</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>399</v>
-      </c>
-      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
         <v>53</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>297</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>76</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>99</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>456</v>
-      </c>
-      <c r="E21" t="s">
+        <v>399</v>
+      </c>
+      <c r="F21" t="s">
         <v>574</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>298</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>381</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>100</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>413</v>
-      </c>
-      <c r="E22" t="s">
+        <v>456</v>
+      </c>
+      <c r="F22" t="s">
         <v>54</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>299</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>505</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>518</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>358</v>
-      </c>
-      <c r="E23" t="s">
+        <v>413</v>
+      </c>
+      <c r="F23" t="s">
         <v>322</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>300</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>37</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>102</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>395</v>
-      </c>
-      <c r="E24" t="s">
+        <v>358</v>
+      </c>
+      <c r="F24" t="s">
         <v>55</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>291</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>393</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>579</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" t="s">
+        <v>395</v>
+      </c>
+      <c r="F25" t="s">
         <v>483</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>280</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>557</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>103</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
         <v>216</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>68</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>77</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>104</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
         <v>217</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>283</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>475</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>105</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s">
         <v>503</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>267</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>38</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>458</v>
-      </c>
-      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" t="s">
         <v>504</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>284</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>39</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>458</v>
+      </c>
+      <c r="F30" t="s">
+        <v>453</v>
+      </c>
+      <c r="H30" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>218</v>
       </c>
-      <c r="E30" t="s">
-        <v>453</v>
-      </c>
-      <c r="G30" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>56</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>208</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="32">
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>57</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>276</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="33">
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>58</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>286</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="34">
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>59</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>541</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="35">
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>60</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>261</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="36">
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>61</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>331</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="37">
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>62</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>309</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="38">
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>63</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>262</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Z38" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="39">
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>310</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="40">
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>268</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="41">
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>70</v>
       </c>
-      <c r="Y41" t="s">
-        <v>561</v>
+      <c r="Z41" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="42">
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>204</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="43">
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>576</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="44">
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>290</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="45">
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>301</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46">
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>302</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="47">
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>344</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="48">
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>343</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="49">
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>203</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="50">
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>303</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="51">
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>340</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52">
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>369</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="53">
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>304</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="54">
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>357</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="55">
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>332</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="56">
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>269</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="57">
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>293</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="58">
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>294</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59">
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>577</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="60">
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>295</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="61">
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>305</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="62">
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>314</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="63">
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>338</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="64">
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>311</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="65">
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>312</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="66">
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>370</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="67">
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>371</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="68">
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>346</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="69">
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>315</v>
       </c>
-      <c r="Y69" t="s">
+      <c r="Z69" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="70">
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>270</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Z70" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="71">
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>562</v>
       </c>
-      <c r="Y71" t="s">
+      <c r="Z71" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="72">
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>316</v>
       </c>
-      <c r="Y72" t="s">
+      <c r="Z72" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="73">
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>409</v>
       </c>
-      <c r="Y73" t="s">
+      <c r="Z73" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="74">
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>306</v>
       </c>
-      <c r="Y74" t="s">
+      <c r="Z74" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="75">
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>410</v>
       </c>
-      <c r="Y75" t="s">
+      <c r="Z75" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="76">
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>263</v>
       </c>
-      <c r="Y76" t="s">
+      <c r="Z76" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="77">
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>542</v>
       </c>
-      <c r="Y77" t="s">
+      <c r="Z77" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="78">
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>345</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="79">
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>281</v>
       </c>
-      <c r="Y79" t="s">
+      <c r="Z79" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="80">
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>287</v>
       </c>
-      <c r="Y80" t="s">
+      <c r="Z80" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="81">
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>292</v>
       </c>
-      <c r="Y81" t="s">
+      <c r="Z81" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="82">
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>464</v>
       </c>
-      <c r="Y82" t="s">
+      <c r="Z82" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="83">
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>333</v>
       </c>
-      <c r="Y83" t="s">
+      <c r="Z83" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="84">
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>271</v>
       </c>
-      <c r="Y84" t="s">
+      <c r="Z84" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="85">
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>282</v>
       </c>
-      <c r="Y85" t="s">
+      <c r="Z85" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="86">
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>288</v>
       </c>
-      <c r="Y86" t="s">
+      <c r="Z86" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="87">
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>277</v>
       </c>
-      <c r="Y87" t="s">
+      <c r="Z87" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="88">
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>563</v>
       </c>
-      <c r="Y88" t="s">
+      <c r="Z88" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="89">
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>272</v>
       </c>
-      <c r="Y89" t="s">
+      <c r="Z89" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="90">
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>289</v>
       </c>
-      <c r="Y90" t="s">
+      <c r="Z90" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="91">
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>273</v>
       </c>
-      <c r="Y91" t="s">
+      <c r="Z91" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="92">
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>274</v>
       </c>
-      <c r="Y92" t="s">
+      <c r="Z92" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="93">
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>307</v>
       </c>
-      <c r="Y93" t="s">
+      <c r="Z93" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="94">
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>313</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Z94" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="95">
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>296</v>
       </c>
-      <c r="Y95" t="s">
+      <c r="Z95" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="96">
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>341</v>
       </c>
-      <c r="Y96" t="s">
+      <c r="Z96" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="97">
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>278</v>
       </c>
-      <c r="Y97" t="s">
+      <c r="Z97" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="98">
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>279</v>
       </c>
-      <c r="Y98" t="s">
+      <c r="Z98" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="99">
-      <c r="Y99" t="s">
+      <c r="Z99" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="100">
-      <c r="Y100" t="s">
+      <c r="Z100" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="101">
-      <c r="Y101" t="s">
+      <c r="Z101" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="102">
-      <c r="Y102" t="s">
+      <c r="Z102" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="103">
-      <c r="Y103" t="s">
+      <c r="Z103" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="104">
-      <c r="Y104" t="s">
+      <c r="Z104" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="105">
-      <c r="Y105" t="s">
+      <c r="Z105" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="106">
-      <c r="Y106" t="s">
+      <c r="Z106" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="107">
-      <c r="Y107" t="s">
+      <c r="Z107" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="Z108" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="108">
-      <c r="Y108" t="s">
+    <row r="109">
+      <c r="Z109" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="109">
-      <c r="Y109" t="s">
+    <row r="110">
+      <c r="Z110" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="110">
-      <c r="Y110" t="s">
+    <row r="111">
+      <c r="Z111" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="111">
-      <c r="Y111" t="s">
+    <row r="112">
+      <c r="Z112" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="112">
-      <c r="Y112" t="s">
+    <row r="113">
+      <c r="Z113" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="113">
-      <c r="Y113" t="s">
+    <row r="114">
+      <c r="Z114" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="114">
-      <c r="Y114" t="s">
+    <row r="115">
+      <c r="Z115" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="115">
-      <c r="Y115" t="s">
+    <row r="116">
+      <c r="Z116" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="116">
-      <c r="Y116" t="s">
+    <row r="117">
+      <c r="Z117" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="117">
-      <c r="Y117" t="s">
+    <row r="118">
+      <c r="Z118" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="118">
-      <c r="Y118" t="s">
+    <row r="119">
+      <c r="Z119" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="119">
-      <c r="Y119" t="s">
+    <row r="120">
+      <c r="Z120" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="120">
-      <c r="Y120" t="s">
+    <row r="121">
+      <c r="Z121" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="121">
-      <c r="Y121" t="s">
+    <row r="122">
+      <c r="Z122" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="122">
-      <c r="Y122" t="s">
+    <row r="123">
+      <c r="Z123" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="123">
-      <c r="Y123" t="s">
+    <row r="124">
+      <c r="Z124" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="124">
-      <c r="Y124" t="s">
+    <row r="125">
+      <c r="Z125" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="125">
-      <c r="Y125" t="s">
+    <row r="126">
+      <c r="Z126" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="126">
-      <c r="Y126" t="s">
+    <row r="127">
+      <c r="Z127" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="127">
-      <c r="Y127" t="s">
+    <row r="128">
+      <c r="Z128" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="128">
-      <c r="Y128" t="s">
+    <row r="129">
+      <c r="Z129" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="129">
-      <c r="Y129" t="s">
+    <row r="130">
+      <c r="Z130" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="130">
-      <c r="Y130" t="s">
+    <row r="131">
+      <c r="Z131" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="131">
-      <c r="Y131" t="s">
+    <row r="132">
+      <c r="Z132" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="132">
-      <c r="Y132" t="s">
+    <row r="133">
+      <c r="Z133" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="133">
-      <c r="Y133" t="s">
+    <row r="134">
+      <c r="Z134" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="134">
-      <c r="Y134" t="s">
+    <row r="135">
+      <c r="Z135" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[system variable] - [`nexial.summary.header`]: **NEW** System variable to allow user to add customized header (HTML) to execution summary. - [`nexial.summary.footer`]: **NEW** System variable to allow user to add customized footer (HTML) to execution summary.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$F$2:$F$39</definedName>
+    <definedName name="base">'#system'!$F$2:$F$40</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21354" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21915" uniqueCount="594">
   <si>
     <t>description</t>
   </si>
@@ -1845,6 +1845,12 @@
   </si>
   <si>
     <t>screenshot(file,locator)</t>
+  </si>
+  <si>
+    <t>clear(variables)</t>
+  </si>
+  <si>
+    <t>saveMatches(var,path,fileFilter,textFilter)</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1858,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="648" x14ac:knownFonts="1">
+  <fonts count="664" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5946,8 +5952,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1110">
+  <fills count="1137">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12233,8 +12340,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1166">
+  <borders count="1198">
     <border>
       <left/>
       <right/>
@@ -20257,6 +20517,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -24027,7 +24613,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="659">
+  <cellXfs count="675">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -25962,52 +26548,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1082" fontId="631" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="632" fillId="1085" borderId="1141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="633" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1141" fillId="1085" fontId="632" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="633" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="634" fillId="1088" borderId="1145" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1145" fillId="1088" fontId="634" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="635" fillId="1091" borderId="1149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1149" fillId="1091" fontId="635" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="636" fillId="1094" borderId="1153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1153" fillId="1094" fontId="636" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="637" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="637" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="638" fillId="1097" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1097" fontId="638" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="639" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="640" fillId="1100" borderId="1157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="641" fillId="1091" borderId="1161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="642" fillId="1103" borderId="1165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="643" fillId="1103" borderId="1165" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="644" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="645" fillId="1106" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="646" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="647" fillId="1109" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="639" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1157" fillId="1100" fontId="640" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1161" fillId="1091" fontId="641" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1165" fillId="1103" fontId="642" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1165" fillId="1103" fontId="643" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1094" fontId="644" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1106" fontId="645" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1094" fontId="646" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1109" fontId="647" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="648" fillId="1112" borderId="1173" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="649" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="650" fillId="1115" borderId="1177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="651" fillId="1118" borderId="1181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="652" fillId="1121" borderId="1185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="653" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="654" fillId="1124" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="655" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="656" fillId="1127" borderId="1189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="657" fillId="1118" borderId="1193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="658" fillId="1130" borderId="1197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="659" fillId="1130" borderId="1197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="660" fillId="1121" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="661" fillId="1133" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="662" fillId="1121" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="663" fillId="1136" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -27262,7 +27896,7 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>411</v>
+        <v>592</v>
       </c>
       <c r="H18" t="s">
         <v>81</v>
@@ -27285,7 +27919,7 @@
         <v>230</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>411</v>
       </c>
       <c r="H19" t="s">
         <v>82</v>
@@ -27305,7 +27939,7 @@
         <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" t="s">
         <v>297</v>
@@ -27325,13 +27959,13 @@
         <v>399</v>
       </c>
       <c r="F21" t="s">
-        <v>574</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
         <v>298</v>
       </c>
       <c r="L21" t="s">
-        <v>381</v>
+        <v>593</v>
       </c>
       <c r="Z21" t="s">
         <v>100</v>
@@ -27345,7 +27979,7 @@
         <v>456</v>
       </c>
       <c r="F22" t="s">
-        <v>54</v>
+        <v>574</v>
       </c>
       <c r="H22" t="s">
         <v>299</v>
@@ -27365,7 +27999,7 @@
         <v>413</v>
       </c>
       <c r="F23" t="s">
-        <v>322</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s">
         <v>300</v>
@@ -27385,7 +28019,7 @@
         <v>358</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>322</v>
       </c>
       <c r="H24" t="s">
         <v>291</v>
@@ -27405,7 +28039,7 @@
         <v>395</v>
       </c>
       <c r="F25" t="s">
-        <v>483</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
         <v>280</v>
@@ -27425,7 +28059,7 @@
         <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>216</v>
+        <v>483</v>
       </c>
       <c r="H26" t="s">
         <v>68</v>
@@ -27445,7 +28079,7 @@
         <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H27" t="s">
         <v>283</v>
@@ -27465,7 +28099,7 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>503</v>
+        <v>217</v>
       </c>
       <c r="H28" t="s">
         <v>267</v>
@@ -27482,7 +28116,7 @@
         <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H29" t="s">
         <v>284</v>
@@ -27499,7 +28133,7 @@
         <v>458</v>
       </c>
       <c r="F30" t="s">
-        <v>453</v>
+        <v>504</v>
       </c>
       <c r="H30" t="s">
         <v>285</v>
@@ -27513,7 +28147,7 @@
         <v>218</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>453</v>
       </c>
       <c r="H31" t="s">
         <v>208</v>
@@ -27524,7 +28158,7 @@
     </row>
     <row r="32">
       <c r="F32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H32" t="s">
         <v>276</v>
@@ -27535,7 +28169,7 @@
     </row>
     <row r="33">
       <c r="F33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H33" t="s">
         <v>286</v>
@@ -27546,7 +28180,7 @@
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H34" t="s">
         <v>541</v>
@@ -27557,7 +28191,7 @@
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H35" t="s">
         <v>261</v>
@@ -27568,7 +28202,7 @@
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H36" t="s">
         <v>331</v>
@@ -27579,7 +28213,7 @@
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H37" t="s">
         <v>309</v>
@@ -27590,7 +28224,7 @@
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H38" t="s">
         <v>262</v>
@@ -27600,6 +28234,9 @@
       </c>
     </row>
     <row r="39">
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
       <c r="H39" t="s">
         <v>310</v>
       </c>

</xml_diff>

<commit_message>
[fixes] - enforce uniqueness of activity names within single scenario to avoid confusion and runtime error. - enforce activity name must not be spaces only (avoid busy finger or typo).
[ws]
- [`nexial.ws.keepAlive`]: *NEW* System variable to allow TCP connection to be reused (or not) over subsequent calls.
- Errors incurred during a web service call are now logged as part of the "detailed log". See [`nexial.ws.logDetail`] for more details.

[web]
- [Browser Performance Metrics]: format all timing information to 2 decimal-places.
- [Browser Performance Metrics]: minor color updates.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,15 +19,15 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$F$2:$F$40</definedName>
+    <definedName name="base">'#system'!$F$2:$F$39</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
     <definedName name="excel">'#system'!$I$2:$I$14</definedName>
-    <definedName name="external">'#system'!$J$2:$J$5</definedName>
+    <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
-    <definedName name="io">'#system'!$L$2:$L$29</definedName>
+    <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$137</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21915" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22479" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1851,6 +1851,21 @@
   </si>
   <si>
     <t>saveMatches(var,path,fileFilter,textFilter)</t>
+  </si>
+  <si>
+    <t>terminate(programName)</t>
+  </si>
+  <si>
+    <t>assertPath(path)</t>
+  </si>
+  <si>
+    <t>assertAttributeContain(locator,attrName,contains)</t>
+  </si>
+  <si>
+    <t>saveSelectedText(var,locator)</t>
+  </si>
+  <si>
+    <t>saveSelectedValue(var,locator)</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1873,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="664" x14ac:knownFonts="1">
+  <fonts count="680" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6053,8 +6068,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1137">
+  <fills count="1164">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -12493,8 +12609,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1198">
+  <borders count="1230">
     <border>
       <left/>
       <right/>
@@ -20517,6 +20786,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -24613,7 +25208,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="675">
+  <cellXfs count="691">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -26596,52 +27191,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1109" fontId="647" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="648" fillId="1112" borderId="1173" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="649" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1173" fillId="1112" fontId="648" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="649" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="650" fillId="1115" borderId="1177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1177" fillId="1115" fontId="650" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="651" fillId="1118" borderId="1181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1181" fillId="1118" fontId="651" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="652" fillId="1121" borderId="1185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1185" fillId="1121" fontId="652" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="653" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="653" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="654" fillId="1124" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1124" fontId="654" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="655" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="656" fillId="1127" borderId="1189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="657" fillId="1118" borderId="1193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="658" fillId="1130" borderId="1197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="659" fillId="1130" borderId="1197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="660" fillId="1121" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="661" fillId="1133" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="662" fillId="1121" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="663" fillId="1136" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="655" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1189" fillId="1127" fontId="656" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1193" fillId="1118" fontId="657" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1197" fillId="1130" fontId="658" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1197" fillId="1130" fontId="659" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1121" fontId="660" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1133" fontId="661" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1121" fontId="662" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1136" fontId="663" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="664" fillId="1139" borderId="1205" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="665" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="666" fillId="1142" borderId="1209" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="667" fillId="1145" borderId="1213" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="668" fillId="1148" borderId="1217" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="669" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="670" fillId="1151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="671" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="672" fillId="1154" borderId="1221" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="673" fillId="1145" borderId="1225" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="674" fillId="1157" borderId="1229" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="675" fillId="1157" borderId="1229" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="676" fillId="1148" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="677" fillId="1160" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="678" fillId="1148" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="679" fillId="1163" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -26939,7 +27582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF135"/>
+  <dimension ref="A1:AF137"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -27253,7 +27896,7 @@
         <v>351</v>
       </c>
       <c r="L4" t="s">
-        <v>229</v>
+        <v>595</v>
       </c>
       <c r="M4" t="s">
         <v>336</v>
@@ -27289,7 +27932,7 @@
         <v>398</v>
       </c>
       <c r="Z4" t="s">
-        <v>355</v>
+        <v>596</v>
       </c>
       <c r="AA4" t="s">
         <v>165</v>
@@ -27336,7 +27979,7 @@
         <v>352</v>
       </c>
       <c r="L5" t="s">
-        <v>495</v>
+        <v>229</v>
       </c>
       <c r="N5" t="s">
         <v>79</v>
@@ -27403,11 +28046,14 @@
       <c r="I6" t="s">
         <v>486</v>
       </c>
+      <c r="J6" t="s">
+        <v>594</v>
+      </c>
       <c r="K6" t="s">
         <v>349</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>495</v>
       </c>
       <c r="N6" t="s">
         <v>22</v>
@@ -27469,7 +28115,7 @@
         <v>564</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
         <v>317</v>
@@ -27528,7 +28174,7 @@
         <v>329</v>
       </c>
       <c r="L8" t="s">
-        <v>538</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
         <v>27</v>
@@ -27584,7 +28230,7 @@
         <v>330</v>
       </c>
       <c r="L9" t="s">
-        <v>72</v>
+        <v>538</v>
       </c>
       <c r="N9" t="s">
         <v>28</v>
@@ -27628,7 +28274,7 @@
         <v>487</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="N10" t="s">
         <v>29</v>
@@ -27669,7 +28315,7 @@
         <v>323</v>
       </c>
       <c r="L11" t="s">
-        <v>539</v>
+        <v>31</v>
       </c>
       <c r="N11" t="s">
         <v>507</v>
@@ -27707,7 +28353,7 @@
         <v>324</v>
       </c>
       <c r="L12" t="s">
-        <v>391</v>
+        <v>539</v>
       </c>
       <c r="N12" t="s">
         <v>565</v>
@@ -27745,7 +28391,7 @@
         <v>325</v>
       </c>
       <c r="L13" t="s">
-        <v>13</v>
+        <v>391</v>
       </c>
       <c r="N13" t="s">
         <v>476</v>
@@ -27780,7 +28426,7 @@
         <v>326</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="N14" t="s">
         <v>506</v>
@@ -27812,7 +28458,7 @@
         <v>265</v>
       </c>
       <c r="L15" t="s">
-        <v>540</v>
+        <v>35</v>
       </c>
       <c r="N15" t="s">
         <v>32</v>
@@ -27844,7 +28490,7 @@
         <v>266</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>540</v>
       </c>
       <c r="N16" t="s">
         <v>578</v>
@@ -27876,7 +28522,7 @@
         <v>319</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N17" t="s">
         <v>33</v>
@@ -27896,13 +28542,13 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>592</v>
+        <v>411</v>
       </c>
       <c r="H18" t="s">
         <v>81</v>
       </c>
       <c r="L18" t="s">
-        <v>491</v>
+        <v>74</v>
       </c>
       <c r="N18" t="s">
         <v>36</v>
@@ -27919,13 +28565,13 @@
         <v>230</v>
       </c>
       <c r="F19" t="s">
-        <v>411</v>
+        <v>52</v>
       </c>
       <c r="H19" t="s">
         <v>82</v>
       </c>
       <c r="L19" t="s">
-        <v>75</v>
+        <v>491</v>
       </c>
       <c r="Z19" t="s">
         <v>98</v>
@@ -27939,13 +28585,13 @@
         <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
         <v>297</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z20" t="s">
         <v>99</v>
@@ -27959,13 +28605,13 @@
         <v>399</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>574</v>
       </c>
       <c r="H21" t="s">
         <v>298</v>
       </c>
       <c r="L21" t="s">
-        <v>593</v>
+        <v>76</v>
       </c>
       <c r="Z21" t="s">
         <v>100</v>
@@ -27979,13 +28625,13 @@
         <v>456</v>
       </c>
       <c r="F22" t="s">
-        <v>574</v>
+        <v>54</v>
       </c>
       <c r="H22" t="s">
         <v>299</v>
       </c>
       <c r="L22" t="s">
-        <v>505</v>
+        <v>593</v>
       </c>
       <c r="Z22" t="s">
         <v>518</v>
@@ -27999,13 +28645,13 @@
         <v>413</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>322</v>
       </c>
       <c r="H23" t="s">
         <v>300</v>
       </c>
       <c r="L23" t="s">
-        <v>37</v>
+        <v>505</v>
       </c>
       <c r="Z23" t="s">
         <v>102</v>
@@ -28019,13 +28665,13 @@
         <v>358</v>
       </c>
       <c r="F24" t="s">
-        <v>322</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>291</v>
       </c>
       <c r="L24" t="s">
-        <v>393</v>
+        <v>37</v>
       </c>
       <c r="Z24" t="s">
         <v>579</v>
@@ -28039,13 +28685,13 @@
         <v>395</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>483</v>
       </c>
       <c r="H25" t="s">
         <v>280</v>
       </c>
       <c r="L25" t="s">
-        <v>557</v>
+        <v>393</v>
       </c>
       <c r="Z25" t="s">
         <v>103</v>
@@ -28059,13 +28705,13 @@
         <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>483</v>
+        <v>216</v>
       </c>
       <c r="H26" t="s">
         <v>68</v>
       </c>
       <c r="L26" t="s">
-        <v>77</v>
+        <v>557</v>
       </c>
       <c r="Z26" t="s">
         <v>104</v>
@@ -28079,13 +28725,13 @@
         <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H27" t="s">
         <v>283</v>
       </c>
       <c r="L27" t="s">
-        <v>475</v>
+        <v>77</v>
       </c>
       <c r="Z27" t="s">
         <v>105</v>
@@ -28099,13 +28745,13 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>503</v>
       </c>
       <c r="H28" t="s">
         <v>267</v>
       </c>
       <c r="L28" t="s">
-        <v>38</v>
+        <v>475</v>
       </c>
       <c r="Z28" t="s">
         <v>106</v>
@@ -28116,13 +28762,13 @@
         <v>49</v>
       </c>
       <c r="F29" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H29" t="s">
         <v>284</v>
       </c>
       <c r="L29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z29" t="s">
         <v>328</v>
@@ -28133,10 +28779,13 @@
         <v>458</v>
       </c>
       <c r="F30" t="s">
-        <v>504</v>
+        <v>453</v>
       </c>
       <c r="H30" t="s">
         <v>285</v>
+      </c>
+      <c r="L30" t="s">
+        <v>39</v>
       </c>
       <c r="Z30" t="s">
         <v>107</v>
@@ -28147,7 +28796,7 @@
         <v>218</v>
       </c>
       <c r="F31" t="s">
-        <v>453</v>
+        <v>56</v>
       </c>
       <c r="H31" t="s">
         <v>208</v>
@@ -28158,7 +28807,7 @@
     </row>
     <row r="32">
       <c r="F32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H32" t="s">
         <v>276</v>
@@ -28169,7 +28818,7 @@
     </row>
     <row r="33">
       <c r="F33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H33" t="s">
         <v>286</v>
@@ -28180,7 +28829,7 @@
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H34" t="s">
         <v>541</v>
@@ -28191,7 +28840,7 @@
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H35" t="s">
         <v>261</v>
@@ -28202,7 +28851,7 @@
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H36" t="s">
         <v>331</v>
@@ -28213,7 +28862,7 @@
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H37" t="s">
         <v>309</v>
@@ -28224,7 +28873,7 @@
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H38" t="s">
         <v>262</v>
@@ -28234,9 +28883,6 @@
       </c>
     </row>
     <row r="39">
-      <c r="F39" t="s">
-        <v>63</v>
-      </c>
       <c r="H39" t="s">
         <v>310</v>
       </c>
@@ -28718,186 +29364,196 @@
     </row>
     <row r="99">
       <c r="Z99" t="s">
-        <v>472</v>
+        <v>597</v>
       </c>
     </row>
     <row r="100">
       <c r="Z100" t="s">
-        <v>196</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101">
       <c r="Z101" t="s">
-        <v>197</v>
+        <v>472</v>
       </c>
     </row>
     <row r="102">
       <c r="Z102" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103">
       <c r="Z103" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104">
       <c r="Z104" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105">
       <c r="Z105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106">
       <c r="Z106" t="s">
-        <v>536</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107">
       <c r="Z107" t="s">
-        <v>591</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108">
       <c r="Z108" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="109">
       <c r="Z109" t="s">
-        <v>141</v>
+        <v>591</v>
       </c>
     </row>
     <row r="110">
       <c r="Z110" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="111">
       <c r="Z111" t="s">
-        <v>384</v>
+        <v>141</v>
       </c>
     </row>
     <row r="112">
       <c r="Z112" t="s">
-        <v>142</v>
+        <v>544</v>
       </c>
     </row>
     <row r="113">
       <c r="Z113" t="s">
-        <v>143</v>
+        <v>384</v>
       </c>
     </row>
     <row r="114">
       <c r="Z114" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115">
       <c r="Z115" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116">
       <c r="Z116" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117">
       <c r="Z117" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118">
       <c r="Z118" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119">
       <c r="Z119" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120">
       <c r="Z120" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="121">
       <c r="Z121" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122">
       <c r="Z122" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123">
       <c r="Z123" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124">
       <c r="Z124" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125">
       <c r="Z125" t="s">
-        <v>479</v>
+        <v>153</v>
       </c>
     </row>
     <row r="126">
       <c r="Z126" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127">
       <c r="Z127" t="s">
-        <v>581</v>
+        <v>479</v>
       </c>
     </row>
     <row r="128">
       <c r="Z128" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129">
       <c r="Z129" t="s">
-        <v>157</v>
+        <v>581</v>
       </c>
     </row>
     <row r="130">
       <c r="Z130" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="131">
       <c r="Z131" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132">
       <c r="Z132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133">
       <c r="Z133" t="s">
-        <v>160</v>
+        <v>40</v>
       </c>
     </row>
     <row r="134">
       <c r="Z134" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135">
       <c r="Z135" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="Z136" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="Z137" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[web] - [`saveBrowserVersion(var)`]: *NEW* command to current browser version ( along with browser name) to `var`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -43,7 +43,7 @@
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$137</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$138</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23043" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23608" uniqueCount="600">
   <si>
     <t>description</t>
   </si>
@@ -1866,6 +1866,9 @@
   </si>
   <si>
     <t>saveSelectedValue(var,locator)</t>
+  </si>
+  <si>
+    <t>saveBrowserVersion(var)</t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1876,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="696" x14ac:knownFonts="1">
+  <fonts count="712" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6270,8 +6273,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1191">
+  <fills count="1218">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13016,8 +13120,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1262">
+  <borders count="1294">
     <border>
       <left/>
       <right/>
@@ -21040,6 +21297,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -25788,7 +26371,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="707">
+  <cellXfs count="723">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -27867,52 +28450,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1163" fontId="679" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="680" fillId="1166" borderId="1237" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="681" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1237" fillId="1166" fontId="680" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="681" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="682" fillId="1169" borderId="1241" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1241" fillId="1169" fontId="682" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="683" fillId="1172" borderId="1245" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1245" fillId="1172" fontId="683" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="684" fillId="1175" borderId="1249" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1249" fillId="1175" fontId="684" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="685" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="685" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="686" fillId="1178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1178" fontId="686" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="687" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="688" fillId="1181" borderId="1253" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="689" fillId="1172" borderId="1257" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="690" fillId="1184" borderId="1261" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="691" fillId="1184" borderId="1261" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="692" fillId="1175" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="693" fillId="1187" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="694" fillId="1175" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="695" fillId="1190" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="687" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1253" fillId="1181" fontId="688" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1257" fillId="1172" fontId="689" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1261" fillId="1184" fontId="690" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1261" fillId="1184" fontId="691" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1175" fontId="692" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1187" fontId="693" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1175" fontId="694" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1190" fontId="695" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="696" fillId="1193" borderId="1269" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="697" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="698" fillId="1196" borderId="1273" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="699" fillId="1199" borderId="1277" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="700" fillId="1202" borderId="1281" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="701" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="702" fillId="1205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="703" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="704" fillId="1208" borderId="1285" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="705" fillId="1199" borderId="1289" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="706" fillId="1211" borderId="1293" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="707" fillId="1211" borderId="1293" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="708" fillId="1202" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="709" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="710" fillId="1202" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="711" fillId="1217" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -28210,7 +28841,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF137"/>
+  <dimension ref="A1:AF138"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -29915,7 +30546,7 @@
         <v>272</v>
       </c>
       <c r="Z89" t="s">
-        <v>192</v>
+        <v>599</v>
       </c>
     </row>
     <row r="90">
@@ -29923,7 +30554,7 @@
         <v>289</v>
       </c>
       <c r="Z90" t="s">
-        <v>488</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91">
@@ -29931,7 +30562,7 @@
         <v>273</v>
       </c>
       <c r="Z91" t="s">
-        <v>193</v>
+        <v>488</v>
       </c>
     </row>
     <row r="92">
@@ -29939,7 +30570,7 @@
         <v>274</v>
       </c>
       <c r="Z92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93">
@@ -29947,7 +30578,7 @@
         <v>307</v>
       </c>
       <c r="Z93" t="s">
-        <v>584</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94">
@@ -29955,7 +30586,7 @@
         <v>313</v>
       </c>
       <c r="Z94" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="95">
@@ -29963,7 +30594,7 @@
         <v>296</v>
       </c>
       <c r="Z95" t="s">
-        <v>207</v>
+        <v>585</v>
       </c>
     </row>
     <row r="96">
@@ -29971,7 +30602,7 @@
         <v>341</v>
       </c>
       <c r="Z96" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97">
@@ -29979,7 +30610,7 @@
         <v>278</v>
       </c>
       <c r="Z97" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="98">
@@ -29987,201 +30618,206 @@
         <v>279</v>
       </c>
       <c r="Z98" t="s">
-        <v>471</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99">
       <c r="Z99" t="s">
-        <v>597</v>
+        <v>471</v>
       </c>
     </row>
     <row r="100">
       <c r="Z100" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="101">
       <c r="Z101" t="s">
-        <v>472</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102">
       <c r="Z102" t="s">
-        <v>196</v>
+        <v>472</v>
       </c>
     </row>
     <row r="103">
       <c r="Z103" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="104">
       <c r="Z104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105">
       <c r="Z105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="106">
       <c r="Z106" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="107">
       <c r="Z107" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="108">
       <c r="Z108" t="s">
-        <v>536</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109">
       <c r="Z109" t="s">
-        <v>591</v>
+        <v>536</v>
       </c>
     </row>
     <row r="110">
       <c r="Z110" t="s">
-        <v>543</v>
+        <v>591</v>
       </c>
     </row>
     <row r="111">
       <c r="Z111" t="s">
-        <v>141</v>
+        <v>543</v>
       </c>
     </row>
     <row r="112">
       <c r="Z112" t="s">
-        <v>544</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113">
       <c r="Z113" t="s">
-        <v>384</v>
+        <v>544</v>
       </c>
     </row>
     <row r="114">
       <c r="Z114" t="s">
-        <v>142</v>
+        <v>384</v>
       </c>
     </row>
     <row r="115">
       <c r="Z115" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116">
       <c r="Z116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117">
       <c r="Z117" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="118">
       <c r="Z118" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="119">
       <c r="Z119" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120">
       <c r="Z120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121">
       <c r="Z121" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="122">
       <c r="Z122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="123">
       <c r="Z123" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124">
       <c r="Z124" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125">
       <c r="Z125" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126">
       <c r="Z126" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="127">
       <c r="Z127" t="s">
-        <v>479</v>
+        <v>154</v>
       </c>
     </row>
     <row r="128">
       <c r="Z128" t="s">
-        <v>155</v>
+        <v>479</v>
       </c>
     </row>
     <row r="129">
       <c r="Z129" t="s">
-        <v>581</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130">
       <c r="Z130" t="s">
-        <v>156</v>
+        <v>581</v>
       </c>
     </row>
     <row r="131">
       <c r="Z131" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="132">
       <c r="Z132" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="133">
       <c r="Z133" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134">
       <c r="Z134" t="s">
-        <v>159</v>
+        <v>40</v>
       </c>
     </row>
     <row r="135">
       <c r="Z135" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136">
       <c r="Z136" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137">
       <c r="Z137" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="Z138" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- [`nexial.outputToCloud`]: now supports subdirectory (or relative paths) when moving execution artifacts to cloud storage. This means that any execution artifacts to be created in a subdirectory under the "output" directory will be move to the cloud storage with said subdirectory intact.
### [csv commands]
- [`compareExtended(var,profile,expected,actual)`]: now supports the comparing of cell content as either an order-significant (via `[profile].compareExt.matchAsOrderedList`) or order-insignificant (via `[profile].compareExt.matchAsUnorderedList`) list.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr documentId="13_ncr:1_{9BE96B42-DF10-4D4C-8649-F64CBD9D5FE1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23608" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24173" uniqueCount="600">
   <si>
     <t>description</t>
   </si>
@@ -1876,7 +1876,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="712" x14ac:knownFonts="1">
+  <fonts count="728" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6374,8 +6374,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1218">
+  <fills count="1245">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13273,8 +13374,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1294">
+  <borders count="1326">
     <border>
       <left/>
       <right/>
@@ -21297,6 +21551,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -26371,7 +26951,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="723">
+  <cellXfs count="739">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -28498,52 +29078,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1190" fontId="695" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="696" fillId="1193" borderId="1269" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="697" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1269" fillId="1193" fontId="696" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="697" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="698" fillId="1196" borderId="1273" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1273" fillId="1196" fontId="698" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="699" fillId="1199" borderId="1277" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1277" fillId="1199" fontId="699" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="700" fillId="1202" borderId="1281" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1281" fillId="1202" fontId="700" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="701" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="701" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="702" fillId="1205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1205" fontId="702" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="703" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="704" fillId="1208" borderId="1285" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="705" fillId="1199" borderId="1289" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="706" fillId="1211" borderId="1293" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="707" fillId="1211" borderId="1293" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="708" fillId="1202" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="709" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="710" fillId="1202" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="711" fillId="1217" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="703" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1285" fillId="1208" fontId="704" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1289" fillId="1199" fontId="705" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1293" fillId="1211" fontId="706" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1293" fillId="1211" fontId="707" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1202" fontId="708" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1214" fontId="709" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1202" fontId="710" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1217" fontId="711" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="712" fillId="1220" borderId="1301" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="713" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="714" fillId="1223" borderId="1305" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="715" fillId="1226" borderId="1309" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="716" fillId="1229" borderId="1313" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="717" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="718" fillId="1232" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="719" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="720" fillId="1235" borderId="1317" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="721" fillId="1226" borderId="1321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="722" fillId="1238" borderId="1325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="723" fillId="1238" borderId="1325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="724" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="725" fillId="1241" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="726" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="727" fillId="1244" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -28843,7 +29471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF138"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
+    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30830,9 +31458,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView tabSelected="true" topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100" zoomScale="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="C22" pane="bottomLeft" sqref="C22"/>
+      <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[image commands] - [`ocr(source,saveVar)`]: **NEW** command to perform OCR (optical character recognition) on image (`source`). This command works best on images containing mostly text with block font (not handwriting). This command internally uses OCR.space API to perform OCR.
Signed-off-by: automike <mliu@firstam.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr documentId="13_ncr:1_{9BE96B42-DF10-4D4C-8649-F64CBD9D5FE1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440" firstSheet="1"/>
+    <workbookView activeTab="1" firstSheet="1" tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="440"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -24,9 +24,9 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$14</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$6</definedName>
-    <definedName name="image">'#system'!$K$2:$K$7</definedName>
+    <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
@@ -35,25 +35,26 @@
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$16</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$17</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
     <definedName name="sound">'#system'!$W$2:$W$5</definedName>
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$138</definedName>
-    <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
-    <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
-    <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
-    <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
+    <definedName name="target">'#system'!$A$2:$A$32</definedName>
+    <definedName name="web">'#system'!$AA$2:$AA$144</definedName>
+    <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
+    <definedName name="ws">'#system'!$AD$2:$AD$17</definedName>
+    <definedName name="ws.async">'#system'!$AE$2:$AE$8</definedName>
+    <definedName name="xml">'#system'!$AF$2:$AF$27</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
+    <definedName name="tn.5250">'#system'!$Z$2:$Z$6</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24173" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24757" uniqueCount="619">
   <si>
     <t>description</t>
   </si>
@@ -1869,6 +1870,63 @@
   </si>
   <si>
     <t>saveBrowserVersion(var)</t>
+  </si>
+  <si>
+    <t>tn.5250</t>
+  </si>
+  <si>
+    <t>saveTotalColumnCount(file,worksheet,row,saveVar)</t>
+  </si>
+  <si>
+    <t>saveTotalRowCount(file,worksheet,saveVar)</t>
+  </si>
+  <si>
+    <t>colorbit(image,bit,saveTo)</t>
+  </si>
+  <si>
+    <t>ocr(image,saveVar)</t>
+  </si>
+  <si>
+    <t>saveAsPdf(profile,content,file)</t>
+  </si>
+  <si>
+    <t>close(profile)</t>
+  </si>
+  <si>
+    <t>open(profile)</t>
+  </si>
+  <si>
+    <t>saveText(profile,var)</t>
+  </si>
+  <si>
+    <t>typeKeys(profile,keystrokes)</t>
+  </si>
+  <si>
+    <t>updateScreenFields(profile)</t>
+  </si>
+  <si>
+    <t>assertElementEnabled(locator)</t>
+  </si>
+  <si>
+    <t>saveTitle(var)</t>
+  </si>
+  <si>
+    <t>selectAllOptions(locator)</t>
+  </si>
+  <si>
+    <t>selectMultiByValue(locator,array)</t>
+  </si>
+  <si>
+    <t>switchBrowser(profile,config)</t>
+  </si>
+  <si>
+    <t>waitForElementsPresent(locators)</t>
+  </si>
+  <si>
+    <t>clearCookieFields(var,remove)</t>
+  </si>
+  <si>
+    <t>saveAllAsText(var,exclude)</t>
   </si>
 </sst>
 </file>
@@ -1876,7 +1934,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="728" x14ac:knownFonts="1">
+  <fonts count="744" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6475,8 +6533,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1245">
+  <fills count="1272">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13527,8 +13686,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1326">
+  <borders count="1358">
     <border>
       <left/>
       <right/>
@@ -21551,6 +21863,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -26951,7 +27589,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="739">
+  <cellXfs count="755">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -29126,52 +29764,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1217" fontId="711" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="712" fillId="1220" borderId="1301" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="713" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1301" fillId="1220" fontId="712" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="713" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="714" fillId="1223" borderId="1305" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1305" fillId="1223" fontId="714" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="715" fillId="1226" borderId="1309" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1309" fillId="1226" fontId="715" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="716" fillId="1229" borderId="1313" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1313" fillId="1229" fontId="716" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="717" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="717" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="718" fillId="1232" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1232" fontId="718" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="719" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="720" fillId="1235" borderId="1317" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="721" fillId="1226" borderId="1321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="722" fillId="1238" borderId="1325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="723" fillId="1238" borderId="1325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="724" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="725" fillId="1241" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="726" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="727" fillId="1244" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="719" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1317" fillId="1235" fontId="720" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1321" fillId="1226" fontId="721" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1325" fillId="1238" fontId="722" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1325" fillId="1238" fontId="723" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1229" fontId="724" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1241" fontId="725" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1229" fontId="726" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1244" fontId="727" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="728" fillId="1247" borderId="1333" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="729" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="730" fillId="1250" borderId="1337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="731" fillId="1253" borderId="1341" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="732" fillId="1256" borderId="1345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="733" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="734" fillId="1259" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="735" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="736" fillId="1262" borderId="1349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="737" fillId="1253" borderId="1353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="738" fillId="1265" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="739" fillId="1265" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="740" fillId="1256" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="741" fillId="1268" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="742" fillId="1256" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="743" fillId="1271" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -29469,9 +30155,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF138"/>
+  <dimension ref="A1:AG144"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false"/>
+    <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29555,21 +30241,24 @@
         <v>395</v>
       </c>
       <c r="Z1" t="s">
+        <v>600</v>
+      </c>
+      <c r="AA1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>458</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -29605,7 +30294,7 @@
         <v>71</v>
       </c>
       <c r="K2" t="s">
-        <v>501</v>
+        <v>603</v>
       </c>
       <c r="L2" t="s">
         <v>317</v>
@@ -29650,21 +30339,24 @@
         <v>396</v>
       </c>
       <c r="Z2" t="s">
+        <v>606</v>
+      </c>
+      <c r="AA2" t="s">
         <v>89</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>163</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>168</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>175</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>468</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>524</v>
       </c>
     </row>
@@ -29736,21 +30428,24 @@
         <v>397</v>
       </c>
       <c r="Z3" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA3" t="s">
         <v>90</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>164</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>169</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>365</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>176</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -29819,21 +30514,24 @@
         <v>398</v>
       </c>
       <c r="Z4" t="s">
+        <v>608</v>
+      </c>
+      <c r="AA4" t="s">
         <v>596</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>165</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>170</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>176</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>459</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>220</v>
       </c>
     </row>
@@ -29893,21 +30591,24 @@
         <v>360</v>
       </c>
       <c r="Z5" t="s">
+        <v>609</v>
+      </c>
+      <c r="AA5" t="s">
         <v>589</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>166</v>
       </c>
-      <c r="AB5" t="s">
-        <v>171</v>
-      </c>
       <c r="AC5" t="s">
+        <v>617</v>
+      </c>
+      <c r="AD5" t="s">
         <v>177</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>460</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>221</v>
       </c>
     </row>
@@ -29937,7 +30638,7 @@
         <v>594</v>
       </c>
       <c r="K6" t="s">
-        <v>349</v>
+        <v>604</v>
       </c>
       <c r="L6" t="s">
         <v>495</v>
@@ -29964,21 +30665,24 @@
         <v>362</v>
       </c>
       <c r="Z6" t="s">
+        <v>610</v>
+      </c>
+      <c r="AA6" t="s">
         <v>91</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>480</v>
       </c>
-      <c r="AB6" t="s">
-        <v>172</v>
-      </c>
       <c r="AC6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD6" t="s">
         <v>178</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>461</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>222</v>
       </c>
     </row>
@@ -29999,7 +30703,7 @@
         <v>482</v>
       </c>
       <c r="K7" t="s">
-        <v>564</v>
+        <v>349</v>
       </c>
       <c r="L7" t="s">
         <v>64</v>
@@ -30025,22 +30729,22 @@
       <c r="X7" t="s">
         <v>361</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>92</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>481</v>
       </c>
-      <c r="AB7" t="s">
-        <v>173</v>
-      </c>
       <c r="AC7" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD7" t="s">
         <v>179</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>462</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>567</v>
       </c>
     </row>
@@ -30060,6 +30764,9 @@
       <c r="I8" t="s">
         <v>329</v>
       </c>
+      <c r="K8" t="s">
+        <v>564</v>
+      </c>
       <c r="L8" t="s">
         <v>12</v>
       </c>
@@ -30081,22 +30788,22 @@
       <c r="X8" t="s">
         <v>363</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>93</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>167</v>
       </c>
-      <c r="AB8" t="s">
-        <v>174</v>
-      </c>
       <c r="AC8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD8" t="s">
         <v>180</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>463</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>568</v>
       </c>
     </row>
@@ -30137,13 +30844,16 @@
       <c r="X9" t="s">
         <v>364</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>201</v>
       </c>
       <c r="AC9" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD9" t="s">
         <v>181</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>569</v>
       </c>
     </row>
@@ -30158,7 +30868,7 @@
         <v>308</v>
       </c>
       <c r="I10" t="s">
-        <v>487</v>
+        <v>601</v>
       </c>
       <c r="L10" t="s">
         <v>72</v>
@@ -30178,13 +30888,16 @@
       <c r="U10" t="s">
         <v>408</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>258</v>
       </c>
       <c r="AC10" t="s">
+        <v>618</v>
+      </c>
+      <c r="AD10" t="s">
         <v>182</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>223</v>
       </c>
     </row>
@@ -30199,7 +30912,7 @@
         <v>353</v>
       </c>
       <c r="I11" t="s">
-        <v>323</v>
+        <v>602</v>
       </c>
       <c r="L11" t="s">
         <v>31</v>
@@ -30216,13 +30929,13 @@
       <c r="S11" t="s">
         <v>239</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>259</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>260</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -30237,7 +30950,7 @@
         <v>275</v>
       </c>
       <c r="I12" t="s">
-        <v>324</v>
+        <v>487</v>
       </c>
       <c r="L12" t="s">
         <v>539</v>
@@ -30254,13 +30967,13 @@
       <c r="S12" t="s">
         <v>240</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>94</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>183</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>225</v>
       </c>
     </row>
@@ -30275,7 +30988,7 @@
         <v>264</v>
       </c>
       <c r="I13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L13" t="s">
         <v>391</v>
@@ -30287,15 +31000,15 @@
         <v>86</v>
       </c>
       <c r="S13" t="s">
-        <v>245</v>
-      </c>
-      <c r="Z13" t="s">
+        <v>605</v>
+      </c>
+      <c r="AA13" t="s">
         <v>327</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>184</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>509</v>
       </c>
     </row>
@@ -30310,7 +31023,7 @@
         <v>318</v>
       </c>
       <c r="I14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L14" t="s">
         <v>13</v>
@@ -30322,15 +31035,15 @@
         <v>87</v>
       </c>
       <c r="S14" t="s">
-        <v>241</v>
-      </c>
-      <c r="Z14" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA14" t="s">
         <v>95</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>185</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>525</v>
       </c>
     </row>
@@ -30344,6 +31057,9 @@
       <c r="H15" t="s">
         <v>265</v>
       </c>
+      <c r="I15" t="s">
+        <v>325</v>
+      </c>
       <c r="L15" t="s">
         <v>35</v>
       </c>
@@ -30354,15 +31070,15 @@
         <v>533</v>
       </c>
       <c r="S15" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC15" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>611</v>
+      </c>
+      <c r="AD15" t="s">
         <v>186</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>526</v>
       </c>
     </row>
@@ -30376,6 +31092,9 @@
       <c r="H16" t="s">
         <v>266</v>
       </c>
+      <c r="I16" t="s">
+        <v>326</v>
+      </c>
       <c r="L16" t="s">
         <v>540</v>
       </c>
@@ -30386,15 +31105,15 @@
         <v>534</v>
       </c>
       <c r="S16" t="s">
-        <v>243</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD16" t="s">
         <v>187</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AF16" t="s">
         <v>530</v>
       </c>
     </row>
@@ -30414,13 +31133,16 @@
       <c r="N17" t="s">
         <v>33</v>
       </c>
-      <c r="Z17" t="s">
-        <v>535</v>
-      </c>
-      <c r="AC17" t="s">
+      <c r="S17" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD17" t="s">
         <v>496</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AF17" t="s">
         <v>531</v>
       </c>
     </row>
@@ -30440,10 +31162,10 @@
       <c r="N18" t="s">
         <v>36</v>
       </c>
-      <c r="Z18" t="s">
-        <v>97</v>
-      </c>
-      <c r="AE18" t="s">
+      <c r="AA18" t="s">
+        <v>535</v>
+      </c>
+      <c r="AF18" t="s">
         <v>510</v>
       </c>
     </row>
@@ -30460,10 +31182,10 @@
       <c r="L19" t="s">
         <v>491</v>
       </c>
-      <c r="Z19" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE19" t="s">
+      <c r="AA19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF19" t="s">
         <v>527</v>
       </c>
     </row>
@@ -30480,10 +31202,10 @@
       <c r="L20" t="s">
         <v>75</v>
       </c>
-      <c r="Z20" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE20" t="s">
+      <c r="AA20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF20" t="s">
         <v>528</v>
       </c>
     </row>
@@ -30500,10 +31222,10 @@
       <c r="L21" t="s">
         <v>76</v>
       </c>
-      <c r="Z21" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE21" t="s">
+      <c r="AA21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF21" t="s">
         <v>532</v>
       </c>
     </row>
@@ -30520,10 +31242,10 @@
       <c r="L22" t="s">
         <v>593</v>
       </c>
-      <c r="Z22" t="s">
-        <v>518</v>
-      </c>
-      <c r="AE22" t="s">
+      <c r="AA22" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF22" t="s">
         <v>226</v>
       </c>
     </row>
@@ -30540,10 +31262,10 @@
       <c r="L23" t="s">
         <v>505</v>
       </c>
-      <c r="Z23" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE23" t="s">
+      <c r="AA23" t="s">
+        <v>518</v>
+      </c>
+      <c r="AF23" t="s">
         <v>570</v>
       </c>
     </row>
@@ -30560,10 +31282,10 @@
       <c r="L24" t="s">
         <v>37</v>
       </c>
-      <c r="Z24" t="s">
-        <v>579</v>
-      </c>
-      <c r="AE24" t="s">
+      <c r="AA24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF24" t="s">
         <v>571</v>
       </c>
     </row>
@@ -30580,16 +31302,16 @@
       <c r="L25" t="s">
         <v>393</v>
       </c>
-      <c r="Z25" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE25" t="s">
+      <c r="AA25" t="s">
+        <v>579</v>
+      </c>
+      <c r="AF25" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>600</v>
       </c>
       <c r="F26" t="s">
         <v>216</v>
@@ -30600,16 +31322,16 @@
       <c r="L26" t="s">
         <v>557</v>
       </c>
-      <c r="Z26" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE26" t="s">
+      <c r="AA26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF26" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
         <v>217</v>
@@ -30620,16 +31342,16 @@
       <c r="L27" t="s">
         <v>77</v>
       </c>
-      <c r="Z27" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE27" t="s">
+      <c r="AA27" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
         <v>503</v>
@@ -30640,13 +31362,13 @@
       <c r="L28" t="s">
         <v>475</v>
       </c>
-      <c r="Z28" t="s">
-        <v>106</v>
+      <c r="AA28" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
         <v>504</v>
@@ -30657,13 +31379,13 @@
       <c r="L29" t="s">
         <v>38</v>
       </c>
-      <c r="Z29" t="s">
-        <v>328</v>
+      <c r="AA29" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>458</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
         <v>453</v>
@@ -30674,13 +31396,13 @@
       <c r="L30" t="s">
         <v>39</v>
       </c>
-      <c r="Z30" t="s">
-        <v>107</v>
+      <c r="AA30" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>458</v>
       </c>
       <c r="F31" t="s">
         <v>56</v>
@@ -30688,19 +31410,22 @@
       <c r="H31" t="s">
         <v>208</v>
       </c>
-      <c r="Z31" t="s">
-        <v>108</v>
+      <c r="AA31" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="s">
+        <v>218</v>
+      </c>
       <c r="F32" t="s">
         <v>57</v>
       </c>
       <c r="H32" t="s">
         <v>276</v>
       </c>
-      <c r="Z32" t="s">
-        <v>109</v>
+      <c r="AA32" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="33">
@@ -30710,8 +31435,8 @@
       <c r="H33" t="s">
         <v>286</v>
       </c>
-      <c r="Z33" t="s">
-        <v>110</v>
+      <c r="AA33" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="34">
@@ -30721,8 +31446,8 @@
       <c r="H34" t="s">
         <v>541</v>
       </c>
-      <c r="Z34" t="s">
-        <v>580</v>
+      <c r="AA34" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35">
@@ -30732,8 +31457,8 @@
       <c r="H35" t="s">
         <v>261</v>
       </c>
-      <c r="Z35" t="s">
-        <v>111</v>
+      <c r="AA35" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="36">
@@ -30743,8 +31468,8 @@
       <c r="H36" t="s">
         <v>331</v>
       </c>
-      <c r="Z36" t="s">
-        <v>112</v>
+      <c r="AA36" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="37">
@@ -30754,8 +31479,8 @@
       <c r="H37" t="s">
         <v>309</v>
       </c>
-      <c r="Z37" t="s">
-        <v>202</v>
+      <c r="AA37" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="38">
@@ -30765,687 +31490,717 @@
       <c r="H38" t="s">
         <v>262</v>
       </c>
-      <c r="Z38" t="s">
-        <v>113</v>
+      <c r="AA38" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="39">
       <c r="H39" t="s">
         <v>310</v>
       </c>
-      <c r="Z39" t="s">
-        <v>339</v>
+      <c r="AA39" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="40">
       <c r="H40" t="s">
         <v>268</v>
       </c>
-      <c r="Z40" t="s">
-        <v>470</v>
+      <c r="AA40" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="41">
       <c r="H41" t="s">
         <v>70</v>
       </c>
-      <c r="Z41" t="s">
-        <v>590</v>
+      <c r="AA41" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="42">
       <c r="H42" t="s">
         <v>204</v>
       </c>
-      <c r="Z42" t="s">
-        <v>394</v>
+      <c r="AA42" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="43">
       <c r="H43" t="s">
         <v>576</v>
       </c>
-      <c r="Z43" t="s">
-        <v>114</v>
+      <c r="AA43" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="44">
       <c r="H44" t="s">
         <v>290</v>
       </c>
-      <c r="Z44" t="s">
-        <v>115</v>
+      <c r="AA44" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="45">
       <c r="H45" t="s">
         <v>301</v>
       </c>
-      <c r="Z45" t="s">
-        <v>116</v>
+      <c r="AA45" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="46">
       <c r="H46" t="s">
         <v>302</v>
       </c>
-      <c r="Z46" t="s">
-        <v>117</v>
+      <c r="AA46" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47">
       <c r="H47" t="s">
         <v>344</v>
       </c>
-      <c r="Z47" t="s">
-        <v>118</v>
+      <c r="AA47" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="48">
       <c r="H48" t="s">
         <v>343</v>
       </c>
-      <c r="Z48" t="s">
-        <v>119</v>
+      <c r="AA48" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="49">
       <c r="H49" t="s">
         <v>203</v>
       </c>
-      <c r="Z49" t="s">
-        <v>477</v>
+      <c r="AA49" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="50">
       <c r="H50" t="s">
         <v>303</v>
       </c>
-      <c r="Z50" t="s">
-        <v>205</v>
+      <c r="AA50" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="51">
       <c r="H51" t="s">
         <v>340</v>
       </c>
-      <c r="Z51" t="s">
-        <v>69</v>
+      <c r="AA51" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="52">
       <c r="H52" t="s">
         <v>369</v>
       </c>
-      <c r="Z52" t="s">
-        <v>566</v>
+      <c r="AA52" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="53">
       <c r="H53" t="s">
         <v>304</v>
       </c>
-      <c r="Z53" t="s">
-        <v>120</v>
+      <c r="AA53" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="54">
       <c r="H54" t="s">
         <v>357</v>
       </c>
-      <c r="Z54" t="s">
-        <v>121</v>
+      <c r="AA54" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="55">
       <c r="H55" t="s">
         <v>332</v>
       </c>
-      <c r="Z55" t="s">
-        <v>122</v>
+      <c r="AA55" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="56">
       <c r="H56" t="s">
         <v>269</v>
       </c>
-      <c r="Z56" t="s">
-        <v>516</v>
+      <c r="AA56" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="57">
       <c r="H57" t="s">
         <v>293</v>
       </c>
-      <c r="Z57" t="s">
-        <v>500</v>
+      <c r="AA57" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="58">
       <c r="H58" t="s">
         <v>294</v>
       </c>
-      <c r="Z58" t="s">
-        <v>123</v>
+      <c r="AA58" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="59">
       <c r="H59" t="s">
         <v>577</v>
       </c>
-      <c r="Z59" t="s">
-        <v>347</v>
+      <c r="AA59" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="60">
       <c r="H60" t="s">
         <v>295</v>
       </c>
-      <c r="Z60" t="s">
-        <v>494</v>
+      <c r="AA60" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="61">
       <c r="H61" t="s">
         <v>305</v>
       </c>
-      <c r="Z61" t="s">
-        <v>124</v>
+      <c r="AA61" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="62">
       <c r="H62" t="s">
         <v>314</v>
       </c>
-      <c r="Z62" t="s">
-        <v>125</v>
+      <c r="AA62" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="63">
       <c r="H63" t="s">
         <v>338</v>
       </c>
-      <c r="Z63" t="s">
-        <v>126</v>
+      <c r="AA63" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="64">
       <c r="H64" t="s">
         <v>311</v>
       </c>
-      <c r="Z64" t="s">
-        <v>127</v>
+      <c r="AA64" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="65">
       <c r="H65" t="s">
         <v>312</v>
       </c>
-      <c r="Z65" t="s">
-        <v>128</v>
+      <c r="AA65" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="66">
       <c r="H66" t="s">
         <v>370</v>
       </c>
-      <c r="Z66" t="s">
-        <v>129</v>
+      <c r="AA66" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="67">
       <c r="H67" t="s">
         <v>371</v>
       </c>
-      <c r="Z67" t="s">
-        <v>130</v>
+      <c r="AA67" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="68">
       <c r="H68" t="s">
         <v>346</v>
       </c>
-      <c r="Z68" t="s">
-        <v>473</v>
+      <c r="AA68" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="69">
       <c r="H69" t="s">
         <v>315</v>
       </c>
-      <c r="Z69" t="s">
-        <v>508</v>
+      <c r="AA69" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="70">
       <c r="H70" t="s">
         <v>270</v>
       </c>
-      <c r="Z70" t="s">
-        <v>206</v>
+      <c r="AA70" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="71">
       <c r="H71" t="s">
         <v>562</v>
       </c>
-      <c r="Z71" t="s">
-        <v>390</v>
+      <c r="AA71" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="72">
       <c r="H72" t="s">
         <v>316</v>
       </c>
-      <c r="Z72" t="s">
-        <v>478</v>
+      <c r="AA72" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="73">
       <c r="H73" t="s">
         <v>409</v>
       </c>
-      <c r="Z73" t="s">
-        <v>131</v>
+      <c r="AA73" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="74">
       <c r="H74" t="s">
         <v>306</v>
       </c>
-      <c r="Z74" t="s">
-        <v>132</v>
+      <c r="AA74" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="75">
       <c r="H75" t="s">
         <v>410</v>
       </c>
-      <c r="Z75" t="s">
-        <v>133</v>
+      <c r="AA75" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="76">
       <c r="H76" t="s">
         <v>263</v>
       </c>
-      <c r="Z76" t="s">
-        <v>134</v>
+      <c r="AA76" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="77">
       <c r="H77" t="s">
         <v>542</v>
       </c>
-      <c r="Z77" t="s">
-        <v>189</v>
+      <c r="AA77" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="78">
       <c r="H78" t="s">
         <v>345</v>
       </c>
-      <c r="Z78" t="s">
-        <v>190</v>
+      <c r="AA78" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="79">
       <c r="H79" t="s">
         <v>281</v>
       </c>
-      <c r="Z79" t="s">
-        <v>489</v>
+      <c r="AA79" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="80">
       <c r="H80" t="s">
         <v>287</v>
       </c>
-      <c r="Z80" t="s">
-        <v>502</v>
+      <c r="AA80" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="81">
       <c r="H81" t="s">
         <v>292</v>
       </c>
-      <c r="Z81" t="s">
-        <v>135</v>
+      <c r="AA81" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="82">
       <c r="H82" t="s">
         <v>464</v>
       </c>
-      <c r="Z82" t="s">
-        <v>136</v>
+      <c r="AA82" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="83">
       <c r="H83" t="s">
         <v>333</v>
       </c>
-      <c r="Z83" t="s">
-        <v>137</v>
+      <c r="AA83" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="84">
       <c r="H84" t="s">
         <v>271</v>
       </c>
-      <c r="Z84" t="s">
-        <v>529</v>
+      <c r="AA84" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="85">
       <c r="H85" t="s">
         <v>282</v>
       </c>
-      <c r="Z85" t="s">
-        <v>138</v>
+      <c r="AA85" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="86">
       <c r="H86" t="s">
         <v>288</v>
       </c>
-      <c r="Z86" t="s">
-        <v>139</v>
+      <c r="AA86" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="87">
       <c r="H87" t="s">
         <v>277</v>
       </c>
-      <c r="Z87" t="s">
-        <v>191</v>
+      <c r="AA87" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="88">
       <c r="H88" t="s">
         <v>563</v>
       </c>
-      <c r="Z88" t="s">
-        <v>517</v>
+      <c r="AA88" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="89">
       <c r="H89" t="s">
         <v>272</v>
       </c>
-      <c r="Z89" t="s">
-        <v>599</v>
+      <c r="AA89" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="90">
       <c r="H90" t="s">
         <v>289</v>
       </c>
-      <c r="Z90" t="s">
-        <v>192</v>
+      <c r="AA90" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="91">
       <c r="H91" t="s">
         <v>273</v>
       </c>
-      <c r="Z91" t="s">
-        <v>488</v>
+      <c r="AA91" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="92">
       <c r="H92" t="s">
         <v>274</v>
       </c>
-      <c r="Z92" t="s">
-        <v>193</v>
+      <c r="AA92" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="93">
       <c r="H93" t="s">
         <v>307</v>
       </c>
-      <c r="Z93" t="s">
-        <v>194</v>
+      <c r="AA93" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="94">
       <c r="H94" t="s">
         <v>313</v>
       </c>
-      <c r="Z94" t="s">
-        <v>584</v>
+      <c r="AA94" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="95">
       <c r="H95" t="s">
         <v>296</v>
       </c>
-      <c r="Z95" t="s">
-        <v>585</v>
+      <c r="AA95" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="96">
       <c r="H96" t="s">
         <v>341</v>
       </c>
-      <c r="Z96" t="s">
-        <v>207</v>
+      <c r="AA96" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="97">
       <c r="H97" t="s">
         <v>278</v>
       </c>
-      <c r="Z97" t="s">
-        <v>140</v>
+      <c r="AA97" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="98">
       <c r="H98" t="s">
         <v>279</v>
       </c>
-      <c r="Z98" t="s">
+      <c r="AA98" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="AA99" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="99">
-      <c r="Z99" t="s">
+    <row r="100">
+      <c r="AA100" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="100">
-      <c r="Z100" t="s">
+    <row r="101">
+      <c r="AA101" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="101">
-      <c r="Z101" t="s">
+    <row r="102">
+      <c r="AA102" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="102">
-      <c r="Z102" t="s">
+    <row r="103">
+      <c r="AA103" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="103">
-      <c r="Z103" t="s">
+    <row r="104">
+      <c r="AA104" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="104">
-      <c r="Z104" t="s">
+    <row r="105">
+      <c r="AA105" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="105">
-      <c r="Z105" t="s">
+    <row r="106">
+      <c r="AA106" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="106">
-      <c r="Z106" t="s">
+    <row r="107">
+      <c r="AA107" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="107">
-      <c r="Z107" t="s">
+    <row r="108">
+      <c r="AA108" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="108">
-      <c r="Z108" t="s">
+    <row r="109">
+      <c r="AA109" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="AA110" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="109">
-      <c r="Z109" t="s">
+    <row r="111">
+      <c r="AA111" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="110">
-      <c r="Z110" t="s">
+    <row r="112">
+      <c r="AA112" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="111">
-      <c r="Z111" t="s">
+    <row r="113">
+      <c r="AA113" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="112">
-      <c r="Z112" t="s">
+    <row r="114">
+      <c r="AA114" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="113">
-      <c r="Z113" t="s">
+    <row r="115">
+      <c r="AA115" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="114">
-      <c r="Z114" t="s">
+    <row r="116">
+      <c r="AA116" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="115">
-      <c r="Z115" t="s">
+    <row r="117">
+      <c r="AA117" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="116">
-      <c r="Z116" t="s">
+    <row r="118">
+      <c r="AA118" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117">
-      <c r="Z117" t="s">
+    <row r="119">
+      <c r="AA119" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="AA120" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="118">
-      <c r="Z118" t="s">
+    <row r="121">
+      <c r="AA121" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="119">
-      <c r="Z119" t="s">
+    <row r="122">
+      <c r="AA122" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="AA123" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120">
-      <c r="Z120" t="s">
+    <row r="124">
+      <c r="AA124" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="121">
-      <c r="Z121" t="s">
+    <row r="125">
+      <c r="AA125" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="122">
-      <c r="Z122" t="s">
+    <row r="126">
+      <c r="AA126" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="123">
-      <c r="Z123" t="s">
+    <row r="127">
+      <c r="AA127" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="124">
-      <c r="Z124" t="s">
+    <row r="128">
+      <c r="AA128" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="125">
-      <c r="Z125" t="s">
+    <row r="129">
+      <c r="AA129" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="AA130" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="126">
-      <c r="Z126" t="s">
+    <row r="131">
+      <c r="AA131" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="127">
-      <c r="Z127" t="s">
+    <row r="132">
+      <c r="AA132" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="128">
-      <c r="Z128" t="s">
+    <row r="133">
+      <c r="AA133" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="129">
-      <c r="Z129" t="s">
+    <row r="134">
+      <c r="AA134" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="130">
-      <c r="Z130" t="s">
+    <row r="135">
+      <c r="AA135" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="131">
-      <c r="Z131" t="s">
+    <row r="136">
+      <c r="AA136" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="132">
-      <c r="Z132" t="s">
+    <row r="137">
+      <c r="AA137" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="133">
-      <c r="Z133" t="s">
+    <row r="138">
+      <c r="AA138" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134">
-      <c r="Z134" t="s">
+    <row r="139">
+      <c r="AA139" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="135">
-      <c r="Z135" t="s">
+    <row r="140">
+      <c r="AA140" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="136">
-      <c r="Z136" t="s">
+    <row r="141">
+      <c r="AA141" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="AA142" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="137">
-      <c r="Z137" t="s">
+    <row r="143">
+      <c r="AA143" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="138">
-      <c r="Z138" t="s">
+    <row r="144">
+      <c r="AA144" t="s">
         <v>162</v>
       </c>
     </row>
@@ -31458,7 +32213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100" zoomScale="100">
+    <sheetView tabSelected="true" topLeftCell="B1" workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
     </sheetView>

</xml_diff>

<commit_message>
[expression] - [`LIST => saveItems(indexAndVar)`]: **NEW** operation to save one or more items from a `LIST` as individual data variables. - [`BINARY`]: support loading of binary data from external file. - [`TEXT => removeLeft(length)`]: **NEW** operation to remove characters off the current text from the left (i.e. beginning). - [`TEXT => removeRight(length)`]: **NEW** operation to remove characters off the current text from the right (i.e. end).
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$F$2:$F$42</definedName>
+    <definedName name="base">'#system'!$F$2:$F$44</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
@@ -27,7 +27,7 @@
     <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
-    <definedName name="io">'#system'!$L$2:$L$30</definedName>
+    <definedName name="io">'#system'!$L$2:$L$31</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
@@ -35,26 +35,26 @@
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$17</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$18</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$9</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
     <definedName name="sound">'#system'!$W$2:$W$5</definedName>
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$32</definedName>
-    <definedName name="web">'#system'!$AA$2:$AA$149</definedName>
-    <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
-    <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
-    <definedName name="ws">'#system'!$AD$2:$AD$17</definedName>
-    <definedName name="ws.async">'#system'!$AE$2:$AE$8</definedName>
-    <definedName name="xml">'#system'!$AF$2:$AF$27</definedName>
+    <definedName name="target">'#system'!$A$2:$A$33</definedName>
+    <definedName name="web">'#system'!$AB$2:$AB$151</definedName>
+    <definedName name="webalert">'#system'!$AC$2:$AC$8</definedName>
+    <definedName name="webcookie">'#system'!$AD$2:$AD$10</definedName>
+    <definedName name="ws">'#system'!$AE$2:$AE$17</definedName>
+    <definedName name="ws.async">'#system'!$AF$2:$AF$8</definedName>
+    <definedName name="xml">'#system'!$AG$2:$AG$27</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
-    <definedName name="tn.5250">'#system'!$Z$2:$Z$6</definedName>
+    <definedName name="tn.5250">'#system'!$AA$2:$AA$38</definedName>
     <definedName name="step.inTime">'#system'!$Z$2:$Z$4</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26536" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27810" uniqueCount="683">
   <si>
     <t>description</t>
   </si>
@@ -1997,6 +1997,129 @@
   </si>
   <si>
     <t>waitForElementPresent(locator,waitMs)</t>
+  </si>
+  <si>
+    <t>waitForCondition(conditions,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>waitForFile(file,minFileSize,waitMs,maxWaitMs)</t>
+  </si>
+  <si>
+    <t>combine(path,fileFilter,saveTo)</t>
+  </si>
+  <si>
+    <t>assertColumnNotPresent(column)</t>
+  </si>
+  <si>
+    <t>assertColumnPresent(column)</t>
+  </si>
+  <si>
+    <t>assertFieldMatch(label,expects)</t>
+  </si>
+  <si>
+    <t>assertFieldNotMatch(label,expects)</t>
+  </si>
+  <si>
+    <t>assertFieldNotPresent(label)</t>
+  </si>
+  <si>
+    <t>assertFieldPresent(label)</t>
+  </si>
+  <si>
+    <t>assertKeyboardLocked()</t>
+  </si>
+  <si>
+    <t>assertKeyboardNotLocked()</t>
+  </si>
+  <si>
+    <t>assertMessageMatch(expects)</t>
+  </si>
+  <si>
+    <t>assertMessageNotMatch(expects)</t>
+  </si>
+  <si>
+    <t>assertScreenContain(list,ordered)</t>
+  </si>
+  <si>
+    <t>assertScreenMatch(text)</t>
+  </si>
+  <si>
+    <t>assertScreenNotContain(list,ordered)</t>
+  </si>
+  <si>
+    <t>assertScreenNotMatch(text)</t>
+  </si>
+  <si>
+    <t>assertTableMatch(column,text)</t>
+  </si>
+  <si>
+    <t>assertTableNotMatch(column,text)</t>
+  </si>
+  <si>
+    <t>assertTablePresent()</t>
+  </si>
+  <si>
+    <t>assertTitle(expects)</t>
+  </si>
+  <si>
+    <t>assertTitleContain(expects)</t>
+  </si>
+  <si>
+    <t>clearField(label)</t>
+  </si>
+  <si>
+    <t>focus(label)</t>
+  </si>
+  <si>
+    <t>inspectNestedScreen(titles)</t>
+  </si>
+  <si>
+    <t>inspectScreen()</t>
+  </si>
+  <si>
+    <t>saveDisplay(var,field)</t>
+  </si>
+  <si>
+    <t>saveDisplayFields(var)</t>
+  </si>
+  <si>
+    <t>saveInputFields(var)</t>
+  </si>
+  <si>
+    <t>saveMessage(var)</t>
+  </si>
+  <si>
+    <t>saveScreenText(var)</t>
+  </si>
+  <si>
+    <t>saveTableAsCSV(csv,maxPage)</t>
+  </si>
+  <si>
+    <t>saveTableMatchCount(var,column,text)</t>
+  </si>
+  <si>
+    <t>saveTableRow(var,criteria)</t>
+  </si>
+  <si>
+    <t>type(label,text)</t>
+  </si>
+  <si>
+    <t>typeKeys(keystrokes)</t>
+  </si>
+  <si>
+    <t>typeOnMatchedRow(column,match,keystrokes)</t>
+  </si>
+  <si>
+    <t>unlockKeyboard()</t>
+  </si>
+  <si>
+    <t>moveTo(x,y)</t>
+  </si>
+  <si>
+    <t>screenshot(file,locator,removeFixed)</t>
+  </si>
+  <si>
+    <t>screenshotInFull(file,timeout,removeFixed)</t>
   </si>
 </sst>
 </file>
@@ -2004,7 +2127,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="792" x14ac:knownFonts="1">
+  <fonts count="826" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7007,8 +7130,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1353">
+  <fills count="1401">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -14669,6 +15006,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="E6E6E6"/>
         <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -29399,7 +30008,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="803">
+  <cellXfs count="837">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -31766,52 +32375,154 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1325" fontId="775" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="776" fillId="1328" borderId="1429" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="777" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1429" fillId="1328" fontId="776" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="777" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="778" fillId="1331" borderId="1433" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1433" fillId="1331" fontId="778" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="779" fillId="1334" borderId="1437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1437" fillId="1334" fontId="779" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="780" fillId="1337" borderId="1441" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1441" fillId="1337" fontId="780" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="781" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="781" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="782" fillId="1340" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1340" fontId="782" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="783" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="784" fillId="1343" borderId="1445" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="785" fillId="1334" borderId="1449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="786" fillId="1346" borderId="1453" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="787" fillId="1346" borderId="1453" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="788" fillId="1337" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="789" fillId="1349" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="790" fillId="1337" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="791" fillId="1352" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="783" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1445" fillId="1343" fontId="784" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1449" fillId="1334" fontId="785" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1453" fillId="1346" fontId="786" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1453" fillId="1346" fontId="787" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1337" fontId="788" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1349" fontId="789" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1337" fontId="790" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1352" fontId="791" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1355" fontId="792" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="793" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1358" fontId="794" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1361" fontId="795" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1364" fontId="796" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="797" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1367" fontId="798" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="799" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1370" fontId="800" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1373" fontId="801" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1361" fontId="802" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="803" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="804" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1364" fontId="805" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1376" fontId="806" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1364" fontId="807" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1373" fontId="808" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="809" fillId="1379" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="810" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="811" fillId="1382" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="812" fillId="1385" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="813" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="814" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="815" fillId="1391" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="816" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="817" fillId="1394" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="818" fillId="1397" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="819" fillId="1385" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="820" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="821" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="822" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="823" fillId="1400" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="824" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="825" fillId="1397" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -32109,7 +32820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG149"/>
+  <dimension ref="A1:AH151"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -32198,21 +32909,24 @@
         <v>619</v>
       </c>
       <c r="AA1" t="s">
+        <v>600</v>
+      </c>
+      <c r="AB1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>458</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -32296,21 +33010,24 @@
         <v>626</v>
       </c>
       <c r="AA2" t="s">
+        <v>645</v>
+      </c>
+      <c r="AB2" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>163</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>168</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>175</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>468</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>524</v>
       </c>
     </row>
@@ -32385,21 +33102,24 @@
         <v>627</v>
       </c>
       <c r="AA3" t="s">
+        <v>646</v>
+      </c>
+      <c r="AB3" t="s">
         <v>90</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>164</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>169</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>365</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>176</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -32471,21 +33191,24 @@
         <v>628</v>
       </c>
       <c r="AA4" t="s">
+        <v>647</v>
+      </c>
+      <c r="AB4" t="s">
         <v>596</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>165</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>170</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>176</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>459</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>220</v>
       </c>
     </row>
@@ -32545,21 +33268,24 @@
         <v>360</v>
       </c>
       <c r="AA5" t="s">
+        <v>648</v>
+      </c>
+      <c r="AB5" t="s">
         <v>589</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>166</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>617</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>177</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>460</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>221</v>
       </c>
     </row>
@@ -32616,21 +33342,24 @@
         <v>362</v>
       </c>
       <c r="AA6" t="s">
+        <v>649</v>
+      </c>
+      <c r="AB6" t="s">
         <v>91</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>480</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>171</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>178</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>461</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>222</v>
       </c>
     </row>
@@ -32678,21 +33407,24 @@
         <v>361</v>
       </c>
       <c r="AA7" t="s">
+        <v>650</v>
+      </c>
+      <c r="AB7" t="s">
         <v>92</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>481</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>172</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>179</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>462</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>567</v>
       </c>
     </row>
@@ -32740,21 +33472,24 @@
         <v>363</v>
       </c>
       <c r="AA8" t="s">
+        <v>651</v>
+      </c>
+      <c r="AB8" t="s">
         <v>93</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>167</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>173</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>180</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>463</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AG8" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32799,15 +33534,18 @@
         <v>364</v>
       </c>
       <c r="AA9" t="s">
+        <v>652</v>
+      </c>
+      <c r="AB9" t="s">
         <v>201</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>174</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>181</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AG9" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32843,15 +33581,18 @@
         <v>408</v>
       </c>
       <c r="AA10" t="s">
+        <v>653</v>
+      </c>
+      <c r="AB10" t="s">
         <v>258</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>618</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>182</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AG10" t="s">
         <v>223</v>
       </c>
     </row>
@@ -32881,15 +33622,18 @@
         <v>85</v>
       </c>
       <c r="S11" t="s">
-        <v>239</v>
+        <v>644</v>
       </c>
       <c r="AA11" t="s">
+        <v>654</v>
+      </c>
+      <c r="AB11" t="s">
         <v>259</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>260</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AG11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -32919,15 +33663,18 @@
         <v>34</v>
       </c>
       <c r="S12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA12" t="s">
+        <v>655</v>
+      </c>
+      <c r="AB12" t="s">
         <v>94</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>183</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>225</v>
       </c>
     </row>
@@ -32957,15 +33704,18 @@
         <v>86</v>
       </c>
       <c r="S13" t="s">
-        <v>605</v>
+        <v>240</v>
       </c>
       <c r="AA13" t="s">
+        <v>656</v>
+      </c>
+      <c r="AB13" t="s">
         <v>327</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>184</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>509</v>
       </c>
     </row>
@@ -32992,15 +33742,18 @@
         <v>87</v>
       </c>
       <c r="S14" t="s">
-        <v>245</v>
+        <v>605</v>
       </c>
       <c r="AA14" t="s">
+        <v>657</v>
+      </c>
+      <c r="AB14" t="s">
         <v>95</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>185</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AG14" t="s">
         <v>525</v>
       </c>
     </row>
@@ -33027,15 +33780,18 @@
         <v>533</v>
       </c>
       <c r="S15" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AA15" t="s">
+        <v>658</v>
+      </c>
+      <c r="AB15" t="s">
         <v>629</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>186</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AG15" t="s">
         <v>526</v>
       </c>
     </row>
@@ -33062,15 +33818,18 @@
         <v>534</v>
       </c>
       <c r="S16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AA16" t="s">
+        <v>659</v>
+      </c>
+      <c r="AB16" t="s">
         <v>611</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>187</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AG16" t="s">
         <v>530</v>
       </c>
     </row>
@@ -33091,15 +33850,18 @@
         <v>33</v>
       </c>
       <c r="S17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AA17" t="s">
+        <v>660</v>
+      </c>
+      <c r="AB17" t="s">
         <v>96</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>496</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AG17" t="s">
         <v>531</v>
       </c>
     </row>
@@ -33119,10 +33881,16 @@
       <c r="N18" t="s">
         <v>36</v>
       </c>
+      <c r="S18" t="s">
+        <v>243</v>
+      </c>
       <c r="AA18" t="s">
+        <v>661</v>
+      </c>
+      <c r="AB18" t="s">
         <v>67</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AG18" t="s">
         <v>510</v>
       </c>
     </row>
@@ -33140,9 +33908,12 @@
         <v>491</v>
       </c>
       <c r="AA19" t="s">
+        <v>662</v>
+      </c>
+      <c r="AB19" t="s">
         <v>535</v>
       </c>
-      <c r="AF19" t="s">
+      <c r="AG19" t="s">
         <v>527</v>
       </c>
     </row>
@@ -33160,9 +33931,12 @@
         <v>75</v>
       </c>
       <c r="AA20" t="s">
+        <v>663</v>
+      </c>
+      <c r="AB20" t="s">
         <v>97</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AG20" t="s">
         <v>528</v>
       </c>
     </row>
@@ -33180,9 +33954,12 @@
         <v>76</v>
       </c>
       <c r="AA21" t="s">
+        <v>664</v>
+      </c>
+      <c r="AB21" t="s">
         <v>98</v>
       </c>
-      <c r="AF21" t="s">
+      <c r="AG21" t="s">
         <v>532</v>
       </c>
     </row>
@@ -33200,9 +33977,12 @@
         <v>593</v>
       </c>
       <c r="AA22" t="s">
+        <v>606</v>
+      </c>
+      <c r="AB22" t="s">
         <v>99</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AG22" t="s">
         <v>226</v>
       </c>
     </row>
@@ -33220,9 +34000,12 @@
         <v>505</v>
       </c>
       <c r="AA23" t="s">
+        <v>665</v>
+      </c>
+      <c r="AB23" t="s">
         <v>100</v>
       </c>
-      <c r="AF23" t="s">
+      <c r="AG23" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33240,9 +34023,12 @@
         <v>37</v>
       </c>
       <c r="AA24" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB24" t="s">
         <v>518</v>
       </c>
-      <c r="AF24" t="s">
+      <c r="AG24" t="s">
         <v>571</v>
       </c>
     </row>
@@ -33260,9 +34046,12 @@
         <v>393</v>
       </c>
       <c r="AA25" t="s">
+        <v>667</v>
+      </c>
+      <c r="AB25" t="s">
         <v>102</v>
       </c>
-      <c r="AF25" t="s">
+      <c r="AG25" t="s">
         <v>572</v>
       </c>
     </row>
@@ -33277,18 +34066,21 @@
         <v>68</v>
       </c>
       <c r="L26" t="s">
-        <v>557</v>
+        <v>643</v>
       </c>
       <c r="AA26" t="s">
+        <v>607</v>
+      </c>
+      <c r="AB26" t="s">
         <v>579</v>
       </c>
-      <c r="AF26" t="s">
+      <c r="AG26" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>600</v>
       </c>
       <c r="F27" t="s">
         <v>55</v>
@@ -33297,18 +34089,21 @@
         <v>283</v>
       </c>
       <c r="L27" t="s">
-        <v>77</v>
+        <v>557</v>
       </c>
       <c r="AA27" t="s">
+        <v>668</v>
+      </c>
+      <c r="AB27" t="s">
         <v>103</v>
       </c>
-      <c r="AF27" t="s">
+      <c r="AG27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
         <v>483</v>
@@ -33317,15 +34112,18 @@
         <v>267</v>
       </c>
       <c r="L28" t="s">
-        <v>475</v>
+        <v>77</v>
       </c>
       <c r="AA28" t="s">
+        <v>669</v>
+      </c>
+      <c r="AB28" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
         <v>216</v>
@@ -33334,15 +34132,18 @@
         <v>284</v>
       </c>
       <c r="L29" t="s">
-        <v>38</v>
+        <v>475</v>
       </c>
       <c r="AA29" t="s">
+        <v>670</v>
+      </c>
+      <c r="AB29" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
         <v>217</v>
@@ -33351,15 +34152,18 @@
         <v>285</v>
       </c>
       <c r="L30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA30" t="s">
+        <v>671</v>
+      </c>
+      <c r="AB30" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>458</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
         <v>503</v>
@@ -33367,13 +34171,19 @@
       <c r="H31" t="s">
         <v>208</v>
       </c>
+      <c r="L31" t="s">
+        <v>39</v>
+      </c>
       <c r="AA31" t="s">
+        <v>672</v>
+      </c>
+      <c r="AB31" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>218</v>
+        <v>458</v>
       </c>
       <c r="F32" t="s">
         <v>504</v>
@@ -33382,10 +34192,16 @@
         <v>276</v>
       </c>
       <c r="AA32" t="s">
+        <v>673</v>
+      </c>
+      <c r="AB32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="s">
+        <v>218</v>
+      </c>
       <c r="F33" t="s">
         <v>453</v>
       </c>
@@ -33393,6 +34209,9 @@
         <v>286</v>
       </c>
       <c r="AA33" t="s">
+        <v>674</v>
+      </c>
+      <c r="AB33" t="s">
         <v>108</v>
       </c>
     </row>
@@ -33404,6 +34223,9 @@
         <v>541</v>
       </c>
       <c r="AA34" t="s">
+        <v>675</v>
+      </c>
+      <c r="AB34" t="s">
         <v>109</v>
       </c>
     </row>
@@ -33415,6 +34237,9 @@
         <v>261</v>
       </c>
       <c r="AA35" t="s">
+        <v>676</v>
+      </c>
+      <c r="AB35" t="s">
         <v>110</v>
       </c>
     </row>
@@ -33426,6 +34251,9 @@
         <v>331</v>
       </c>
       <c r="AA36" t="s">
+        <v>677</v>
+      </c>
+      <c r="AB36" t="s">
         <v>580</v>
       </c>
     </row>
@@ -33437,6 +34265,9 @@
         <v>309</v>
       </c>
       <c r="AA37" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB37" t="s">
         <v>111</v>
       </c>
     </row>
@@ -33448,6 +34279,9 @@
         <v>262</v>
       </c>
       <c r="AA38" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB38" t="s">
         <v>112</v>
       </c>
     </row>
@@ -33458,7 +34292,7 @@
       <c r="H39" t="s">
         <v>310</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AB39" t="s">
         <v>202</v>
       </c>
     </row>
@@ -33469,7 +34303,7 @@
       <c r="H40" t="s">
         <v>268</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AB40" t="s">
         <v>113</v>
       </c>
     </row>
@@ -33480,15 +34314,18 @@
       <c r="H41" t="s">
         <v>70</v>
       </c>
-      <c r="AA41" t="s">
+      <c r="AB41" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="42">
+      <c r="F42" t="s">
+        <v>642</v>
+      </c>
       <c r="H42" t="s">
         <v>204</v>
       </c>
-      <c r="AA42" t="s">
+      <c r="AB42" t="s">
         <v>470</v>
       </c>
     </row>
@@ -33496,7 +34333,7 @@
       <c r="H43" t="s">
         <v>576</v>
       </c>
-      <c r="AA43" t="s">
+      <c r="AB43" t="s">
         <v>590</v>
       </c>
     </row>
@@ -33504,7 +34341,7 @@
       <c r="H44" t="s">
         <v>290</v>
       </c>
-      <c r="AA44" t="s">
+      <c r="AB44" t="s">
         <v>394</v>
       </c>
     </row>
@@ -33512,7 +34349,7 @@
       <c r="H45" t="s">
         <v>301</v>
       </c>
-      <c r="AA45" t="s">
+      <c r="AB45" t="s">
         <v>114</v>
       </c>
     </row>
@@ -33520,7 +34357,7 @@
       <c r="H46" t="s">
         <v>302</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AB46" t="s">
         <v>115</v>
       </c>
     </row>
@@ -33528,7 +34365,7 @@
       <c r="H47" t="s">
         <v>344</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="AB47" t="s">
         <v>116</v>
       </c>
     </row>
@@ -33536,7 +34373,7 @@
       <c r="H48" t="s">
         <v>343</v>
       </c>
-      <c r="AA48" t="s">
+      <c r="AB48" t="s">
         <v>117</v>
       </c>
     </row>
@@ -33544,7 +34381,7 @@
       <c r="H49" t="s">
         <v>203</v>
       </c>
-      <c r="AA49" t="s">
+      <c r="AB49" t="s">
         <v>118</v>
       </c>
     </row>
@@ -33552,7 +34389,7 @@
       <c r="H50" t="s">
         <v>303</v>
       </c>
-      <c r="AA50" t="s">
+      <c r="AB50" t="s">
         <v>119</v>
       </c>
     </row>
@@ -33560,7 +34397,7 @@
       <c r="H51" t="s">
         <v>340</v>
       </c>
-      <c r="AA51" t="s">
+      <c r="AB51" t="s">
         <v>630</v>
       </c>
     </row>
@@ -33568,7 +34405,7 @@
       <c r="H52" t="s">
         <v>369</v>
       </c>
-      <c r="AA52" t="s">
+      <c r="AB52" t="s">
         <v>205</v>
       </c>
     </row>
@@ -33576,7 +34413,7 @@
       <c r="H53" t="s">
         <v>304</v>
       </c>
-      <c r="AA53" t="s">
+      <c r="AB53" t="s">
         <v>69</v>
       </c>
     </row>
@@ -33584,7 +34421,7 @@
       <c r="H54" t="s">
         <v>357</v>
       </c>
-      <c r="AA54" t="s">
+      <c r="AB54" t="s">
         <v>566</v>
       </c>
     </row>
@@ -33592,7 +34429,7 @@
       <c r="H55" t="s">
         <v>332</v>
       </c>
-      <c r="AA55" t="s">
+      <c r="AB55" t="s">
         <v>120</v>
       </c>
     </row>
@@ -33600,7 +34437,7 @@
       <c r="H56" t="s">
         <v>269</v>
       </c>
-      <c r="AA56" t="s">
+      <c r="AB56" t="s">
         <v>121</v>
       </c>
     </row>
@@ -33608,7 +34445,7 @@
       <c r="H57" t="s">
         <v>293</v>
       </c>
-      <c r="AA57" t="s">
+      <c r="AB57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -33616,7 +34453,7 @@
       <c r="H58" t="s">
         <v>294</v>
       </c>
-      <c r="AA58" t="s">
+      <c r="AB58" t="s">
         <v>516</v>
       </c>
     </row>
@@ -33624,7 +34461,7 @@
       <c r="H59" t="s">
         <v>577</v>
       </c>
-      <c r="AA59" t="s">
+      <c r="AB59" t="s">
         <v>500</v>
       </c>
     </row>
@@ -33632,7 +34469,7 @@
       <c r="H60" t="s">
         <v>295</v>
       </c>
-      <c r="AA60" t="s">
+      <c r="AB60" t="s">
         <v>123</v>
       </c>
     </row>
@@ -33640,7 +34477,7 @@
       <c r="H61" t="s">
         <v>305</v>
       </c>
-      <c r="AA61" t="s">
+      <c r="AB61" t="s">
         <v>347</v>
       </c>
     </row>
@@ -33648,7 +34485,7 @@
       <c r="H62" t="s">
         <v>314</v>
       </c>
-      <c r="AA62" t="s">
+      <c r="AB62" t="s">
         <v>494</v>
       </c>
     </row>
@@ -33656,7 +34493,7 @@
       <c r="H63" t="s">
         <v>338</v>
       </c>
-      <c r="AA63" t="s">
+      <c r="AB63" t="s">
         <v>124</v>
       </c>
     </row>
@@ -33664,7 +34501,7 @@
       <c r="H64" t="s">
         <v>311</v>
       </c>
-      <c r="AA64" t="s">
+      <c r="AB64" t="s">
         <v>125</v>
       </c>
     </row>
@@ -33672,7 +34509,7 @@
       <c r="H65" t="s">
         <v>312</v>
       </c>
-      <c r="AA65" t="s">
+      <c r="AB65" t="s">
         <v>126</v>
       </c>
     </row>
@@ -33680,7 +34517,7 @@
       <c r="H66" t="s">
         <v>370</v>
       </c>
-      <c r="AA66" t="s">
+      <c r="AB66" t="s">
         <v>127</v>
       </c>
     </row>
@@ -33688,7 +34525,7 @@
       <c r="H67" t="s">
         <v>371</v>
       </c>
-      <c r="AA67" t="s">
+      <c r="AB67" t="s">
         <v>128</v>
       </c>
     </row>
@@ -33696,7 +34533,7 @@
       <c r="H68" t="s">
         <v>346</v>
       </c>
-      <c r="AA68" t="s">
+      <c r="AB68" t="s">
         <v>129</v>
       </c>
     </row>
@@ -33704,7 +34541,7 @@
       <c r="H69" t="s">
         <v>315</v>
       </c>
-      <c r="AA69" t="s">
+      <c r="AB69" t="s">
         <v>130</v>
       </c>
     </row>
@@ -33712,7 +34549,7 @@
       <c r="H70" t="s">
         <v>270</v>
       </c>
-      <c r="AA70" t="s">
+      <c r="AB70" t="s">
         <v>473</v>
       </c>
     </row>
@@ -33720,7 +34557,7 @@
       <c r="H71" t="s">
         <v>562</v>
       </c>
-      <c r="AA71" t="s">
+      <c r="AB71" t="s">
         <v>508</v>
       </c>
     </row>
@@ -33728,7 +34565,7 @@
       <c r="H72" t="s">
         <v>316</v>
       </c>
-      <c r="AA72" t="s">
+      <c r="AB72" t="s">
         <v>206</v>
       </c>
     </row>
@@ -33736,7 +34573,7 @@
       <c r="H73" t="s">
         <v>409</v>
       </c>
-      <c r="AA73" t="s">
+      <c r="AB73" t="s">
         <v>390</v>
       </c>
     </row>
@@ -33744,7 +34581,7 @@
       <c r="H74" t="s">
         <v>306</v>
       </c>
-      <c r="AA74" t="s">
+      <c r="AB74" t="s">
         <v>478</v>
       </c>
     </row>
@@ -33752,7 +34589,7 @@
       <c r="H75" t="s">
         <v>410</v>
       </c>
-      <c r="AA75" t="s">
+      <c r="AB75" t="s">
         <v>131</v>
       </c>
     </row>
@@ -33760,7 +34597,7 @@
       <c r="H76" t="s">
         <v>263</v>
       </c>
-      <c r="AA76" t="s">
+      <c r="AB76" t="s">
         <v>132</v>
       </c>
     </row>
@@ -33768,7 +34605,7 @@
       <c r="H77" t="s">
         <v>542</v>
       </c>
-      <c r="AA77" t="s">
+      <c r="AB77" t="s">
         <v>133</v>
       </c>
     </row>
@@ -33776,7 +34613,7 @@
       <c r="H78" t="s">
         <v>345</v>
       </c>
-      <c r="AA78" t="s">
+      <c r="AB78" t="s">
         <v>134</v>
       </c>
     </row>
@@ -33784,414 +34621,424 @@
       <c r="H79" t="s">
         <v>281</v>
       </c>
-      <c r="AA79" t="s">
-        <v>189</v>
+      <c r="AB79" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="80">
       <c r="H80" t="s">
         <v>287</v>
       </c>
-      <c r="AA80" t="s">
-        <v>190</v>
+      <c r="AB80" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="81">
       <c r="H81" t="s">
         <v>292</v>
       </c>
-      <c r="AA81" t="s">
-        <v>489</v>
+      <c r="AB81" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="82">
       <c r="H82" t="s">
         <v>464</v>
       </c>
-      <c r="AA82" t="s">
-        <v>502</v>
+      <c r="AB82" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="83">
       <c r="H83" t="s">
         <v>333</v>
       </c>
-      <c r="AA83" t="s">
-        <v>135</v>
+      <c r="AB83" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="84">
       <c r="H84" t="s">
         <v>271</v>
       </c>
-      <c r="AA84" t="s">
-        <v>136</v>
+      <c r="AB84" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="85">
       <c r="H85" t="s">
         <v>282</v>
       </c>
-      <c r="AA85" t="s">
-        <v>137</v>
+      <c r="AB85" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="86">
       <c r="H86" t="s">
         <v>288</v>
       </c>
-      <c r="AA86" t="s">
-        <v>529</v>
+      <c r="AB86" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="87">
       <c r="H87" t="s">
         <v>277</v>
       </c>
-      <c r="AA87" t="s">
-        <v>138</v>
+      <c r="AB87" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="88">
       <c r="H88" t="s">
         <v>563</v>
       </c>
-      <c r="AA88" t="s">
-        <v>139</v>
+      <c r="AB88" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="89">
       <c r="H89" t="s">
         <v>272</v>
       </c>
-      <c r="AA89" t="s">
-        <v>191</v>
+      <c r="AB89" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="90">
       <c r="H90" t="s">
         <v>289</v>
       </c>
-      <c r="AA90" t="s">
-        <v>517</v>
+      <c r="AB90" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="91">
       <c r="H91" t="s">
         <v>273</v>
       </c>
-      <c r="AA91" t="s">
-        <v>599</v>
+      <c r="AB91" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="92">
       <c r="H92" t="s">
         <v>274</v>
       </c>
-      <c r="AA92" t="s">
-        <v>192</v>
+      <c r="AB92" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="93">
       <c r="H93" t="s">
         <v>307</v>
       </c>
-      <c r="AA93" t="s">
-        <v>488</v>
+      <c r="AB93" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="94">
       <c r="H94" t="s">
         <v>313</v>
       </c>
-      <c r="AA94" t="s">
-        <v>193</v>
+      <c r="AB94" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="95">
       <c r="H95" t="s">
         <v>296</v>
       </c>
-      <c r="AA95" t="s">
-        <v>194</v>
+      <c r="AB95" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="96">
       <c r="H96" t="s">
         <v>341</v>
       </c>
-      <c r="AA96" t="s">
-        <v>584</v>
+      <c r="AB96" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="97">
       <c r="H97" t="s">
         <v>278</v>
       </c>
-      <c r="AA97" t="s">
-        <v>585</v>
+      <c r="AB97" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="98">
       <c r="H98" t="s">
         <v>279</v>
       </c>
-      <c r="AA98" t="s">
+      <c r="AB98" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="AB99" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="99">
-      <c r="AA99" t="s">
+    <row r="100">
+      <c r="AB100" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="100">
-      <c r="AA100" t="s">
+    <row r="101">
+      <c r="AB101" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="101">
-      <c r="AA101" t="s">
+    <row r="102">
+      <c r="AB102" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="102">
-      <c r="AA102" t="s">
+    <row r="103">
+      <c r="AB103" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="103">
-      <c r="AA103" t="s">
+    <row r="104">
+      <c r="AB104" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="104">
-      <c r="AA104" t="s">
+    <row r="105">
+      <c r="AB105" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="105">
-      <c r="AA105" t="s">
+    <row r="106">
+      <c r="AB106" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="106">
-      <c r="AA106" t="s">
+    <row r="107">
+      <c r="AB107" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="107">
-      <c r="AA107" t="s">
+    <row r="108">
+      <c r="AB108" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="108">
-      <c r="AA108" t="s">
+    <row r="109">
+      <c r="AB109" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="109">
-      <c r="AA109" t="s">
+    <row r="110">
+      <c r="AB110" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="110">
-      <c r="AA110" t="s">
+    <row r="111">
+      <c r="AB111" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="111">
-      <c r="AA111" t="s">
+    <row r="112">
+      <c r="AB112" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="112">
-      <c r="AA112" t="s">
+    <row r="113">
+      <c r="AB113" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="113">
-      <c r="AA113" t="s">
-        <v>591</v>
-      </c>
-    </row>
     <row r="114">
-      <c r="AA114" t="s">
+      <c r="AB114" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="AB115" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="AB116" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="115">
-      <c r="AA115" t="s">
+    <row r="117">
+      <c r="AB117" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="116">
-      <c r="AA116" t="s">
+    <row r="118">
+      <c r="AB118" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="117">
-      <c r="AA117" t="s">
+    <row r="119">
+      <c r="AB119" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="118">
-      <c r="AA118" t="s">
+    <row r="120">
+      <c r="AB120" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="119">
-      <c r="AA119" t="s">
+    <row r="121">
+      <c r="AB121" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="120">
-      <c r="AA120" t="s">
+    <row r="122">
+      <c r="AB122" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="121">
-      <c r="AA121" t="s">
+    <row r="123">
+      <c r="AB123" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="122">
-      <c r="AA122" t="s">
+    <row r="124">
+      <c r="AB124" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="123">
-      <c r="AA123" t="s">
+    <row r="125">
+      <c r="AB125" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="124">
-      <c r="AA124" t="s">
+    <row r="126">
+      <c r="AB126" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="125">
-      <c r="AA125" t="s">
+    <row r="127">
+      <c r="AB127" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="126">
-      <c r="AA126" t="s">
+    <row r="128">
+      <c r="AB128" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="127">
-      <c r="AA127" t="s">
+    <row r="129">
+      <c r="AB129" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="128">
-      <c r="AA128" t="s">
+    <row r="130">
+      <c r="AB130" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="129">
-      <c r="AA129" t="s">
+    <row r="131">
+      <c r="AB131" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="130">
-      <c r="AA130" t="s">
+    <row r="132">
+      <c r="AB132" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="131">
-      <c r="AA131" t="s">
+    <row r="133">
+      <c r="AB133" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="132">
-      <c r="AA132" t="s">
+    <row r="134">
+      <c r="AB134" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="133">
-      <c r="AA133" t="s">
+    <row r="135">
+      <c r="AB135" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="134">
-      <c r="AA134" t="s">
+    <row r="136">
+      <c r="AB136" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="135">
-      <c r="AA135" t="s">
+    <row r="137">
+      <c r="AB137" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="136">
-      <c r="AA136" t="s">
+    <row r="138">
+      <c r="AB138" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="137">
-      <c r="AA137" t="s">
+    <row r="139">
+      <c r="AB139" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="138">
-      <c r="AA138" t="s">
+    <row r="140">
+      <c r="AB140" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="139">
-      <c r="AA139" t="s">
+    <row r="141">
+      <c r="AB141" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="140">
-      <c r="AA140" t="s">
+    <row r="142">
+      <c r="AB142" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="141">
-      <c r="AA141" t="s">
+    <row r="143">
+      <c r="AB143" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="142">
-      <c r="AA142" t="s">
+    <row r="144">
+      <c r="AB144" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="143">
-      <c r="AA143" t="s">
+    <row r="145">
+      <c r="AB145" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="144">
-      <c r="AA144" t="s">
+    <row r="146">
+      <c r="AB146" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="145">
-      <c r="AA145" t="s">
+    <row r="147">
+      <c r="AB147" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="146">
-      <c r="AA146" t="s">
+    <row r="148">
+      <c r="AB148" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="147">
-      <c r="AA147" t="s">
+    <row r="149">
+      <c r="AB149" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="148">
-      <c r="AA148" t="s">
+    <row r="150">
+      <c r="AB150" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="149">
-      <c r="AA149" t="s">
+    <row r="151">
+      <c r="AB151" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[base commands] - [`assertMatch(text,regex)`]: *NEW* command to check for text value via   regular expression.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -19,13 +19,13 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$F$2:$F$44</definedName>
+    <definedName name="base">'#system'!$F$2:$F$45</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
     <definedName name="excel">'#system'!$I$2:$I$16</definedName>
-    <definedName name="external">'#system'!$J$2:$J$6</definedName>
+    <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$31</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
@@ -42,13 +42,13 @@
     <definedName name="sound">'#system'!$W$2:$W$5</definedName>
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$33</definedName>
-    <definedName name="web">'#system'!$AB$2:$AB$151</definedName>
-    <definedName name="webalert">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="webcookie">'#system'!$AD$2:$AD$10</definedName>
-    <definedName name="ws">'#system'!$AE$2:$AE$17</definedName>
-    <definedName name="ws.async">'#system'!$AF$2:$AF$8</definedName>
-    <definedName name="xml">'#system'!$AG$2:$AG$27</definedName>
+    <definedName name="target">'#system'!$A$2:$A$32</definedName>
+    <definedName name="web">'#system'!$AA$2:$AA$151</definedName>
+    <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
+    <definedName name="ws">'#system'!$AD$2:$AD$17</definedName>
+    <definedName name="ws.async">'#system'!$AE$2:$AE$8</definedName>
+    <definedName name="xml">'#system'!$AF$2:$AF$27</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27810" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28410" uniqueCount="685">
   <si>
     <t>description</t>
   </si>
@@ -2120,6 +2120,12 @@
   </si>
   <si>
     <t>screenshotInFull(file,timeout,removeFixed)</t>
+  </si>
+  <si>
+    <t>assertMatch(text,regex)</t>
+  </si>
+  <si>
+    <t>openFile(filePath)</t>
   </si>
 </sst>
 </file>
@@ -2127,7 +2133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="826" x14ac:knownFonts="1">
+  <fonts count="843" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7344,8 +7350,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1401">
+  <fills count="1425">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15006,6 +15119,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="E6E6E6"/>
         <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -30008,7 +30257,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="837">
+  <cellXfs count="854">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -32474,55 +32723,106 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1373" fontId="808" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="809" fillId="1379" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="810" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1379" fontId="809" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="810" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="811" fillId="1382" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1382" fontId="811" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="812" fillId="1385" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1385" fontId="812" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="813" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1388" fontId="813" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="814" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="814" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="815" fillId="1391" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1391" fontId="815" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="816" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="817" fillId="1394" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="816" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1394" fontId="817" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="818" fillId="1397" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1397" fontId="818" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="819" fillId="1385" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1385" fontId="819" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="820" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="821" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="822" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="823" fillId="1400" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="824" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="825" fillId="1397" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="820" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="821" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1388" fontId="822" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1400" fontId="823" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1388" fontId="824" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1397" fontId="825" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="826" fillId="1403" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="827" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="828" fillId="1406" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="829" fillId="1409" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="830" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="831" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="832" fillId="1415" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="833" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="834" fillId="1418" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="835" fillId="1421" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="836" fillId="1409" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="837" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="838" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="839" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="840" fillId="1424" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="841" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="842" fillId="1421" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -32820,7 +33120,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH151"/>
+  <dimension ref="A1:AG151"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -32909,24 +33209,21 @@
         <v>619</v>
       </c>
       <c r="AA1" t="s">
-        <v>600</v>
+        <v>46</v>
       </c>
       <c r="AB1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AD1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AE1" t="s">
-        <v>49</v>
+        <v>458</v>
       </c>
       <c r="AF1" t="s">
-        <v>458</v>
-      </c>
-      <c r="AG1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -32959,7 +33256,7 @@
         <v>484</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>684</v>
       </c>
       <c r="K2" t="s">
         <v>603</v>
@@ -33010,24 +33307,21 @@
         <v>626</v>
       </c>
       <c r="AA2" t="s">
-        <v>645</v>
+        <v>89</v>
       </c>
       <c r="AB2" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="AC2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="AD2" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="AE2" t="s">
-        <v>175</v>
+        <v>468</v>
       </c>
       <c r="AF2" t="s">
-        <v>468</v>
-      </c>
-      <c r="AG2" t="s">
         <v>524</v>
       </c>
     </row>
@@ -33057,7 +33351,7 @@
         <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>511</v>
+        <v>71</v>
       </c>
       <c r="K3" t="s">
         <v>350</v>
@@ -33102,24 +33396,21 @@
         <v>627</v>
       </c>
       <c r="AA3" t="s">
-        <v>646</v>
+        <v>90</v>
       </c>
       <c r="AB3" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="AC3" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="AD3" t="s">
-        <v>169</v>
+        <v>365</v>
       </c>
       <c r="AE3" t="s">
-        <v>365</v>
+        <v>176</v>
       </c>
       <c r="AF3" t="s">
-        <v>176</v>
-      </c>
-      <c r="AG3" t="s">
         <v>219</v>
       </c>
     </row>
@@ -33146,7 +33437,7 @@
         <v>485</v>
       </c>
       <c r="J4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K4" t="s">
         <v>351</v>
@@ -33191,24 +33482,21 @@
         <v>628</v>
       </c>
       <c r="AA4" t="s">
-        <v>647</v>
+        <v>596</v>
       </c>
       <c r="AB4" t="s">
-        <v>596</v>
+        <v>165</v>
       </c>
       <c r="AC4" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="AD4" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AE4" t="s">
-        <v>176</v>
+        <v>459</v>
       </c>
       <c r="AF4" t="s">
-        <v>459</v>
-      </c>
-      <c r="AG4" t="s">
         <v>220</v>
       </c>
     </row>
@@ -33235,7 +33523,7 @@
         <v>490</v>
       </c>
       <c r="J5" t="s">
-        <v>560</v>
+        <v>512</v>
       </c>
       <c r="K5" t="s">
         <v>352</v>
@@ -33268,24 +33556,21 @@
         <v>360</v>
       </c>
       <c r="AA5" t="s">
-        <v>648</v>
+        <v>589</v>
       </c>
       <c r="AB5" t="s">
-        <v>589</v>
+        <v>166</v>
       </c>
       <c r="AC5" t="s">
-        <v>166</v>
+        <v>617</v>
       </c>
       <c r="AD5" t="s">
-        <v>617</v>
+        <v>177</v>
       </c>
       <c r="AE5" t="s">
-        <v>177</v>
+        <v>460</v>
       </c>
       <c r="AF5" t="s">
-        <v>460</v>
-      </c>
-      <c r="AG5" t="s">
         <v>221</v>
       </c>
     </row>
@@ -33312,7 +33597,7 @@
         <v>486</v>
       </c>
       <c r="J6" t="s">
-        <v>594</v>
+        <v>560</v>
       </c>
       <c r="K6" t="s">
         <v>604</v>
@@ -33342,24 +33627,21 @@
         <v>362</v>
       </c>
       <c r="AA6" t="s">
-        <v>649</v>
+        <v>91</v>
       </c>
       <c r="AB6" t="s">
-        <v>91</v>
+        <v>480</v>
       </c>
       <c r="AC6" t="s">
-        <v>480</v>
+        <v>171</v>
       </c>
       <c r="AD6" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="AE6" t="s">
-        <v>178</v>
+        <v>461</v>
       </c>
       <c r="AF6" t="s">
-        <v>461</v>
-      </c>
-      <c r="AG6" t="s">
         <v>222</v>
       </c>
     </row>
@@ -33379,6 +33661,9 @@
       <c r="I7" t="s">
         <v>482</v>
       </c>
+      <c r="J7" t="s">
+        <v>594</v>
+      </c>
       <c r="K7" t="s">
         <v>349</v>
       </c>
@@ -33407,24 +33692,21 @@
         <v>361</v>
       </c>
       <c r="AA7" t="s">
-        <v>650</v>
+        <v>92</v>
       </c>
       <c r="AB7" t="s">
-        <v>92</v>
+        <v>481</v>
       </c>
       <c r="AC7" t="s">
-        <v>481</v>
+        <v>172</v>
       </c>
       <c r="AD7" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="AE7" t="s">
-        <v>179</v>
+        <v>462</v>
       </c>
       <c r="AF7" t="s">
-        <v>462</v>
-      </c>
-      <c r="AG7" t="s">
         <v>567</v>
       </c>
     </row>
@@ -33472,24 +33754,21 @@
         <v>363</v>
       </c>
       <c r="AA8" t="s">
-        <v>651</v>
+        <v>93</v>
       </c>
       <c r="AB8" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="AC8" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="AD8" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="AE8" t="s">
-        <v>180</v>
+        <v>463</v>
       </c>
       <c r="AF8" t="s">
-        <v>463</v>
-      </c>
-      <c r="AG8" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33534,18 +33813,15 @@
         <v>364</v>
       </c>
       <c r="AA9" t="s">
-        <v>652</v>
-      </c>
-      <c r="AB9" t="s">
         <v>201</v>
       </c>
+      <c r="AC9" t="s">
+        <v>174</v>
+      </c>
       <c r="AD9" t="s">
-        <v>174</v>
-      </c>
-      <c r="AE9" t="s">
         <v>181</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AF9" t="s">
         <v>569</v>
       </c>
     </row>
@@ -33581,18 +33857,15 @@
         <v>408</v>
       </c>
       <c r="AA10" t="s">
-        <v>653</v>
-      </c>
-      <c r="AB10" t="s">
         <v>258</v>
       </c>
+      <c r="AC10" t="s">
+        <v>618</v>
+      </c>
       <c r="AD10" t="s">
-        <v>618</v>
-      </c>
-      <c r="AE10" t="s">
         <v>182</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AF10" t="s">
         <v>223</v>
       </c>
     </row>
@@ -33601,7 +33874,7 @@
         <v>348</v>
       </c>
       <c r="F11" t="s">
-        <v>588</v>
+        <v>683</v>
       </c>
       <c r="H11" t="s">
         <v>353</v>
@@ -33625,15 +33898,12 @@
         <v>644</v>
       </c>
       <c r="AA11" t="s">
-        <v>654</v>
-      </c>
-      <c r="AB11" t="s">
         <v>259</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AD11" t="s">
         <v>260</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AF11" t="s">
         <v>224</v>
       </c>
     </row>
@@ -33642,7 +33912,7 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>321</v>
+        <v>588</v>
       </c>
       <c r="H12" t="s">
         <v>275</v>
@@ -33666,15 +33936,12 @@
         <v>239</v>
       </c>
       <c r="AA12" t="s">
-        <v>655</v>
-      </c>
-      <c r="AB12" t="s">
         <v>94</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AD12" t="s">
         <v>183</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AF12" t="s">
         <v>225</v>
       </c>
     </row>
@@ -33683,7 +33950,7 @@
         <v>334</v>
       </c>
       <c r="F13" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="H13" t="s">
         <v>264</v>
@@ -33707,15 +33974,12 @@
         <v>240</v>
       </c>
       <c r="AA13" t="s">
-        <v>656</v>
-      </c>
-      <c r="AB13" t="s">
         <v>327</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AD13" t="s">
         <v>184</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AF13" t="s">
         <v>509</v>
       </c>
     </row>
@@ -33724,7 +33988,7 @@
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>342</v>
       </c>
       <c r="H14" t="s">
         <v>318</v>
@@ -33745,15 +34009,12 @@
         <v>605</v>
       </c>
       <c r="AA14" t="s">
-        <v>657</v>
-      </c>
-      <c r="AB14" t="s">
         <v>95</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AD14" t="s">
         <v>185</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AF14" t="s">
         <v>525</v>
       </c>
     </row>
@@ -33762,7 +34023,7 @@
         <v>545</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="H15" t="s">
         <v>265</v>
@@ -33783,15 +34044,12 @@
         <v>245</v>
       </c>
       <c r="AA15" t="s">
-        <v>658</v>
-      </c>
-      <c r="AB15" t="s">
         <v>629</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AD15" t="s">
         <v>186</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AF15" t="s">
         <v>526</v>
       </c>
     </row>
@@ -33800,7 +34058,7 @@
         <v>246</v>
       </c>
       <c r="F16" t="s">
-        <v>386</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s">
         <v>266</v>
@@ -33821,15 +34079,12 @@
         <v>241</v>
       </c>
       <c r="AA16" t="s">
-        <v>659</v>
-      </c>
-      <c r="AB16" t="s">
         <v>611</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AD16" t="s">
         <v>187</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AF16" t="s">
         <v>530</v>
       </c>
     </row>
@@ -33838,7 +34093,7 @@
         <v>188</v>
       </c>
       <c r="F17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H17" t="s">
         <v>319</v>
@@ -33853,15 +34108,12 @@
         <v>242</v>
       </c>
       <c r="AA17" t="s">
-        <v>660</v>
-      </c>
-      <c r="AB17" t="s">
         <v>96</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AD17" t="s">
         <v>496</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AF17" t="s">
         <v>531</v>
       </c>
     </row>
@@ -33870,7 +34122,7 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="H18" t="s">
         <v>81</v>
@@ -33885,12 +34137,9 @@
         <v>243</v>
       </c>
       <c r="AA18" t="s">
-        <v>661</v>
-      </c>
-      <c r="AB18" t="s">
         <v>67</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AF18" t="s">
         <v>510</v>
       </c>
     </row>
@@ -33899,7 +34148,7 @@
         <v>230</v>
       </c>
       <c r="F19" t="s">
-        <v>620</v>
+        <v>411</v>
       </c>
       <c r="H19" t="s">
         <v>82</v>
@@ -33908,12 +34157,9 @@
         <v>491</v>
       </c>
       <c r="AA19" t="s">
-        <v>662</v>
-      </c>
-      <c r="AB19" t="s">
         <v>535</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AF19" t="s">
         <v>527</v>
       </c>
     </row>
@@ -33922,7 +34168,7 @@
         <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H20" t="s">
         <v>297</v>
@@ -33931,12 +34177,9 @@
         <v>75</v>
       </c>
       <c r="AA20" t="s">
-        <v>663</v>
-      </c>
-      <c r="AB20" t="s">
         <v>97</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AF20" t="s">
         <v>528</v>
       </c>
     </row>
@@ -33945,7 +34188,7 @@
         <v>399</v>
       </c>
       <c r="F21" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H21" t="s">
         <v>298</v>
@@ -33954,12 +34197,9 @@
         <v>76</v>
       </c>
       <c r="AA21" t="s">
-        <v>664</v>
-      </c>
-      <c r="AB21" t="s">
         <v>98</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AF21" t="s">
         <v>532</v>
       </c>
     </row>
@@ -33968,7 +34208,7 @@
         <v>456</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>622</v>
       </c>
       <c r="H22" t="s">
         <v>299</v>
@@ -33977,12 +34217,9 @@
         <v>593</v>
       </c>
       <c r="AA22" t="s">
-        <v>606</v>
-      </c>
-      <c r="AB22" t="s">
         <v>99</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AF22" t="s">
         <v>226</v>
       </c>
     </row>
@@ -33991,7 +34228,7 @@
         <v>413</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" t="s">
         <v>300</v>
@@ -34000,12 +34237,9 @@
         <v>505</v>
       </c>
       <c r="AA23" t="s">
-        <v>665</v>
-      </c>
-      <c r="AB23" t="s">
         <v>100</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AF23" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34014,7 +34248,7 @@
         <v>358</v>
       </c>
       <c r="F24" t="s">
-        <v>574</v>
+        <v>53</v>
       </c>
       <c r="H24" t="s">
         <v>291</v>
@@ -34023,12 +34257,9 @@
         <v>37</v>
       </c>
       <c r="AA24" t="s">
-        <v>666</v>
-      </c>
-      <c r="AB24" t="s">
         <v>518</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AF24" t="s">
         <v>571</v>
       </c>
     </row>
@@ -34037,7 +34268,7 @@
         <v>395</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>574</v>
       </c>
       <c r="H25" t="s">
         <v>280</v>
@@ -34046,12 +34277,9 @@
         <v>393</v>
       </c>
       <c r="AA25" t="s">
-        <v>667</v>
-      </c>
-      <c r="AB25" t="s">
         <v>102</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AF25" t="s">
         <v>572</v>
       </c>
     </row>
@@ -34060,7 +34288,7 @@
         <v>619</v>
       </c>
       <c r="F26" t="s">
-        <v>322</v>
+        <v>54</v>
       </c>
       <c r="H26" t="s">
         <v>68</v>
@@ -34069,21 +34297,18 @@
         <v>643</v>
       </c>
       <c r="AA26" t="s">
-        <v>607</v>
-      </c>
-      <c r="AB26" t="s">
         <v>579</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AF26" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>600</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>322</v>
       </c>
       <c r="H27" t="s">
         <v>283</v>
@@ -34092,21 +34317,18 @@
         <v>557</v>
       </c>
       <c r="AA27" t="s">
-        <v>668</v>
-      </c>
-      <c r="AB27" t="s">
         <v>103</v>
       </c>
-      <c r="AG27" t="s">
+      <c r="AF27" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>483</v>
+        <v>55</v>
       </c>
       <c r="H28" t="s">
         <v>267</v>
@@ -34115,18 +34337,15 @@
         <v>77</v>
       </c>
       <c r="AA28" t="s">
-        <v>669</v>
-      </c>
-      <c r="AB28" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>216</v>
+        <v>483</v>
       </c>
       <c r="H29" t="s">
         <v>284</v>
@@ -34135,18 +34354,15 @@
         <v>475</v>
       </c>
       <c r="AA29" t="s">
-        <v>670</v>
-      </c>
-      <c r="AB29" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H30" t="s">
         <v>285</v>
@@ -34155,18 +34371,15 @@
         <v>38</v>
       </c>
       <c r="AA30" t="s">
-        <v>671</v>
-      </c>
-      <c r="AB30" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>458</v>
       </c>
       <c r="F31" t="s">
-        <v>503</v>
+        <v>217</v>
       </c>
       <c r="H31" t="s">
         <v>208</v>
@@ -34175,165 +34388,141 @@
         <v>39</v>
       </c>
       <c r="AA31" t="s">
-        <v>672</v>
-      </c>
-      <c r="AB31" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>458</v>
+        <v>218</v>
       </c>
       <c r="F32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H32" t="s">
         <v>276</v>
       </c>
       <c r="AA32" t="s">
-        <v>673</v>
-      </c>
-      <c r="AB32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>218</v>
-      </c>
       <c r="F33" t="s">
-        <v>453</v>
+        <v>504</v>
       </c>
       <c r="H33" t="s">
         <v>286</v>
       </c>
       <c r="AA33" t="s">
-        <v>674</v>
-      </c>
-      <c r="AB33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>56</v>
+        <v>453</v>
       </c>
       <c r="H34" t="s">
         <v>541</v>
       </c>
       <c r="AA34" t="s">
-        <v>675</v>
-      </c>
-      <c r="AB34" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H35" t="s">
         <v>261</v>
       </c>
       <c r="AA35" t="s">
-        <v>676</v>
-      </c>
-      <c r="AB35" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H36" t="s">
         <v>331</v>
       </c>
       <c r="AA36" t="s">
-        <v>677</v>
-      </c>
-      <c r="AB36" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H37" t="s">
         <v>309</v>
       </c>
       <c r="AA37" t="s">
-        <v>678</v>
-      </c>
-      <c r="AB37" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H38" t="s">
         <v>262</v>
       </c>
       <c r="AA38" t="s">
-        <v>679</v>
-      </c>
-      <c r="AB38" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="39">
       <c r="F39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H39" t="s">
         <v>310</v>
       </c>
-      <c r="AB39" t="s">
+      <c r="AA39" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="40">
       <c r="F40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H40" t="s">
         <v>268</v>
       </c>
-      <c r="AB40" t="s">
+      <c r="AA40" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="41">
       <c r="F41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H41" t="s">
         <v>70</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AA41" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="42">
       <c r="F42" t="s">
-        <v>642</v>
+        <v>63</v>
       </c>
       <c r="H42" t="s">
         <v>204</v>
       </c>
-      <c r="AB42" t="s">
+      <c r="AA42" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="43">
+      <c r="F43" t="s">
+        <v>642</v>
+      </c>
       <c r="H43" t="s">
         <v>576</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AA43" t="s">
         <v>590</v>
       </c>
     </row>
@@ -34341,7 +34530,7 @@
       <c r="H44" t="s">
         <v>290</v>
       </c>
-      <c r="AB44" t="s">
+      <c r="AA44" t="s">
         <v>394</v>
       </c>
     </row>
@@ -34349,7 +34538,7 @@
       <c r="H45" t="s">
         <v>301</v>
       </c>
-      <c r="AB45" t="s">
+      <c r="AA45" t="s">
         <v>114</v>
       </c>
     </row>
@@ -34357,7 +34546,7 @@
       <c r="H46" t="s">
         <v>302</v>
       </c>
-      <c r="AB46" t="s">
+      <c r="AA46" t="s">
         <v>115</v>
       </c>
     </row>
@@ -34365,7 +34554,7 @@
       <c r="H47" t="s">
         <v>344</v>
       </c>
-      <c r="AB47" t="s">
+      <c r="AA47" t="s">
         <v>116</v>
       </c>
     </row>
@@ -34373,7 +34562,7 @@
       <c r="H48" t="s">
         <v>343</v>
       </c>
-      <c r="AB48" t="s">
+      <c r="AA48" t="s">
         <v>117</v>
       </c>
     </row>
@@ -34381,7 +34570,7 @@
       <c r="H49" t="s">
         <v>203</v>
       </c>
-      <c r="AB49" t="s">
+      <c r="AA49" t="s">
         <v>118</v>
       </c>
     </row>
@@ -34389,7 +34578,7 @@
       <c r="H50" t="s">
         <v>303</v>
       </c>
-      <c r="AB50" t="s">
+      <c r="AA50" t="s">
         <v>119</v>
       </c>
     </row>
@@ -34397,7 +34586,7 @@
       <c r="H51" t="s">
         <v>340</v>
       </c>
-      <c r="AB51" t="s">
+      <c r="AA51" t="s">
         <v>630</v>
       </c>
     </row>
@@ -34405,7 +34594,7 @@
       <c r="H52" t="s">
         <v>369</v>
       </c>
-      <c r="AB52" t="s">
+      <c r="AA52" t="s">
         <v>205</v>
       </c>
     </row>
@@ -34413,7 +34602,7 @@
       <c r="H53" t="s">
         <v>304</v>
       </c>
-      <c r="AB53" t="s">
+      <c r="AA53" t="s">
         <v>69</v>
       </c>
     </row>
@@ -34421,7 +34610,7 @@
       <c r="H54" t="s">
         <v>357</v>
       </c>
-      <c r="AB54" t="s">
+      <c r="AA54" t="s">
         <v>566</v>
       </c>
     </row>
@@ -34429,7 +34618,7 @@
       <c r="H55" t="s">
         <v>332</v>
       </c>
-      <c r="AB55" t="s">
+      <c r="AA55" t="s">
         <v>120</v>
       </c>
     </row>
@@ -34437,7 +34626,7 @@
       <c r="H56" t="s">
         <v>269</v>
       </c>
-      <c r="AB56" t="s">
+      <c r="AA56" t="s">
         <v>121</v>
       </c>
     </row>
@@ -34445,7 +34634,7 @@
       <c r="H57" t="s">
         <v>293</v>
       </c>
-      <c r="AB57" t="s">
+      <c r="AA57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -34453,7 +34642,7 @@
       <c r="H58" t="s">
         <v>294</v>
       </c>
-      <c r="AB58" t="s">
+      <c r="AA58" t="s">
         <v>516</v>
       </c>
     </row>
@@ -34461,7 +34650,7 @@
       <c r="H59" t="s">
         <v>577</v>
       </c>
-      <c r="AB59" t="s">
+      <c r="AA59" t="s">
         <v>500</v>
       </c>
     </row>
@@ -34469,7 +34658,7 @@
       <c r="H60" t="s">
         <v>295</v>
       </c>
-      <c r="AB60" t="s">
+      <c r="AA60" t="s">
         <v>123</v>
       </c>
     </row>
@@ -34477,7 +34666,7 @@
       <c r="H61" t="s">
         <v>305</v>
       </c>
-      <c r="AB61" t="s">
+      <c r="AA61" t="s">
         <v>347</v>
       </c>
     </row>
@@ -34485,7 +34674,7 @@
       <c r="H62" t="s">
         <v>314</v>
       </c>
-      <c r="AB62" t="s">
+      <c r="AA62" t="s">
         <v>494</v>
       </c>
     </row>
@@ -34493,7 +34682,7 @@
       <c r="H63" t="s">
         <v>338</v>
       </c>
-      <c r="AB63" t="s">
+      <c r="AA63" t="s">
         <v>124</v>
       </c>
     </row>
@@ -34501,7 +34690,7 @@
       <c r="H64" t="s">
         <v>311</v>
       </c>
-      <c r="AB64" t="s">
+      <c r="AA64" t="s">
         <v>125</v>
       </c>
     </row>
@@ -34509,7 +34698,7 @@
       <c r="H65" t="s">
         <v>312</v>
       </c>
-      <c r="AB65" t="s">
+      <c r="AA65" t="s">
         <v>126</v>
       </c>
     </row>
@@ -34517,7 +34706,7 @@
       <c r="H66" t="s">
         <v>370</v>
       </c>
-      <c r="AB66" t="s">
+      <c r="AA66" t="s">
         <v>127</v>
       </c>
     </row>
@@ -34525,7 +34714,7 @@
       <c r="H67" t="s">
         <v>371</v>
       </c>
-      <c r="AB67" t="s">
+      <c r="AA67" t="s">
         <v>128</v>
       </c>
     </row>
@@ -34533,7 +34722,7 @@
       <c r="H68" t="s">
         <v>346</v>
       </c>
-      <c r="AB68" t="s">
+      <c r="AA68" t="s">
         <v>129</v>
       </c>
     </row>
@@ -34541,7 +34730,7 @@
       <c r="H69" t="s">
         <v>315</v>
       </c>
-      <c r="AB69" t="s">
+      <c r="AA69" t="s">
         <v>130</v>
       </c>
     </row>
@@ -34549,7 +34738,7 @@
       <c r="H70" t="s">
         <v>270</v>
       </c>
-      <c r="AB70" t="s">
+      <c r="AA70" t="s">
         <v>473</v>
       </c>
     </row>
@@ -34557,7 +34746,7 @@
       <c r="H71" t="s">
         <v>562</v>
       </c>
-      <c r="AB71" t="s">
+      <c r="AA71" t="s">
         <v>508</v>
       </c>
     </row>
@@ -34565,7 +34754,7 @@
       <c r="H72" t="s">
         <v>316</v>
       </c>
-      <c r="AB72" t="s">
+      <c r="AA72" t="s">
         <v>206</v>
       </c>
     </row>
@@ -34573,7 +34762,7 @@
       <c r="H73" t="s">
         <v>409</v>
       </c>
-      <c r="AB73" t="s">
+      <c r="AA73" t="s">
         <v>390</v>
       </c>
     </row>
@@ -34581,7 +34770,7 @@
       <c r="H74" t="s">
         <v>306</v>
       </c>
-      <c r="AB74" t="s">
+      <c r="AA74" t="s">
         <v>478</v>
       </c>
     </row>
@@ -34589,7 +34778,7 @@
       <c r="H75" t="s">
         <v>410</v>
       </c>
-      <c r="AB75" t="s">
+      <c r="AA75" t="s">
         <v>131</v>
       </c>
     </row>
@@ -34597,7 +34786,7 @@
       <c r="H76" t="s">
         <v>263</v>
       </c>
-      <c r="AB76" t="s">
+      <c r="AA76" t="s">
         <v>132</v>
       </c>
     </row>
@@ -34605,7 +34794,7 @@
       <c r="H77" t="s">
         <v>542</v>
       </c>
-      <c r="AB77" t="s">
+      <c r="AA77" t="s">
         <v>133</v>
       </c>
     </row>
@@ -34613,7 +34802,7 @@
       <c r="H78" t="s">
         <v>345</v>
       </c>
-      <c r="AB78" t="s">
+      <c r="AA78" t="s">
         <v>134</v>
       </c>
     </row>
@@ -34621,7 +34810,7 @@
       <c r="H79" t="s">
         <v>281</v>
       </c>
-      <c r="AB79" t="s">
+      <c r="AA79" t="s">
         <v>680</v>
       </c>
     </row>
@@ -34629,7 +34818,7 @@
       <c r="H80" t="s">
         <v>287</v>
       </c>
-      <c r="AB80" t="s">
+      <c r="AA80" t="s">
         <v>189</v>
       </c>
     </row>
@@ -34637,7 +34826,7 @@
       <c r="H81" t="s">
         <v>292</v>
       </c>
-      <c r="AB81" t="s">
+      <c r="AA81" t="s">
         <v>190</v>
       </c>
     </row>
@@ -34645,7 +34834,7 @@
       <c r="H82" t="s">
         <v>464</v>
       </c>
-      <c r="AB82" t="s">
+      <c r="AA82" t="s">
         <v>489</v>
       </c>
     </row>
@@ -34653,7 +34842,7 @@
       <c r="H83" t="s">
         <v>333</v>
       </c>
-      <c r="AB83" t="s">
+      <c r="AA83" t="s">
         <v>502</v>
       </c>
     </row>
@@ -34661,7 +34850,7 @@
       <c r="H84" t="s">
         <v>271</v>
       </c>
-      <c r="AB84" t="s">
+      <c r="AA84" t="s">
         <v>135</v>
       </c>
     </row>
@@ -34669,7 +34858,7 @@
       <c r="H85" t="s">
         <v>282</v>
       </c>
-      <c r="AB85" t="s">
+      <c r="AA85" t="s">
         <v>136</v>
       </c>
     </row>
@@ -34677,7 +34866,7 @@
       <c r="H86" t="s">
         <v>288</v>
       </c>
-      <c r="AB86" t="s">
+      <c r="AA86" t="s">
         <v>137</v>
       </c>
     </row>
@@ -34685,7 +34874,7 @@
       <c r="H87" t="s">
         <v>277</v>
       </c>
-      <c r="AB87" t="s">
+      <c r="AA87" t="s">
         <v>529</v>
       </c>
     </row>
@@ -34693,7 +34882,7 @@
       <c r="H88" t="s">
         <v>563</v>
       </c>
-      <c r="AB88" t="s">
+      <c r="AA88" t="s">
         <v>138</v>
       </c>
     </row>
@@ -34701,7 +34890,7 @@
       <c r="H89" t="s">
         <v>272</v>
       </c>
-      <c r="AB89" t="s">
+      <c r="AA89" t="s">
         <v>139</v>
       </c>
     </row>
@@ -34709,7 +34898,7 @@
       <c r="H90" t="s">
         <v>289</v>
       </c>
-      <c r="AB90" t="s">
+      <c r="AA90" t="s">
         <v>191</v>
       </c>
     </row>
@@ -34717,7 +34906,7 @@
       <c r="H91" t="s">
         <v>273</v>
       </c>
-      <c r="AB91" t="s">
+      <c r="AA91" t="s">
         <v>517</v>
       </c>
     </row>
@@ -34725,7 +34914,7 @@
       <c r="H92" t="s">
         <v>274</v>
       </c>
-      <c r="AB92" t="s">
+      <c r="AA92" t="s">
         <v>599</v>
       </c>
     </row>
@@ -34733,7 +34922,7 @@
       <c r="H93" t="s">
         <v>307</v>
       </c>
-      <c r="AB93" t="s">
+      <c r="AA93" t="s">
         <v>192</v>
       </c>
     </row>
@@ -34741,7 +34930,7 @@
       <c r="H94" t="s">
         <v>313</v>
       </c>
-      <c r="AB94" t="s">
+      <c r="AA94" t="s">
         <v>488</v>
       </c>
     </row>
@@ -34749,7 +34938,7 @@
       <c r="H95" t="s">
         <v>296</v>
       </c>
-      <c r="AB95" t="s">
+      <c r="AA95" t="s">
         <v>193</v>
       </c>
     </row>
@@ -34757,7 +34946,7 @@
       <c r="H96" t="s">
         <v>341</v>
       </c>
-      <c r="AB96" t="s">
+      <c r="AA96" t="s">
         <v>194</v>
       </c>
     </row>
@@ -34765,7 +34954,7 @@
       <c r="H97" t="s">
         <v>278</v>
       </c>
-      <c r="AB97" t="s">
+      <c r="AA97" t="s">
         <v>584</v>
       </c>
     </row>
@@ -34773,272 +34962,272 @@
       <c r="H98" t="s">
         <v>279</v>
       </c>
-      <c r="AB98" t="s">
+      <c r="AA98" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="99">
-      <c r="AB99" t="s">
+      <c r="AA99" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="100">
-      <c r="AB100" t="s">
+      <c r="AA100" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="101">
-      <c r="AB101" t="s">
+      <c r="AA101" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="102">
-      <c r="AB102" t="s">
+      <c r="AA102" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="103">
-      <c r="AB103" t="s">
+      <c r="AA103" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="104">
-      <c r="AB104" t="s">
+      <c r="AA104" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="105">
-      <c r="AB105" t="s">
+      <c r="AA105" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="106">
-      <c r="AB106" t="s">
+      <c r="AA106" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="107">
-      <c r="AB107" t="s">
+      <c r="AA107" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="108">
-      <c r="AB108" t="s">
+      <c r="AA108" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="109">
-      <c r="AB109" t="s">
+      <c r="AA109" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="110">
-      <c r="AB110" t="s">
+      <c r="AA110" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="111">
-      <c r="AB111" t="s">
+      <c r="AA111" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="112">
-      <c r="AB112" t="s">
+      <c r="AA112" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="113">
-      <c r="AB113" t="s">
+      <c r="AA113" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="114">
-      <c r="AB114" t="s">
+      <c r="AA114" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="115">
-      <c r="AB115" t="s">
+      <c r="AA115" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="116">
-      <c r="AB116" t="s">
+      <c r="AA116" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="117">
-      <c r="AB117" t="s">
+      <c r="AA117" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="118">
-      <c r="AB118" t="s">
+      <c r="AA118" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="119">
-      <c r="AB119" t="s">
+      <c r="AA119" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="120">
-      <c r="AB120" t="s">
+      <c r="AA120" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="121">
-      <c r="AB121" t="s">
+      <c r="AA121" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="122">
-      <c r="AB122" t="s">
+      <c r="AA122" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="123">
-      <c r="AB123" t="s">
+      <c r="AA123" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="124">
-      <c r="AB124" t="s">
+      <c r="AA124" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="125">
-      <c r="AB125" t="s">
+      <c r="AA125" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="126">
-      <c r="AB126" t="s">
+      <c r="AA126" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="127">
-      <c r="AB127" t="s">
+      <c r="AA127" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="128">
-      <c r="AB128" t="s">
+      <c r="AA128" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="129">
-      <c r="AB129" t="s">
+      <c r="AA129" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="130">
-      <c r="AB130" t="s">
+      <c r="AA130" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="131">
-      <c r="AB131" t="s">
+      <c r="AA131" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="132">
-      <c r="AB132" t="s">
+      <c r="AA132" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="133">
-      <c r="AB133" t="s">
+      <c r="AA133" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="134">
-      <c r="AB134" t="s">
+      <c r="AA134" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="135">
-      <c r="AB135" t="s">
+      <c r="AA135" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="136">
-      <c r="AB136" t="s">
+      <c r="AA136" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="137">
-      <c r="AB137" t="s">
+      <c r="AA137" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="138">
-      <c r="AB138" t="s">
+      <c r="AA138" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="139">
-      <c r="AB139" t="s">
+      <c r="AA139" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="140">
-      <c r="AB140" t="s">
+      <c r="AA140" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="141">
-      <c r="AB141" t="s">
+      <c r="AA141" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="142">
-      <c r="AB142" t="s">
+      <c r="AA142" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="143">
-      <c r="AB143" t="s">
+      <c r="AA143" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="144">
-      <c r="AB144" t="s">
+      <c r="AA144" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="145">
-      <c r="AB145" t="s">
+      <c r="AA145" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="146">
-      <c r="AB146" t="s">
+      <c r="AA146" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="147">
-      <c r="AB147" t="s">
+      <c r="AA147" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="148">
-      <c r="AB148" t="s">
+      <c r="AA148" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="149">
-      <c r="AB149" t="s">
+      <c r="AA149" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="150">
-      <c r="AB150" t="s">
+      <c r="AA150" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="151">
-      <c r="AB151" t="s">
+      <c r="AA151" t="s">
         <v>640</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed invalid activity names
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28410" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29010" uniqueCount="685">
   <si>
     <t>description</t>
   </si>
@@ -2133,7 +2133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="843" x14ac:knownFonts="1">
+  <fonts count="860" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7457,8 +7457,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1425">
+  <fills count="1449">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15119,6 +15226,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="E6E6E6"/>
         <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -30257,7 +30500,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="854">
+  <cellXfs count="871">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -32774,55 +33017,106 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1397" fontId="825" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="826" fillId="1403" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="827" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1403" fontId="826" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="827" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="828" fillId="1406" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1406" fontId="828" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="829" fillId="1409" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1409" fontId="829" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="830" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1412" fontId="830" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="831" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="831" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="832" fillId="1415" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1415" fontId="832" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="833" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="834" fillId="1418" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="833" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1418" fontId="834" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="835" fillId="1421" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1421" fontId="835" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="836" fillId="1409" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1409" fontId="836" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="837" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="838" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="839" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="840" fillId="1424" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="841" fillId="1412" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="842" fillId="1421" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="837" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="838" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1412" fontId="839" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1424" fontId="840" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1412" fontId="841" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1421" fontId="842" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="843" fillId="1427" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="844" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="845" fillId="1430" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="846" fillId="1433" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="847" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="848" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="849" fillId="1439" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="850" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="851" fillId="1442" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="852" fillId="1445" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="853" fillId="1433" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="854" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="855" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="856" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="857" fillId="1448" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="858" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="859" fillId="1445" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[word] - [`extractText(var,file)`]: *NEW* command to extract text from a Word document. - [`readOnly(file,password)`]: *NEW* command to restrict update access on a Word document. - [`removeProtection(file)`]: *NEW* command to remove update restriction from a Word document.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
+++ b/src/test/resources/showcase/artifact/script/base-showcase-macro.xlsx
@@ -27,15 +27,15 @@
     <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
-    <definedName name="io">'#system'!$L$2:$L$31</definedName>
+    <definedName name="io">'#system'!$L$2:$L$32</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
-    <definedName name="mail">'#system'!$Q$2:$Q$2</definedName>
+    <definedName name="mail">'#system'!$Q$2:$Q$5</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$18</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$21</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$9</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29010" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29617" uniqueCount="692">
   <si>
     <t>description</t>
   </si>
@@ -2126,6 +2126,27 @@
   </si>
   <si>
     <t>openFile(filePath)</t>
+  </si>
+  <si>
+    <t>checksum(var,file)</t>
+  </si>
+  <si>
+    <t>clearComposed(var)</t>
+  </si>
+  <si>
+    <t>compose(var,config,value)</t>
+  </si>
+  <si>
+    <t>sendComposed(profile,var)</t>
+  </si>
+  <si>
+    <t>ocr(pdf,saveTo)</t>
+  </si>
+  <si>
+    <t>savePageCount(pdf,var)</t>
+  </si>
+  <si>
+    <t>split(pdf,saveTo)</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2154,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="860" x14ac:knownFonts="1">
+  <fonts count="877" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7564,8 +7585,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1449">
+  <fills count="1473">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15226,6 +15354,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="E6E6E6"/>
         <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -30500,7 +30764,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="871">
+  <cellXfs count="888">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -33068,55 +33332,106 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1421" fontId="842" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="843" fillId="1427" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="844" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1427" fontId="843" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="844" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="845" fillId="1430" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1430" fontId="845" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="846" fillId="1433" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1433" fontId="846" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="847" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1436" fontId="847" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="848" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="848" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="849" fillId="1439" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1439" fontId="849" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="850" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="851" fillId="1442" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="850" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1442" fontId="851" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="852" fillId="1445" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1445" fontId="852" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="853" fillId="1433" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1433" fontId="853" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="854" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="855" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="856" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="857" fillId="1448" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="858" fillId="1436" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="859" fillId="1445" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="854" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="855" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1436" fontId="856" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1448" fontId="857" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1436" fontId="858" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1445" fontId="859" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="860" fillId="1451" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="861" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="862" fillId="1454" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="863" fillId="1457" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="864" fillId="1460" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="865" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="866" fillId="1463" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="867" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="868" fillId="1466" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="869" fillId="1469" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="870" fillId="1457" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="871" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="872" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="873" fillId="1460" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="874" fillId="1472" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="875" fillId="1460" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="876" fillId="1469" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -33571,7 +33886,7 @@
         <v>513</v>
       </c>
       <c r="Q2" t="s">
-        <v>412</v>
+        <v>686</v>
       </c>
       <c r="R2" t="s">
         <v>466</v>
@@ -33665,6 +33980,9 @@
       <c r="P3" t="s">
         <v>514</v>
       </c>
+      <c r="Q3" t="s">
+        <v>687</v>
+      </c>
       <c r="R3" t="s">
         <v>467</v>
       </c>
@@ -33751,6 +34069,9 @@
       <c r="P4" t="s">
         <v>515</v>
       </c>
+      <c r="Q4" t="s">
+        <v>412</v>
+      </c>
       <c r="R4" t="s">
         <v>19</v>
       </c>
@@ -33831,6 +34152,9 @@
       <c r="O5" t="s">
         <v>558</v>
       </c>
+      <c r="Q5" t="s">
+        <v>688</v>
+      </c>
       <c r="R5" t="s">
         <v>23</v>
       </c>
@@ -33962,7 +34286,7 @@
         <v>349</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>685</v>
       </c>
       <c r="N7" t="s">
         <v>317</v>
@@ -34024,7 +34348,7 @@
         <v>564</v>
       </c>
       <c r="L8" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="N8" t="s">
         <v>27</v>
@@ -34083,7 +34407,7 @@
         <v>330</v>
       </c>
       <c r="L9" t="s">
-        <v>538</v>
+        <v>12</v>
       </c>
       <c r="N9" t="s">
         <v>28</v>
@@ -34133,7 +34457,7 @@
         <v>601</v>
       </c>
       <c r="L10" t="s">
-        <v>72</v>
+        <v>538</v>
       </c>
       <c r="N10" t="s">
         <v>29</v>
@@ -34177,7 +34501,7 @@
         <v>602</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="N11" t="s">
         <v>507</v>
@@ -34215,7 +34539,7 @@
         <v>487</v>
       </c>
       <c r="L12" t="s">
-        <v>539</v>
+        <v>31</v>
       </c>
       <c r="N12" t="s">
         <v>565</v>
@@ -34253,7 +34577,7 @@
         <v>323</v>
       </c>
       <c r="L13" t="s">
-        <v>391</v>
+        <v>539</v>
       </c>
       <c r="N13" t="s">
         <v>476</v>
@@ -34265,7 +34589,7 @@
         <v>86</v>
       </c>
       <c r="S13" t="s">
-        <v>240</v>
+        <v>689</v>
       </c>
       <c r="AA13" t="s">
         <v>327</v>
@@ -34291,7 +34615,7 @@
         <v>324</v>
       </c>
       <c r="L14" t="s">
-        <v>13</v>
+        <v>391</v>
       </c>
       <c r="N14" t="s">
         <v>506</v>
@@ -34300,7 +34624,7 @@
         <v>87</v>
       </c>
       <c r="S14" t="s">
-        <v>605</v>
+        <v>240</v>
       </c>
       <c r="AA14" t="s">
         <v>95</v>
@@ -34326,7 +34650,7 @@
         <v>325</v>
       </c>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="N15" t="s">
         <v>32</v>
@@ -34335,7 +34659,7 @@
         <v>533</v>
       </c>
       <c r="S15" t="s">
-        <v>245</v>
+        <v>605</v>
       </c>
       <c r="AA15" t="s">
         <v>629</v>
@@ -34361,7 +34685,7 @@
         <v>326</v>
       </c>
       <c r="L16" t="s">
-        <v>540</v>
+        <v>35</v>
       </c>
       <c r="N16" t="s">
         <v>578</v>
@@ -34370,7 +34694,7 @@
         <v>534</v>
       </c>
       <c r="S16" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AA16" t="s">
         <v>611</v>
@@ -34393,13 +34717,13 @@
         <v>319</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>540</v>
       </c>
       <c r="N17" t="s">
         <v>33</v>
       </c>
       <c r="S17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AA17" t="s">
         <v>96</v>
@@ -34422,13 +34746,13 @@
         <v>81</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N18" t="s">
         <v>36</v>
       </c>
       <c r="S18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AA18" t="s">
         <v>67</v>
@@ -34448,7 +34772,10 @@
         <v>82</v>
       </c>
       <c r="L19" t="s">
-        <v>491</v>
+        <v>74</v>
+      </c>
+      <c r="S19" t="s">
+        <v>690</v>
       </c>
       <c r="AA19" t="s">
         <v>535</v>
@@ -34468,7 +34795,10 @@
         <v>297</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>491</v>
+      </c>
+      <c r="S20" t="s">
+        <v>243</v>
       </c>
       <c r="AA20" t="s">
         <v>97</v>
@@ -34488,7 +34818,10 @@
         <v>298</v>
       </c>
       <c r="L21" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="S21" t="s">
+        <v>691</v>
       </c>
       <c r="AA21" t="s">
         <v>98</v>
@@ -34508,7 +34841,7 @@
         <v>299</v>
       </c>
       <c r="L22" t="s">
-        <v>593</v>
+        <v>76</v>
       </c>
       <c r="AA22" t="s">
         <v>99</v>
@@ -34528,7 +34861,7 @@
         <v>300</v>
       </c>
       <c r="L23" t="s">
-        <v>505</v>
+        <v>593</v>
       </c>
       <c r="AA23" t="s">
         <v>100</v>
@@ -34548,7 +34881,7 @@
         <v>291</v>
       </c>
       <c r="L24" t="s">
-        <v>37</v>
+        <v>505</v>
       </c>
       <c r="AA24" t="s">
         <v>518</v>
@@ -34568,7 +34901,7 @@
         <v>280</v>
       </c>
       <c r="L25" t="s">
-        <v>393</v>
+        <v>37</v>
       </c>
       <c r="AA25" t="s">
         <v>102</v>
@@ -34588,7 +34921,7 @@
         <v>68</v>
       </c>
       <c r="L26" t="s">
-        <v>643</v>
+        <v>393</v>
       </c>
       <c r="AA26" t="s">
         <v>579</v>
@@ -34608,7 +34941,7 @@
         <v>283</v>
       </c>
       <c r="L27" t="s">
-        <v>557</v>
+        <v>643</v>
       </c>
       <c r="AA27" t="s">
         <v>103</v>
@@ -34628,7 +34961,7 @@
         <v>267</v>
       </c>
       <c r="L28" t="s">
-        <v>77</v>
+        <v>557</v>
       </c>
       <c r="AA28" t="s">
         <v>104</v>
@@ -34645,7 +34978,7 @@
         <v>284</v>
       </c>
       <c r="L29" t="s">
-        <v>475</v>
+        <v>77</v>
       </c>
       <c r="AA29" t="s">
         <v>105</v>
@@ -34662,7 +34995,7 @@
         <v>285</v>
       </c>
       <c r="L30" t="s">
-        <v>38</v>
+        <v>475</v>
       </c>
       <c r="AA30" t="s">
         <v>106</v>
@@ -34679,7 +35012,7 @@
         <v>208</v>
       </c>
       <c r="L31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA31" t="s">
         <v>328</v>
@@ -34694,6 +35027,9 @@
       </c>
       <c r="H32" t="s">
         <v>276</v>
+      </c>
+      <c r="L32" t="s">
+        <v>39</v>
       </c>
       <c r="AA32" t="s">
         <v>107</v>

</xml_diff>